<commit_message>
Update stubble sim.xls using latest data from Property_GSW.xl Unexplained increase in profit of $55500. Unexplained because not sure what data/code changes have been made since sim last run.
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.05988132675614952</v>
+        <v>0.05891273035340159</v>
       </c>
       <c r="B1">
-        <v>0.2767500477278779</v>
+        <v>0.2870057404054701</v>
       </c>
       <c r="C1">
-        <v>0.07471151065916186</v>
+        <v>0.07350303208347805</v>
       </c>
       <c r="D1">
-        <v>0.05988132675614952</v>
+        <v>0.05891273035340159</v>
       </c>
       <c r="E1">
-        <v>0.2767500477278779</v>
+        <v>0.2870057404054701</v>
       </c>
       <c r="F1">
-        <v>0.07471151065916186</v>
+        <v>0.07350303208347805</v>
       </c>
       <c r="G1">
-        <v>0.0521744500435975</v>
+        <v>0.0504892938067427</v>
       </c>
       <c r="H1">
-        <v>0.2574457951240353</v>
+        <v>0.2669861185227384</v>
       </c>
       <c r="I1">
-        <v>0.08103691176984291</v>
+        <v>0.07841954144451525</v>
       </c>
       <c r="J1">
-        <v>0.00914922352952397</v>
+        <v>0.009001232403096171</v>
       </c>
       <c r="K1">
-        <v>0.0517739155603892</v>
+        <v>0.05369253263403487</v>
       </c>
       <c r="L1">
-        <v>0.01397689892382598</v>
+        <v>0.01375081886260223</v>
       </c>
       <c r="M1">
-        <v>0.0521744500435975</v>
+        <v>0.0504892938067427</v>
       </c>
       <c r="N1">
-        <v>0.2574457951240353</v>
+        <v>0.2669861185227384</v>
       </c>
       <c r="O1">
-        <v>0.08103691176984291</v>
+        <v>0.07841954144451525</v>
       </c>
       <c r="P1">
-        <v>0.0521744500435975</v>
+        <v>0.0504892938067427</v>
       </c>
       <c r="Q1">
-        <v>0.2574457951240353</v>
+        <v>0.2669861185227384</v>
       </c>
       <c r="R1">
-        <v>0.08103691176984291</v>
+        <v>0.07841954144451525</v>
       </c>
       <c r="S1">
-        <v>0.0521744500435975</v>
+        <v>0.0504892938067427</v>
       </c>
       <c r="T1">
-        <v>0.2574457951240353</v>
+        <v>0.2669861185227384</v>
       </c>
       <c r="U1">
-        <v>0.08103691176984291</v>
+        <v>0.07841954144451525</v>
       </c>
       <c r="V1">
-        <v>0.05115735724039348</v>
+        <v>0.05032987336718341</v>
       </c>
       <c r="W1">
-        <v>0.251590952479889</v>
+        <v>0.2609143094595183</v>
       </c>
       <c r="X1">
-        <v>0.06791955514469261</v>
+        <v>0.06682093825770732</v>
       </c>
       <c r="Y1">
-        <v>0.05115735724039348</v>
+        <v>0.05032987336718341</v>
       </c>
       <c r="Z1">
-        <v>0.251590952479889</v>
+        <v>0.2609143094595183</v>
       </c>
       <c r="AA1">
-        <v>0.06791955514469261</v>
+        <v>0.06682093825770732</v>
       </c>
       <c r="AB1">
-        <v>0.05115592128470829</v>
+        <v>0.05032846063846373</v>
       </c>
       <c r="AC1">
-        <v>0.2515838904759458</v>
+        <v>0.260906985754655</v>
       </c>
       <c r="AD1">
-        <v>0.06791764868437865</v>
+        <v>0.06681906263489652</v>
       </c>
       <c r="AE1">
-        <v>0.04244178852572304</v>
+        <v>0.04107098261252931</v>
       </c>
       <c r="AF1">
-        <v>0.2312244641391799</v>
+        <v>0.2397930879324596</v>
       </c>
       <c r="AG1">
-        <v>0.0727831522377293</v>
+        <v>0.07043236592701835</v>
       </c>
       <c r="AH1">
-        <v>0.04244178852572304</v>
+        <v>0.04107098261252931</v>
       </c>
       <c r="AI1">
-        <v>0.2312244641391799</v>
+        <v>0.2397930879324596</v>
       </c>
       <c r="AJ1">
-        <v>0.0727831522377293</v>
+        <v>0.07043236592701835</v>
       </c>
       <c r="AK1">
-        <v>0.0521744500435975</v>
+        <v>0.0504892938067427</v>
       </c>
       <c r="AL1">
-        <v>0.2574457951240353</v>
+        <v>0.2669861185227384</v>
       </c>
       <c r="AM1">
-        <v>0.08103691176984291</v>
+        <v>0.07841954144451525</v>
       </c>
       <c r="AN1">
-        <v>0.05538384081940814</v>
+        <v>0.05448799244907232</v>
       </c>
       <c r="AO1">
-        <v>0.2641705001038834</v>
+        <v>0.2739600249324942</v>
       </c>
       <c r="AP1">
-        <v>0.07131553290192723</v>
+        <v>0.07016198517059269</v>
       </c>
       <c r="AQ1">
-        <v>0.05538384081940814</v>
+        <v>0.05448799244907232</v>
       </c>
       <c r="AR1">
-        <v>0.2641705001038834</v>
+        <v>0.2739600249324942</v>
       </c>
       <c r="AS1">
-        <v>0.07131553290192723</v>
+        <v>0.07016198517059269</v>
       </c>
       <c r="AT1">
-        <v>0.04244178852572304</v>
+        <v>0.04107098261252931</v>
       </c>
       <c r="AU1">
-        <v>0.2312244641391799</v>
+        <v>0.2397930879324596</v>
       </c>
       <c r="AV1">
-        <v>0.0727831522377293</v>
+        <v>0.07043236592701835</v>
       </c>
       <c r="AW1">
-        <v>0.04244178852572304</v>
+        <v>0.04107098261252931</v>
       </c>
       <c r="AX1">
-        <v>0.2312244641391799</v>
+        <v>0.2397930879324596</v>
       </c>
       <c r="AY1">
-        <v>0.0727831522377293</v>
+        <v>0.07043236592701835</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.0126434043002024</v>
+        <v>0.01756326854460394</v>
       </c>
       <c r="B2">
-        <v>0.0251590952479889</v>
+        <v>0.03592642471042405</v>
       </c>
       <c r="C2">
-        <v>0.01577466442901848</v>
+        <v>0.02191298015862926</v>
       </c>
       <c r="D2">
-        <v>0.0126434043002024</v>
+        <v>0.01756326854460394</v>
       </c>
       <c r="E2">
-        <v>0.0251590952479889</v>
+        <v>0.03592642471042405</v>
       </c>
       <c r="F2">
-        <v>0.01577466442901848</v>
+        <v>0.02191298015862926</v>
       </c>
       <c r="G2">
-        <v>0.01893955208721895</v>
+        <v>0.01999642032776401</v>
       </c>
       <c r="H2">
-        <v>0.02340416319309412</v>
+        <v>0.03342043497905139</v>
       </c>
       <c r="I2">
-        <v>0.02941675111419113</v>
+        <v>0.0310582698707824</v>
       </c>
       <c r="J2">
-        <v>0.001931776371418104</v>
+        <v>0.002683478782592881</v>
       </c>
       <c r="K2">
-        <v>0.004706719596399019</v>
+        <v>0.006721052786134014</v>
       </c>
       <c r="L2">
-        <v>0.002951096669528083</v>
+        <v>0.004099442055109974</v>
       </c>
       <c r="M2">
-        <v>0.01893955208721895</v>
+        <v>0.01999642032776401</v>
       </c>
       <c r="N2">
-        <v>0.02340416319309412</v>
+        <v>0.03342043497905139</v>
       </c>
       <c r="O2">
-        <v>0.02941675111419113</v>
+        <v>0.0310582698707824</v>
       </c>
       <c r="P2">
-        <v>0.01893955208721895</v>
+        <v>0.01999642032776401</v>
       </c>
       <c r="Q2">
-        <v>0.02340416319309412</v>
+        <v>0.03342043497905139</v>
       </c>
       <c r="R2">
-        <v>0.02941675111419113</v>
+        <v>0.0310582698707824</v>
       </c>
       <c r="S2">
-        <v>0.01893955208721895</v>
+        <v>0.01999642032776401</v>
       </c>
       <c r="T2">
-        <v>0.02340416319309412</v>
+        <v>0.03342043497905139</v>
       </c>
       <c r="U2">
-        <v>0.02941675111419113</v>
+        <v>0.0310582698707824</v>
       </c>
       <c r="V2">
-        <v>0.01080141649422886</v>
+        <v>0.01500451729976071</v>
       </c>
       <c r="W2">
-        <v>0.022871904770899</v>
+        <v>0.03266038610038551</v>
       </c>
       <c r="X2">
-        <v>0.01434060402638044</v>
+        <v>0.01992089105329933</v>
       </c>
       <c r="Y2">
-        <v>0.01080141649422886</v>
+        <v>0.01500451729976071</v>
       </c>
       <c r="Z2">
-        <v>0.022871904770899</v>
+        <v>0.03266038610038551</v>
       </c>
       <c r="AA2">
-        <v>0.01434060402638044</v>
+        <v>0.01992089105329933</v>
       </c>
       <c r="AB2">
-        <v>0.01080111330508345</v>
+        <v>0.01500409613214999</v>
       </c>
       <c r="AC2">
-        <v>0.02287126277054053</v>
+        <v>0.0326594693433513</v>
       </c>
       <c r="AD2">
-        <v>0.01434020149440867</v>
+        <v>0.01992033188608849</v>
       </c>
       <c r="AE2">
-        <v>0.01540655366344975</v>
+        <v>0.01626627290011224</v>
       </c>
       <c r="AF2">
-        <v>0.02102040583083454</v>
+        <v>0.0300165017867406</v>
       </c>
       <c r="AG2">
-        <v>0.02642060053774574</v>
+        <v>0.02789492756912864</v>
       </c>
       <c r="AH2">
-        <v>0.01540655366344975</v>
+        <v>0.01626627290011224</v>
       </c>
       <c r="AI2">
-        <v>0.02102040583083454</v>
+        <v>0.0300165017867406</v>
       </c>
       <c r="AJ2">
-        <v>0.02642060053774574</v>
+        <v>0.02789492756912864</v>
       </c>
       <c r="AK2">
-        <v>0.01893955208721895</v>
+        <v>0.01999642032776401</v>
       </c>
       <c r="AL2">
-        <v>0.02340416319309412</v>
+        <v>0.03342043497905139</v>
       </c>
       <c r="AM2">
-        <v>0.02941675111419113</v>
+        <v>0.0310582698707824</v>
       </c>
       <c r="AN2">
-        <v>0.01169380054034823</v>
+        <v>0.01624415025578853</v>
       </c>
       <c r="AO2">
-        <v>0.02401550000944395</v>
+        <v>0.03429340540540477</v>
       </c>
       <c r="AP2">
-        <v>0.01505763422769946</v>
+        <v>0.02091693560596429</v>
       </c>
       <c r="AQ2">
-        <v>0.01169380054034823</v>
+        <v>0.01624415025578853</v>
       </c>
       <c r="AR2">
-        <v>0.02401550000944395</v>
+        <v>0.03429340540540477</v>
       </c>
       <c r="AS2">
-        <v>0.01505763422769946</v>
+        <v>0.02091693560596429</v>
       </c>
       <c r="AT2">
-        <v>0.01540655366344975</v>
+        <v>0.01626627290011224</v>
       </c>
       <c r="AU2">
-        <v>0.02102040583083454</v>
+        <v>0.0300165017867406</v>
       </c>
       <c r="AV2">
-        <v>0.02642060053774574</v>
+        <v>0.02789492756912864</v>
       </c>
       <c r="AW2">
-        <v>0.01540655366344975</v>
+        <v>0.01626627290011224</v>
       </c>
       <c r="AX2">
-        <v>0.02102040583083454</v>
+        <v>0.0300165017867406</v>
       </c>
       <c r="AY2">
-        <v>0.02642060053774574</v>
+        <v>0.02789492756912864</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.02064126044938914</v>
+        <v>0.01460385865728181</v>
       </c>
       <c r="B3">
-        <v>0.03432010394244681</v>
+        <v>0.0368205150526488</v>
       </c>
       <c r="C3">
-        <v>0.02575326622876977</v>
+        <v>0.01822064407793628</v>
       </c>
       <c r="D3">
-        <v>0.02064126044938914</v>
+        <v>0.01460385865728181</v>
       </c>
       <c r="E3">
-        <v>0.03432010394244681</v>
+        <v>0.0368205150526488</v>
       </c>
       <c r="F3">
-        <v>0.02575326622876977</v>
+        <v>0.01822064407793628</v>
       </c>
       <c r="G3">
-        <v>0.02039971166164056</v>
+        <v>0.01857346232618267</v>
       </c>
       <c r="H3">
-        <v>0.03192616052189654</v>
+        <v>0.03425215949348797</v>
       </c>
       <c r="I3">
-        <v>0.03168465853829278</v>
+        <v>0.02884814361300712</v>
       </c>
       <c r="J3">
-        <v>0.003153762884239861</v>
+        <v>0.002231312739498103</v>
       </c>
       <c r="K3">
-        <v>0.006420545102442743</v>
+        <v>0.006888317645749215</v>
       </c>
       <c r="L3">
-        <v>0.004817876065711105</v>
+        <v>0.003408686270126889</v>
       </c>
       <c r="M3">
-        <v>0.02039971166164056</v>
+        <v>0.01857346232618267</v>
       </c>
       <c r="N3">
-        <v>0.03192616052189654</v>
+        <v>0.03425215949348797</v>
       </c>
       <c r="O3">
-        <v>0.03168465853829278</v>
+        <v>0.02884814361300712</v>
       </c>
       <c r="P3">
-        <v>0.02039971166164056</v>
+        <v>0.01857346232618267</v>
       </c>
       <c r="Q3">
-        <v>0.03192616052189654</v>
+        <v>0.03425215949348797</v>
       </c>
       <c r="R3">
-        <v>0.03168465853829278</v>
+        <v>0.02884814361300712</v>
       </c>
       <c r="S3">
-        <v>0.02039971166164056</v>
+        <v>0.01857346232618267</v>
       </c>
       <c r="T3">
-        <v>0.03192616052189654</v>
+        <v>0.03425215949348797</v>
       </c>
       <c r="U3">
-        <v>0.03168465853829278</v>
+        <v>0.02884814361300712</v>
       </c>
       <c r="V3">
-        <v>0.01763408381049212</v>
+        <v>0.01247625687154728</v>
       </c>
       <c r="W3">
-        <v>0.03120009449313346</v>
+        <v>0.033473195502408</v>
       </c>
       <c r="X3">
-        <v>0.02341206020797252</v>
+        <v>0.01656422188903298</v>
       </c>
       <c r="Y3">
-        <v>0.01763408381049212</v>
+        <v>0.01247625687154728</v>
       </c>
       <c r="Z3">
-        <v>0.03120009449313346</v>
+        <v>0.033473195502408</v>
       </c>
       <c r="AA3">
-        <v>0.02341206020797252</v>
+        <v>0.01656422188903298</v>
       </c>
       <c r="AB3">
-        <v>0.01763358883255998</v>
+        <v>0.01247590667065828</v>
       </c>
       <c r="AC3">
-        <v>0.03119921872559029</v>
+        <v>0.03347225593031171</v>
       </c>
       <c r="AD3">
-        <v>0.02341140304578176</v>
+        <v>0.01656375694146971</v>
       </c>
       <c r="AE3">
-        <v>0.01659433396242037</v>
+        <v>0.01510875456434375</v>
       </c>
       <c r="AF3">
-        <v>0.0286744219502219</v>
+        <v>0.03076351361915124</v>
       </c>
       <c r="AG3">
-        <v>0.02845751739087408</v>
+        <v>0.02590990676353418</v>
       </c>
       <c r="AH3">
-        <v>0.01659433396242037</v>
+        <v>0.01510875456434375</v>
       </c>
       <c r="AI3">
-        <v>0.0286744219502219</v>
+        <v>0.03076351361915124</v>
       </c>
       <c r="AJ3">
-        <v>0.02845751739087408</v>
+        <v>0.02590990676353418</v>
       </c>
       <c r="AK3">
-        <v>0.02039971166164056</v>
+        <v>0.01857346232618267</v>
       </c>
       <c r="AL3">
-        <v>0.03192616052189654</v>
+        <v>0.03425215949348797</v>
       </c>
       <c r="AM3">
-        <v>0.03168465853829278</v>
+        <v>0.02884814361300712</v>
       </c>
       <c r="AN3">
-        <v>0.01909096449543033</v>
+        <v>0.01350701173535654</v>
       </c>
       <c r="AO3">
-        <v>0.03276009921779013</v>
+        <v>0.0351468552775284</v>
       </c>
       <c r="AP3">
-        <v>0.02458266321837114</v>
+        <v>0.01739243298348463</v>
       </c>
       <c r="AQ3">
-        <v>0.01909096449543033</v>
+        <v>0.01350701173535654</v>
       </c>
       <c r="AR3">
-        <v>0.03276009921779013</v>
+        <v>0.0351468552775284</v>
       </c>
       <c r="AS3">
-        <v>0.02458266321837114</v>
+        <v>0.01739243298348463</v>
       </c>
       <c r="AT3">
-        <v>0.01659433396242037</v>
+        <v>0.01510875456434375</v>
       </c>
       <c r="AU3">
-        <v>0.0286744219502219</v>
+        <v>0.03076351361915124</v>
       </c>
       <c r="AV3">
-        <v>0.02845751739087408</v>
+        <v>0.02590990676353418</v>
       </c>
       <c r="AW3">
-        <v>0.01659433396242037</v>
+        <v>0.01510875456434375</v>
       </c>
       <c r="AX3">
-        <v>0.0286744219502219</v>
+        <v>0.03076351361915124</v>
       </c>
       <c r="AY3">
-        <v>0.02845751739087408</v>
+        <v>0.02590990676353418</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.01843537451228727</v>
+        <v>0.02380038338468012</v>
       </c>
       <c r="B4">
-        <v>0.03515292291467025</v>
+        <v>0.03771460539487354</v>
       </c>
       <c r="C4">
-        <v>0.02300107151916011</v>
+        <v>0.02969477620590728</v>
       </c>
       <c r="D4">
-        <v>0.01843537451228727</v>
+        <v>0.02380038338468012</v>
       </c>
       <c r="E4">
-        <v>0.03515292291467025</v>
+        <v>0.03771460539487354</v>
       </c>
       <c r="F4">
-        <v>0.02300107151916011</v>
+        <v>0.02969477620590728</v>
       </c>
       <c r="G4">
-        <v>0.02194479730016959</v>
+        <v>0.02636481726938018</v>
       </c>
       <c r="H4">
-        <v>0.03270088755178767</v>
+        <v>0.03508388400792455</v>
       </c>
       <c r="I4">
-        <v>0.03408447240239106</v>
+        <v>0.04094960980137772</v>
       </c>
       <c r="J4">
-        <v>0.002816727206968299</v>
+        <v>0.003636442935901455</v>
       </c>
       <c r="K4">
-        <v>0.00657634742117399</v>
+        <v>0.007055582505364415</v>
       </c>
       <c r="L4">
-        <v>0.00430300028638987</v>
+        <v>0.005555246868036689</v>
       </c>
       <c r="M4">
-        <v>0.02194479730016959</v>
+        <v>0.02636481726938018</v>
       </c>
       <c r="N4">
-        <v>0.03270088755178767</v>
+        <v>0.03508388400792455</v>
       </c>
       <c r="O4">
-        <v>0.03408447240239106</v>
+        <v>0.04094960980137772</v>
       </c>
       <c r="P4">
-        <v>0.02194479730016959</v>
+        <v>0.02636481726938018</v>
       </c>
       <c r="Q4">
-        <v>0.03270088755178767</v>
+        <v>0.03508388400792455</v>
       </c>
       <c r="R4">
-        <v>0.03408447240239106</v>
+        <v>0.04094960980137772</v>
       </c>
       <c r="S4">
-        <v>0.02194479730016959</v>
+        <v>0.02636481726938018</v>
       </c>
       <c r="T4">
-        <v>0.03270088755178767</v>
+        <v>0.03508388400792455</v>
       </c>
       <c r="U4">
-        <v>0.03408447240239106</v>
+        <v>0.04094960980137772</v>
       </c>
       <c r="V4">
-        <v>0.01574956820222211</v>
+        <v>0.02033296156290272</v>
       </c>
       <c r="W4">
-        <v>0.03195720264970024</v>
+        <v>0.0342860049044305</v>
       </c>
       <c r="X4">
-        <v>0.02091006501741828</v>
+        <v>0.02699525109627935</v>
       </c>
       <c r="Y4">
-        <v>0.01574956820222211</v>
+        <v>0.02033296156290272</v>
       </c>
       <c r="Z4">
-        <v>0.03195720264970024</v>
+        <v>0.0342860049044305</v>
       </c>
       <c r="AA4">
-        <v>0.02091006501741828</v>
+        <v>0.02699525109627935</v>
       </c>
       <c r="AB4">
-        <v>0.01574912612148887</v>
+        <v>0.02033239082912506</v>
       </c>
       <c r="AC4">
-        <v>0.03195630563059481</v>
+        <v>0.03428504251727212</v>
       </c>
       <c r="AD4">
-        <v>0.02090947808470011</v>
+        <v>0.02699449335611496</v>
       </c>
       <c r="AE4">
-        <v>0.01785119815303061</v>
+        <v>0.02144670424185289</v>
       </c>
       <c r="AF4">
-        <v>0.02937024159743893</v>
+        <v>0.03151052545156188</v>
       </c>
       <c r="AG4">
-        <v>0.0306129057688142</v>
+        <v>0.03677881621049666</v>
       </c>
       <c r="AH4">
-        <v>0.01785119815303061</v>
+        <v>0.02144670424185289</v>
       </c>
       <c r="AI4">
-        <v>0.02937024159743893</v>
+        <v>0.03151052545156188</v>
       </c>
       <c r="AJ4">
-        <v>0.0306129057688142</v>
+        <v>0.03677881621049666</v>
       </c>
       <c r="AK4">
-        <v>0.02194479730016959</v>
+        <v>0.02636481726938018</v>
       </c>
       <c r="AL4">
-        <v>0.03270088755178767</v>
+        <v>0.03508388400792455</v>
       </c>
       <c r="AM4">
-        <v>0.03408447240239106</v>
+        <v>0.04094960980137772</v>
       </c>
       <c r="AN4">
-        <v>0.01705075526453391</v>
+        <v>0.02201281628554834</v>
       </c>
       <c r="AO4">
-        <v>0.03355506278218524</v>
+        <v>0.03600030514965202</v>
       </c>
       <c r="AP4">
-        <v>0.0219555682682892</v>
+        <v>0.02834501365109331</v>
       </c>
       <c r="AQ4">
-        <v>0.01705075526453391</v>
+        <v>0.02201281628554834</v>
       </c>
       <c r="AR4">
-        <v>0.03355506278218524</v>
+        <v>0.03600030514965202</v>
       </c>
       <c r="AS4">
-        <v>0.0219555682682892</v>
+        <v>0.02834501365109331</v>
       </c>
       <c r="AT4">
-        <v>0.01785119815303061</v>
+        <v>0.02144670424185289</v>
       </c>
       <c r="AU4">
-        <v>0.02937024159743893</v>
+        <v>0.03151052545156188</v>
       </c>
       <c r="AV4">
-        <v>0.0306129057688142</v>
+        <v>0.03677881621049666</v>
       </c>
       <c r="AW4">
-        <v>0.01785119815303061</v>
+        <v>0.02144670424185289</v>
       </c>
       <c r="AX4">
-        <v>0.02937024159743893</v>
+        <v>0.03151052545156188</v>
       </c>
       <c r="AY4">
-        <v>0.0306129057688142</v>
+        <v>0.03677881621049666</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.01953414552244474</v>
+        <v>0.02123983564831252</v>
       </c>
       <c r="B5">
-        <v>0.03598574188689369</v>
+        <v>0.0386086957370983</v>
       </c>
       <c r="C5">
-        <v>0.02437196369013105</v>
+        <v>0.02650008430674565</v>
       </c>
       <c r="D5">
-        <v>0.01953414552244474</v>
+        <v>0.02123983564831252</v>
       </c>
       <c r="E5">
-        <v>0.03598574188689369</v>
+        <v>0.0386086957370983</v>
       </c>
       <c r="F5">
-        <v>0.02437196369013105</v>
+        <v>0.02650008430674565</v>
       </c>
       <c r="G5">
-        <v>0.02374497521172172</v>
+        <v>0.02856714344291116</v>
       </c>
       <c r="H5">
-        <v>0.0334756145816788</v>
+        <v>0.03591560852236114</v>
       </c>
       <c r="I5">
-        <v>0.03688049341395075</v>
+        <v>0.04437024407090457</v>
       </c>
       <c r="J5">
-        <v>0.002984607615173503</v>
+        <v>0.003245218745204344</v>
       </c>
       <c r="K5">
-        <v>0.006732149739905238</v>
+        <v>0.007222847364979616</v>
       </c>
       <c r="L5">
-        <v>0.00455946439935016</v>
+        <v>0.004957589487354721</v>
       </c>
       <c r="M5">
-        <v>0.02374497521172172</v>
+        <v>0.02856714344291116</v>
       </c>
       <c r="N5">
-        <v>0.0334756145816788</v>
+        <v>0.03591560852236114</v>
       </c>
       <c r="O5">
-        <v>0.03688049341395075</v>
+        <v>0.04437024407090457</v>
       </c>
       <c r="P5">
-        <v>0.02374497521172172</v>
+        <v>0.02856714344291116</v>
       </c>
       <c r="Q5">
-        <v>0.0334756145816788</v>
+        <v>0.03591560852236114</v>
       </c>
       <c r="R5">
-        <v>0.03688049341395075</v>
+        <v>0.04437024407090457</v>
       </c>
       <c r="S5">
-        <v>0.02374497521172172</v>
+        <v>0.02856714344291116</v>
       </c>
       <c r="T5">
-        <v>0.0334756145816788</v>
+        <v>0.03591560852236114</v>
       </c>
       <c r="U5">
-        <v>0.03688049341395075</v>
+        <v>0.04437024407090457</v>
       </c>
       <c r="V5">
-        <v>0.0166882618507599</v>
+        <v>0.01814545399791734</v>
       </c>
       <c r="W5">
-        <v>0.032714310806267</v>
+        <v>0.035098814306453</v>
       </c>
       <c r="X5">
-        <v>0.02215633062739187</v>
+        <v>0.02409098573340514</v>
       </c>
       <c r="Y5">
-        <v>0.0166882618507599</v>
+        <v>0.01814545399791734</v>
       </c>
       <c r="Z5">
-        <v>0.032714310806267</v>
+        <v>0.035098814306453</v>
       </c>
       <c r="AA5">
-        <v>0.02215633062739187</v>
+        <v>0.02409098573340514</v>
       </c>
       <c r="AB5">
-        <v>0.01668779342147088</v>
+        <v>0.01814494466613724</v>
       </c>
       <c r="AC5">
-        <v>0.03271339253559933</v>
+        <v>0.03509782910423253</v>
       </c>
       <c r="AD5">
-        <v>0.02215570871276133</v>
+        <v>0.0240903095141907</v>
       </c>
       <c r="AE5">
-        <v>0.01931556951040822</v>
+        <v>0.02323820681914047</v>
       </c>
       <c r="AF5">
-        <v>0.03006606124465596</v>
+        <v>0.03225753728397251</v>
       </c>
       <c r="AG5">
-        <v>0.03312414686252985</v>
+        <v>0.03985105254516429</v>
       </c>
       <c r="AH5">
-        <v>0.01931556951040822</v>
+        <v>0.02323820681914047</v>
       </c>
       <c r="AI5">
-        <v>0.03006606124465596</v>
+        <v>0.03225753728397251</v>
       </c>
       <c r="AJ5">
-        <v>0.03312414686252985</v>
+        <v>0.03985105254516429</v>
       </c>
       <c r="AK5">
-        <v>0.02374497521172172</v>
+        <v>0.02856714344291116</v>
       </c>
       <c r="AL5">
-        <v>0.0334756145816788</v>
+        <v>0.03591560852236114</v>
       </c>
       <c r="AM5">
-        <v>0.03688049341395075</v>
+        <v>0.04437024407090457</v>
       </c>
       <c r="AN5">
-        <v>0.01806700126341356</v>
+        <v>0.01964458271552452</v>
       </c>
       <c r="AO5">
-        <v>0.03435002634658035</v>
+        <v>0.03685375502177565</v>
       </c>
       <c r="AP5">
-        <v>0.02326414715876146</v>
+        <v>0.0252955350200754</v>
       </c>
       <c r="AQ5">
-        <v>0.01806700126341356</v>
+        <v>0.01964458271552452</v>
       </c>
       <c r="AR5">
-        <v>0.03435002634658035</v>
+        <v>0.03685375502177565</v>
       </c>
       <c r="AS5">
-        <v>0.02326414715876146</v>
+        <v>0.0252955350200754</v>
       </c>
       <c r="AT5">
-        <v>0.01931556951040822</v>
+        <v>0.02323820681914047</v>
       </c>
       <c r="AU5">
-        <v>0.03006606124465596</v>
+        <v>0.03225753728397251</v>
       </c>
       <c r="AV5">
-        <v>0.03312414686252985</v>
+        <v>0.03985105254516429</v>
       </c>
       <c r="AW5">
-        <v>0.01931556951040822</v>
+        <v>0.02323820681914047</v>
       </c>
       <c r="AX5">
-        <v>0.03006606124465596</v>
+        <v>0.03225753728397251</v>
       </c>
       <c r="AY5">
-        <v>0.03312414686252985</v>
+        <v>0.03985105254516429</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.01697010025346673</v>
+        <v>0.02261615274301138</v>
       </c>
       <c r="B6">
-        <v>0.0370674477993577</v>
+        <v>0.03977248296902747</v>
       </c>
       <c r="C6">
-        <v>0.02117290806092104</v>
+        <v>0.02821725950745078</v>
       </c>
       <c r="D6">
-        <v>0.01697010025346673</v>
+        <v>0.02261615274301138</v>
       </c>
       <c r="E6">
-        <v>0.0370674477993577</v>
+        <v>0.03977248296902747</v>
       </c>
       <c r="F6">
-        <v>0.02117290806092104</v>
+        <v>0.02821725950745078</v>
       </c>
       <c r="G6">
-        <v>0.01915551567472249</v>
+        <v>0.02397922234784575</v>
       </c>
       <c r="H6">
-        <v>0.03448186784526808</v>
+        <v>0.03699821765554477</v>
       </c>
       <c r="I6">
-        <v>0.02975218392031365</v>
+        <v>0.03724432407218595</v>
       </c>
       <c r="J6">
-        <v>0.002592849039061308</v>
+        <v>0.003455505213942476</v>
       </c>
       <c r="K6">
-        <v>0.006934513392713539</v>
+        <v>0.007440566647671146</v>
       </c>
       <c r="L6">
-        <v>0.003960990659672381</v>
+        <v>0.005278835624703611</v>
       </c>
       <c r="M6">
-        <v>0.01915551567472249</v>
+        <v>0.02397922234784575</v>
       </c>
       <c r="N6">
-        <v>0.03448186784526808</v>
+        <v>0.03699821765554477</v>
       </c>
       <c r="O6">
-        <v>0.02975218392031365</v>
+        <v>0.03724432407218595</v>
       </c>
       <c r="P6">
-        <v>0.01915551567472249</v>
+        <v>0.02397922234784575</v>
       </c>
       <c r="Q6">
-        <v>0.03448186784526808</v>
+        <v>0.03699821765554477</v>
       </c>
       <c r="R6">
-        <v>0.02975218392031365</v>
+        <v>0.03724432407218595</v>
       </c>
       <c r="S6">
-        <v>0.01915551567472249</v>
+        <v>0.02397922234784575</v>
       </c>
       <c r="T6">
-        <v>0.03448186784526808</v>
+        <v>0.03699821765554477</v>
       </c>
       <c r="U6">
-        <v>0.02975218392031365</v>
+        <v>0.03724432407218595</v>
       </c>
       <c r="V6">
-        <v>0.01449776630045585</v>
+        <v>0.01932125869536986</v>
       </c>
       <c r="W6">
-        <v>0.03369767981759791</v>
+        <v>0.03615680269911589</v>
       </c>
       <c r="X6">
-        <v>0.01924809823720095</v>
+        <v>0.02565205409768254</v>
       </c>
       <c r="Y6">
-        <v>0.01449776630045585</v>
+        <v>0.01932125869536986</v>
       </c>
       <c r="Z6">
-        <v>0.03369767981759791</v>
+        <v>0.03615680269911589</v>
       </c>
       <c r="AA6">
-        <v>0.01924809823720095</v>
+        <v>0.02565205409768254</v>
       </c>
       <c r="AB6">
-        <v>0.0144973593570353</v>
+        <v>0.01932071635947205</v>
       </c>
       <c r="AC6">
-        <v>0.03369673394436439</v>
+        <v>0.03615578779980922</v>
       </c>
       <c r="AD6">
-        <v>0.01924755795487239</v>
+        <v>0.02565133406023523</v>
       </c>
       <c r="AE6">
-        <v>0.0155822312393978</v>
+        <v>0.01950612000793767</v>
       </c>
       <c r="AF6">
-        <v>0.0309698257499167</v>
+        <v>0.03322988067210966</v>
       </c>
       <c r="AG6">
-        <v>0.02672186889139282</v>
+        <v>0.03345092069446332</v>
       </c>
       <c r="AH6">
-        <v>0.0155822312393978</v>
+        <v>0.01950612000793767</v>
       </c>
       <c r="AI6">
-        <v>0.0309698257499167</v>
+        <v>0.03322988067210966</v>
       </c>
       <c r="AJ6">
-        <v>0.02672186889139282</v>
+        <v>0.03345092069446332</v>
       </c>
       <c r="AK6">
-        <v>0.01915551567472249</v>
+        <v>0.02397922234784575</v>
       </c>
       <c r="AL6">
-        <v>0.03448186784526808</v>
+        <v>0.03699821765554477</v>
       </c>
       <c r="AM6">
-        <v>0.02975218392031365</v>
+        <v>0.03724432407218595</v>
       </c>
       <c r="AN6">
-        <v>0.01569553284874202</v>
+        <v>0.02091752924191397</v>
       </c>
       <c r="AO6">
-        <v>0.03538256380847781</v>
+        <v>0.03796464283407167</v>
       </c>
       <c r="AP6">
-        <v>0.020210503149061</v>
+        <v>0.02693465680256666</v>
       </c>
       <c r="AQ6">
-        <v>0.01569553284874202</v>
+        <v>0.02091752924191397</v>
       </c>
       <c r="AR6">
-        <v>0.03538256380847781</v>
+        <v>0.03796464283407167</v>
       </c>
       <c r="AS6">
-        <v>0.020210503149061</v>
+        <v>0.02693465680256666</v>
       </c>
       <c r="AT6">
-        <v>0.0155822312393978</v>
+        <v>0.01950612000793767</v>
       </c>
       <c r="AU6">
-        <v>0.0309698257499167</v>
+        <v>0.03322988067210966</v>
       </c>
       <c r="AV6">
-        <v>0.02672186889139282</v>
+        <v>0.03345092069446332</v>
       </c>
       <c r="AW6">
-        <v>0.0155822312393978</v>
+        <v>0.01950612000793767</v>
       </c>
       <c r="AX6">
-        <v>0.0309698257499167</v>
+        <v>0.03322988067210966</v>
       </c>
       <c r="AY6">
-        <v>0.02672186889139282</v>
+        <v>0.03345092069446332</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.01765538706564372</v>
+        <v>0.02389526882647277</v>
       </c>
       <c r="B7">
-        <v>0.03792289285705757</v>
+        <v>0.04069109121031626</v>
       </c>
       <c r="C7">
-        <v>0.02202791271339038</v>
+        <v>0.02981316093583751</v>
       </c>
       <c r="D7">
-        <v>0.01765538706564372</v>
+        <v>0.02389526882647277</v>
       </c>
       <c r="E7">
-        <v>0.03792289285705757</v>
+        <v>0.04069109121031626</v>
       </c>
       <c r="F7">
-        <v>0.02202791271339038</v>
+        <v>0.02981316093583751</v>
       </c>
       <c r="G7">
-        <v>0.02040475168892487</v>
+        <v>0.02214616139544141</v>
       </c>
       <c r="H7">
-        <v>0.03527764271458631</v>
+        <v>0.03785274986259472</v>
       </c>
       <c r="I7">
-        <v>0.03169248666577692</v>
+        <v>0.03439722940143027</v>
       </c>
       <c r="J7">
-        <v>0.00269755350314198</v>
+        <v>0.003650940412221474</v>
       </c>
       <c r="K7">
-        <v>0.007094548559997247</v>
+        <v>0.007612418273020559</v>
       </c>
       <c r="L7">
-        <v>0.004120943436714769</v>
+        <v>0.00557739407654259</v>
       </c>
       <c r="M7">
-        <v>0.02040475168892487</v>
+        <v>0.02214616139544141</v>
       </c>
       <c r="N7">
-        <v>0.03527764271458631</v>
+        <v>0.03785274986259472</v>
       </c>
       <c r="O7">
-        <v>0.03169248666577692</v>
+        <v>0.03439722940143027</v>
       </c>
       <c r="P7">
-        <v>0.02040475168892487</v>
+        <v>0.02214616139544141</v>
       </c>
       <c r="Q7">
-        <v>0.03527764271458631</v>
+        <v>0.03785274986259472</v>
       </c>
       <c r="R7">
-        <v>0.03169248666577692</v>
+        <v>0.03439722940143027</v>
       </c>
       <c r="S7">
-        <v>0.02040475168892487</v>
+        <v>0.02214616139544141</v>
       </c>
       <c r="T7">
-        <v>0.03527764271458631</v>
+        <v>0.03785274986259472</v>
       </c>
       <c r="U7">
-        <v>0.03169248666577692</v>
+        <v>0.03439722940143027</v>
       </c>
       <c r="V7">
-        <v>0.01508321529034598</v>
+        <v>0.02041402336807056</v>
       </c>
       <c r="W7">
-        <v>0.03447535714277961</v>
+        <v>0.03699190110028751</v>
       </c>
       <c r="X7">
-        <v>0.02002537519399126</v>
+        <v>0.0271028735780341</v>
       </c>
       <c r="Y7">
-        <v>0.01508321529034598</v>
+        <v>0.02041402336807056</v>
       </c>
       <c r="Z7">
-        <v>0.03447535714277961</v>
+        <v>0.03699190110028751</v>
       </c>
       <c r="AA7">
-        <v>0.02002537519399126</v>
+        <v>0.0271028735780341</v>
       </c>
       <c r="AB7">
-        <v>0.01508279191373086</v>
+        <v>0.02041345035893768</v>
       </c>
       <c r="AC7">
-        <v>0.03447438944061988</v>
+        <v>0.0369908627602802</v>
       </c>
       <c r="AD7">
-        <v>0.02002481309397458</v>
+        <v>0.02710211281697257</v>
       </c>
       <c r="AE7">
-        <v>0.01659843381918907</v>
+        <v>0.01801499963711063</v>
       </c>
       <c r="AF7">
-        <v>0.03168454947513771</v>
+        <v>0.03399737719140453</v>
       </c>
       <c r="AG7">
-        <v>0.02846454820907742</v>
+        <v>0.03089380788832164</v>
       </c>
       <c r="AH7">
-        <v>0.01659843381918907</v>
+        <v>0.01801499963711063</v>
       </c>
       <c r="AI7">
-        <v>0.03168454947513771</v>
+        <v>0.03399737719140453</v>
       </c>
       <c r="AJ7">
-        <v>0.02846454820907742</v>
+        <v>0.03089380788832164</v>
       </c>
       <c r="AK7">
-        <v>0.02040475168892487</v>
+        <v>0.02214616139544141</v>
       </c>
       <c r="AL7">
-        <v>0.03527764271458631</v>
+        <v>0.03785274986259472</v>
       </c>
       <c r="AM7">
-        <v>0.03169248666577692</v>
+        <v>0.03439722940143027</v>
       </c>
       <c r="AN7">
-        <v>0.01632935006317694</v>
+        <v>0.02210057519953706</v>
       </c>
       <c r="AO7">
-        <v>0.03619912499991858</v>
+        <v>0.03884149615530188</v>
       </c>
       <c r="AP7">
-        <v>0.02102664395369082</v>
+        <v>0.0284580172569358</v>
       </c>
       <c r="AQ7">
-        <v>0.01632935006317694</v>
+        <v>0.02210057519953706</v>
       </c>
       <c r="AR7">
-        <v>0.03619912499991858</v>
+        <v>0.03884149615530188</v>
       </c>
       <c r="AS7">
-        <v>0.02102664395369082</v>
+        <v>0.0284580172569358</v>
       </c>
       <c r="AT7">
-        <v>0.01659843381918907</v>
+        <v>0.01801499963711063</v>
       </c>
       <c r="AU7">
-        <v>0.03168454947513771</v>
+        <v>0.03399737719140453</v>
       </c>
       <c r="AV7">
-        <v>0.02846454820907742</v>
+        <v>0.03089380788832164</v>
       </c>
       <c r="AW7">
-        <v>0.01659843381918907</v>
+        <v>0.01801499963711063</v>
       </c>
       <c r="AX7">
-        <v>0.03168454947513771</v>
+        <v>0.03399737719140453</v>
       </c>
       <c r="AY7">
-        <v>0.02846454820907742</v>
+        <v>0.03089380788832164</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.01457159641084726</v>
+        <v>0.01647820741399939</v>
       </c>
       <c r="B8">
-        <v>0.02936844228005895</v>
+        <v>0.0315050087974284</v>
       </c>
       <c r="C8">
-        <v>0.01818039177727837</v>
+        <v>0.02055919325014732</v>
       </c>
       <c r="D8">
-        <v>0.01457159641084726</v>
+        <v>0.01647820741399939</v>
       </c>
       <c r="E8">
-        <v>0.02936844228005895</v>
+        <v>0.0315050087974284</v>
       </c>
       <c r="F8">
-        <v>0.01818039177727837</v>
+        <v>0.02055919325014732</v>
       </c>
       <c r="G8">
-        <v>0.01809256628032066</v>
+        <v>0.02307927789969434</v>
       </c>
       <c r="H8">
-        <v>0.02731989402140397</v>
+        <v>0.0293074277920952</v>
       </c>
       <c r="I8">
-        <v>0.02810121996730656</v>
+        <v>0.03584653801441887</v>
       </c>
       <c r="J8">
-        <v>0.002226383414778959</v>
+        <v>0.00251769309672246</v>
       </c>
       <c r="K8">
-        <v>0.005494196887160175</v>
+        <v>0.005893902019526435</v>
       </c>
       <c r="L8">
-        <v>0.003401155940024026</v>
+        <v>0.003846177964780267</v>
       </c>
       <c r="M8">
-        <v>0.01809256628032066</v>
+        <v>0.02307927789969434</v>
       </c>
       <c r="N8">
-        <v>0.02731989402140397</v>
+        <v>0.0293074277920952</v>
       </c>
       <c r="O8">
-        <v>0.02810121996730656</v>
+        <v>0.03584653801441887</v>
       </c>
       <c r="P8">
-        <v>0.01809256628032066</v>
+        <v>0.02307927789969434</v>
       </c>
       <c r="Q8">
-        <v>0.02731989402140397</v>
+        <v>0.0293074277920952</v>
       </c>
       <c r="R8">
-        <v>0.02810121996730656</v>
+        <v>0.03584653801441887</v>
       </c>
       <c r="S8">
-        <v>0.01809256628032066</v>
+        <v>0.02307927789969434</v>
       </c>
       <c r="T8">
-        <v>0.02731989402140397</v>
+        <v>0.0293074277920952</v>
       </c>
       <c r="U8">
-        <v>0.02810121996730656</v>
+        <v>0.03584653801441887</v>
       </c>
       <c r="V8">
-        <v>0.01244869483584038</v>
+        <v>0.01407753617070111</v>
       </c>
       <c r="W8">
-        <v>0.02669858389096269</v>
+        <v>0.02864091708857127</v>
       </c>
       <c r="X8">
-        <v>0.01652762888843488</v>
+        <v>0.01869017568195212</v>
       </c>
       <c r="Y8">
-        <v>0.01244869483584038</v>
+        <v>0.01407753617070111</v>
       </c>
       <c r="Z8">
-        <v>0.02669858389096269</v>
+        <v>0.02864091708857127</v>
       </c>
       <c r="AA8">
-        <v>0.01652762888843488</v>
+        <v>0.01869017568195212</v>
       </c>
       <c r="AB8">
-        <v>0.01244834540860084</v>
+        <v>0.01407714102288293</v>
       </c>
       <c r="AC8">
-        <v>0.02669783447806506</v>
+        <v>0.02864011315557041</v>
       </c>
       <c r="AD8">
-        <v>0.01652716496801472</v>
+        <v>0.01868965106016797</v>
       </c>
       <c r="AE8">
-        <v>0.01471756523193533</v>
+        <v>0.01877405188031151</v>
       </c>
       <c r="AF8">
-        <v>0.02453731222292764</v>
+        <v>0.02632241199845588</v>
       </c>
       <c r="AG8">
-        <v>0.02523905867434015</v>
+        <v>0.03219550173517251</v>
       </c>
       <c r="AH8">
-        <v>0.01471756523193533</v>
+        <v>0.01877405188031151</v>
       </c>
       <c r="AI8">
-        <v>0.02453731222292764</v>
+        <v>0.02632241199845588</v>
       </c>
       <c r="AJ8">
-        <v>0.02523905867434015</v>
+        <v>0.03219550173517251</v>
       </c>
       <c r="AK8">
-        <v>0.01809256628032066</v>
+        <v>0.02307927789969434</v>
       </c>
       <c r="AL8">
-        <v>0.02731989402140397</v>
+        <v>0.0293074277920952</v>
       </c>
       <c r="AM8">
-        <v>0.02810121996730656</v>
+        <v>0.03584653801441887</v>
       </c>
       <c r="AN8">
-        <v>0.01347717259821979</v>
+        <v>0.01524058443331687</v>
       </c>
       <c r="AO8">
-        <v>0.02803351308551082</v>
+        <v>0.03007296294299983</v>
       </c>
       <c r="AP8">
-        <v>0.01735401033285662</v>
+        <v>0.01962468446604972</v>
       </c>
       <c r="AQ8">
-        <v>0.01347717259821979</v>
+        <v>0.01524058443331687</v>
       </c>
       <c r="AR8">
-        <v>0.02803351308551082</v>
+        <v>0.03007296294299983</v>
       </c>
       <c r="AS8">
-        <v>0.01735401033285662</v>
+        <v>0.01962468446604972</v>
       </c>
       <c r="AT8">
-        <v>0.01471756523193533</v>
+        <v>0.01877405188031151</v>
       </c>
       <c r="AU8">
-        <v>0.02453731222292764</v>
+        <v>0.02632241199845588</v>
       </c>
       <c r="AV8">
-        <v>0.02523905867434015</v>
+        <v>0.03219550173517251</v>
       </c>
       <c r="AW8">
-        <v>0.01471756523193533</v>
+        <v>0.01877405188031151</v>
       </c>
       <c r="AX8">
-        <v>0.02453731222292764</v>
+        <v>0.02632241199845588</v>
       </c>
       <c r="AY8">
-        <v>0.02523905867434015</v>
+        <v>0.03219550173517251</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.01491423981693576</v>
+        <v>0.01686857906728747</v>
       </c>
       <c r="B9">
-        <v>0.03877833791475743</v>
+        <v>0.04160969945160504</v>
       </c>
       <c r="C9">
-        <v>0.01860789410351303</v>
+        <v>0.02104624418097312</v>
       </c>
       <c r="D9">
-        <v>0.01491423981693576</v>
+        <v>0.01686857906728747</v>
       </c>
       <c r="E9">
-        <v>0.03877833791475743</v>
+        <v>0.04160969945160504</v>
       </c>
       <c r="F9">
-        <v>0.01860789410351303</v>
+        <v>0.02104624418097312</v>
       </c>
       <c r="G9">
-        <v>0.01867061263247171</v>
+        <v>0.01716954003942577</v>
       </c>
       <c r="H9">
-        <v>0.03607341758390455</v>
+        <v>0.03870728206964467</v>
       </c>
       <c r="I9">
-        <v>0.02899903664192415</v>
+        <v>0.02666758346549108</v>
       </c>
       <c r="J9">
-        <v>0.002278735646819294</v>
+        <v>0.002577337692275039</v>
       </c>
       <c r="K9">
-        <v>0.007254583727280954</v>
+        <v>0.00778426989836997</v>
       </c>
       <c r="L9">
-        <v>0.003481132328545219</v>
+        <v>0.003937294602241443</v>
       </c>
       <c r="M9">
-        <v>0.01867061263247171</v>
+        <v>0.01716954003942577</v>
       </c>
       <c r="N9">
-        <v>0.03607341758390455</v>
+        <v>0.03870728206964467</v>
       </c>
       <c r="O9">
-        <v>0.02899903664192415</v>
+        <v>0.02666758346549108</v>
       </c>
       <c r="P9">
-        <v>0.01867061263247171</v>
+        <v>0.01716954003942577</v>
       </c>
       <c r="Q9">
-        <v>0.03607341758390455</v>
+        <v>0.03870728206964467</v>
       </c>
       <c r="R9">
-        <v>0.02899903664192415</v>
+        <v>0.02666758346549108</v>
       </c>
       <c r="S9">
-        <v>0.01867061263247171</v>
+        <v>0.01716954003942577</v>
       </c>
       <c r="T9">
-        <v>0.03607341758390455</v>
+        <v>0.03870728206964467</v>
       </c>
       <c r="U9">
-        <v>0.02899903664192415</v>
+        <v>0.02666758346549108</v>
       </c>
       <c r="V9">
-        <v>0.01274141933078544</v>
+        <v>0.01441103549687845</v>
       </c>
       <c r="W9">
-        <v>0.0352530344679613</v>
+        <v>0.03782699950145913</v>
       </c>
       <c r="X9">
-        <v>0.01691626736683003</v>
+        <v>0.01913294925543011</v>
       </c>
       <c r="Y9">
-        <v>0.01274141933078544</v>
+        <v>0.01441103549687845</v>
       </c>
       <c r="Z9">
-        <v>0.0352530344679613</v>
+        <v>0.03782699950145913</v>
       </c>
       <c r="AA9">
-        <v>0.01691626736683003</v>
+        <v>0.01913294925543011</v>
       </c>
       <c r="AB9">
-        <v>0.01274106168694862</v>
+        <v>0.01441063098793844</v>
       </c>
       <c r="AC9">
-        <v>0.03525204493687535</v>
+        <v>0.03782593772075118</v>
       </c>
       <c r="AD9">
-        <v>0.01691579253756582</v>
+        <v>0.01913241220526295</v>
       </c>
       <c r="AE9">
-        <v>0.01518778237874876</v>
+        <v>0.01396672100670594</v>
       </c>
       <c r="AF9">
-        <v>0.03239927320035871</v>
+        <v>0.03476487371069939</v>
       </c>
       <c r="AG9">
-        <v>0.02604543105802447</v>
+        <v>0.02395144070511699</v>
       </c>
       <c r="AH9">
-        <v>0.01518778237874876</v>
+        <v>0.01396672100670594</v>
       </c>
       <c r="AI9">
-        <v>0.03239927320035871</v>
+        <v>0.03476487371069939</v>
       </c>
       <c r="AJ9">
-        <v>0.02604543105802447</v>
+        <v>0.02395144070511699</v>
       </c>
       <c r="AK9">
-        <v>0.01867061263247171</v>
+        <v>0.01716954003942577</v>
       </c>
       <c r="AL9">
-        <v>0.03607341758390455</v>
+        <v>0.03870728206964467</v>
       </c>
       <c r="AM9">
-        <v>0.02899903664192415</v>
+        <v>0.02666758346549108</v>
       </c>
       <c r="AN9">
-        <v>0.01379408120543725</v>
+        <v>0.0156016365789074</v>
       </c>
       <c r="AO9">
-        <v>0.03701568619135936</v>
+        <v>0.03971834947653208</v>
       </c>
       <c r="AP9">
-        <v>0.01776208073517153</v>
+        <v>0.02008959671820162</v>
       </c>
       <c r="AQ9">
-        <v>0.01379408120543725</v>
+        <v>0.0156016365789074</v>
       </c>
       <c r="AR9">
-        <v>0.03701568619135936</v>
+        <v>0.03971834947653208</v>
       </c>
       <c r="AS9">
-        <v>0.01776208073517153</v>
+        <v>0.02008959671820162</v>
       </c>
       <c r="AT9">
-        <v>0.01518778237874876</v>
+        <v>0.01396672100670594</v>
       </c>
       <c r="AU9">
-        <v>0.03239927320035871</v>
+        <v>0.03476487371069939</v>
       </c>
       <c r="AV9">
-        <v>0.02604543105802447</v>
+        <v>0.02395144070511699</v>
       </c>
       <c r="AW9">
-        <v>0.01518778237874876</v>
+        <v>0.01396672100670594</v>
       </c>
       <c r="AX9">
-        <v>0.03239927320035871</v>
+        <v>0.03476487371069939</v>
       </c>
       <c r="AY9">
-        <v>0.02604543105802447</v>
+        <v>0.02395144070511699</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.1312819359299788</v>
+        <v>0.141998875151762</v>
       </c>
       <c r="B10">
-        <v>0.2764956699217879</v>
+        <v>0.2969460008586314</v>
       </c>
       <c r="C10">
-        <v>0.1637951643177437</v>
+        <v>0.1771662561467941</v>
       </c>
       <c r="D10">
-        <v>0.1312819359299788</v>
+        <v>0.141998875151762</v>
       </c>
       <c r="E10">
-        <v>0.2764956699217879</v>
+        <v>0.2969460008586314</v>
       </c>
       <c r="F10">
-        <v>0.1637951643177437</v>
+        <v>0.1771662561467941</v>
       </c>
       <c r="G10">
-        <v>0.05931741052837072</v>
+        <v>0.06402290023288615</v>
       </c>
       <c r="H10">
-        <v>0.2572091610309669</v>
+        <v>0.2762330121623753</v>
       </c>
       <c r="I10">
-        <v>0.09213129720363962</v>
+        <v>0.09943982376597209</v>
       </c>
       <c r="J10">
-        <v>0.02005846968126287</v>
+        <v>0.02169590288129376</v>
       </c>
       <c r="K10">
-        <v>0.05172632700471933</v>
+        <v>0.05555213919806441</v>
       </c>
       <c r="L10">
-        <v>0.03064251325775902</v>
+        <v>0.03314395376333812</v>
       </c>
       <c r="M10">
-        <v>0.05931741052837072</v>
+        <v>0.06402290023288615</v>
       </c>
       <c r="N10">
-        <v>0.2572091610309669</v>
+        <v>0.2762330121623753</v>
       </c>
       <c r="O10">
-        <v>0.09213129720363962</v>
+        <v>0.09943982376597209</v>
       </c>
       <c r="P10">
-        <v>0.05931741052837072</v>
+        <v>0.06402290023288615</v>
       </c>
       <c r="Q10">
-        <v>0.2572091610309669</v>
+        <v>0.2762330121623753</v>
       </c>
       <c r="R10">
-        <v>0.09213129720363962</v>
+        <v>0.09943982376597209</v>
       </c>
       <c r="S10">
-        <v>0.05931741052837072</v>
+        <v>0.06402290023288615</v>
       </c>
       <c r="T10">
-        <v>0.2572091610309669</v>
+        <v>0.2762330121623753</v>
       </c>
       <c r="U10">
-        <v>0.09213129720363962</v>
+        <v>0.09943982376597209</v>
       </c>
       <c r="V10">
-        <v>0.1121557797630239</v>
+        <v>0.1213113933406079</v>
       </c>
       <c r="W10">
-        <v>0.2513596999288981</v>
+        <v>0.2699509098714831</v>
       </c>
       <c r="X10">
-        <v>0.1489046948343125</v>
+        <v>0.1610602328607219</v>
       </c>
       <c r="Y10">
-        <v>0.1121557797630239</v>
+        <v>0.1213113933406079</v>
       </c>
       <c r="Z10">
-        <v>0.2513596999288981</v>
+        <v>0.2699509098714831</v>
       </c>
       <c r="AA10">
-        <v>0.1489046948343125</v>
+        <v>0.1610602328607219</v>
       </c>
       <c r="AB10">
-        <v>0.1121526316189784</v>
+        <v>0.1213079882040969</v>
       </c>
       <c r="AC10">
-        <v>0.2513526444160724</v>
+        <v>0.2699433325147809</v>
       </c>
       <c r="AD10">
-        <v>0.1489005151707287</v>
+        <v>0.1610557119986307</v>
       </c>
       <c r="AE10">
-        <v>0.04825229573929248</v>
+        <v>0.05208001982228964</v>
       </c>
       <c r="AF10">
-        <v>0.2310119316667018</v>
+        <v>0.2480981683310223</v>
       </c>
       <c r="AG10">
-        <v>0.08274755396993559</v>
+        <v>0.08931169356758606</v>
       </c>
       <c r="AH10">
-        <v>0.04825229573929248</v>
+        <v>0.05208001982228964</v>
       </c>
       <c r="AI10">
-        <v>0.2310119316667018</v>
+        <v>0.2480981683310223</v>
       </c>
       <c r="AJ10">
-        <v>0.08274755396993559</v>
+        <v>0.08931169356758606</v>
       </c>
       <c r="AK10">
-        <v>0.05931741052837072</v>
+        <v>0.06402290023288615</v>
       </c>
       <c r="AL10">
-        <v>0.2572091610309669</v>
+        <v>0.2762330121623753</v>
       </c>
       <c r="AM10">
-        <v>0.09213129720363962</v>
+        <v>0.09943982376597209</v>
       </c>
       <c r="AN10">
-        <v>0.1214217893270542</v>
+        <v>0.1313338151301491</v>
       </c>
       <c r="AO10">
-        <v>0.263927684925343</v>
+        <v>0.2834484553650572</v>
       </c>
       <c r="AP10">
-        <v>0.1563499295760281</v>
+        <v>0.169113244503758</v>
       </c>
       <c r="AQ10">
-        <v>0.1214217893270542</v>
+        <v>0.1313338151301491</v>
       </c>
       <c r="AR10">
-        <v>0.263927684925343</v>
+        <v>0.2834484553650572</v>
       </c>
       <c r="AS10">
-        <v>0.1563499295760281</v>
+        <v>0.169113244503758</v>
       </c>
       <c r="AT10">
-        <v>0.04825229573929248</v>
+        <v>0.05208001982228964</v>
       </c>
       <c r="AU10">
-        <v>0.2310119316667018</v>
+        <v>0.2480981683310223</v>
       </c>
       <c r="AV10">
-        <v>0.08274755396993559</v>
+        <v>0.08931169356758606</v>
       </c>
       <c r="AW10">
-        <v>0.04825229573929248</v>
+        <v>0.05208001982228964</v>
       </c>
       <c r="AX10">
-        <v>0.2310119316667018</v>
+        <v>0.2480981683310223</v>
       </c>
       <c r="AY10">
-        <v>0.08274755396993559</v>
+        <v>0.08931169356758606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Re-run CropResidueSim without any assumption changes. Profit reduction $2000. 1% increase in sheep numbers
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.05891273035340159</v>
+        <v>0.05482790899252283</v>
       </c>
       <c r="B1">
-        <v>0.2870057404054701</v>
+        <v>0.2868948076594419</v>
       </c>
       <c r="C1">
-        <v>0.07350303208347805</v>
+        <v>0.06840656560258593</v>
       </c>
       <c r="D1">
-        <v>0.05891273035340159</v>
+        <v>0.05482790899252283</v>
       </c>
       <c r="E1">
-        <v>0.2870057404054701</v>
+        <v>0.2868948076594419</v>
       </c>
       <c r="F1">
-        <v>0.07350303208347805</v>
+        <v>0.06840656560258593</v>
       </c>
       <c r="G1">
-        <v>0.0504892938067427</v>
+        <v>0.04740812681074145</v>
       </c>
       <c r="H1">
-        <v>0.2669861185227384</v>
+        <v>0.2668829237112434</v>
       </c>
       <c r="I1">
-        <v>0.07841954144451525</v>
+        <v>0.07363389908902396</v>
       </c>
       <c r="J1">
-        <v>0.009001232403096171</v>
+        <v>0.008377115575140016</v>
       </c>
       <c r="K1">
-        <v>0.05369253263403487</v>
+        <v>0.05367177952966182</v>
       </c>
       <c r="L1">
-        <v>0.01375081886260223</v>
+        <v>0.01279738081478836</v>
       </c>
       <c r="M1">
-        <v>0.0504892938067427</v>
+        <v>0.04740812681074145</v>
       </c>
       <c r="N1">
-        <v>0.2669861185227384</v>
+        <v>0.2668829237112434</v>
       </c>
       <c r="O1">
-        <v>0.07841954144451525</v>
+        <v>0.07363389908902396</v>
       </c>
       <c r="P1">
-        <v>0.0504892938067427</v>
+        <v>0.04740812681074145</v>
       </c>
       <c r="Q1">
-        <v>0.2669861185227384</v>
+        <v>0.2668829237112434</v>
       </c>
       <c r="R1">
-        <v>0.07841954144451525</v>
+        <v>0.07363389908902396</v>
       </c>
       <c r="S1">
-        <v>0.0504892938067427</v>
+        <v>0.04740812681074145</v>
       </c>
       <c r="T1">
-        <v>0.2669861185227384</v>
+        <v>0.2668829237112434</v>
       </c>
       <c r="U1">
-        <v>0.07841954144451525</v>
+        <v>0.07363389908902396</v>
       </c>
       <c r="V1">
-        <v>0.05032987336718341</v>
+        <v>0.04684016001342569</v>
       </c>
       <c r="W1">
-        <v>0.2609143094595183</v>
+        <v>0.2608134615085836</v>
       </c>
       <c r="X1">
-        <v>0.06682093825770732</v>
+        <v>0.06218778691144176</v>
       </c>
       <c r="Y1">
-        <v>0.05032987336718341</v>
+        <v>0.04684016001342569</v>
       </c>
       <c r="Z1">
-        <v>0.2609143094595183</v>
+        <v>0.2608134615085836</v>
       </c>
       <c r="AA1">
-        <v>0.06682093825770732</v>
+        <v>0.06218778691144176</v>
       </c>
       <c r="AB1">
-        <v>0.05032846063846373</v>
+        <v>0.04683884523882249</v>
       </c>
       <c r="AC1">
-        <v>0.260906985754655</v>
+        <v>0.2608061406344605</v>
       </c>
       <c r="AD1">
-        <v>0.06681906263489652</v>
+        <v>0.06218604133835155</v>
       </c>
       <c r="AE1">
-        <v>0.04107098261252931</v>
+        <v>0.03856457884694195</v>
       </c>
       <c r="AF1">
-        <v>0.2397930879324596</v>
+        <v>0.2397004037036168</v>
       </c>
       <c r="AG1">
-        <v>0.07043236592701835</v>
+        <v>0.06613415010773449</v>
       </c>
       <c r="AH1">
-        <v>0.04107098261252931</v>
+        <v>0.03856457884694195</v>
       </c>
       <c r="AI1">
-        <v>0.2397930879324596</v>
+        <v>0.2397004037036168</v>
       </c>
       <c r="AJ1">
-        <v>0.07043236592701835</v>
+        <v>0.06613415010773449</v>
       </c>
       <c r="AK1">
-        <v>0.0504892938067427</v>
+        <v>0.04740812681074145</v>
       </c>
       <c r="AL1">
-        <v>0.2669861185227384</v>
+        <v>0.2668829237112434</v>
       </c>
       <c r="AM1">
-        <v>0.07841954144451525</v>
+        <v>0.07363389908902396</v>
       </c>
       <c r="AN1">
-        <v>0.05448799244907232</v>
+        <v>0.05070996834236039</v>
       </c>
       <c r="AO1">
-        <v>0.2739600249324942</v>
+        <v>0.2738541345840128</v>
       </c>
       <c r="AP1">
-        <v>0.07016198517059269</v>
+        <v>0.06529717625701384</v>
       </c>
       <c r="AQ1">
-        <v>0.05448799244907232</v>
+        <v>0.05070996834236039</v>
       </c>
       <c r="AR1">
-        <v>0.2739600249324942</v>
+        <v>0.2738541345840128</v>
       </c>
       <c r="AS1">
-        <v>0.07016198517059269</v>
+        <v>0.06529717625701384</v>
       </c>
       <c r="AT1">
-        <v>0.04107098261252931</v>
+        <v>0.03856457884694195</v>
       </c>
       <c r="AU1">
-        <v>0.2397930879324596</v>
+        <v>0.2397004037036168</v>
       </c>
       <c r="AV1">
-        <v>0.07043236592701835</v>
+        <v>0.06613415010773449</v>
       </c>
       <c r="AW1">
-        <v>0.04107098261252931</v>
+        <v>0.03856457884694195</v>
       </c>
       <c r="AX1">
-        <v>0.2397930879324596</v>
+        <v>0.2397004037036168</v>
       </c>
       <c r="AY1">
-        <v>0.07043236592701835</v>
+        <v>0.06613415010773449</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.01756326854460394</v>
+        <v>0.01717818715579903</v>
       </c>
       <c r="B2">
-        <v>0.03592642471042405</v>
+        <v>0.03590688454940147</v>
       </c>
       <c r="C2">
-        <v>0.02191298015862926</v>
+        <v>0.02143252967693735</v>
       </c>
       <c r="D2">
-        <v>0.01756326854460394</v>
+        <v>0.01717818715579903</v>
       </c>
       <c r="E2">
-        <v>0.03592642471042405</v>
+        <v>0.03590688454940147</v>
       </c>
       <c r="F2">
-        <v>0.02191298015862926</v>
+        <v>0.02143252967693735</v>
       </c>
       <c r="G2">
-        <v>0.01999642032776401</v>
+        <v>0.01655864727677222</v>
       </c>
       <c r="H2">
-        <v>0.03342043497905139</v>
+        <v>0.03340225781040188</v>
       </c>
       <c r="I2">
-        <v>0.0310582698707824</v>
+        <v>0.02571875002562493</v>
       </c>
       <c r="J2">
-        <v>0.002683478782592881</v>
+        <v>0.002624642482629406</v>
       </c>
       <c r="K2">
-        <v>0.006721052786134014</v>
+        <v>0.006717397246938537</v>
       </c>
       <c r="L2">
-        <v>0.004099442055109974</v>
+        <v>0.004009560218144497</v>
       </c>
       <c r="M2">
-        <v>0.01999642032776401</v>
+        <v>0.01655864727677222</v>
       </c>
       <c r="N2">
-        <v>0.03342043497905139</v>
+        <v>0.03340225781040188</v>
       </c>
       <c r="O2">
-        <v>0.0310582698707824</v>
+        <v>0.02571875002562493</v>
       </c>
       <c r="P2">
-        <v>0.01999642032776401</v>
+        <v>0.01655864727677222</v>
       </c>
       <c r="Q2">
-        <v>0.03342043497905139</v>
+        <v>0.03340225781040188</v>
       </c>
       <c r="R2">
-        <v>0.0310582698707824</v>
+        <v>0.02571875002562493</v>
       </c>
       <c r="S2">
-        <v>0.01999642032776401</v>
+        <v>0.01655864727677222</v>
       </c>
       <c r="T2">
-        <v>0.03342043497905139</v>
+        <v>0.03340225781040188</v>
       </c>
       <c r="U2">
-        <v>0.0310582698707824</v>
+        <v>0.02571875002562493</v>
       </c>
       <c r="V2">
-        <v>0.01500451729976071</v>
+        <v>0.01467553751188892</v>
       </c>
       <c r="W2">
-        <v>0.03266038610038551</v>
+        <v>0.0326426223176377</v>
       </c>
       <c r="X2">
-        <v>0.01992089105329933</v>
+        <v>0.01948411788812486</v>
       </c>
       <c r="Y2">
-        <v>0.01500451729976071</v>
+        <v>0.01467553751188892</v>
       </c>
       <c r="Z2">
-        <v>0.03266038610038551</v>
+        <v>0.0326426223176377</v>
       </c>
       <c r="AA2">
-        <v>0.01992089105329933</v>
+        <v>0.01948411788812486</v>
       </c>
       <c r="AB2">
-        <v>0.01500409613214999</v>
+        <v>0.01467512557853935</v>
       </c>
       <c r="AC2">
-        <v>0.0326594693433513</v>
+        <v>0.032641706059222</v>
       </c>
       <c r="AD2">
-        <v>0.01992033188608849</v>
+        <v>0.01948357098086926</v>
       </c>
       <c r="AE2">
-        <v>0.01626627290011224</v>
+        <v>0.01346978464373956</v>
       </c>
       <c r="AF2">
-        <v>0.0300165017867406</v>
+        <v>0.03000017599637947</v>
       </c>
       <c r="AG2">
-        <v>0.02789492756912864</v>
+        <v>0.02309924770820018</v>
       </c>
       <c r="AH2">
-        <v>0.01626627290011224</v>
+        <v>0.01346978464373956</v>
       </c>
       <c r="AI2">
-        <v>0.0300165017867406</v>
+        <v>0.03000017599637947</v>
       </c>
       <c r="AJ2">
-        <v>0.02789492756912864</v>
+        <v>0.02309924770820018</v>
       </c>
       <c r="AK2">
-        <v>0.01999642032776401</v>
+        <v>0.01655864727677222</v>
       </c>
       <c r="AL2">
-        <v>0.03342043497905139</v>
+        <v>0.03340225781040188</v>
       </c>
       <c r="AM2">
-        <v>0.0310582698707824</v>
+        <v>0.02571875002562493</v>
       </c>
       <c r="AN2">
-        <v>0.01624415025578853</v>
+        <v>0.01588799104063057</v>
       </c>
       <c r="AO2">
-        <v>0.03429340540540477</v>
+        <v>0.03427475343351959</v>
       </c>
       <c r="AP2">
-        <v>0.02091693560596429</v>
+        <v>0.0204583237825311</v>
       </c>
       <c r="AQ2">
-        <v>0.01624415025578853</v>
+        <v>0.01588799104063057</v>
       </c>
       <c r="AR2">
-        <v>0.03429340540540477</v>
+        <v>0.03427475343351959</v>
       </c>
       <c r="AS2">
-        <v>0.02091693560596429</v>
+        <v>0.0204583237825311</v>
       </c>
       <c r="AT2">
-        <v>0.01626627290011224</v>
+        <v>0.01346978464373956</v>
       </c>
       <c r="AU2">
-        <v>0.0300165017867406</v>
+        <v>0.03000017599637947</v>
       </c>
       <c r="AV2">
-        <v>0.02789492756912864</v>
+        <v>0.02309924770820018</v>
       </c>
       <c r="AW2">
-        <v>0.01626627290011224</v>
+        <v>0.01346978464373956</v>
       </c>
       <c r="AX2">
-        <v>0.0300165017867406</v>
+        <v>0.03000017599637947</v>
       </c>
       <c r="AY2">
-        <v>0.02789492756912864</v>
+        <v>0.02309924770820018</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.01460385865728181</v>
+        <v>0.01422210672117057</v>
       </c>
       <c r="B3">
-        <v>0.0368205150526488</v>
+        <v>0.03680011531290539</v>
       </c>
       <c r="C3">
-        <v>0.01822064407793628</v>
+        <v>0.01774434761977536</v>
       </c>
       <c r="D3">
-        <v>0.01460385865728181</v>
+        <v>0.01422210672117057</v>
       </c>
       <c r="E3">
-        <v>0.0368205150526488</v>
+        <v>0.03680011531290539</v>
       </c>
       <c r="F3">
-        <v>0.01822064407793628</v>
+        <v>0.01774434761977536</v>
       </c>
       <c r="G3">
-        <v>0.01857346232618267</v>
+        <v>0.02106457809051863</v>
       </c>
       <c r="H3">
-        <v>0.03425215949348797</v>
+        <v>0.034233182704643</v>
       </c>
       <c r="I3">
-        <v>0.02884814361300712</v>
+        <v>0.03271732341718851</v>
       </c>
       <c r="J3">
-        <v>0.002231312739498103</v>
+        <v>0.002172985144143821</v>
       </c>
       <c r="K3">
-        <v>0.006888317645749215</v>
+        <v>0.006884501298067975</v>
       </c>
       <c r="L3">
-        <v>0.003408686270126889</v>
+        <v>0.003319581560628219</v>
       </c>
       <c r="M3">
-        <v>0.01857346232618267</v>
+        <v>0.02106457809051863</v>
       </c>
       <c r="N3">
-        <v>0.03425215949348797</v>
+        <v>0.034233182704643</v>
       </c>
       <c r="O3">
-        <v>0.02884814361300712</v>
+        <v>0.03271732341718851</v>
       </c>
       <c r="P3">
-        <v>0.01857346232618267</v>
+        <v>0.02106457809051863</v>
       </c>
       <c r="Q3">
-        <v>0.03425215949348797</v>
+        <v>0.034233182704643</v>
       </c>
       <c r="R3">
-        <v>0.02884814361300712</v>
+        <v>0.03271732341718851</v>
       </c>
       <c r="S3">
-        <v>0.01857346232618267</v>
+        <v>0.02106457809051863</v>
       </c>
       <c r="T3">
-        <v>0.03425215949348797</v>
+        <v>0.034233182704643</v>
       </c>
       <c r="U3">
-        <v>0.02884814361300712</v>
+        <v>0.03271732341718851</v>
       </c>
       <c r="V3">
-        <v>0.01247625687154728</v>
+        <v>0.01215012147624479</v>
       </c>
       <c r="W3">
-        <v>0.033473195502408</v>
+        <v>0.03345465028445944</v>
       </c>
       <c r="X3">
-        <v>0.01656422188903298</v>
+        <v>0.0161312251088867</v>
       </c>
       <c r="Y3">
-        <v>0.01247625687154728</v>
+        <v>0.01215012147624479</v>
       </c>
       <c r="Z3">
-        <v>0.033473195502408</v>
+        <v>0.03345465028445944</v>
       </c>
       <c r="AA3">
-        <v>0.01656422188903298</v>
+        <v>0.0161312251088867</v>
       </c>
       <c r="AB3">
-        <v>0.01247590667065828</v>
+        <v>0.01214978042977658</v>
       </c>
       <c r="AC3">
-        <v>0.03347225593031171</v>
+        <v>0.03345371123291607</v>
       </c>
       <c r="AD3">
-        <v>0.01656375694146971</v>
+        <v>0.01613077231527784</v>
       </c>
       <c r="AE3">
-        <v>0.01510875456434375</v>
+        <v>0.01713517570294119</v>
       </c>
       <c r="AF3">
-        <v>0.03076351361915124</v>
+        <v>0.03074646965139233</v>
       </c>
       <c r="AG3">
-        <v>0.02590990676353418</v>
+        <v>0.02938500343951191</v>
       </c>
       <c r="AH3">
-        <v>0.01510875456434375</v>
+        <v>0.01713517570294119</v>
       </c>
       <c r="AI3">
-        <v>0.03076351361915124</v>
+        <v>0.03074646965139233</v>
       </c>
       <c r="AJ3">
-        <v>0.02590990676353418</v>
+        <v>0.02938500343951191</v>
       </c>
       <c r="AK3">
-        <v>0.01857346232618267</v>
+        <v>0.02106457809051863</v>
       </c>
       <c r="AL3">
-        <v>0.03425215949348797</v>
+        <v>0.034233182704643</v>
       </c>
       <c r="AM3">
-        <v>0.02884814361300712</v>
+        <v>0.03271732341718851</v>
       </c>
       <c r="AN3">
-        <v>0.01350701173535654</v>
+        <v>0.01315393190884928</v>
       </c>
       <c r="AO3">
-        <v>0.0351468552775284</v>
+        <v>0.03512738279868242</v>
       </c>
       <c r="AP3">
-        <v>0.01739243298348463</v>
+        <v>0.01693778636433103</v>
       </c>
       <c r="AQ3">
-        <v>0.01350701173535654</v>
+        <v>0.01315393190884928</v>
       </c>
       <c r="AR3">
-        <v>0.0351468552775284</v>
+        <v>0.03512738279868242</v>
       </c>
       <c r="AS3">
-        <v>0.01739243298348463</v>
+        <v>0.01693778636433103</v>
       </c>
       <c r="AT3">
-        <v>0.01510875456434375</v>
+        <v>0.01713517570294119</v>
       </c>
       <c r="AU3">
-        <v>0.03076351361915124</v>
+        <v>0.03074646965139233</v>
       </c>
       <c r="AV3">
-        <v>0.02590990676353418</v>
+        <v>0.02938500343951191</v>
       </c>
       <c r="AW3">
-        <v>0.01510875456434375</v>
+        <v>0.01713517570294119</v>
       </c>
       <c r="AX3">
-        <v>0.03076351361915124</v>
+        <v>0.03074646965139233</v>
       </c>
       <c r="AY3">
-        <v>0.02590990676353418</v>
+        <v>0.02938500343951191</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.02380038338468012</v>
+        <v>0.02747950361229071</v>
       </c>
       <c r="B4">
-        <v>0.03771460539487354</v>
+        <v>0.03769334607640931</v>
       </c>
       <c r="C4">
-        <v>0.02969477620590728</v>
+        <v>0.03428506578350483</v>
       </c>
       <c r="D4">
-        <v>0.02380038338468012</v>
+        <v>0.02747950361229071</v>
       </c>
       <c r="E4">
-        <v>0.03771460539487354</v>
+        <v>0.03769334607640931</v>
       </c>
       <c r="F4">
-        <v>0.02969477620590728</v>
+        <v>0.03428506578350483</v>
       </c>
       <c r="G4">
-        <v>0.02636481726938018</v>
+        <v>0.02598224740166624</v>
       </c>
       <c r="H4">
-        <v>0.03508388400792455</v>
+        <v>0.03506410759888413</v>
       </c>
       <c r="I4">
-        <v>0.04094960980137772</v>
+        <v>0.0403554055387582</v>
       </c>
       <c r="J4">
-        <v>0.003636442935901455</v>
+        <v>0.004198572988421467</v>
       </c>
       <c r="K4">
-        <v>0.007055582505364415</v>
+        <v>0.007051605349197413</v>
       </c>
       <c r="L4">
-        <v>0.005555246868036689</v>
+        <v>0.006413990224865134</v>
       </c>
       <c r="M4">
-        <v>0.02636481726938018</v>
+        <v>0.02598224740166624</v>
       </c>
       <c r="N4">
-        <v>0.03508388400792455</v>
+        <v>0.03506410759888413</v>
       </c>
       <c r="O4">
-        <v>0.04094960980137772</v>
+        <v>0.0403554055387582</v>
       </c>
       <c r="P4">
-        <v>0.02636481726938018</v>
+        <v>0.02598224740166624</v>
       </c>
       <c r="Q4">
-        <v>0.03508388400792455</v>
+        <v>0.03506410759888413</v>
       </c>
       <c r="R4">
-        <v>0.04094960980137772</v>
+        <v>0.0403554055387582</v>
       </c>
       <c r="S4">
-        <v>0.02636481726938018</v>
+        <v>0.02598224740166624</v>
       </c>
       <c r="T4">
-        <v>0.03508388400792455</v>
+        <v>0.03506410759888413</v>
       </c>
       <c r="U4">
-        <v>0.04094960980137772</v>
+        <v>0.0403554055387582</v>
       </c>
       <c r="V4">
-        <v>0.02033296156290272</v>
+        <v>0.02347607942635092</v>
       </c>
       <c r="W4">
-        <v>0.0342860049044305</v>
+        <v>0.03426667825128119</v>
       </c>
       <c r="X4">
-        <v>0.02699525109627935</v>
+        <v>0.03116824162136803</v>
       </c>
       <c r="Y4">
-        <v>0.02033296156290272</v>
+        <v>0.02347607942635092</v>
       </c>
       <c r="Z4">
-        <v>0.0342860049044305</v>
+        <v>0.03426667825128119</v>
       </c>
       <c r="AA4">
-        <v>0.02699525109627935</v>
+        <v>0.03116824162136803</v>
       </c>
       <c r="AB4">
-        <v>0.02033239082912506</v>
+        <v>0.02347542046717991</v>
       </c>
       <c r="AC4">
-        <v>0.03428504251727212</v>
+        <v>0.03426571640661012</v>
       </c>
       <c r="AD4">
-        <v>0.02699449335611496</v>
+        <v>0.03116736674791545</v>
       </c>
       <c r="AE4">
-        <v>0.02144670424185289</v>
+        <v>0.02113549924767929</v>
       </c>
       <c r="AF4">
-        <v>0.03151052545156188</v>
+        <v>0.03149276330640521</v>
       </c>
       <c r="AG4">
-        <v>0.03677881621049666</v>
+        <v>0.03624513275240321</v>
       </c>
       <c r="AH4">
-        <v>0.02144670424185289</v>
+        <v>0.02113549924767929</v>
       </c>
       <c r="AI4">
-        <v>0.03151052545156188</v>
+        <v>0.03149276330640521</v>
       </c>
       <c r="AJ4">
-        <v>0.03677881621049666</v>
+        <v>0.03624513275240321</v>
       </c>
       <c r="AK4">
-        <v>0.02636481726938018</v>
+        <v>0.02598224740166624</v>
       </c>
       <c r="AL4">
-        <v>0.03508388400792455</v>
+        <v>0.03506410759888413</v>
       </c>
       <c r="AM4">
-        <v>0.04094960980137772</v>
+        <v>0.0403554055387582</v>
       </c>
       <c r="AN4">
-        <v>0.02201281628554834</v>
+        <v>0.02541561011259934</v>
       </c>
       <c r="AO4">
-        <v>0.03600030514965202</v>
+        <v>0.03598001216384524</v>
       </c>
       <c r="AP4">
-        <v>0.02834501365109331</v>
+        <v>0.03272665370243642</v>
       </c>
       <c r="AQ4">
-        <v>0.02201281628554834</v>
+        <v>0.02541561011259934</v>
       </c>
       <c r="AR4">
-        <v>0.03600030514965202</v>
+        <v>0.03598001216384524</v>
       </c>
       <c r="AS4">
-        <v>0.02834501365109331</v>
+        <v>0.03272665370243642</v>
       </c>
       <c r="AT4">
-        <v>0.02144670424185289</v>
+        <v>0.02113549924767929</v>
       </c>
       <c r="AU4">
-        <v>0.03151052545156188</v>
+        <v>0.03149276330640521</v>
       </c>
       <c r="AV4">
-        <v>0.03677881621049666</v>
+        <v>0.03624513275240321</v>
       </c>
       <c r="AW4">
-        <v>0.02144670424185289</v>
+        <v>0.02113549924767929</v>
       </c>
       <c r="AX4">
-        <v>0.03151052545156188</v>
+        <v>0.03149276330640521</v>
       </c>
       <c r="AY4">
-        <v>0.03677881621049666</v>
+        <v>0.03624513275240321</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.02123983564831252</v>
+        <v>0.02122733677867073</v>
       </c>
       <c r="B5">
-        <v>0.0386086957370983</v>
+        <v>0.03858657683991322</v>
       </c>
       <c r="C5">
-        <v>0.02650008430674565</v>
+        <v>0.02648448997236706</v>
       </c>
       <c r="D5">
-        <v>0.02123983564831252</v>
+        <v>0.02122733677867073</v>
       </c>
       <c r="E5">
-        <v>0.0386086957370983</v>
+        <v>0.03858657683991322</v>
       </c>
       <c r="F5">
-        <v>0.02650008430674565</v>
+        <v>0.02648448997236706</v>
       </c>
       <c r="G5">
-        <v>0.02856714344291116</v>
+        <v>0.0281744581498477</v>
       </c>
       <c r="H5">
-        <v>0.03591560852236114</v>
+        <v>0.03589503249312527</v>
       </c>
       <c r="I5">
-        <v>0.04437024407090457</v>
+        <v>0.04376032861572089</v>
       </c>
       <c r="J5">
-        <v>0.003245218745204344</v>
+        <v>0.003243309052176254</v>
       </c>
       <c r="K5">
-        <v>0.007222847364979616</v>
+        <v>0.007218709400326851</v>
       </c>
       <c r="L5">
-        <v>0.004957589487354721</v>
+        <v>0.004954672126516063</v>
       </c>
       <c r="M5">
-        <v>0.02856714344291116</v>
+        <v>0.0281744581498477</v>
       </c>
       <c r="N5">
-        <v>0.03591560852236114</v>
+        <v>0.03589503249312527</v>
       </c>
       <c r="O5">
-        <v>0.04437024407090457</v>
+        <v>0.04376032861572089</v>
       </c>
       <c r="P5">
-        <v>0.02856714344291116</v>
+        <v>0.0281744581498477</v>
       </c>
       <c r="Q5">
-        <v>0.03591560852236114</v>
+        <v>0.03589503249312527</v>
       </c>
       <c r="R5">
-        <v>0.04437024407090457</v>
+        <v>0.04376032861572089</v>
       </c>
       <c r="S5">
-        <v>0.02856714344291116</v>
+        <v>0.0281744581498477</v>
       </c>
       <c r="T5">
-        <v>0.03591560852236114</v>
+        <v>0.03589503249312527</v>
       </c>
       <c r="U5">
-        <v>0.04437024407090457</v>
+        <v>0.04376032861572089</v>
       </c>
       <c r="V5">
-        <v>0.01814545399791734</v>
+        <v>0.01813477605916743</v>
       </c>
       <c r="W5">
-        <v>0.035098814306453</v>
+        <v>0.03507870621810293</v>
       </c>
       <c r="X5">
-        <v>0.02409098573340514</v>
+        <v>0.02407680906578824</v>
       </c>
       <c r="Y5">
-        <v>0.01814545399791734</v>
+        <v>0.01813477605916743</v>
       </c>
       <c r="Z5">
-        <v>0.035098814306453</v>
+        <v>0.03507870621810293</v>
       </c>
       <c r="AA5">
-        <v>0.02409098573340514</v>
+        <v>0.02407680906578824</v>
       </c>
       <c r="AB5">
-        <v>0.01814494466613724</v>
+        <v>0.01813426702711052</v>
       </c>
       <c r="AC5">
-        <v>0.03509782910423253</v>
+        <v>0.03507772158030419</v>
       </c>
       <c r="AD5">
-        <v>0.0240903095141907</v>
+        <v>0.02407613324450418</v>
       </c>
       <c r="AE5">
-        <v>0.02323820681914047</v>
+        <v>0.02291877333874088</v>
       </c>
       <c r="AF5">
-        <v>0.03225753728397251</v>
+        <v>0.03223905696141807</v>
       </c>
       <c r="AG5">
-        <v>0.03985105254516429</v>
+        <v>0.03930325810856414</v>
       </c>
       <c r="AH5">
-        <v>0.02323820681914047</v>
+        <v>0.02291877333874088</v>
       </c>
       <c r="AI5">
-        <v>0.03225753728397251</v>
+        <v>0.03223905696141807</v>
       </c>
       <c r="AJ5">
-        <v>0.03985105254516429</v>
+        <v>0.03930325810856414</v>
       </c>
       <c r="AK5">
-        <v>0.02856714344291116</v>
+        <v>0.0281744581498477</v>
       </c>
       <c r="AL5">
-        <v>0.03591560852236114</v>
+        <v>0.03589503249312527</v>
       </c>
       <c r="AM5">
-        <v>0.04437024407090457</v>
+        <v>0.04376032861572089</v>
       </c>
       <c r="AN5">
-        <v>0.01964458271552452</v>
+        <v>0.01963302259412838</v>
       </c>
       <c r="AO5">
-        <v>0.03685375502177565</v>
+        <v>0.03683264152900807</v>
       </c>
       <c r="AP5">
-        <v>0.0252955350200754</v>
+        <v>0.02528064951907764</v>
       </c>
       <c r="AQ5">
-        <v>0.01964458271552452</v>
+        <v>0.01963302259412838</v>
       </c>
       <c r="AR5">
-        <v>0.03685375502177565</v>
+        <v>0.03683264152900807</v>
       </c>
       <c r="AS5">
-        <v>0.0252955350200754</v>
+        <v>0.02528064951907764</v>
       </c>
       <c r="AT5">
-        <v>0.02323820681914047</v>
+        <v>0.02291877333874088</v>
       </c>
       <c r="AU5">
-        <v>0.03225753728397251</v>
+        <v>0.03223905696141807</v>
       </c>
       <c r="AV5">
-        <v>0.03985105254516429</v>
+        <v>0.03930325810856414</v>
       </c>
       <c r="AW5">
-        <v>0.02323820681914047</v>
+        <v>0.02291877333874088</v>
       </c>
       <c r="AX5">
-        <v>0.03225753728397251</v>
+        <v>0.03223905696141807</v>
       </c>
       <c r="AY5">
-        <v>0.03985105254516429</v>
+        <v>0.03930325810856414</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.02261615274301138</v>
+        <v>0.02260565303072172</v>
       </c>
       <c r="B6">
-        <v>0.03977248296902747</v>
+        <v>0.03974627504669438</v>
       </c>
       <c r="C6">
-        <v>0.02821725950745078</v>
+        <v>0.02820415944088344</v>
       </c>
       <c r="D6">
-        <v>0.02261615274301138</v>
+        <v>0.02260565303072172</v>
       </c>
       <c r="E6">
-        <v>0.03977248296902747</v>
+        <v>0.03974627504669438</v>
       </c>
       <c r="F6">
-        <v>0.02821725950745078</v>
+        <v>0.02820415944088344</v>
       </c>
       <c r="G6">
-        <v>0.02397922234784575</v>
+        <v>0.02699715920064775</v>
       </c>
       <c r="H6">
-        <v>0.03699821765554477</v>
+        <v>0.03697383782450595</v>
       </c>
       <c r="I6">
-        <v>0.03724432407218595</v>
+        <v>0.04193175790738905</v>
       </c>
       <c r="J6">
-        <v>0.003455505213942476</v>
+        <v>0.003453900970684391</v>
       </c>
       <c r="K6">
-        <v>0.007440566647671146</v>
+        <v>0.007435663715335535</v>
       </c>
       <c r="L6">
-        <v>0.005278835624703611</v>
+        <v>0.005276384887130622</v>
       </c>
       <c r="M6">
-        <v>0.02397922234784575</v>
+        <v>0.02699715920064775</v>
       </c>
       <c r="N6">
-        <v>0.03699821765554477</v>
+        <v>0.03697383782450595</v>
       </c>
       <c r="O6">
-        <v>0.03724432407218595</v>
+        <v>0.04193175790738905</v>
       </c>
       <c r="P6">
-        <v>0.02397922234784575</v>
+        <v>0.02699715920064775</v>
       </c>
       <c r="Q6">
-        <v>0.03699821765554477</v>
+        <v>0.03697383782450595</v>
       </c>
       <c r="R6">
-        <v>0.03724432407218595</v>
+        <v>0.04193175790738905</v>
       </c>
       <c r="S6">
-        <v>0.02397922234784575</v>
+        <v>0.02699715920064775</v>
       </c>
       <c r="T6">
-        <v>0.03699821765554477</v>
+        <v>0.03697383782450595</v>
       </c>
       <c r="U6">
-        <v>0.03724432407218595</v>
+        <v>0.04193175790738905</v>
       </c>
       <c r="V6">
-        <v>0.01932125869536986</v>
+        <v>0.01931228866144409</v>
       </c>
       <c r="W6">
-        <v>0.03615680269911589</v>
+        <v>0.03613297731517671</v>
       </c>
       <c r="X6">
-        <v>0.02565205409768254</v>
+        <v>0.02564014494625768</v>
       </c>
       <c r="Y6">
-        <v>0.01932125869536986</v>
+        <v>0.01931228866144409</v>
       </c>
       <c r="Z6">
-        <v>0.03615680269911589</v>
+        <v>0.03613297731517671</v>
       </c>
       <c r="AA6">
-        <v>0.02565205409768254</v>
+        <v>0.02564014494625768</v>
       </c>
       <c r="AB6">
-        <v>0.01932071635947205</v>
+        <v>0.01931174657732963</v>
       </c>
       <c r="AC6">
-        <v>0.03615578779980922</v>
+        <v>0.03613196308463398</v>
       </c>
       <c r="AD6">
-        <v>0.02565133406023523</v>
+        <v>0.02563942524309295</v>
       </c>
       <c r="AE6">
-        <v>0.01950612000793767</v>
+        <v>0.02196108862923752</v>
       </c>
       <c r="AF6">
-        <v>0.03322988067210966</v>
+        <v>0.03320798397200998</v>
       </c>
       <c r="AG6">
-        <v>0.03345092069446332</v>
+        <v>0.03766093071311795</v>
       </c>
       <c r="AH6">
-        <v>0.01950612000793767</v>
+        <v>0.02196108862923752</v>
       </c>
       <c r="AI6">
-        <v>0.03322988067210966</v>
+        <v>0.03320798397200998</v>
       </c>
       <c r="AJ6">
-        <v>0.03345092069446332</v>
+        <v>0.03766093071311795</v>
       </c>
       <c r="AK6">
-        <v>0.02397922234784575</v>
+        <v>0.02699715920064775</v>
       </c>
       <c r="AL6">
-        <v>0.03699821765554477</v>
+        <v>0.03697383782450595</v>
       </c>
       <c r="AM6">
-        <v>0.03724432407218595</v>
+        <v>0.04193175790738905</v>
       </c>
       <c r="AN6">
-        <v>0.02091752924191397</v>
+        <v>0.02090781812785552</v>
       </c>
       <c r="AO6">
-        <v>0.03796464283407167</v>
+        <v>0.03793962618093554</v>
       </c>
       <c r="AP6">
-        <v>0.02693465680256666</v>
+        <v>0.02692215219357056</v>
       </c>
       <c r="AQ6">
-        <v>0.02091752924191397</v>
+        <v>0.02090781812785552</v>
       </c>
       <c r="AR6">
-        <v>0.03796464283407167</v>
+        <v>0.03793962618093554</v>
       </c>
       <c r="AS6">
-        <v>0.02693465680256666</v>
+        <v>0.02692215219357056</v>
       </c>
       <c r="AT6">
-        <v>0.01950612000793767</v>
+        <v>0.02196108862923752</v>
       </c>
       <c r="AU6">
-        <v>0.03322988067210966</v>
+        <v>0.03320798397200998</v>
       </c>
       <c r="AV6">
-        <v>0.03345092069446332</v>
+        <v>0.03766093071311795</v>
       </c>
       <c r="AW6">
-        <v>0.01950612000793767</v>
+        <v>0.02196108862923752</v>
       </c>
       <c r="AX6">
-        <v>0.03322988067210966</v>
+        <v>0.03320798397200998</v>
       </c>
       <c r="AY6">
-        <v>0.03345092069446332</v>
+        <v>0.03766093071311795</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.02389526882647277</v>
+        <v>0.02388567210132279</v>
       </c>
       <c r="B7">
-        <v>0.04069109121031626</v>
+        <v>0.0406637301232235</v>
       </c>
       <c r="C7">
-        <v>0.02981316093583751</v>
+        <v>0.0298011874898206</v>
       </c>
       <c r="D7">
-        <v>0.02389526882647277</v>
+        <v>0.02388567210132279</v>
       </c>
       <c r="E7">
-        <v>0.04069109121031626</v>
+        <v>0.0406637301232235</v>
       </c>
       <c r="F7">
-        <v>0.02981316093583751</v>
+        <v>0.0298011874898206</v>
       </c>
       <c r="G7">
-        <v>0.02214616139544141</v>
+        <v>0.02556141052849559</v>
       </c>
       <c r="H7">
-        <v>0.03785274986259472</v>
+        <v>0.03782729730394159</v>
       </c>
       <c r="I7">
-        <v>0.03439722940143027</v>
+        <v>0.03970176528893996</v>
       </c>
       <c r="J7">
-        <v>0.003650940412221474</v>
+        <v>0.003649474135699143</v>
       </c>
       <c r="K7">
-        <v>0.007612418273020559</v>
+        <v>0.007607299608635814</v>
       </c>
       <c r="L7">
-        <v>0.00557739407654259</v>
+        <v>0.005575154105174434</v>
       </c>
       <c r="M7">
-        <v>0.02214616139544141</v>
+        <v>0.02556141052849559</v>
       </c>
       <c r="N7">
-        <v>0.03785274986259472</v>
+        <v>0.03782729730394159</v>
       </c>
       <c r="O7">
-        <v>0.03439722940143027</v>
+        <v>0.03970176528893996</v>
       </c>
       <c r="P7">
-        <v>0.02214616139544141</v>
+        <v>0.02556141052849559</v>
       </c>
       <c r="Q7">
-        <v>0.03785274986259472</v>
+        <v>0.03782729730394159</v>
       </c>
       <c r="R7">
-        <v>0.03439722940143027</v>
+        <v>0.03970176528893996</v>
       </c>
       <c r="S7">
-        <v>0.02214616139544141</v>
+        <v>0.02556141052849559</v>
       </c>
       <c r="T7">
-        <v>0.03785274986259472</v>
+        <v>0.03782729730394159</v>
       </c>
       <c r="U7">
-        <v>0.03439722940143027</v>
+        <v>0.03970176528893996</v>
       </c>
       <c r="V7">
-        <v>0.02041402336807056</v>
+        <v>0.02040582476721399</v>
       </c>
       <c r="W7">
-        <v>0.03699190110028751</v>
+        <v>0.03696702738474864</v>
       </c>
       <c r="X7">
-        <v>0.0271028735780341</v>
+        <v>0.02709198862710964</v>
       </c>
       <c r="Y7">
-        <v>0.02041402336807056</v>
+        <v>0.02040582476721399</v>
       </c>
       <c r="Z7">
-        <v>0.03699190110028751</v>
+        <v>0.03696702738474864</v>
       </c>
       <c r="AA7">
-        <v>0.0271028735780341</v>
+        <v>0.02709198862710964</v>
       </c>
       <c r="AB7">
-        <v>0.02041345035893768</v>
+        <v>0.02040525198821081</v>
       </c>
       <c r="AC7">
-        <v>0.0369908627602802</v>
+        <v>0.03696598974293129</v>
       </c>
       <c r="AD7">
-        <v>0.02710211281697257</v>
+        <v>0.02709122817158201</v>
       </c>
       <c r="AE7">
-        <v>0.01801499963711063</v>
+        <v>0.02079316560429617</v>
       </c>
       <c r="AF7">
-        <v>0.03399737719140453</v>
+        <v>0.03397451702298458</v>
       </c>
       <c r="AG7">
-        <v>0.03089380788832164</v>
+        <v>0.03565806697247385</v>
       </c>
       <c r="AH7">
-        <v>0.01801499963711063</v>
+        <v>0.02079316560429617</v>
       </c>
       <c r="AI7">
-        <v>0.03399737719140453</v>
+        <v>0.03397451702298458</v>
       </c>
       <c r="AJ7">
-        <v>0.03089380788832164</v>
+        <v>0.03565806697247385</v>
       </c>
       <c r="AK7">
-        <v>0.02214616139544141</v>
+        <v>0.02556141052849559</v>
       </c>
       <c r="AL7">
-        <v>0.03785274986259472</v>
+        <v>0.03782729730394159</v>
       </c>
       <c r="AM7">
-        <v>0.03439722940143027</v>
+        <v>0.03970176528893996</v>
       </c>
       <c r="AN7">
-        <v>0.02210057519953706</v>
+        <v>0.02209169925227794</v>
       </c>
       <c r="AO7">
-        <v>0.03884149615530188</v>
+        <v>0.03881537875398607</v>
       </c>
       <c r="AP7">
-        <v>0.0284580172569358</v>
+        <v>0.02844658805846512</v>
       </c>
       <c r="AQ7">
-        <v>0.02210057519953706</v>
+        <v>0.02209169925227794</v>
       </c>
       <c r="AR7">
-        <v>0.03884149615530188</v>
+        <v>0.03881537875398607</v>
       </c>
       <c r="AS7">
-        <v>0.0284580172569358</v>
+        <v>0.02844658805846512</v>
       </c>
       <c r="AT7">
-        <v>0.01801499963711063</v>
+        <v>0.02079316560429617</v>
       </c>
       <c r="AU7">
-        <v>0.03399737719140453</v>
+        <v>0.03397451702298458</v>
       </c>
       <c r="AV7">
-        <v>0.03089380788832164</v>
+        <v>0.03565806697247385</v>
       </c>
       <c r="AW7">
-        <v>0.01801499963711063</v>
+        <v>0.02079316560429617</v>
       </c>
       <c r="AX7">
-        <v>0.03399737719140453</v>
+        <v>0.03397451702298458</v>
       </c>
       <c r="AY7">
-        <v>0.03089380788832164</v>
+        <v>0.03565806697247385</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.01647820741399939</v>
+        <v>0.01647060556068213</v>
       </c>
       <c r="B8">
-        <v>0.0315050087974284</v>
+        <v>0.03148917935793227</v>
       </c>
       <c r="C8">
-        <v>0.02055919325014732</v>
+        <v>0.02054970872507234</v>
       </c>
       <c r="D8">
-        <v>0.01647820741399939</v>
+        <v>0.01647060556068213</v>
       </c>
       <c r="E8">
-        <v>0.0315050087974284</v>
+        <v>0.03148917935793227</v>
       </c>
       <c r="F8">
-        <v>0.02055919325014732</v>
+        <v>0.02054970872507234</v>
       </c>
       <c r="G8">
-        <v>0.02307927789969434</v>
+        <v>0.01996357207874159</v>
       </c>
       <c r="H8">
-        <v>0.0293074277920952</v>
+        <v>0.02929270250958521</v>
       </c>
       <c r="I8">
-        <v>0.03584653801441887</v>
+        <v>0.03100725024996033</v>
       </c>
       <c r="J8">
-        <v>0.00251769309672246</v>
+        <v>0.0025165316151888</v>
       </c>
       <c r="K8">
-        <v>0.005893902019526435</v>
+        <v>0.005890940675633023</v>
       </c>
       <c r="L8">
-        <v>0.003846177964780267</v>
+        <v>0.003844403616394805</v>
       </c>
       <c r="M8">
-        <v>0.02307927789969434</v>
+        <v>0.01996357207874159</v>
       </c>
       <c r="N8">
-        <v>0.0293074277920952</v>
+        <v>0.02929270250958521</v>
       </c>
       <c r="O8">
-        <v>0.03584653801441887</v>
+        <v>0.03100725024996033</v>
       </c>
       <c r="P8">
-        <v>0.02307927789969434</v>
+        <v>0.01996357207874159</v>
       </c>
       <c r="Q8">
-        <v>0.0293074277920952</v>
+        <v>0.02929270250958521</v>
       </c>
       <c r="R8">
-        <v>0.03584653801441887</v>
+        <v>0.03100725024996033</v>
       </c>
       <c r="S8">
-        <v>0.02307927789969434</v>
+        <v>0.01996357207874159</v>
       </c>
       <c r="T8">
-        <v>0.0293074277920952</v>
+        <v>0.02929270250958521</v>
       </c>
       <c r="U8">
-        <v>0.03584653801441887</v>
+        <v>0.03100725024996033</v>
       </c>
       <c r="V8">
-        <v>0.01407753617070111</v>
+        <v>0.01407104181349651</v>
       </c>
       <c r="W8">
-        <v>0.02864091708857127</v>
+        <v>0.02862652668902934</v>
       </c>
       <c r="X8">
-        <v>0.01869017568195212</v>
+        <v>0.0186815533864294</v>
       </c>
       <c r="Y8">
-        <v>0.01407753617070111</v>
+        <v>0.01407104181349651</v>
       </c>
       <c r="Z8">
-        <v>0.02864091708857127</v>
+        <v>0.02862652668902934</v>
       </c>
       <c r="AA8">
-        <v>0.01869017568195212</v>
+        <v>0.0186815533864294</v>
       </c>
       <c r="AB8">
-        <v>0.01407714102288293</v>
+        <v>0.01407064684797095</v>
       </c>
       <c r="AC8">
-        <v>0.02864011315557041</v>
+        <v>0.02862572315995818</v>
       </c>
       <c r="AD8">
-        <v>0.01868965106016797</v>
+        <v>0.01868102900666781</v>
       </c>
       <c r="AE8">
-        <v>0.01877405188031151</v>
+        <v>0.01623955218839826</v>
       </c>
       <c r="AF8">
-        <v>0.02632241199845588</v>
+        <v>0.02630918651323857</v>
       </c>
       <c r="AG8">
-        <v>0.03219550173517251</v>
+        <v>0.02784910439116808</v>
       </c>
       <c r="AH8">
-        <v>0.01877405188031151</v>
+        <v>0.01623955218839826</v>
       </c>
       <c r="AI8">
-        <v>0.02632241199845588</v>
+        <v>0.02630918651323857</v>
       </c>
       <c r="AJ8">
-        <v>0.03219550173517251</v>
+        <v>0.02784910439116808</v>
       </c>
       <c r="AK8">
-        <v>0.02307927789969434</v>
+        <v>0.01996357207874159</v>
       </c>
       <c r="AL8">
-        <v>0.0293074277920952</v>
+        <v>0.02929270250958521</v>
       </c>
       <c r="AM8">
-        <v>0.03584653801441887</v>
+        <v>0.03100725024996033</v>
       </c>
       <c r="AN8">
-        <v>0.01524058443331687</v>
+        <v>0.01523355352974704</v>
       </c>
       <c r="AO8">
-        <v>0.03007296294299983</v>
+        <v>0.03005785302348081</v>
       </c>
       <c r="AP8">
-        <v>0.01962468446604972</v>
+        <v>0.01961563105575087</v>
       </c>
       <c r="AQ8">
-        <v>0.01524058443331687</v>
+        <v>0.01523355352974704</v>
       </c>
       <c r="AR8">
-        <v>0.03007296294299983</v>
+        <v>0.03005785302348081</v>
       </c>
       <c r="AS8">
-        <v>0.01962468446604972</v>
+        <v>0.01961563105575087</v>
       </c>
       <c r="AT8">
-        <v>0.01877405188031151</v>
+        <v>0.01623955218839826</v>
       </c>
       <c r="AU8">
-        <v>0.02632241199845588</v>
+        <v>0.02630918651323857</v>
       </c>
       <c r="AV8">
-        <v>0.03219550173517251</v>
+        <v>0.02784910439116808</v>
       </c>
       <c r="AW8">
-        <v>0.01877405188031151</v>
+        <v>0.01623955218839826</v>
       </c>
       <c r="AX8">
-        <v>0.02632241199845588</v>
+        <v>0.02630918651323857</v>
       </c>
       <c r="AY8">
-        <v>0.03219550173517251</v>
+        <v>0.02784910439116808</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.01686857906728747</v>
+        <v>0.02127595415812239</v>
       </c>
       <c r="B9">
-        <v>0.04160969945160504</v>
+        <v>0.04158118519975262</v>
       </c>
       <c r="C9">
-        <v>0.02104624418097312</v>
+        <v>0.02654514791132546</v>
       </c>
       <c r="D9">
-        <v>0.01686857906728747</v>
+        <v>0.02127595415812239</v>
       </c>
       <c r="E9">
-        <v>0.04160969945160504</v>
+        <v>0.04158118519975262</v>
       </c>
       <c r="F9">
-        <v>0.02104624418097312</v>
+        <v>0.02654514791132546</v>
       </c>
       <c r="G9">
-        <v>0.01716954003942577</v>
+        <v>0.02068289050448551</v>
       </c>
       <c r="H9">
-        <v>0.03870728206964467</v>
+        <v>0.03868075678337723</v>
       </c>
       <c r="I9">
-        <v>0.02666758346549108</v>
+        <v>0.03212448950696685</v>
       </c>
       <c r="J9">
-        <v>0.002577337692275039</v>
+        <v>0.003250737265546246</v>
       </c>
       <c r="K9">
-        <v>0.00778426989836997</v>
+        <v>0.007778935501936093</v>
       </c>
       <c r="L9">
-        <v>0.003937294602241443</v>
+        <v>0.004966019907791924</v>
       </c>
       <c r="M9">
-        <v>0.01716954003942577</v>
+        <v>0.02068289050448551</v>
       </c>
       <c r="N9">
-        <v>0.03870728206964467</v>
+        <v>0.03868075678337723</v>
       </c>
       <c r="O9">
-        <v>0.02666758346549108</v>
+        <v>0.03212448950696685</v>
       </c>
       <c r="P9">
-        <v>0.01716954003942577</v>
+        <v>0.02068289050448551</v>
       </c>
       <c r="Q9">
-        <v>0.03870728206964467</v>
+        <v>0.03868075678337723</v>
       </c>
       <c r="R9">
-        <v>0.02666758346549108</v>
+        <v>0.03212448950696685</v>
       </c>
       <c r="S9">
-        <v>0.01716954003942577</v>
+        <v>0.02068289050448551</v>
       </c>
       <c r="T9">
-        <v>0.03870728206964467</v>
+        <v>0.03868075678337723</v>
       </c>
       <c r="U9">
-        <v>0.02666758346549108</v>
+        <v>0.03212448950696685</v>
       </c>
       <c r="V9">
-        <v>0.01441103549687845</v>
+        <v>0.01817631048706727</v>
       </c>
       <c r="W9">
-        <v>0.03782699950145913</v>
+        <v>0.03780107745432057</v>
       </c>
       <c r="X9">
-        <v>0.01913294925543011</v>
+        <v>0.02413195264665952</v>
       </c>
       <c r="Y9">
-        <v>0.01441103549687845</v>
+        <v>0.01817631048706727</v>
       </c>
       <c r="Z9">
-        <v>0.03782699950145913</v>
+        <v>0.03780107745432057</v>
       </c>
       <c r="AA9">
-        <v>0.01913294925543011</v>
+        <v>0.02413195264665952</v>
       </c>
       <c r="AB9">
-        <v>0.01441063098793844</v>
+        <v>0.01817580028916441</v>
       </c>
       <c r="AC9">
-        <v>0.03782593772075118</v>
+        <v>0.0378000164012286</v>
       </c>
       <c r="AD9">
-        <v>0.01913241220526295</v>
+        <v>0.02413127527752892</v>
       </c>
       <c r="AE9">
-        <v>0.01396672100670594</v>
+        <v>0.0168246884089539</v>
       </c>
       <c r="AF9">
-        <v>0.03476487371069939</v>
+        <v>0.03474105007395918</v>
       </c>
       <c r="AG9">
-        <v>0.02395144070511699</v>
+        <v>0.0288525507608869</v>
       </c>
       <c r="AH9">
-        <v>0.01396672100670594</v>
+        <v>0.0168246884089539</v>
       </c>
       <c r="AI9">
-        <v>0.03476487371069939</v>
+        <v>0.03474105007395918</v>
       </c>
       <c r="AJ9">
-        <v>0.02395144070511699</v>
+        <v>0.0288525507608869</v>
       </c>
       <c r="AK9">
-        <v>0.01716954003942577</v>
+        <v>0.02068289050448551</v>
       </c>
       <c r="AL9">
-        <v>0.03870728206964467</v>
+        <v>0.03868075678337723</v>
       </c>
       <c r="AM9">
-        <v>0.02666758346549108</v>
+        <v>0.03212448950696685</v>
       </c>
       <c r="AN9">
-        <v>0.0156016365789074</v>
+        <v>0.01967798848500739</v>
       </c>
       <c r="AO9">
-        <v>0.03971834947653208</v>
+        <v>0.03969113132703659</v>
       </c>
       <c r="AP9">
-        <v>0.02008959671820162</v>
+        <v>0.02533855027899249</v>
       </c>
       <c r="AQ9">
-        <v>0.0156016365789074</v>
+        <v>0.01967798848500739</v>
       </c>
       <c r="AR9">
-        <v>0.03971834947653208</v>
+        <v>0.03969113132703659</v>
       </c>
       <c r="AS9">
-        <v>0.02008959671820162</v>
+        <v>0.02533855027899249</v>
       </c>
       <c r="AT9">
-        <v>0.01396672100670594</v>
+        <v>0.0168246884089539</v>
       </c>
       <c r="AU9">
-        <v>0.03476487371069939</v>
+        <v>0.03474105007395918</v>
       </c>
       <c r="AV9">
-        <v>0.02395144070511699</v>
+        <v>0.0288525507608869</v>
       </c>
       <c r="AW9">
-        <v>0.01396672100670594</v>
+        <v>0.0168246884089539</v>
       </c>
       <c r="AX9">
-        <v>0.03476487371069939</v>
+        <v>0.03474105007395918</v>
       </c>
       <c r="AY9">
-        <v>0.02395144070511699</v>
+        <v>0.0288525507608869</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.141998875151762</v>
+        <v>0.137943802762931</v>
       </c>
       <c r="B10">
-        <v>0.2969460008586314</v>
+        <v>0.2964693904867735</v>
       </c>
       <c r="C10">
-        <v>0.1771662561467941</v>
+        <v>0.172106906255708</v>
       </c>
       <c r="D10">
-        <v>0.141998875151762</v>
+        <v>0.137943802762931</v>
       </c>
       <c r="E10">
-        <v>0.2969460008586314</v>
+        <v>0.2964693904867735</v>
       </c>
       <c r="F10">
-        <v>0.1771662561467941</v>
+        <v>0.172106906255708</v>
       </c>
       <c r="G10">
-        <v>0.06402290023288615</v>
+        <v>0.06081241335533492</v>
       </c>
       <c r="H10">
-        <v>0.2762330121623753</v>
+        <v>0.2757896469772391</v>
       </c>
       <c r="I10">
-        <v>0.09943982376597209</v>
+        <v>0.0944533228710521</v>
       </c>
       <c r="J10">
-        <v>0.02169590288129376</v>
+        <v>0.0210763313767261</v>
       </c>
       <c r="K10">
-        <v>0.05555213919806441</v>
+        <v>0.0554629757621396</v>
       </c>
       <c r="L10">
-        <v>0.03314395376333812</v>
+        <v>0.03219745942231773</v>
       </c>
       <c r="M10">
-        <v>0.06402290023288615</v>
+        <v>0.06081241335533492</v>
       </c>
       <c r="N10">
-        <v>0.2762330121623753</v>
+        <v>0.2757896469772391</v>
       </c>
       <c r="O10">
-        <v>0.09943982376597209</v>
+        <v>0.0944533228710521</v>
       </c>
       <c r="P10">
-        <v>0.06402290023288615</v>
+        <v>0.06081241335533492</v>
       </c>
       <c r="Q10">
-        <v>0.2762330121623753</v>
+        <v>0.2757896469772391</v>
       </c>
       <c r="R10">
-        <v>0.09943982376597209</v>
+        <v>0.0944533228710521</v>
       </c>
       <c r="S10">
-        <v>0.06402290023288615</v>
+        <v>0.06081241335533492</v>
       </c>
       <c r="T10">
-        <v>0.2762330121623753</v>
+        <v>0.2757896469772391</v>
       </c>
       <c r="U10">
-        <v>0.09943982376597209</v>
+        <v>0.0944533228710521</v>
       </c>
       <c r="V10">
-        <v>0.1213113933406079</v>
+        <v>0.1178470949011987</v>
       </c>
       <c r="W10">
-        <v>0.2699509098714831</v>
+        <v>0.2695176277152487</v>
       </c>
       <c r="X10">
-        <v>0.1610602328607219</v>
+        <v>0.1564608238688254</v>
       </c>
       <c r="Y10">
-        <v>0.1213113933406079</v>
+        <v>0.1178470949011987</v>
       </c>
       <c r="Z10">
-        <v>0.2699509098714831</v>
+        <v>0.2695176277152487</v>
       </c>
       <c r="AA10">
-        <v>0.1610602328607219</v>
+        <v>0.1564608238688254</v>
       </c>
       <c r="AB10">
-        <v>0.1213079882040969</v>
+        <v>0.1178437870054231</v>
       </c>
       <c r="AC10">
-        <v>0.2699433325147809</v>
+        <v>0.2695100625205112</v>
       </c>
       <c r="AD10">
-        <v>0.1610557119986307</v>
+        <v>0.1564564321093276</v>
       </c>
       <c r="AE10">
-        <v>0.05208001982228964</v>
+        <v>0.04946841960402613</v>
       </c>
       <c r="AF10">
-        <v>0.2480981683310223</v>
+        <v>0.2476999607110389</v>
       </c>
       <c r="AG10">
-        <v>0.08931169356758606</v>
+        <v>0.08483307702307459</v>
       </c>
       <c r="AH10">
-        <v>0.05208001982228964</v>
+        <v>0.04946841960402613</v>
       </c>
       <c r="AI10">
-        <v>0.2480981683310223</v>
+        <v>0.2476999607110389</v>
       </c>
       <c r="AJ10">
-        <v>0.08931169356758606</v>
+        <v>0.08483307702307459</v>
       </c>
       <c r="AK10">
-        <v>0.06402290023288615</v>
+        <v>0.06081241335533492</v>
       </c>
       <c r="AL10">
-        <v>0.2762330121623753</v>
+        <v>0.2757896469772391</v>
       </c>
       <c r="AM10">
-        <v>0.09943982376597209</v>
+        <v>0.0944533228710521</v>
       </c>
       <c r="AN10">
-        <v>0.1313338151301491</v>
+        <v>0.1275833056498106</v>
       </c>
       <c r="AO10">
-        <v>0.2834484553650572</v>
+        <v>0.2829935091010111</v>
       </c>
       <c r="AP10">
-        <v>0.169113244503758</v>
+        <v>0.1642838650622667</v>
       </c>
       <c r="AQ10">
-        <v>0.1313338151301491</v>
+        <v>0.1275833056498106</v>
       </c>
       <c r="AR10">
-        <v>0.2834484553650572</v>
+        <v>0.2829935091010111</v>
       </c>
       <c r="AS10">
-        <v>0.169113244503758</v>
+        <v>0.1642838650622667</v>
       </c>
       <c r="AT10">
-        <v>0.05208001982228964</v>
+        <v>0.04946841960402613</v>
       </c>
       <c r="AU10">
-        <v>0.2480981683310223</v>
+        <v>0.2476999607110389</v>
       </c>
       <c r="AV10">
-        <v>0.08931169356758606</v>
+        <v>0.08483307702307459</v>
       </c>
       <c r="AW10">
-        <v>0.05208001982228964</v>
+        <v>0.04946841960402613</v>
       </c>
       <c r="AX10">
-        <v>0.2480981683310223</v>
+        <v>0.2476999607110389</v>
       </c>
       <c r="AY10">
-        <v>0.08931169356758606</v>
+        <v>0.08483307702307459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change the calculation of the LW quadratic to work on grazing days rather than days and separate wheat and barley stubble. Profit +$65K, +25% stock numbers
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDCE2DB-4E4E-415F-B6C2-875F99FD70B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +68,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +122,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -130,9 +154,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,6 +206,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -339,1561 +399,1563 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection sqref="A1:AY10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.05482790899252283</v>
+        <v>0.17069334575684059</v>
       </c>
       <c r="B1">
-        <v>0.2868948076594419</v>
+        <v>0.17729592423753929</v>
       </c>
       <c r="C1">
-        <v>0.06840656560258593</v>
+        <v>0.21296718713151341</v>
       </c>
       <c r="D1">
-        <v>0.05482790899252283</v>
+        <v>0.17069334575684059</v>
       </c>
       <c r="E1">
-        <v>0.2868948076594419</v>
+        <v>0.17729592423753929</v>
       </c>
       <c r="F1">
-        <v>0.06840656560258593</v>
+        <v>0.21296718713151341</v>
       </c>
       <c r="G1">
-        <v>0.04740812681074145</v>
+        <v>1.297240195222021E-2</v>
       </c>
       <c r="H1">
-        <v>0.2668829237112434</v>
+        <v>0.16492893339069939</v>
       </c>
       <c r="I1">
-        <v>0.07363389908902396</v>
+        <v>2.0148624308767561E-2</v>
       </c>
       <c r="J1">
-        <v>0.008377115575140016</v>
+        <v>2.648605191673075E-3</v>
       </c>
       <c r="K1">
-        <v>0.05367177952966182</v>
+        <v>1.7435530794102039E-2</v>
       </c>
       <c r="L1">
-        <v>0.01279738081478836</v>
+        <v>4.0461670800452506E-3</v>
       </c>
       <c r="M1">
-        <v>0.04740812681074145</v>
+        <v>1.297240195222021E-2</v>
       </c>
       <c r="N1">
-        <v>0.2668829237112434</v>
+        <v>0.16492893339069939</v>
       </c>
       <c r="O1">
-        <v>0.07363389908902396</v>
+        <v>2.0148624308767561E-2</v>
       </c>
       <c r="P1">
-        <v>0.04740812681074145</v>
+        <v>1.297240195222021E-2</v>
       </c>
       <c r="Q1">
-        <v>0.2668829237112434</v>
+        <v>0.16492893339069939</v>
       </c>
       <c r="R1">
-        <v>0.07363389908902396</v>
+        <v>2.0148624308767561E-2</v>
       </c>
       <c r="S1">
-        <v>0.04740812681074145</v>
+        <v>6.1451309414891804E-3</v>
       </c>
       <c r="T1">
-        <v>0.2668829237112434</v>
+        <v>0.1599499218526465</v>
       </c>
       <c r="U1">
-        <v>0.07363389908902396</v>
+        <v>9.5445650793342558E-3</v>
       </c>
       <c r="V1">
-        <v>0.04684016001342569</v>
+        <v>1.480952362153405E-2</v>
       </c>
       <c r="W1">
-        <v>0.2608134615085836</v>
+        <v>8.4726483442497266E-2</v>
       </c>
       <c r="X1">
-        <v>0.06218778691144176</v>
+        <v>1.966200582944095E-2</v>
       </c>
       <c r="Y1">
-        <v>0.04684016001342569</v>
+        <v>1.480952362153405E-2</v>
       </c>
       <c r="Z1">
-        <v>0.2608134615085836</v>
+        <v>8.4726483442497266E-2</v>
       </c>
       <c r="AA1">
-        <v>0.06218778691144176</v>
+        <v>1.966200582944095E-2</v>
       </c>
       <c r="AB1">
-        <v>0.04683884523882249</v>
+        <v>1.480910792727644E-2</v>
       </c>
       <c r="AC1">
-        <v>0.2608061406344605</v>
+        <v>8.4724105221999801E-2</v>
       </c>
       <c r="AD1">
-        <v>0.06218604133835155</v>
+        <v>1.9661453928979781E-2</v>
       </c>
       <c r="AE1">
-        <v>0.03856457884694195</v>
+        <v>2.4282338717033108E-3</v>
       </c>
       <c r="AF1">
-        <v>0.2397004037036168</v>
+        <v>0.14813061610090589</v>
       </c>
       <c r="AG1">
-        <v>0.06613415010773449</v>
+        <v>4.1641627672188699E-3</v>
       </c>
       <c r="AH1">
-        <v>0.03856457884694195</v>
+        <v>2.4282338717033108E-3</v>
       </c>
       <c r="AI1">
-        <v>0.2397004037036168</v>
+        <v>0.14813061610090589</v>
       </c>
       <c r="AJ1">
-        <v>0.06613415010773449</v>
+        <v>4.1641627672188699E-3</v>
       </c>
       <c r="AK1">
-        <v>0.04740812681074145</v>
+        <v>6.1451309414891804E-3</v>
       </c>
       <c r="AL1">
-        <v>0.2668829237112434</v>
+        <v>0.1599499218526465</v>
       </c>
       <c r="AM1">
-        <v>0.07363389908902396</v>
+        <v>9.5445650793342558E-3</v>
       </c>
       <c r="AN1">
-        <v>0.05070996834236039</v>
+        <v>3.7293384562146182E-3</v>
       </c>
       <c r="AO1">
-        <v>0.2738541345840128</v>
+        <v>0.16923701859037851</v>
       </c>
       <c r="AP1">
-        <v>0.06529717625701384</v>
+        <v>4.80211836957678E-3</v>
       </c>
       <c r="AQ1">
-        <v>0.05070996834236039</v>
+        <v>3.7293384562146182E-3</v>
       </c>
       <c r="AR1">
-        <v>0.2738541345840128</v>
+        <v>0.16923701859037851</v>
       </c>
       <c r="AS1">
-        <v>0.06529717625701384</v>
+        <v>4.80211836957678E-3</v>
       </c>
       <c r="AT1">
-        <v>0.03856457884694195</v>
+        <v>2.4282338717033108E-3</v>
       </c>
       <c r="AU1">
-        <v>0.2397004037036168</v>
+        <v>0.14813061610090589</v>
       </c>
       <c r="AV1">
-        <v>0.06613415010773449</v>
+        <v>4.1641627672188699E-3</v>
       </c>
       <c r="AW1">
-        <v>0.03856457884694195</v>
+        <v>2.4282338717033108E-3</v>
       </c>
       <c r="AX1">
-        <v>0.2397004037036168</v>
+        <v>0.14813061610090589</v>
       </c>
       <c r="AY1">
-        <v>0.06613415010773449</v>
+        <v>4.1641627672188699E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.01717818715579903</v>
+        <v>3.4935840886530872E-2</v>
       </c>
       <c r="B2">
-        <v>0.03590688454940147</v>
+        <v>1.6117811294321761E-2</v>
       </c>
       <c r="C2">
-        <v>0.02143252967693735</v>
+        <v>4.3588036374173827E-2</v>
       </c>
       <c r="D2">
-        <v>0.01717818715579903</v>
+        <v>3.4935840886530872E-2</v>
       </c>
       <c r="E2">
-        <v>0.03590688454940147</v>
+        <v>1.6117811294321761E-2</v>
       </c>
       <c r="F2">
-        <v>0.02143252967693735</v>
+        <v>4.3588036374173827E-2</v>
       </c>
       <c r="G2">
-        <v>0.01655864727677222</v>
+        <v>4.7365913074357252E-2</v>
       </c>
       <c r="H2">
-        <v>0.03340225781040188</v>
+        <v>1.4993539399154489E-2</v>
       </c>
       <c r="I2">
-        <v>0.02571875002562493</v>
+        <v>7.3568333072937836E-2</v>
       </c>
       <c r="J2">
-        <v>0.002624642482629406</v>
+        <v>5.4147474403530467E-3</v>
       </c>
       <c r="K2">
-        <v>0.006717397246938537</v>
+        <v>1.585048254009276E-3</v>
       </c>
       <c r="L2">
-        <v>0.004009560218144497</v>
+        <v>8.271890770581887E-3</v>
       </c>
       <c r="M2">
-        <v>0.01655864727677222</v>
+        <v>4.7365913074357252E-2</v>
       </c>
       <c r="N2">
-        <v>0.03340225781040188</v>
+        <v>1.4993539399154489E-2</v>
       </c>
       <c r="O2">
-        <v>0.02571875002562493</v>
+        <v>7.3568333072937836E-2</v>
       </c>
       <c r="P2">
-        <v>0.01655864727677222</v>
+        <v>4.7365913074357252E-2</v>
       </c>
       <c r="Q2">
-        <v>0.03340225781040188</v>
+        <v>1.4993539399154489E-2</v>
       </c>
       <c r="R2">
-        <v>0.02571875002562493</v>
+        <v>7.3568333072937836E-2</v>
       </c>
       <c r="S2">
-        <v>0.01655864727677222</v>
+        <v>5.5864826740810729E-4</v>
       </c>
       <c r="T2">
-        <v>0.03340225781040188</v>
+        <v>1.4540901986604231E-2</v>
       </c>
       <c r="U2">
-        <v>0.02571875002562493</v>
+        <v>8.6768773448493242E-4</v>
       </c>
       <c r="V2">
-        <v>0.01467553751188892</v>
+        <v>3.027624893836859E-2</v>
       </c>
       <c r="W2">
-        <v>0.0326426223176377</v>
+        <v>7.7024075856815689E-3</v>
       </c>
       <c r="X2">
-        <v>0.01948411788812486</v>
+        <v>4.0196551782004243E-2</v>
       </c>
       <c r="Y2">
-        <v>0.01467553751188892</v>
+        <v>3.027624893836859E-2</v>
       </c>
       <c r="Z2">
-        <v>0.0326426223176377</v>
+        <v>7.7024075856815689E-3</v>
       </c>
       <c r="AA2">
-        <v>0.01948411788812486</v>
+        <v>4.0196551782004243E-2</v>
       </c>
       <c r="AB2">
-        <v>0.01467512557853935</v>
+        <v>3.0275399102604302E-2</v>
       </c>
       <c r="AC2">
-        <v>0.032641706059222</v>
+        <v>7.7021913838181627E-3</v>
       </c>
       <c r="AD2">
-        <v>0.01948357098086926</v>
+        <v>4.0195423489415058E-2</v>
       </c>
       <c r="AE2">
-        <v>0.01346978464373956</v>
+        <v>2.2074853379121009E-4</v>
       </c>
       <c r="AF2">
-        <v>0.03000017599637947</v>
+        <v>1.34664196455369E-2</v>
       </c>
       <c r="AG2">
-        <v>0.02309924770820018</v>
+        <v>3.7856025156535167E-4</v>
       </c>
       <c r="AH2">
-        <v>0.01346978464373956</v>
+        <v>2.2074853379121009E-4</v>
       </c>
       <c r="AI2">
-        <v>0.03000017599637947</v>
+        <v>1.34664196455369E-2</v>
       </c>
       <c r="AJ2">
-        <v>0.02309924770820018</v>
+        <v>3.7856025156535167E-4</v>
       </c>
       <c r="AK2">
-        <v>0.01655864727677222</v>
+        <v>5.5864826740810729E-4</v>
       </c>
       <c r="AL2">
-        <v>0.03340225781040188</v>
+        <v>1.4540901986604231E-2</v>
       </c>
       <c r="AM2">
-        <v>0.02571875002562493</v>
+        <v>8.6768773448493242E-4</v>
       </c>
       <c r="AN2">
-        <v>0.01588799104063057</v>
+        <v>3.3903076874678339E-4</v>
       </c>
       <c r="AO2">
-        <v>0.03427475343351959</v>
+        <v>1.5385183508216219E-2</v>
       </c>
       <c r="AP2">
-        <v>0.0204583237825311</v>
+        <v>4.3655621541607089E-4</v>
       </c>
       <c r="AQ2">
-        <v>0.01588799104063057</v>
+        <v>3.3903076874678339E-4</v>
       </c>
       <c r="AR2">
-        <v>0.03427475343351959</v>
+        <v>1.5385183508216219E-2</v>
       </c>
       <c r="AS2">
-        <v>0.0204583237825311</v>
+        <v>4.3655621541607089E-4</v>
       </c>
       <c r="AT2">
-        <v>0.01346978464373956</v>
+        <v>2.2074853379121009E-4</v>
       </c>
       <c r="AU2">
-        <v>0.03000017599637947</v>
+        <v>1.34664196455369E-2</v>
       </c>
       <c r="AV2">
-        <v>0.02309924770820018</v>
+        <v>3.7856025156535167E-4</v>
       </c>
       <c r="AW2">
-        <v>0.01346978464373956</v>
+        <v>2.2074853379121009E-4</v>
       </c>
       <c r="AX2">
-        <v>0.03000017599637947</v>
+        <v>1.34664196455369E-2</v>
       </c>
       <c r="AY2">
-        <v>0.02309924770820018</v>
+        <v>3.7856025156535167E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.01422210672117057</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="B3">
-        <v>0.03680011531290539</v>
+        <v>0.22635979242130261</v>
       </c>
       <c r="C3">
-        <v>0.01774434761977536</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="D3">
-        <v>0.01422210672117057</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="E3">
-        <v>0.03680011531290539</v>
+        <v>0.22635979242130261</v>
       </c>
       <c r="F3">
-        <v>0.01774434761977536</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="G3">
-        <v>0.02106457809051863</v>
+        <v>9.076573040146127E-2</v>
       </c>
       <c r="H3">
-        <v>0.034233182704643</v>
+        <v>0.2105704306917219</v>
       </c>
       <c r="I3">
-        <v>0.03271732341718851</v>
+        <v>0.14097655998524841</v>
       </c>
       <c r="J3">
-        <v>0.002172985144143821</v>
+        <v>2.6848141865304379E-2</v>
       </c>
       <c r="K3">
-        <v>0.006884501298067975</v>
+        <v>4.0916750876948918E-2</v>
       </c>
       <c r="L3">
-        <v>0.003319581560628219</v>
+        <v>4.1014820977209668E-2</v>
       </c>
       <c r="M3">
-        <v>0.02106457809051863</v>
+        <v>9.076573040146127E-2</v>
       </c>
       <c r="N3">
-        <v>0.034233182704643</v>
+        <v>0.2105704306917219</v>
       </c>
       <c r="O3">
-        <v>0.03271732341718851</v>
+        <v>0.14097655998524841</v>
       </c>
       <c r="P3">
-        <v>0.02106457809051863</v>
+        <v>9.076573040146127E-2</v>
       </c>
       <c r="Q3">
-        <v>0.034233182704643</v>
+        <v>0.2105704306917219</v>
       </c>
       <c r="R3">
-        <v>0.03271732341718851</v>
+        <v>0.14097655998524841</v>
       </c>
       <c r="S3">
-        <v>0.02106457809051863</v>
+        <v>0.1325050224731904</v>
       </c>
       <c r="T3">
-        <v>0.034233182704643</v>
+        <v>1.4540901986604231E-2</v>
       </c>
       <c r="U3">
-        <v>0.03271732341718851</v>
+        <v>0.20580567320304041</v>
       </c>
       <c r="V3">
-        <v>0.01215012147624479</v>
+        <v>0.15011984134085329</v>
       </c>
       <c r="W3">
-        <v>0.03345465028445944</v>
+        <v>0.19883148133748241</v>
       </c>
       <c r="X3">
-        <v>0.0161312251088867</v>
+        <v>0.19930804467381369</v>
       </c>
       <c r="Y3">
-        <v>0.01215012147624479</v>
+        <v>0.15011984134085329</v>
       </c>
       <c r="Z3">
-        <v>0.03345465028445944</v>
+        <v>0.19883148133748241</v>
       </c>
       <c r="AA3">
-        <v>0.0161312251088867</v>
+        <v>0.19930804467381369</v>
       </c>
       <c r="AB3">
-        <v>0.01214978042977658</v>
+        <v>0.15011562756885141</v>
       </c>
       <c r="AC3">
-        <v>0.03345371123291607</v>
+        <v>0.1988259002595803</v>
       </c>
       <c r="AD3">
-        <v>0.01613077231527784</v>
+        <v>0.1993024502190707</v>
       </c>
       <c r="AE3">
-        <v>0.01713517570294119</v>
+        <v>0.1097450235421261</v>
       </c>
       <c r="AF3">
-        <v>0.03074646965139233</v>
+        <v>0.189123442380528</v>
       </c>
       <c r="AG3">
-        <v>0.02938500343951191</v>
+        <v>0.18820104037224189</v>
       </c>
       <c r="AH3">
-        <v>0.01713517570294119</v>
+        <v>0.1097450235421261</v>
       </c>
       <c r="AI3">
-        <v>0.03074646965139233</v>
+        <v>0.189123442380528</v>
       </c>
       <c r="AJ3">
-        <v>0.02938500343951191</v>
+        <v>0.18820104037224189</v>
       </c>
       <c r="AK3">
-        <v>0.02106457809051863</v>
+        <v>0.1325050224731904</v>
       </c>
       <c r="AL3">
-        <v>0.034233182704643</v>
+        <v>1.4540901986604231E-2</v>
       </c>
       <c r="AM3">
-        <v>0.03271732341718851</v>
+        <v>0.20580567320304041</v>
       </c>
       <c r="AN3">
-        <v>0.01315393190884928</v>
+        <v>0.14144991040144761</v>
       </c>
       <c r="AO3">
-        <v>0.03512738279868242</v>
+        <v>0.21607071094760699</v>
       </c>
       <c r="AP3">
-        <v>0.01693778636433103</v>
+        <v>0.18213933143607669</v>
       </c>
       <c r="AQ3">
-        <v>0.01315393190884928</v>
+        <v>0.14144991040144761</v>
       </c>
       <c r="AR3">
-        <v>0.03512738279868242</v>
+        <v>0.21607071094760699</v>
       </c>
       <c r="AS3">
-        <v>0.01693778636433103</v>
+        <v>0.18213933143607669</v>
       </c>
       <c r="AT3">
-        <v>0.01713517570294119</v>
+        <v>0.1097450235421261</v>
       </c>
       <c r="AU3">
-        <v>0.03074646965139233</v>
+        <v>0.189123442380528</v>
       </c>
       <c r="AV3">
-        <v>0.02938500343951191</v>
+        <v>0.18820104037224189</v>
       </c>
       <c r="AW3">
-        <v>0.01713517570294119</v>
+        <v>0.1097450235421261</v>
       </c>
       <c r="AX3">
-        <v>0.03074646965139233</v>
+        <v>0.189123442380528</v>
       </c>
       <c r="AY3">
-        <v>0.02938500343951191</v>
+        <v>0.18820104037224189</v>
       </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.02747950361229071</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="B4">
-        <v>0.03769334607640931</v>
+        <v>0.22409796236541021</v>
       </c>
       <c r="C4">
-        <v>0.03428506578350483</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="D4">
-        <v>0.02747950361229071</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="E4">
-        <v>0.03769334607640931</v>
+        <v>0.22409796236541021</v>
       </c>
       <c r="F4">
-        <v>0.03428506578350483</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="G4">
-        <v>0.02598224740166624</v>
+        <v>7.298818546593154E-2</v>
       </c>
       <c r="H4">
-        <v>0.03506410759888413</v>
+        <v>0.2084663709383259</v>
       </c>
       <c r="I4">
-        <v>0.0403554055387582</v>
+        <v>0.1133646284896383</v>
       </c>
       <c r="J4">
-        <v>0.004198572988421467</v>
+        <v>1.087073643375785E-2</v>
       </c>
       <c r="K4">
-        <v>0.007051605349197413</v>
+        <v>4.0493611660579687E-2</v>
       </c>
       <c r="L4">
-        <v>0.006413990224865134</v>
+        <v>1.6606784594549229E-2</v>
       </c>
       <c r="M4">
-        <v>0.02598224740166624</v>
+        <v>7.298818546593154E-2</v>
       </c>
       <c r="N4">
-        <v>0.03506410759888413</v>
+        <v>0.2084663709383259</v>
       </c>
       <c r="O4">
-        <v>0.0403554055387582</v>
+        <v>0.1133646284896383</v>
       </c>
       <c r="P4">
-        <v>0.02598224740166624</v>
+        <v>7.298818546593154E-2</v>
       </c>
       <c r="Q4">
-        <v>0.03506410759888413</v>
+        <v>0.2084663709383259</v>
       </c>
       <c r="R4">
-        <v>0.0403554055387582</v>
+        <v>0.1133646284896383</v>
       </c>
       <c r="S4">
-        <v>0.02598224740166624</v>
+        <v>7.2401354595038783E-2</v>
       </c>
       <c r="T4">
-        <v>0.03506410759888413</v>
+        <v>6.4787130329130305E-2</v>
       </c>
       <c r="U4">
-        <v>0.0403554055387582</v>
+        <v>0.11245316777527301</v>
       </c>
       <c r="V4">
-        <v>0.02347607942635092</v>
+        <v>6.0783097649035799E-2</v>
       </c>
       <c r="W4">
-        <v>0.03426667825128119</v>
+        <v>0.19677527219576199</v>
       </c>
       <c r="X4">
-        <v>0.03116824162136803</v>
+        <v>8.0699261559570926E-2</v>
       </c>
       <c r="Y4">
-        <v>0.02347607942635092</v>
+        <v>6.0783097649035799E-2</v>
       </c>
       <c r="Z4">
-        <v>0.03426667825128119</v>
+        <v>0.19677527219576199</v>
       </c>
       <c r="AA4">
-        <v>0.03116824162136803</v>
+        <v>8.0699261559570926E-2</v>
       </c>
       <c r="AB4">
-        <v>0.02347542046717991</v>
+        <v>6.0781391504712859E-2</v>
       </c>
       <c r="AC4">
-        <v>0.03426571640661012</v>
+        <v>0.19676974883439119</v>
       </c>
       <c r="AD4">
-        <v>0.03116736674791545</v>
+        <v>8.0696996380725139E-2</v>
       </c>
       <c r="AE4">
-        <v>0.02113549924767929</v>
+        <v>5.8708077211763743E-2</v>
       </c>
       <c r="AF4">
-        <v>0.03149276330640521</v>
+        <v>0.18723368500942231</v>
       </c>
       <c r="AG4">
-        <v>0.03624513275240321</v>
+        <v>0.1006781068780459</v>
       </c>
       <c r="AH4">
-        <v>0.02113549924767929</v>
+        <v>5.8708077211763743E-2</v>
       </c>
       <c r="AI4">
-        <v>0.03149276330640521</v>
+        <v>0.18723368500942231</v>
       </c>
       <c r="AJ4">
-        <v>0.03624513275240321</v>
+        <v>0.1006781068780459</v>
       </c>
       <c r="AK4">
-        <v>0.02598224740166624</v>
+        <v>7.2401354595038783E-2</v>
       </c>
       <c r="AL4">
-        <v>0.03506410759888413</v>
+        <v>6.4787130329130305E-2</v>
       </c>
       <c r="AM4">
-        <v>0.0403554055387582</v>
+        <v>0.11245316777527301</v>
       </c>
       <c r="AN4">
-        <v>0.02541561011259934</v>
+        <v>0.1112871408980786</v>
       </c>
       <c r="AO4">
-        <v>0.03598001216384524</v>
+        <v>0.21391169134880059</v>
       </c>
       <c r="AP4">
-        <v>0.03272665370243642</v>
+        <v>0.14329995249258959</v>
       </c>
       <c r="AQ4">
-        <v>0.02541561011259934</v>
+        <v>0.1112871408980786</v>
       </c>
       <c r="AR4">
-        <v>0.03598001216384524</v>
+        <v>0.21391169134880059</v>
       </c>
       <c r="AS4">
-        <v>0.03272665370243642</v>
+        <v>0.14329995249258959</v>
       </c>
       <c r="AT4">
-        <v>0.02113549924767929</v>
+        <v>5.8708077211763743E-2</v>
       </c>
       <c r="AU4">
-        <v>0.03149276330640521</v>
+        <v>0.18723368500942231</v>
       </c>
       <c r="AV4">
-        <v>0.03624513275240321</v>
+        <v>0.1006781068780459</v>
       </c>
       <c r="AW4">
-        <v>0.02113549924767929</v>
+        <v>5.8708077211763743E-2</v>
       </c>
       <c r="AX4">
-        <v>0.03149276330640521</v>
+        <v>0.18723368500942231</v>
       </c>
       <c r="AY4">
-        <v>0.03624513275240321</v>
+        <v>0.1006781068780459</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.02122733677867073</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="B5">
-        <v>0.03858657683991322</v>
+        <v>9.653105386736166E-2</v>
       </c>
       <c r="C5">
-        <v>0.02648448997236706</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="D5">
-        <v>0.02122733677867073</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="E5">
-        <v>0.03858657683991322</v>
+        <v>9.653105386736166E-2</v>
       </c>
       <c r="F5">
-        <v>0.02648448997236706</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="G5">
-        <v>0.0281744581498477</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="H5">
-        <v>0.03589503249312527</v>
+        <v>8.9797686110897973E-2</v>
       </c>
       <c r="I5">
-        <v>0.04376032861572089</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="J5">
-        <v>0.003243309052176254</v>
+        <v>3.7948247542115591E-3</v>
       </c>
       <c r="K5">
-        <v>0.007218709400326851</v>
+        <v>1.6628617225702289E-2</v>
       </c>
       <c r="L5">
-        <v>0.004954672126516063</v>
+        <v>5.7972003691997842E-3</v>
       </c>
       <c r="M5">
-        <v>0.0281744581498477</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="N5">
-        <v>0.03589503249312527</v>
+        <v>8.9797686110897973E-2</v>
       </c>
       <c r="O5">
-        <v>0.04376032861572089</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="P5">
-        <v>0.0281744581498477</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="Q5">
-        <v>0.03589503249312527</v>
+        <v>8.9797686110897973E-2</v>
       </c>
       <c r="R5">
-        <v>0.04376032861572089</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="S5">
-        <v>0.0281744581498477</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="T5">
-        <v>0.03589503249312527</v>
+        <v>0.24834049582135209</v>
       </c>
       <c r="U5">
-        <v>0.04376032861572089</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="V5">
-        <v>0.01813477605916743</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="W5">
-        <v>0.03507870621810293</v>
+        <v>8.0805355379354224E-2</v>
       </c>
       <c r="X5">
-        <v>0.02407680906578824</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="Y5">
-        <v>0.01813477605916743</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="Z5">
-        <v>0.03507870621810293</v>
+        <v>8.0805355379354224E-2</v>
       </c>
       <c r="AA5">
-        <v>0.02407680906578824</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="AB5">
-        <v>0.01813426702711052</v>
+        <v>2.121794880071198E-2</v>
       </c>
       <c r="AC5">
-        <v>0.03507772158030419</v>
+        <v>8.0803087222519915E-2</v>
       </c>
       <c r="AD5">
-        <v>0.02407613324450418</v>
+        <v>2.8170212875838881E-2</v>
       </c>
       <c r="AE5">
-        <v>0.02291877333874088</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AF5">
-        <v>0.03223905696141807</v>
+        <v>8.065162548849171E-2</v>
       </c>
       <c r="AG5">
-        <v>0.03930325810856414</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AH5">
-        <v>0.02291877333874088</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AI5">
-        <v>0.03223905696141807</v>
+        <v>8.065162548849171E-2</v>
       </c>
       <c r="AJ5">
-        <v>0.03930325810856414</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AK5">
-        <v>0.0281744581498477</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="AL5">
-        <v>0.03589503249312527</v>
+        <v>0.24834049582135209</v>
       </c>
       <c r="AM5">
-        <v>0.04376032861572089</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="AN5">
-        <v>0.01963302259412838</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AO5">
-        <v>0.03683264152900807</v>
+        <v>9.2143278691572489E-2</v>
       </c>
       <c r="AP5">
-        <v>0.02528064951907764</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AQ5">
-        <v>0.01963302259412838</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AR5">
-        <v>0.03683264152900807</v>
+        <v>9.2143278691572489E-2</v>
       </c>
       <c r="AS5">
-        <v>0.02528064951907764</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AT5">
-        <v>0.02291877333874088</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AU5">
-        <v>0.03223905696141807</v>
+        <v>8.065162548849171E-2</v>
       </c>
       <c r="AV5">
-        <v>0.03930325810856414</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AW5">
-        <v>0.02291877333874088</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AX5">
-        <v>0.03223905696141807</v>
+        <v>8.065162548849171E-2</v>
       </c>
       <c r="AY5">
-        <v>0.03930325810856414</v>
+        <v>2.501921987221041E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.02260565303072172</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="B6">
-        <v>0.03974627504669438</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="C6">
-        <v>0.02820415944088344</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="D6">
-        <v>0.02260565303072172</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="E6">
-        <v>0.03974627504669438</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="F6">
-        <v>0.02820415944088344</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="G6">
-        <v>0.02699715920064775</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="H6">
-        <v>0.03697383782450595</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="I6">
-        <v>0.04193175790738905</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="J6">
-        <v>0.003453900970684391</v>
+        <v>3.7948247542115591E-3</v>
       </c>
       <c r="K6">
-        <v>0.007435663715335535</v>
+        <v>9.1232782183906184E-3</v>
       </c>
       <c r="L6">
-        <v>0.005276384887130622</v>
+        <v>5.7972003691997842E-3</v>
       </c>
       <c r="M6">
-        <v>0.02699715920064775</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="N6">
-        <v>0.03697383782450595</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="O6">
-        <v>0.04193175790738905</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="P6">
-        <v>0.02699715920064775</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="Q6">
-        <v>0.03697383782450595</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="R6">
-        <v>0.04193175790738905</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="S6">
-        <v>0.02699715920064775</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="T6">
-        <v>0.03697383782450595</v>
+        <v>0.16034481276636189</v>
       </c>
       <c r="U6">
-        <v>0.04193175790738905</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="V6">
-        <v>0.01931228866144409</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="W6">
-        <v>0.03613297731517671</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="X6">
-        <v>0.02564014494625768</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="Y6">
-        <v>0.01931228866144409</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="Z6">
-        <v>0.03613297731517671</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="AA6">
-        <v>0.02564014494625768</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="AB6">
-        <v>0.01931174657732963</v>
+        <v>2.121794880071198E-2</v>
       </c>
       <c r="AC6">
-        <v>0.03613196308463398</v>
+        <v>4.4332552468432873E-2</v>
       </c>
       <c r="AD6">
-        <v>0.02563942524309295</v>
+        <v>2.8170212875838881E-2</v>
       </c>
       <c r="AE6">
-        <v>0.02196108862923752</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AF6">
-        <v>0.03320798397200998</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AG6">
-        <v>0.03766093071311795</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AH6">
-        <v>0.02196108862923752</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AI6">
-        <v>0.03320798397200998</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AJ6">
-        <v>0.03766093071311795</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AK6">
-        <v>0.02699715920064775</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="AL6">
-        <v>0.03697383782450595</v>
+        <v>0.16034481276636189</v>
       </c>
       <c r="AM6">
-        <v>0.04193175790738905</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="AN6">
-        <v>0.02090781812785552</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AO6">
-        <v>0.03793962618093554</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AP6">
-        <v>0.02692215219357056</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AQ6">
-        <v>0.02090781812785552</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AR6">
-        <v>0.03793962618093554</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AS6">
-        <v>0.02692215219357056</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AT6">
-        <v>0.02196108862923752</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AU6">
-        <v>0.03320798397200998</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AV6">
-        <v>0.03766093071311795</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AW6">
-        <v>0.02196108862923752</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AX6">
-        <v>0.03320798397200998</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AY6">
-        <v>0.03766093071311795</v>
+        <v>2.501921987221041E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.02388567210132279</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="B7">
-        <v>0.0406637301232235</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="C7">
-        <v>0.0298011874898206</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="D7">
-        <v>0.02388567210132279</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="E7">
-        <v>0.0406637301232235</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="F7">
-        <v>0.0298011874898206</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="G7">
-        <v>0.02556141052849559</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="H7">
-        <v>0.03782729730394159</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="I7">
-        <v>0.03970176528893996</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="J7">
-        <v>0.003649474135699143</v>
+        <v>3.7948247542115591E-3</v>
       </c>
       <c r="K7">
-        <v>0.007607299608635814</v>
+        <v>9.1232782183906184E-3</v>
       </c>
       <c r="L7">
-        <v>0.005575154105174434</v>
+        <v>5.7972003691997842E-3</v>
       </c>
       <c r="M7">
-        <v>0.02556141052849559</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="N7">
-        <v>0.03782729730394159</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="O7">
-        <v>0.03970176528893996</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="P7">
-        <v>0.02556141052849559</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="Q7">
-        <v>0.03782729730394159</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="R7">
-        <v>0.03970176528893996</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="S7">
-        <v>0.02556141052849559</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="T7">
-        <v>0.03782729730394159</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="U7">
-        <v>0.03970176528893996</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="V7">
-        <v>0.02040582476721399</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="W7">
-        <v>0.03696702738474864</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="X7">
-        <v>0.02709198862710964</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="Y7">
-        <v>0.02040582476721399</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="Z7">
-        <v>0.03696702738474864</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="AA7">
-        <v>0.02709198862710964</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="AB7">
-        <v>0.02040525198821081</v>
+        <v>2.121794880071198E-2</v>
       </c>
       <c r="AC7">
-        <v>0.03696598974293129</v>
+        <v>4.4332552468432873E-2</v>
       </c>
       <c r="AD7">
-        <v>0.02709122817158201</v>
+        <v>2.8170212875838881E-2</v>
       </c>
       <c r="AE7">
-        <v>0.02079316560429617</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AF7">
-        <v>0.03397451702298458</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AG7">
-        <v>0.03565806697247385</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AH7">
-        <v>0.02079316560429617</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AI7">
-        <v>0.03397451702298458</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AJ7">
-        <v>0.03565806697247385</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AK7">
-        <v>0.02556141052849559</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="AL7">
-        <v>0.03782729730394159</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="AM7">
-        <v>0.03970176528893996</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="AN7">
-        <v>0.02209169925227794</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AO7">
-        <v>0.03881537875398607</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AP7">
-        <v>0.02844658805846512</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AQ7">
-        <v>0.02209169925227794</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AR7">
-        <v>0.03881537875398607</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AS7">
-        <v>0.02844658805846512</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AT7">
-        <v>0.02079316560429617</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AU7">
-        <v>0.03397451702298458</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AV7">
-        <v>0.03565806697247385</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AW7">
-        <v>0.02079316560429617</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AX7">
-        <v>0.03397451702298458</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AY7">
-        <v>0.03565806697247385</v>
+        <v>2.501921987221041E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.01647060556068213</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="B8">
-        <v>0.03148917935793227</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="C8">
-        <v>0.02054970872507234</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="D8">
-        <v>0.01647060556068213</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="E8">
-        <v>0.03148917935793227</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="F8">
-        <v>0.02054970872507234</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="G8">
-        <v>0.01996357207874159</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="H8">
-        <v>0.02929270250958521</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="I8">
-        <v>0.03100725024996033</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="J8">
-        <v>0.0025165316151888</v>
+        <v>3.7948247542115591E-3</v>
       </c>
       <c r="K8">
-        <v>0.005890940675633023</v>
+        <v>9.1232782183906184E-3</v>
       </c>
       <c r="L8">
-        <v>0.003844403616394805</v>
+        <v>5.7972003691997842E-3</v>
       </c>
       <c r="M8">
-        <v>0.01996357207874159</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="N8">
-        <v>0.02929270250958521</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="O8">
-        <v>0.03100725024996033</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="P8">
-        <v>0.01996357207874159</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="Q8">
-        <v>0.02929270250958521</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="R8">
-        <v>0.03100725024996033</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="S8">
-        <v>0.01996357207874159</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="T8">
-        <v>0.02929270250958521</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="U8">
-        <v>0.03100725024996033</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="V8">
-        <v>0.01407104181349651</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="W8">
-        <v>0.02862652668902934</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="X8">
-        <v>0.0186815533864294</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="Y8">
-        <v>0.01407104181349651</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="Z8">
-        <v>0.02862652668902934</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="AA8">
-        <v>0.0186815533864294</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="AB8">
-        <v>0.01407064684797095</v>
+        <v>2.121794880071198E-2</v>
       </c>
       <c r="AC8">
-        <v>0.02862572315995818</v>
+        <v>4.4332552468432873E-2</v>
       </c>
       <c r="AD8">
-        <v>0.01868102900666781</v>
+        <v>2.8170212875838881E-2</v>
       </c>
       <c r="AE8">
-        <v>0.01623955218839826</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AF8">
-        <v>0.02630918651323857</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AG8">
-        <v>0.02784910439116808</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AH8">
-        <v>0.01623955218839826</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AI8">
-        <v>0.02630918651323857</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AJ8">
-        <v>0.02784910439116808</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AK8">
-        <v>0.01996357207874159</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="AL8">
-        <v>0.02929270250958521</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="AM8">
-        <v>0.03100725024996033</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="AN8">
-        <v>0.01523355352974704</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AO8">
-        <v>0.03005785302348081</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AP8">
-        <v>0.01961563105575087</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AQ8">
-        <v>0.01523355352974704</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AR8">
-        <v>0.03005785302348081</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AS8">
-        <v>0.01961563105575087</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AT8">
-        <v>0.01623955218839826</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AU8">
-        <v>0.02630918651323857</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AV8">
-        <v>0.02784910439116808</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AW8">
-        <v>0.01623955218839826</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AX8">
-        <v>0.02630918651323857</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AY8">
-        <v>0.02784910439116808</v>
+        <v>2.501921987221041E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.02127595415812239</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="B9">
-        <v>0.04158118519975262</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="C9">
-        <v>0.02654514791132546</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="D9">
-        <v>0.02127595415812239</v>
+        <v>1.7282873614216911E-2</v>
       </c>
       <c r="E9">
-        <v>0.04158118519975262</v>
+        <v>5.641233953012615E-2</v>
       </c>
       <c r="F9">
-        <v>0.02654514791132546</v>
+        <v>2.156314273909956E-2</v>
       </c>
       <c r="G9">
-        <v>0.02068289050448551</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="H9">
-        <v>0.03868075678337723</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="I9">
-        <v>0.03212448950696685</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="J9">
-        <v>0.003250737265546246</v>
+        <v>3.7948247542115591E-3</v>
       </c>
       <c r="K9">
-        <v>0.007778935501936093</v>
+        <v>9.1232782183906184E-3</v>
       </c>
       <c r="L9">
-        <v>0.004966019907791924</v>
+        <v>5.7972003691997842E-3</v>
       </c>
       <c r="M9">
-        <v>0.02068289050448551</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="N9">
-        <v>0.03868075678337723</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="O9">
-        <v>0.03212448950696685</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="P9">
-        <v>0.02068289050448551</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="Q9">
-        <v>0.03868075678337723</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="R9">
-        <v>0.03212448950696685</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="S9">
-        <v>0.02068289050448551</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="T9">
-        <v>0.03868075678337723</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="U9">
-        <v>0.03212448950696685</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="V9">
-        <v>0.01817631048706727</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="W9">
-        <v>0.03780107745432057</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="X9">
-        <v>0.02413195264665952</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="Y9">
-        <v>0.01817631048706727</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="Z9">
-        <v>0.03780107745432057</v>
+        <v>4.4333796890958288E-2</v>
       </c>
       <c r="AA9">
-        <v>0.02413195264665952</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="AB9">
-        <v>0.01817580028916441</v>
+        <v>2.121794880071198E-2</v>
       </c>
       <c r="AC9">
-        <v>0.0378000164012286</v>
+        <v>4.4332552468432873E-2</v>
       </c>
       <c r="AD9">
-        <v>0.02413127527752892</v>
+        <v>2.8170212875838881E-2</v>
       </c>
       <c r="AE9">
-        <v>0.0168246884089539</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AF9">
-        <v>0.03474105007395918</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AG9">
-        <v>0.0288525507608869</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AH9">
-        <v>0.0168246884089539</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AI9">
-        <v>0.03474105007395918</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AJ9">
-        <v>0.0288525507608869</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AK9">
-        <v>0.02068289050448551</v>
+        <v>1.7994462413373071E-2</v>
       </c>
       <c r="AL9">
-        <v>0.03868075678337723</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="AM9">
-        <v>0.03212448950696685</v>
+        <v>2.7948845876090089E-2</v>
       </c>
       <c r="AN9">
-        <v>0.01967798848500739</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AO9">
-        <v>0.03969113132703659</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AP9">
-        <v>0.02533855027899249</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AQ9">
-        <v>0.01967798848500739</v>
+        <v>2.2087278766677831E-2</v>
       </c>
       <c r="AR9">
-        <v>0.03969113132703659</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AS9">
-        <v>0.02533855027899249</v>
+        <v>2.8440895977858351E-2</v>
       </c>
       <c r="AT9">
-        <v>0.0168246884089539</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AU9">
-        <v>0.03474105007395918</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AV9">
-        <v>0.0288525507608869</v>
+        <v>2.501921987221041E-2</v>
       </c>
       <c r="AW9">
-        <v>0.0168246884089539</v>
+        <v>1.4589371389502351E-2</v>
       </c>
       <c r="AX9">
-        <v>0.03474105007395918</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AY9">
-        <v>0.0288525507608869</v>
+        <v>2.501921987221041E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.137943802762931</v>
+        <v>2.3879560197959209E-2</v>
       </c>
       <c r="B10">
-        <v>0.2964693904867735</v>
+        <v>3.3948097693559776E-2</v>
       </c>
       <c r="C10">
-        <v>0.172106906255708</v>
+        <v>2.97935619150708E-2</v>
       </c>
       <c r="D10">
-        <v>0.137943802762931</v>
+        <v>2.3879560197959209E-2</v>
       </c>
       <c r="E10">
-        <v>0.2964693904867735</v>
+        <v>3.3948097693559776E-2</v>
       </c>
       <c r="F10">
-        <v>0.172106906255708</v>
+        <v>2.97935619150708E-2</v>
       </c>
       <c r="G10">
-        <v>0.06081241335533492</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="H10">
-        <v>0.2757896469772391</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="I10">
-        <v>0.0944533228710521</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="J10">
-        <v>0.0210763313767261</v>
+        <v>3.7948247542115591E-3</v>
       </c>
       <c r="K10">
-        <v>0.0554629757621396</v>
+        <v>2.485595926756648E-2</v>
       </c>
       <c r="L10">
-        <v>0.03219745942231773</v>
+        <v>5.7972003691997842E-3</v>
       </c>
       <c r="M10">
-        <v>0.06081241335533492</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="N10">
-        <v>0.2757896469772391</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="O10">
-        <v>0.0944533228710521</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="P10">
-        <v>0.06081241335533492</v>
+        <v>1.8581293284265839E-2</v>
       </c>
       <c r="Q10">
-        <v>0.2757896469772391</v>
+        <v>5.2477387897040713E-2</v>
       </c>
       <c r="R10">
-        <v>0.0944533228710521</v>
+        <v>2.8860306590455451E-2</v>
       </c>
       <c r="S10">
-        <v>0.06081241335533492</v>
+        <v>2.4842262226883429E-2</v>
       </c>
       <c r="T10">
-        <v>0.2757896469772391</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="U10">
-        <v>0.0944533228710521</v>
+        <v>3.858479026728702E-2</v>
       </c>
       <c r="V10">
-        <v>0.1178470949011987</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="W10">
-        <v>0.2695176277152487</v>
+        <v>0.12078542639167859</v>
       </c>
       <c r="X10">
-        <v>0.1564608238688254</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="Y10">
-        <v>0.1178470949011987</v>
+        <v>2.1218544392257271E-2</v>
       </c>
       <c r="Z10">
-        <v>0.2695176277152487</v>
+        <v>0.12078542639167859</v>
       </c>
       <c r="AA10">
-        <v>0.1564608238688254</v>
+        <v>2.8171003618656449E-2</v>
       </c>
       <c r="AB10">
-        <v>0.1178437870054231</v>
+        <v>2.121794880071198E-2</v>
       </c>
       <c r="AC10">
-        <v>0.2695100625205112</v>
+        <v>0.1207820360187377</v>
       </c>
       <c r="AD10">
-        <v>0.1564564321093276</v>
+        <v>2.8170212875838881E-2</v>
       </c>
       <c r="AE10">
-        <v>0.04946841960402613</v>
+        <v>2.014096224549702E-2</v>
       </c>
       <c r="AF10">
-        <v>0.2476999607110389</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AG10">
-        <v>0.08483307702307459</v>
+        <v>3.4539607595469361E-2</v>
       </c>
       <c r="AH10">
-        <v>0.04946841960402613</v>
+        <v>2.014096224549702E-2</v>
       </c>
       <c r="AI10">
-        <v>0.2476999607110389</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AJ10">
-        <v>0.08483307702307459</v>
+        <v>3.4539607595469361E-2</v>
       </c>
       <c r="AK10">
-        <v>0.06081241335533492</v>
+        <v>2.4842262226883429E-2</v>
       </c>
       <c r="AL10">
-        <v>0.2757896469772391</v>
+        <v>5.0893156953114797E-2</v>
       </c>
       <c r="AM10">
-        <v>0.0944533228710521</v>
+        <v>3.858479026728702E-2</v>
       </c>
       <c r="AN10">
-        <v>0.1275833056498106</v>
+        <v>3.4563604879611229E-2</v>
       </c>
       <c r="AO10">
-        <v>0.2829935091010111</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AP10">
-        <v>0.1642838650622667</v>
+        <v>4.450615675136322E-2</v>
       </c>
       <c r="AQ10">
-        <v>0.1275833056498106</v>
+        <v>3.4563604879611229E-2</v>
       </c>
       <c r="AR10">
-        <v>0.2829935091010111</v>
+        <v>5.3848142278756783E-2</v>
       </c>
       <c r="AS10">
-        <v>0.1642838650622667</v>
+        <v>4.450615675136322E-2</v>
       </c>
       <c r="AT10">
-        <v>0.04946841960402613</v>
+        <v>2.014096224549702E-2</v>
       </c>
       <c r="AU10">
-        <v>0.2476999607110389</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AV10">
-        <v>0.08483307702307459</v>
+        <v>3.4539607595469361E-2</v>
       </c>
       <c r="AW10">
-        <v>0.04946841960402613</v>
+        <v>2.014096224549702E-2</v>
       </c>
       <c r="AX10">
-        <v>0.2476999607110389</v>
+        <v>4.7132468759379161E-2</v>
       </c>
       <c r="AY10">
-        <v>0.08483307702307459</v>
+        <v>3.4539607595469361E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change calibration of lupin fodder crop to Murdoch trials - Scanlon and Watts Profit no change
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDCE2DB-4E4E-415F-B6C2-875F99FD70B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26978B26-E1DF-40B1-9170-60B9E4F21FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -402,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:AY10"/>
     </sheetView>
   </sheetViews>
@@ -467,7 +467,7 @@
         <v>6.1451309414891804E-3</v>
       </c>
       <c r="T1">
-        <v>0.1599499218526465</v>
+        <v>0.1892678598946218</v>
       </c>
       <c r="U1">
         <v>9.5445650793342558E-3</v>
@@ -622,7 +622,7 @@
         <v>5.5864826740810729E-4</v>
       </c>
       <c r="T2">
-        <v>1.4540901986604231E-2</v>
+        <v>3.2302043749510331E-2</v>
       </c>
       <c r="U2">
         <v>8.6768773448493242E-4</v>
@@ -777,7 +777,7 @@
         <v>0.1325050224731904</v>
       </c>
       <c r="T3">
-        <v>1.4540901986604231E-2</v>
+        <v>2.6238275402749485E-2</v>
       </c>
       <c r="U3">
         <v>0.20580567320304041</v>
@@ -932,7 +932,7 @@
         <v>7.2401354595038783E-2</v>
       </c>
       <c r="T4">
-        <v>6.4787130329130305E-2</v>
+        <v>0.16905002841257127</v>
       </c>
       <c r="U4">
         <v>0.11245316777527301</v>
@@ -1087,7 +1087,7 @@
         <v>1.7994462413373071E-2</v>
       </c>
       <c r="T5">
-        <v>0.24834049582135209</v>
+        <v>0.19504265042326546</v>
       </c>
       <c r="U5">
         <v>2.7948845876090089E-2</v>
@@ -1242,7 +1242,7 @@
         <v>1.7994462413373071E-2</v>
       </c>
       <c r="T6">
-        <v>0.16034481276636189</v>
+        <v>0.15611659276390244</v>
       </c>
       <c r="U6">
         <v>2.7948845876090089E-2</v>
@@ -1397,7 +1397,7 @@
         <v>1.7994462413373071E-2</v>
       </c>
       <c r="T7">
-        <v>5.0893156953114797E-2</v>
+        <v>0.10617299893863949</v>
       </c>
       <c r="U7">
         <v>2.7948845876090089E-2</v>
@@ -1552,7 +1552,7 @@
         <v>1.7994462413373071E-2</v>
       </c>
       <c r="T8">
-        <v>5.0893156953114797E-2</v>
+        <v>6.1919466480956781E-2</v>
       </c>
       <c r="U8">
         <v>2.7948845876090089E-2</v>
@@ -1707,7 +1707,7 @@
         <v>1.7994462413373071E-2</v>
       </c>
       <c r="T9">
-        <v>5.0893156953114797E-2</v>
+        <v>6.1919466480956781E-2</v>
       </c>
       <c r="U9">
         <v>2.7948845876090089E-2</v>
@@ -1862,7 +1862,7 @@
         <v>2.4842262226883429E-2</v>
       </c>
       <c r="T10">
-        <v>5.0893156953114797E-2</v>
+        <v>1.9706174528261178E-3</v>
       </c>
       <c r="U10">
         <v>3.858479026728702E-2</v>

</xml_diff>

<commit_message>
Adjust stubble decay assumptions (halve deterioration because grain is included in the DM decline) Add capacity to specify supp feeding by week Change the quadratic parameters to be EBG rather than LWC Fixed error that stubble intake was based on PI rather than intake of forage Changed calculation of LWC in the trial to the derivative of the equation Increased profit $24K
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -8,24 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26978B26-E1DF-40B1-9170-60B9E4F21FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A60702-8A15-4A01-B71C-AD9491915AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30075" yWindow="315" windowWidth="25140" windowHeight="15075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -410,1552 +400,1552 @@
   <sheetData>
     <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.17069334575684059</v>
+        <v>6.0646152631832567E-2</v>
       </c>
       <c r="B1">
-        <v>0.17729592423753929</v>
+        <v>0.53088441236560147</v>
       </c>
       <c r="C1">
-        <v>0.21296718713151341</v>
+        <v>7.5665752985758755E-2</v>
       </c>
       <c r="D1">
-        <v>0.17069334575684059</v>
+        <v>6.0646152631832567E-2</v>
       </c>
       <c r="E1">
-        <v>0.17729592423753929</v>
+        <v>0.53088441236560147</v>
       </c>
       <c r="F1">
-        <v>0.21296718713151341</v>
+        <v>7.5665752985758755E-2</v>
       </c>
       <c r="G1">
-        <v>1.297240195222021E-2</v>
+        <v>0.1572352033654765</v>
       </c>
       <c r="H1">
-        <v>0.16492893339069939</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="I1">
-        <v>2.0148624308767561E-2</v>
+        <v>0.24421637969531451</v>
       </c>
       <c r="J1">
-        <v>2.648605191673075E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K1">
-        <v>1.7435530794102039E-2</v>
+        <v>0.2279970962331436</v>
       </c>
       <c r="L1">
-        <v>4.0461670800452506E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M1">
-        <v>1.297240195222021E-2</v>
+        <v>0.1572352033654765</v>
       </c>
       <c r="N1">
-        <v>0.16492893339069939</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="O1">
-        <v>2.0148624308767561E-2</v>
+        <v>0.24421637969531451</v>
       </c>
       <c r="P1">
-        <v>1.297240195222021E-2</v>
+        <v>0.1572352033654765</v>
       </c>
       <c r="Q1">
-        <v>0.16492893339069939</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="R1">
-        <v>2.0148624308767561E-2</v>
+        <v>0.24421637969531451</v>
       </c>
       <c r="S1">
-        <v>6.1451309414891804E-3</v>
+        <v>2.769971914895164E-2</v>
       </c>
       <c r="T1">
-        <v>0.1892678598946218</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="U1">
-        <v>9.5445650793342558E-3</v>
+        <v>4.3022968039861047E-2</v>
       </c>
       <c r="V1">
-        <v>1.480952362153405E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W1">
-        <v>8.4726483442497266E-2</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="X1">
-        <v>1.966200582944095E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y1">
-        <v>1.480952362153405E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z1">
-        <v>8.4726483442497266E-2</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AA1">
-        <v>1.966200582944095E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB1">
-        <v>1.480910792727644E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC1">
-        <v>8.4724105221999801E-2</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AD1">
-        <v>1.9661453928979781E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE1">
-        <v>2.4282338717033108E-3</v>
+        <v>2.4753777129460398E-2</v>
       </c>
       <c r="AF1">
-        <v>0.14813061610090589</v>
+        <v>0.44355354146056142</v>
       </c>
       <c r="AG1">
-        <v>4.1641627672188699E-3</v>
+        <v>4.2450094396478899E-2</v>
       </c>
       <c r="AH1">
-        <v>2.4282338717033108E-3</v>
+        <v>2.4753777129460398E-2</v>
       </c>
       <c r="AI1">
-        <v>0.14813061610090589</v>
+        <v>0.44355354146056142</v>
       </c>
       <c r="AJ1">
-        <v>4.1641627672188699E-3</v>
+        <v>4.2450094396478899E-2</v>
       </c>
       <c r="AK1">
-        <v>6.1451309414891804E-3</v>
+        <v>2.769971914895164E-2</v>
       </c>
       <c r="AL1">
-        <v>0.1599499218526465</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="AM1">
-        <v>9.5445650793342558E-3</v>
+        <v>4.3022968039861047E-2</v>
       </c>
       <c r="AN1">
-        <v>3.7293384562146182E-3</v>
+        <v>2.7530400947871809E-2</v>
       </c>
       <c r="AO1">
-        <v>0.16923701859037851</v>
+        <v>0.50675330271261954</v>
       </c>
       <c r="AP1">
-        <v>4.80211836957678E-3</v>
+        <v>3.5449784369472381E-2</v>
       </c>
       <c r="AQ1">
-        <v>3.7293384562146182E-3</v>
+        <v>2.7530400947871809E-2</v>
       </c>
       <c r="AR1">
-        <v>0.16923701859037851</v>
+        <v>0.50675330271261954</v>
       </c>
       <c r="AS1">
-        <v>4.80211836957678E-3</v>
+        <v>3.5449784369472381E-2</v>
       </c>
       <c r="AT1">
-        <v>2.4282338717033108E-3</v>
+        <v>2.4753777129460398E-2</v>
       </c>
       <c r="AU1">
-        <v>0.14813061610090589</v>
+        <v>0.44355354146056142</v>
       </c>
       <c r="AV1">
-        <v>4.1641627672188699E-3</v>
+        <v>4.2450094396478899E-2</v>
       </c>
       <c r="AW1">
-        <v>2.4282338717033108E-3</v>
+        <v>2.4753777129460398E-2</v>
       </c>
       <c r="AX1">
-        <v>0.14813061610090589</v>
+        <v>0.44355354146056142</v>
       </c>
       <c r="AY1">
-        <v>4.1641627672188699E-3</v>
+        <v>4.2450094396478899E-2</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3.4935840886530872E-2</v>
+        <v>1.7248569401469811E-2</v>
       </c>
       <c r="B2">
-        <v>1.6117811294321761E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C2">
-        <v>4.3588036374173827E-2</v>
+        <v>2.1520342759621058E-2</v>
       </c>
       <c r="D2">
-        <v>3.4935840886530872E-2</v>
+        <v>1.7248569401469811E-2</v>
       </c>
       <c r="E2">
-        <v>1.6117811294321761E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F2">
-        <v>4.3588036374173827E-2</v>
+        <v>2.1520342759621058E-2</v>
       </c>
       <c r="G2">
-        <v>4.7365913074357252E-2</v>
+        <v>1.770553379233198E-2</v>
       </c>
       <c r="H2">
-        <v>1.4993539399154489E-2</v>
+        <v>0.12524239478063742</v>
       </c>
       <c r="I2">
-        <v>7.3568333072937836E-2</v>
+        <v>2.7500084400856051E-2</v>
       </c>
       <c r="J2">
-        <v>5.4147474403530467E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K2">
-        <v>1.585048254009276E-3</v>
+        <v>7.003318336585281E-3</v>
       </c>
       <c r="L2">
-        <v>8.271890770581887E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M2">
-        <v>4.7365913074357252E-2</v>
+        <v>1.770553379233198E-2</v>
       </c>
       <c r="N2">
-        <v>1.4993539399154489E-2</v>
+        <v>0.12524239478063742</v>
       </c>
       <c r="O2">
-        <v>7.3568333072937836E-2</v>
+        <v>2.7500084400856051E-2</v>
       </c>
       <c r="P2">
-        <v>4.7365913074357252E-2</v>
+        <v>1.770553379233198E-2</v>
       </c>
       <c r="Q2">
-        <v>1.4993539399154489E-2</v>
+        <v>0.12524239478063742</v>
       </c>
       <c r="R2">
-        <v>7.3568333072937836E-2</v>
+        <v>2.7500084400856051E-2</v>
       </c>
       <c r="S2">
-        <v>5.5864826740810729E-4</v>
+        <v>1.525120165427472E-2</v>
       </c>
       <c r="T2">
-        <v>3.2302043749510331E-2</v>
+        <v>0.12524239478063742</v>
       </c>
       <c r="U2">
-        <v>8.6768773448493242E-4</v>
+        <v>2.3688036611958611E-2</v>
       </c>
       <c r="V2">
-        <v>3.027624893836859E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W2">
-        <v>7.7024075856815689E-3</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="X2">
-        <v>4.0196551782004243E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y2">
-        <v>3.027624893836859E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z2">
-        <v>7.7024075856815689E-3</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AA2">
-        <v>4.0196551782004243E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB2">
-        <v>3.0275399102604302E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC2">
-        <v>7.7021913838181627E-3</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AD2">
-        <v>4.0195423489415058E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE2">
-        <v>2.2074853379121009E-4</v>
+        <v>8.2558821479480574E-3</v>
       </c>
       <c r="AF2">
-        <v>1.34664196455369E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG2">
-        <v>3.7856025156535167E-4</v>
+        <v>1.415795959839603E-2</v>
       </c>
       <c r="AH2">
-        <v>2.2074853379121009E-4</v>
+        <v>8.2558821479480574E-3</v>
       </c>
       <c r="AI2">
-        <v>1.34664196455369E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ2">
-        <v>3.7856025156535167E-4</v>
+        <v>1.415795959839603E-2</v>
       </c>
       <c r="AK2">
-        <v>5.5864826740810729E-4</v>
+        <v>1.525120165427472E-2</v>
       </c>
       <c r="AL2">
-        <v>1.4540901986604231E-2</v>
+        <v>0.12524239478063742</v>
       </c>
       <c r="AM2">
-        <v>8.6768773448493242E-4</v>
+        <v>2.3688036611958611E-2</v>
       </c>
       <c r="AN2">
-        <v>3.3903076874678339E-4</v>
+        <v>9.4738022711688043E-3</v>
       </c>
       <c r="AO2">
-        <v>1.5385183508216219E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP2">
-        <v>4.3655621541607089E-4</v>
+        <v>1.2199032201088001E-2</v>
       </c>
       <c r="AQ2">
-        <v>3.3903076874678339E-4</v>
+        <v>9.4738022711688043E-3</v>
       </c>
       <c r="AR2">
-        <v>1.5385183508216219E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS2">
-        <v>4.3655621541607089E-4</v>
+        <v>1.2199032201088001E-2</v>
       </c>
       <c r="AT2">
-        <v>2.2074853379121009E-4</v>
+        <v>8.2558821479480574E-3</v>
       </c>
       <c r="AU2">
-        <v>1.34664196455369E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV2">
-        <v>3.7856025156535167E-4</v>
+        <v>1.415795959839603E-2</v>
       </c>
       <c r="AW2">
-        <v>2.2074853379121009E-4</v>
+        <v>8.2558821479480574E-3</v>
       </c>
       <c r="AX2">
-        <v>1.34664196455369E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY2">
-        <v>3.7856025156535167E-4</v>
+        <v>1.415795959839603E-2</v>
       </c>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.7282873614216911E-2</v>
+        <v>1.8062496090622038E-2</v>
       </c>
       <c r="B3">
-        <v>0.22635979242130261</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C3">
-        <v>2.156314273909956E-2</v>
+        <v>2.2535846186256939E-2</v>
       </c>
       <c r="D3">
-        <v>1.7282873614216911E-2</v>
+        <v>1.8062496090622038E-2</v>
       </c>
       <c r="E3">
-        <v>0.22635979242130261</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F3">
-        <v>2.156314273909956E-2</v>
+        <v>2.2535846186256939E-2</v>
       </c>
       <c r="G3">
-        <v>9.076573040146127E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H3">
-        <v>0.2105704306917219</v>
+        <v>0.37022630621646846</v>
       </c>
       <c r="I3">
-        <v>0.14097655998524841</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J3">
-        <v>2.6848141865304379E-2</v>
+        <v>3.2661458119004942E-2</v>
       </c>
       <c r="K3">
-        <v>4.0916750876948918E-2</v>
+        <v>6.3396164068368838E-3</v>
       </c>
       <c r="L3">
-        <v>4.1014820977209668E-2</v>
+        <v>4.9895589211586253E-2</v>
       </c>
       <c r="M3">
-        <v>9.076573040146127E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N3">
-        <v>0.2105704306917219</v>
+        <v>0.37022630621646846</v>
       </c>
       <c r="O3">
-        <v>0.14097655998524841</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P3">
-        <v>9.076573040146127E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q3">
-        <v>0.2105704306917219</v>
+        <v>0.37022630621646846</v>
       </c>
       <c r="R3">
-        <v>0.14097655998524841</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S3">
-        <v>0.1325050224731904</v>
+        <v>9.2237484816381603E-3</v>
       </c>
       <c r="T3">
-        <v>2.6238275402749485E-2</v>
+        <v>0.37022630621646846</v>
       </c>
       <c r="U3">
-        <v>0.20580567320304041</v>
+        <v>1.432624764169331E-2</v>
       </c>
       <c r="V3">
-        <v>0.15011984134085329</v>
+        <v>3.7581613668983251E-2</v>
       </c>
       <c r="W3">
-        <v>0.19883148133748241</v>
+        <v>0.51047441656239501</v>
       </c>
       <c r="X3">
-        <v>0.19930804467381369</v>
+        <v>4.989558921158626E-2</v>
       </c>
       <c r="Y3">
-        <v>0.15011984134085329</v>
+        <v>3.7581613668983251E-2</v>
       </c>
       <c r="Z3">
-        <v>0.19883148133748241</v>
+        <v>0.51047441656239501</v>
       </c>
       <c r="AA3">
-        <v>0.19930804467381369</v>
+        <v>4.989558921158626E-2</v>
       </c>
       <c r="AB3">
-        <v>0.15011562756885141</v>
+        <v>3.7580558776105319E-2</v>
       </c>
       <c r="AC3">
-        <v>0.1988259002595803</v>
+        <v>0.51047441656239501</v>
       </c>
       <c r="AD3">
-        <v>0.1993024502190707</v>
+        <v>4.9894188672956842E-2</v>
       </c>
       <c r="AE3">
-        <v>0.1097450235421261</v>
+        <v>3.745079023766351E-3</v>
       </c>
       <c r="AF3">
-        <v>0.189123442380528</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG3">
-        <v>0.18820104037224189</v>
+        <v>6.4224121130971876E-3</v>
       </c>
       <c r="AH3">
-        <v>0.1097450235421261</v>
+        <v>3.745079023766351E-3</v>
       </c>
       <c r="AI3">
-        <v>0.189123442380528</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ3">
-        <v>0.18820104037224189</v>
+        <v>6.4224121130971876E-3</v>
       </c>
       <c r="AK3">
-        <v>0.1325050224731904</v>
+        <v>9.2237484816381603E-3</v>
       </c>
       <c r="AL3">
-        <v>1.4540901986604231E-2</v>
+        <v>0.37022630621646846</v>
       </c>
       <c r="AM3">
-        <v>0.20580567320304041</v>
+        <v>1.432624764169331E-2</v>
       </c>
       <c r="AN3">
-        <v>0.14144991040144761</v>
+        <v>5.7225157293905376E-3</v>
       </c>
       <c r="AO3">
-        <v>0.21607071094760699</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP3">
-        <v>0.18213933143607669</v>
+        <v>7.3686521689939437E-3</v>
       </c>
       <c r="AQ3">
-        <v>0.14144991040144761</v>
+        <v>5.7225157293905376E-3</v>
       </c>
       <c r="AR3">
-        <v>0.21607071094760699</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS3">
-        <v>0.18213933143607669</v>
+        <v>7.3686521689939437E-3</v>
       </c>
       <c r="AT3">
-        <v>0.1097450235421261</v>
+        <v>3.745079023766351E-3</v>
       </c>
       <c r="AU3">
-        <v>0.189123442380528</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV3">
-        <v>0.18820104037224189</v>
+        <v>6.4224121130971876E-3</v>
       </c>
       <c r="AW3">
-        <v>0.1097450235421261</v>
+        <v>3.745079023766351E-3</v>
       </c>
       <c r="AX3">
-        <v>0.189123442380528</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY3">
-        <v>0.18820104037224189</v>
+        <v>6.4224121130971876E-3</v>
       </c>
     </row>
     <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.7282873614216911E-2</v>
+        <v>1.8398354443743381E-2</v>
       </c>
       <c r="B4">
-        <v>0.22409796236541021</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C4">
-        <v>2.156314273909956E-2</v>
+        <v>2.295488307619387E-2</v>
       </c>
       <c r="D4">
-        <v>1.7282873614216911E-2</v>
+        <v>1.8398354443743381E-2</v>
       </c>
       <c r="E4">
-        <v>0.22409796236541021</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F4">
-        <v>2.156314273909956E-2</v>
+        <v>2.295488307619387E-2</v>
       </c>
       <c r="G4">
-        <v>7.298818546593154E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H4">
-        <v>0.2084663709383259</v>
+        <v>0.21027741069319272</v>
       </c>
       <c r="I4">
-        <v>0.1133646284896383</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J4">
-        <v>1.087073643375785E-2</v>
+        <v>0.1007043548491684</v>
       </c>
       <c r="K4">
-        <v>4.0493611660579687E-2</v>
+        <v>5.6759139045950641E-3</v>
       </c>
       <c r="L4">
-        <v>1.6606784594549229E-2</v>
+        <v>0.1538419718759636</v>
       </c>
       <c r="M4">
-        <v>7.298818546593154E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N4">
-        <v>0.2084663709383259</v>
+        <v>0.21027741069319272</v>
       </c>
       <c r="O4">
-        <v>0.1133646284896383</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P4">
-        <v>7.298818546593154E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q4">
-        <v>0.2084663709383259</v>
+        <v>0.21027741069319272</v>
       </c>
       <c r="R4">
-        <v>0.1133646284896383</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S4">
-        <v>7.2401354595038783E-2</v>
+        <v>1.035289848004251E-2</v>
       </c>
       <c r="T4">
-        <v>0.16905002841257127</v>
+        <v>0.21027741069319272</v>
       </c>
       <c r="U4">
-        <v>0.11245316777527301</v>
+        <v>1.608003380942773E-2</v>
       </c>
       <c r="V4">
-        <v>6.0783097649035799E-2</v>
+        <v>0.11587456215016489</v>
       </c>
       <c r="W4">
-        <v>0.19677527219576199</v>
+        <v>0.26808365097208692</v>
       </c>
       <c r="X4">
-        <v>8.0699261559570926E-2</v>
+        <v>0.1538419718759636</v>
       </c>
       <c r="Y4">
-        <v>6.0783097649035799E-2</v>
+        <v>0.11587456215016489</v>
       </c>
       <c r="Z4">
-        <v>0.19677527219576199</v>
+        <v>0.26808365097208692</v>
       </c>
       <c r="AA4">
-        <v>8.0699261559570926E-2</v>
+        <v>0.1538419718759636</v>
       </c>
       <c r="AB4">
-        <v>6.0781391504712859E-2</v>
+        <v>0.1158713096221755</v>
       </c>
       <c r="AC4">
-        <v>0.19676974883439119</v>
+        <v>0.26808365097208692</v>
       </c>
       <c r="AD4">
-        <v>8.0696996380725139E-2</v>
+        <v>0.15383765362603721</v>
       </c>
       <c r="AE4">
-        <v>5.8708077211763743E-2</v>
+        <v>5.0332879722065071E-3</v>
       </c>
       <c r="AF4">
-        <v>0.18723368500942231</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG4">
-        <v>0.1006781068780459</v>
+        <v>8.6315534161669032E-3</v>
       </c>
       <c r="AH4">
-        <v>5.8708077211763743E-2</v>
+        <v>5.0332879722065071E-3</v>
       </c>
       <c r="AI4">
-        <v>0.18723368500942231</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ4">
-        <v>0.1006781068780459</v>
+        <v>8.6315534161669032E-3</v>
       </c>
       <c r="AK4">
-        <v>7.2401354595038783E-2</v>
+        <v>1.035289848004251E-2</v>
       </c>
       <c r="AL4">
-        <v>6.4787130329130305E-2</v>
+        <v>0.21027741069319272</v>
       </c>
       <c r="AM4">
-        <v>0.11245316777527301</v>
+        <v>1.608003380942773E-2</v>
       </c>
       <c r="AN4">
-        <v>0.1112871408980786</v>
+        <v>5.1380843197396126E-3</v>
       </c>
       <c r="AO4">
-        <v>0.21391169134880059</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP4">
-        <v>0.14329995249258959</v>
+        <v>6.6161034687370508E-3</v>
       </c>
       <c r="AQ4">
-        <v>0.1112871408980786</v>
+        <v>5.1380843197396126E-3</v>
       </c>
       <c r="AR4">
-        <v>0.21391169134880059</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS4">
-        <v>0.14329995249258959</v>
+        <v>6.6161034687370508E-3</v>
       </c>
       <c r="AT4">
-        <v>5.8708077211763743E-2</v>
+        <v>5.0332879722065071E-3</v>
       </c>
       <c r="AU4">
-        <v>0.18723368500942231</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV4">
-        <v>0.1006781068780459</v>
+        <v>8.6315534161669032E-3</v>
       </c>
       <c r="AW4">
-        <v>5.8708077211763743E-2</v>
+        <v>5.0332879722065071E-3</v>
       </c>
       <c r="AX4">
-        <v>0.18723368500942231</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY4">
-        <v>0.1006781068780459</v>
+        <v>8.6315534161669032E-3</v>
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1.7282873614216911E-2</v>
+        <v>1.0276499738658519E-2</v>
       </c>
       <c r="B5">
-        <v>9.653105386736166E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C5">
-        <v>2.156314273909956E-2</v>
+        <v>1.2821573290956069E-2</v>
       </c>
       <c r="D5">
-        <v>1.7282873614216911E-2</v>
+        <v>1.0276499738658519E-2</v>
       </c>
       <c r="E5">
-        <v>9.653105386736166E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F5">
-        <v>2.156314273909956E-2</v>
+        <v>1.2821573290956069E-2</v>
       </c>
       <c r="G5">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H5">
-        <v>8.9797686110897973E-2</v>
+        <v>0.14045064295904497</v>
       </c>
       <c r="I5">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J5">
-        <v>3.7948247542115591E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K5">
-        <v>1.6628617225702289E-2</v>
+        <v>5.012211974846666E-3</v>
       </c>
       <c r="L5">
-        <v>5.7972003691997842E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M5">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N5">
-        <v>8.9797686110897973E-2</v>
+        <v>0.14045064295904497</v>
       </c>
       <c r="O5">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P5">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q5">
-        <v>8.9797686110897973E-2</v>
+        <v>0.14045064295904497</v>
       </c>
       <c r="R5">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S5">
-        <v>1.7994462413373071E-2</v>
+        <v>1.2824127246370481E-2</v>
       </c>
       <c r="T5">
-        <v>0.19504265042326546</v>
+        <v>0.14045064295904497</v>
       </c>
       <c r="U5">
-        <v>2.7948845876090089E-2</v>
+        <v>1.9918325297554142E-2</v>
       </c>
       <c r="V5">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W5">
-        <v>8.0805355379354224E-2</v>
+        <v>0.1281600317902849</v>
       </c>
       <c r="X5">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y5">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z5">
-        <v>8.0805355379354224E-2</v>
+        <v>0.1281600317902849</v>
       </c>
       <c r="AA5">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB5">
-        <v>2.121794880071198E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC5">
-        <v>8.0803087222519915E-2</v>
+        <v>0.1281600317902849</v>
       </c>
       <c r="AD5">
-        <v>2.8170212875838881E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE5">
-        <v>1.4589371389502351E-2</v>
+        <v>5.9346588902596574E-3</v>
       </c>
       <c r="AF5">
-        <v>8.065162548849171E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG5">
-        <v>2.501921987221041E-2</v>
+        <v>1.017730865010486E-2</v>
       </c>
       <c r="AH5">
-        <v>1.4589371389502351E-2</v>
+        <v>5.9346588902596574E-3</v>
       </c>
       <c r="AI5">
-        <v>8.065162548849171E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ5">
-        <v>2.501921987221041E-2</v>
+        <v>1.017730865010486E-2</v>
       </c>
       <c r="AK5">
-        <v>1.7994462413373071E-2</v>
+        <v>1.2824127246370481E-2</v>
       </c>
       <c r="AL5">
-        <v>0.24834049582135209</v>
+        <v>0.14045064295904497</v>
       </c>
       <c r="AM5">
-        <v>2.7948845876090089E-2</v>
+        <v>1.9918325297554142E-2</v>
       </c>
       <c r="AN5">
-        <v>2.2087278766677831E-2</v>
+        <v>6.8242095401696333E-3</v>
       </c>
       <c r="AO5">
-        <v>9.2143278691572489E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP5">
-        <v>2.8440895977858351E-2</v>
+        <v>8.7872587525758758E-3</v>
       </c>
       <c r="AQ5">
-        <v>2.2087278766677831E-2</v>
+        <v>6.8242095401696333E-3</v>
       </c>
       <c r="AR5">
-        <v>9.2143278691572489E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS5">
-        <v>2.8440895977858351E-2</v>
+        <v>8.7872587525758758E-3</v>
       </c>
       <c r="AT5">
-        <v>1.4589371389502351E-2</v>
+        <v>5.9346588902596574E-3</v>
       </c>
       <c r="AU5">
-        <v>8.065162548849171E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV5">
-        <v>2.501921987221041E-2</v>
+        <v>1.017730865010486E-2</v>
       </c>
       <c r="AW5">
-        <v>1.4589371389502351E-2</v>
+        <v>5.9346588902596574E-3</v>
       </c>
       <c r="AX5">
-        <v>8.065162548849171E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY5">
-        <v>2.501921987221041E-2</v>
+        <v>1.017730865010486E-2</v>
       </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1.7282873614216911E-2</v>
+        <v>8.9932497576223937E-3</v>
       </c>
       <c r="B6">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C6">
-        <v>2.156314273909956E-2</v>
+        <v>1.1220514165680359E-2</v>
       </c>
       <c r="D6">
-        <v>1.7282873614216911E-2</v>
+        <v>8.9932497576223937E-3</v>
       </c>
       <c r="E6">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F6">
-        <v>2.156314273909956E-2</v>
+        <v>1.1220514165680359E-2</v>
       </c>
       <c r="G6">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H6">
-        <v>5.2477387897040713E-2</v>
+        <v>0.16735104985882043</v>
       </c>
       <c r="I6">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J6">
-        <v>3.7948247542115591E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K6">
-        <v>9.1232782183906184E-3</v>
+        <v>4.3485094726048454E-3</v>
       </c>
       <c r="L6">
-        <v>5.7972003691997842E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M6">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N6">
-        <v>5.2477387897040713E-2</v>
+        <v>0.16735104985882043</v>
       </c>
       <c r="O6">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P6">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q6">
-        <v>5.2477387897040713E-2</v>
+        <v>0.16735104985882043</v>
       </c>
       <c r="R6">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S6">
-        <v>1.7994462413373071E-2</v>
+        <v>9.5537979509848613E-3</v>
       </c>
       <c r="T6">
-        <v>0.15611659276390244</v>
+        <v>0.16735104985882043</v>
       </c>
       <c r="U6">
-        <v>2.7948845876090089E-2</v>
+        <v>1.4838877668550949E-2</v>
       </c>
       <c r="V6">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W6">
-        <v>4.4333796890958288E-2</v>
+        <v>0.1563592930333936</v>
       </c>
       <c r="X6">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y6">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z6">
-        <v>4.4333796890958288E-2</v>
+        <v>0.1563592930333936</v>
       </c>
       <c r="AA6">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB6">
-        <v>2.121794880071198E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC6">
-        <v>4.4332552468432873E-2</v>
+        <v>0.1563592930333936</v>
       </c>
       <c r="AD6">
-        <v>2.8170212875838881E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE6">
-        <v>1.4589371389502351E-2</v>
+        <v>5.1528116666491224E-3</v>
       </c>
       <c r="AF6">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG6">
-        <v>2.501921987221041E-2</v>
+        <v>8.8365238368493439E-3</v>
       </c>
       <c r="AH6">
-        <v>1.4589371389502351E-2</v>
+        <v>5.1528116666491224E-3</v>
       </c>
       <c r="AI6">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ6">
-        <v>2.501921987221041E-2</v>
+        <v>8.8365238368493439E-3</v>
       </c>
       <c r="AK6">
-        <v>1.7994462413373071E-2</v>
+        <v>9.5537979509848613E-3</v>
       </c>
       <c r="AL6">
-        <v>0.16034481276636189</v>
+        <v>0.16735104985882043</v>
       </c>
       <c r="AM6">
-        <v>2.7948845876090089E-2</v>
+        <v>1.4838877668550949E-2</v>
       </c>
       <c r="AN6">
-        <v>2.2087278766677831E-2</v>
+        <v>5.9279110381232356E-3</v>
       </c>
       <c r="AO6">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP6">
-        <v>2.8440895977858351E-2</v>
+        <v>7.6331314048344303E-3</v>
       </c>
       <c r="AQ6">
-        <v>2.2087278766677831E-2</v>
+        <v>5.9279110381232356E-3</v>
       </c>
       <c r="AR6">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS6">
-        <v>2.8440895977858351E-2</v>
+        <v>7.6331314048344303E-3</v>
       </c>
       <c r="AT6">
-        <v>1.4589371389502351E-2</v>
+        <v>5.1528116666491224E-3</v>
       </c>
       <c r="AU6">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV6">
-        <v>2.501921987221041E-2</v>
+        <v>8.8365238368493439E-3</v>
       </c>
       <c r="AW6">
-        <v>1.4589371389502351E-2</v>
+        <v>5.1528116666491224E-3</v>
       </c>
       <c r="AX6">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY6">
-        <v>2.501921987221041E-2</v>
+        <v>8.8365238368493439E-3</v>
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1.7282873614216911E-2</v>
+        <v>6.1174443165379873E-3</v>
       </c>
       <c r="B7">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C7">
-        <v>2.156314273909956E-2</v>
+        <v>7.6324879728039896E-3</v>
       </c>
       <c r="D7">
-        <v>1.7282873614216911E-2</v>
+        <v>6.1174443165379873E-3</v>
       </c>
       <c r="E7">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F7">
-        <v>2.156314273909956E-2</v>
+        <v>7.6324879728039896E-3</v>
       </c>
       <c r="G7">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H7">
-        <v>5.2477387897040713E-2</v>
+        <v>4.2944511169081545E-2</v>
       </c>
       <c r="I7">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J7">
-        <v>3.7948247542115591E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K7">
-        <v>9.1232782183906184E-3</v>
+        <v>3.685644441736035E-3</v>
       </c>
       <c r="L7">
-        <v>5.7972003691997842E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M7">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N7">
-        <v>5.2477387897040713E-2</v>
+        <v>4.2944511169081545E-2</v>
       </c>
       <c r="O7">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P7">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q7">
-        <v>5.2477387897040713E-2</v>
+        <v>4.2944511169081545E-2</v>
       </c>
       <c r="R7">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S7">
-        <v>1.7994462413373071E-2</v>
+        <v>6.7497814487402748E-3</v>
       </c>
       <c r="T7">
-        <v>0.10617299893863949</v>
+        <v>4.2944511169081545E-2</v>
       </c>
       <c r="U7">
-        <v>2.7948845876090089E-2</v>
+        <v>1.0483703101234891E-2</v>
       </c>
       <c r="V7">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W7">
-        <v>4.4333796890958288E-2</v>
+        <v>0.1508147044740282</v>
       </c>
       <c r="X7">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y7">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z7">
-        <v>4.4333796890958288E-2</v>
+        <v>0.1508147044740282</v>
       </c>
       <c r="AA7">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB7">
-        <v>2.121794880071198E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC7">
-        <v>4.4332552468432873E-2</v>
+        <v>0.1508147044740282</v>
       </c>
       <c r="AD7">
-        <v>2.8170212875838881E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE7">
-        <v>1.4589371389502351E-2</v>
+        <v>3.28225000874757E-3</v>
       </c>
       <c r="AF7">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG7">
-        <v>2.501921987221041E-2</v>
+        <v>5.6287095894692364E-3</v>
       </c>
       <c r="AH7">
-        <v>1.4589371389502351E-2</v>
+        <v>3.28225000874757E-3</v>
       </c>
       <c r="AI7">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ7">
-        <v>2.501921987221041E-2</v>
+        <v>5.6287095894692364E-3</v>
       </c>
       <c r="AK7">
-        <v>1.7994462413373071E-2</v>
+        <v>6.7497814487402748E-3</v>
       </c>
       <c r="AL7">
-        <v>5.0893156953114797E-2</v>
+        <v>4.2944511169081545E-2</v>
       </c>
       <c r="AM7">
-        <v>2.7948845876090089E-2</v>
+        <v>1.0483703101234891E-2</v>
       </c>
       <c r="AN7">
-        <v>2.2087278766677831E-2</v>
+        <v>5.0386361581330856E-3</v>
       </c>
       <c r="AO7">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP7">
-        <v>2.8440895977858351E-2</v>
+        <v>6.488048091281156E-3</v>
       </c>
       <c r="AQ7">
-        <v>2.2087278766677831E-2</v>
+        <v>5.0386361581330856E-3</v>
       </c>
       <c r="AR7">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS7">
-        <v>2.8440895977858351E-2</v>
+        <v>6.488048091281156E-3</v>
       </c>
       <c r="AT7">
-        <v>1.4589371389502351E-2</v>
+        <v>3.28225000874757E-3</v>
       </c>
       <c r="AU7">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV7">
-        <v>2.501921987221041E-2</v>
+        <v>5.6287095894692364E-3</v>
       </c>
       <c r="AW7">
-        <v>1.4589371389502351E-2</v>
+        <v>3.28225000874757E-3</v>
       </c>
       <c r="AX7">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY7">
-        <v>2.501921987221041E-2</v>
+        <v>5.6287095894692364E-3</v>
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1.7282873614216911E-2</v>
+        <v>3.8072249886750469E-3</v>
       </c>
       <c r="B8">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C8">
-        <v>2.156314273909956E-2</v>
+        <v>4.7501207092745688E-3</v>
       </c>
       <c r="D8">
-        <v>1.7282873614216911E-2</v>
+        <v>3.8072249886750469E-3</v>
       </c>
       <c r="E8">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F8">
-        <v>2.156314273909956E-2</v>
+        <v>4.7501207092745688E-3</v>
       </c>
       <c r="G8">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H8">
-        <v>5.2477387897040713E-2</v>
+        <v>2.6082369580643704E-2</v>
       </c>
       <c r="I8">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J8">
-        <v>3.7948247542115591E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K8">
-        <v>9.1232782183906184E-3</v>
+        <v>3.018032415910987E-3</v>
       </c>
       <c r="L8">
-        <v>5.7972003691997842E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M8">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N8">
-        <v>5.2477387897040713E-2</v>
+        <v>2.6082369580643704E-2</v>
       </c>
       <c r="O8">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P8">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q8">
-        <v>5.2477387897040713E-2</v>
+        <v>2.6082369580643704E-2</v>
       </c>
       <c r="R8">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S8">
-        <v>1.7994462413373071E-2</v>
+        <v>4.4206640911911687E-3</v>
       </c>
       <c r="T8">
-        <v>6.1919466480956781E-2</v>
+        <v>2.6082369580643704E-2</v>
       </c>
       <c r="U8">
-        <v>2.7948845876090089E-2</v>
+        <v>6.8661378437650062E-3</v>
       </c>
       <c r="V8">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W8">
-        <v>4.4333796890958288E-2</v>
+        <v>1.014142284416838E-2</v>
       </c>
       <c r="X8">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y8">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z8">
-        <v>4.4333796890958288E-2</v>
+        <v>1.014142284416838E-2</v>
       </c>
       <c r="AA8">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB8">
-        <v>2.121794880071198E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC8">
-        <v>4.4332552468432873E-2</v>
+        <v>1.014142284416838E-2</v>
       </c>
       <c r="AD8">
-        <v>2.8170212875838881E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE8">
-        <v>1.4589371389502351E-2</v>
+        <v>1.7940372941328271E-3</v>
       </c>
       <c r="AF8">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG8">
-        <v>2.501921987221041E-2</v>
+        <v>3.0765831044065068E-3</v>
       </c>
       <c r="AH8">
-        <v>1.4589371389502351E-2</v>
+        <v>1.7940372941328271E-3</v>
       </c>
       <c r="AI8">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ8">
-        <v>2.501921987221041E-2</v>
+        <v>3.0765831044065068E-3</v>
       </c>
       <c r="AK8">
-        <v>1.7994462413373071E-2</v>
+        <v>4.4206640911911687E-3</v>
       </c>
       <c r="AL8">
-        <v>5.0893156953114797E-2</v>
+        <v>2.6082369580643704E-2</v>
       </c>
       <c r="AM8">
-        <v>2.7948845876090089E-2</v>
+        <v>6.8661378437650062E-3</v>
       </c>
       <c r="AN8">
-        <v>2.2087278766677831E-2</v>
+        <v>2.757420428824129E-3</v>
       </c>
       <c r="AO8">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP8">
-        <v>2.8440895977858351E-2</v>
+        <v>3.550618816009282E-3</v>
       </c>
       <c r="AQ8">
-        <v>2.2087278766677831E-2</v>
+        <v>2.757420428824129E-3</v>
       </c>
       <c r="AR8">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS8">
-        <v>2.8440895977858351E-2</v>
+        <v>3.550618816009282E-3</v>
       </c>
       <c r="AT8">
-        <v>1.4589371389502351E-2</v>
+        <v>1.7940372941328271E-3</v>
       </c>
       <c r="AU8">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV8">
-        <v>2.501921987221041E-2</v>
+        <v>3.0765831044065068E-3</v>
       </c>
       <c r="AW8">
-        <v>1.4589371389502351E-2</v>
+        <v>1.7940372941328271E-3</v>
       </c>
       <c r="AX8">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY8">
-        <v>2.501921987221041E-2</v>
+        <v>3.0765831044065068E-3</v>
       </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1.7282873614216911E-2</v>
+        <v>2.0263856999000749E-3</v>
       </c>
       <c r="B9">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C9">
-        <v>2.156314273909956E-2</v>
+        <v>2.528239520045539E-3</v>
       </c>
       <c r="D9">
-        <v>1.7282873614216911E-2</v>
+        <v>2.0263856999000749E-3</v>
       </c>
       <c r="E9">
-        <v>5.641233953012615E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F9">
-        <v>2.156314273909956E-2</v>
+        <v>2.528239520045539E-3</v>
       </c>
       <c r="G9">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H9">
-        <v>5.2477387897040713E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="I9">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J9">
-        <v>3.7948247542115591E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K9">
-        <v>9.1232782183906184E-3</v>
+        <v>2.3504202449427299E-3</v>
       </c>
       <c r="L9">
-        <v>5.7972003691997842E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M9">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N9">
-        <v>5.2477387897040713E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="O9">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P9">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q9">
-        <v>5.2477387897040713E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="R9">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S9">
-        <v>1.7994462413373071E-2</v>
+        <v>2.57512443744353E-3</v>
       </c>
       <c r="T9">
-        <v>6.1919466480956781E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="U9">
-        <v>2.7948845876090089E-2</v>
+        <v>3.9996613602846318E-3</v>
       </c>
       <c r="V9">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W9">
-        <v>4.4333796890958288E-2</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="X9">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y9">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z9">
-        <v>4.4333796890958288E-2</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AA9">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB9">
-        <v>2.121794880071198E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC9">
-        <v>4.4332552468432873E-2</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AD9">
-        <v>2.8170212875838881E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE9">
-        <v>1.4589371389502351E-2</v>
+        <v>1.399907830034044E-3</v>
       </c>
       <c r="AF9">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG9">
-        <v>2.501921987221041E-2</v>
+        <v>2.400693002143487E-3</v>
       </c>
       <c r="AH9">
-        <v>1.4589371389502351E-2</v>
+        <v>1.399907830034044E-3</v>
       </c>
       <c r="AI9">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ9">
-        <v>2.501921987221041E-2</v>
+        <v>2.400693002143487E-3</v>
       </c>
       <c r="AK9">
-        <v>1.7994462413373071E-2</v>
+        <v>2.57512443744353E-3</v>
       </c>
       <c r="AL9">
-        <v>5.0893156953114797E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="AM9">
-        <v>2.7948845876090089E-2</v>
+        <v>3.9996613602846318E-3</v>
       </c>
       <c r="AN9">
-        <v>2.2087278766677831E-2</v>
+        <v>1.077875042779767E-3</v>
       </c>
       <c r="AO9">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP9">
-        <v>2.8440895977858351E-2</v>
+        <v>1.387936118915564E-3</v>
       </c>
       <c r="AQ9">
-        <v>2.2087278766677831E-2</v>
+        <v>1.077875042779767E-3</v>
       </c>
       <c r="AR9">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS9">
-        <v>2.8440895977858351E-2</v>
+        <v>1.387936118915564E-3</v>
       </c>
       <c r="AT9">
-        <v>1.4589371389502351E-2</v>
+        <v>1.399907830034044E-3</v>
       </c>
       <c r="AU9">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV9">
-        <v>2.501921987221041E-2</v>
+        <v>2.400693002143487E-3</v>
       </c>
       <c r="AW9">
-        <v>1.4589371389502351E-2</v>
+        <v>1.399907830034044E-3</v>
       </c>
       <c r="AX9">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY9">
-        <v>2.501921987221041E-2</v>
+        <v>2.400693002143487E-3</v>
       </c>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2.3879560197959209E-2</v>
+        <v>2.869662986828103E-3</v>
       </c>
       <c r="B10">
-        <v>3.3948097693559776E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="C10">
-        <v>2.97935619150708E-2</v>
+        <v>3.580362501012764E-3</v>
       </c>
       <c r="D10">
-        <v>2.3879560197959209E-2</v>
+        <v>2.869662986828103E-3</v>
       </c>
       <c r="E10">
-        <v>3.3948097693559776E-2</v>
+        <v>1.4512280701754391E-4</v>
       </c>
       <c r="F10">
-        <v>2.97935619150708E-2</v>
+        <v>3.580362501012764E-3</v>
       </c>
       <c r="G10">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="H10">
-        <v>5.2477387897040713E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="I10">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="J10">
-        <v>3.7948247542115591E-3</v>
+        <v>1.837462737624004E-4</v>
       </c>
       <c r="K10">
-        <v>2.485595926756648E-2</v>
+        <v>4.157237073223638E-2</v>
       </c>
       <c r="L10">
-        <v>5.7972003691997842E-3</v>
+        <v>2.8070175438596478E-4</v>
       </c>
       <c r="M10">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="N10">
-        <v>5.2477387897040713E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="O10">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="P10">
-        <v>1.8581293284265839E-2</v>
+        <v>1.8493150684931509E-4</v>
       </c>
       <c r="Q10">
-        <v>5.2477387897040713E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="R10">
-        <v>2.8860306590455451E-2</v>
+        <v>2.8723404255319142E-4</v>
       </c>
       <c r="S10">
-        <v>2.4842262226883429E-2</v>
+        <v>7.8944083302602309E-3</v>
       </c>
       <c r="T10">
-        <v>1.9706174528261178E-3</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="U10">
-        <v>3.858479026728702E-2</v>
+        <v>1.226152783210631E-2</v>
       </c>
       <c r="V10">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="W10">
-        <v>0.12078542639167859</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="X10">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="Y10">
-        <v>2.1218544392257271E-2</v>
+        <v>2.114260008996851E-4</v>
       </c>
       <c r="Z10">
-        <v>0.12078542639167859</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AA10">
-        <v>2.8171003618656449E-2</v>
+        <v>2.8070175438596489E-4</v>
       </c>
       <c r="AB10">
-        <v>2.121794880071198E-2</v>
+        <v>2.1142006630133281E-4</v>
       </c>
       <c r="AC10">
-        <v>0.1207820360187377</v>
+        <v>2.0102283623599451E-4</v>
       </c>
       <c r="AD10">
-        <v>2.8170212875838881E-2</v>
+        <v>2.8069387525964183E-4</v>
       </c>
       <c r="AE10">
-        <v>2.014096224549702E-2</v>
+        <v>1.388676662940631E-2</v>
       </c>
       <c r="AF10">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AG10">
-        <v>3.4539607595469361E-2</v>
+        <v>2.381432745383295E-2</v>
       </c>
       <c r="AH10">
-        <v>2.014096224549702E-2</v>
+        <v>1.388676662940631E-2</v>
       </c>
       <c r="AI10">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AJ10">
-        <v>3.4539607595469361E-2</v>
+        <v>2.381432745383295E-2</v>
       </c>
       <c r="AK10">
-        <v>2.4842262226883429E-2</v>
+        <v>7.8944083302602309E-3</v>
       </c>
       <c r="AL10">
-        <v>5.0893156953114797E-2</v>
+        <v>1.6749982328865065E-4</v>
       </c>
       <c r="AM10">
-        <v>3.858479026728702E-2</v>
+        <v>1.226152783210631E-2</v>
       </c>
       <c r="AN10">
-        <v>3.4563604879611229E-2</v>
+        <v>2.7537160616379151E-2</v>
       </c>
       <c r="AO10">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AP10">
-        <v>4.450615675136322E-2</v>
+        <v>3.5458488521346081E-2</v>
       </c>
       <c r="AQ10">
-        <v>3.4563604879611229E-2</v>
+        <v>2.7537160616379151E-2</v>
       </c>
       <c r="AR10">
-        <v>5.3848142278756783E-2</v>
+        <v>1.3852631578947371E-4</v>
       </c>
       <c r="AS10">
-        <v>4.450615675136322E-2</v>
+        <v>3.5458488521346081E-2</v>
       </c>
       <c r="AT10">
-        <v>2.014096224549702E-2</v>
+        <v>1.388676662940631E-2</v>
       </c>
       <c r="AU10">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AV10">
-        <v>3.4539607595469361E-2</v>
+        <v>2.381432745383295E-2</v>
       </c>
       <c r="AW10">
-        <v>2.014096224549702E-2</v>
+        <v>1.388676662940631E-2</v>
       </c>
       <c r="AX10">
-        <v>4.7132468759379161E-2</v>
+        <v>1.2125000000000001E-4</v>
       </c>
       <c r="AY10">
-        <v>3.4539607595469361E-2</v>
+        <v>2.381432745383295E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add t axis to residue sim and swap a and b params so quadratic formula is consistent with elsewhere ax2 + bx +c (before we were doing ax + bx2 + c). And add csiro trials but didnt turn them on. No profit change because i didnt change anything
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\ExcelInputs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26978B26-E1DF-40B1-9170-60B9E4F21FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,14 +52,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -122,7 +98,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -154,27 +130,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,24 +164,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,409 +339,407 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AY10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AY10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.17069334575684059</v>
+        <v>0.1706933457568406</v>
       </c>
       <c r="B1">
-        <v>0.17729592423753929</v>
+        <v>0.1772959242375393</v>
       </c>
       <c r="C1">
-        <v>0.21296718713151341</v>
+        <v>0.2129671871315134</v>
       </c>
       <c r="D1">
-        <v>0.17069334575684059</v>
+        <v>0.1706933457568406</v>
       </c>
       <c r="E1">
-        <v>0.17729592423753929</v>
+        <v>0.1772959242375393</v>
       </c>
       <c r="F1">
-        <v>0.21296718713151341</v>
+        <v>0.2129671871315134</v>
       </c>
       <c r="G1">
-        <v>1.297240195222021E-2</v>
+        <v>0.01297240195222021</v>
       </c>
       <c r="H1">
-        <v>0.16492893339069939</v>
+        <v>0.1649289333906994</v>
       </c>
       <c r="I1">
-        <v>2.0148624308767561E-2</v>
+        <v>0.02014862430876756</v>
       </c>
       <c r="J1">
-        <v>2.648605191673075E-3</v>
+        <v>0.002648605191673075</v>
       </c>
       <c r="K1">
-        <v>1.7435530794102039E-2</v>
+        <v>0.01743553079410204</v>
       </c>
       <c r="L1">
-        <v>4.0461670800452506E-3</v>
+        <v>0.004046167080045251</v>
       </c>
       <c r="M1">
-        <v>1.297240195222021E-2</v>
+        <v>0.01297240195222021</v>
       </c>
       <c r="N1">
-        <v>0.16492893339069939</v>
+        <v>0.1649289333906994</v>
       </c>
       <c r="O1">
-        <v>2.0148624308767561E-2</v>
+        <v>0.02014862430876756</v>
       </c>
       <c r="P1">
-        <v>1.297240195222021E-2</v>
+        <v>0.01297240195222021</v>
       </c>
       <c r="Q1">
-        <v>0.16492893339069939</v>
+        <v>0.1649289333906994</v>
       </c>
       <c r="R1">
-        <v>2.0148624308767561E-2</v>
+        <v>0.02014862430876756</v>
       </c>
       <c r="S1">
-        <v>6.1451309414891804E-3</v>
+        <v>0.00614513094148918</v>
       </c>
       <c r="T1">
-        <v>0.1892678598946218</v>
+        <v>0.1892714792784908</v>
       </c>
       <c r="U1">
-        <v>9.5445650793342558E-3</v>
+        <v>0.009544565079334256</v>
       </c>
       <c r="V1">
-        <v>1.480952362153405E-2</v>
+        <v>0.01480952362153405</v>
       </c>
       <c r="W1">
-        <v>8.4726483442497266E-2</v>
+        <v>0.08472648344249727</v>
       </c>
       <c r="X1">
-        <v>1.966200582944095E-2</v>
+        <v>0.01966200582944095</v>
       </c>
       <c r="Y1">
-        <v>1.480952362153405E-2</v>
+        <v>0.01480952362153405</v>
       </c>
       <c r="Z1">
-        <v>8.4726483442497266E-2</v>
+        <v>0.08472648344249727</v>
       </c>
       <c r="AA1">
-        <v>1.966200582944095E-2</v>
+        <v>0.01966200582944095</v>
       </c>
       <c r="AB1">
-        <v>1.480910792727644E-2</v>
+        <v>0.01480910792727644</v>
       </c>
       <c r="AC1">
-        <v>8.4724105221999801E-2</v>
+        <v>0.0847241052219998</v>
       </c>
       <c r="AD1">
-        <v>1.9661453928979781E-2</v>
+        <v>0.01966145392897978</v>
       </c>
       <c r="AE1">
-        <v>2.4282338717033108E-3</v>
+        <v>0.002428233871703311</v>
       </c>
       <c r="AF1">
-        <v>0.14813061610090589</v>
+        <v>0.1481306161009059</v>
       </c>
       <c r="AG1">
-        <v>4.1641627672188699E-3</v>
+        <v>0.00416416276721887</v>
       </c>
       <c r="AH1">
-        <v>2.4282338717033108E-3</v>
+        <v>0.002428233871703311</v>
       </c>
       <c r="AI1">
-        <v>0.14813061610090589</v>
+        <v>0.1481306161009059</v>
       </c>
       <c r="AJ1">
-        <v>4.1641627672188699E-3</v>
+        <v>0.00416416276721887</v>
       </c>
       <c r="AK1">
-        <v>6.1451309414891804E-3</v>
+        <v>0.00614513094148918</v>
       </c>
       <c r="AL1">
         <v>0.1599499218526465</v>
       </c>
       <c r="AM1">
-        <v>9.5445650793342558E-3</v>
+        <v>0.009544565079334256</v>
       </c>
       <c r="AN1">
-        <v>3.7293384562146182E-3</v>
+        <v>0.003729338456214618</v>
       </c>
       <c r="AO1">
-        <v>0.16923701859037851</v>
+        <v>0.1692370185903785</v>
       </c>
       <c r="AP1">
-        <v>4.80211836957678E-3</v>
+        <v>0.00480211836957678</v>
       </c>
       <c r="AQ1">
-        <v>3.7293384562146182E-3</v>
+        <v>0.003729338456214618</v>
       </c>
       <c r="AR1">
-        <v>0.16923701859037851</v>
+        <v>0.1692370185903785</v>
       </c>
       <c r="AS1">
-        <v>4.80211836957678E-3</v>
+        <v>0.00480211836957678</v>
       </c>
       <c r="AT1">
-        <v>2.4282338717033108E-3</v>
+        <v>0.002428233871703311</v>
       </c>
       <c r="AU1">
-        <v>0.14813061610090589</v>
+        <v>0.1481306161009059</v>
       </c>
       <c r="AV1">
-        <v>4.1641627672188699E-3</v>
+        <v>0.00416416276721887</v>
       </c>
       <c r="AW1">
-        <v>2.4282338717033108E-3</v>
+        <v>0.002428233871703311</v>
       </c>
       <c r="AX1">
-        <v>0.14813061610090589</v>
+        <v>0.1481306161009059</v>
       </c>
       <c r="AY1">
-        <v>4.1641627672188699E-3</v>
+        <v>0.00416416276721887</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51">
       <c r="A2">
-        <v>3.4935840886530872E-2</v>
+        <v>0.03493584088653087</v>
       </c>
       <c r="B2">
-        <v>1.6117811294321761E-2</v>
+        <v>0.01611781129432176</v>
       </c>
       <c r="C2">
-        <v>4.3588036374173827E-2</v>
+        <v>0.04358803637417383</v>
       </c>
       <c r="D2">
-        <v>3.4935840886530872E-2</v>
+        <v>0.03493584088653087</v>
       </c>
       <c r="E2">
-        <v>1.6117811294321761E-2</v>
+        <v>0.01611781129432176</v>
       </c>
       <c r="F2">
-        <v>4.3588036374173827E-2</v>
+        <v>0.04358803637417383</v>
       </c>
       <c r="G2">
-        <v>4.7365913074357252E-2</v>
+        <v>0.04736591307435725</v>
       </c>
       <c r="H2">
-        <v>1.4993539399154489E-2</v>
+        <v>0.01499353939915449</v>
       </c>
       <c r="I2">
-        <v>7.3568333072937836E-2</v>
+        <v>0.07356833307293784</v>
       </c>
       <c r="J2">
-        <v>5.4147474403530467E-3</v>
+        <v>0.005414747440353047</v>
       </c>
       <c r="K2">
-        <v>1.585048254009276E-3</v>
+        <v>0.001585048254009276</v>
       </c>
       <c r="L2">
-        <v>8.271890770581887E-3</v>
+        <v>0.008271890770581887</v>
       </c>
       <c r="M2">
-        <v>4.7365913074357252E-2</v>
+        <v>0.04736591307435725</v>
       </c>
       <c r="N2">
-        <v>1.4993539399154489E-2</v>
+        <v>0.01499353939915449</v>
       </c>
       <c r="O2">
-        <v>7.3568333072937836E-2</v>
+        <v>0.07356833307293784</v>
       </c>
       <c r="P2">
-        <v>4.7365913074357252E-2</v>
+        <v>0.04736591307435725</v>
       </c>
       <c r="Q2">
-        <v>1.4993539399154489E-2</v>
+        <v>0.01499353939915449</v>
       </c>
       <c r="R2">
-        <v>7.3568333072937836E-2</v>
+        <v>0.07356833307293784</v>
       </c>
       <c r="S2">
-        <v>5.5864826740810729E-4</v>
+        <v>0.0005586482674081073</v>
       </c>
       <c r="T2">
-        <v>3.2302043749510331E-2</v>
+        <v>0.03230281627140072</v>
       </c>
       <c r="U2">
-        <v>8.6768773448493242E-4</v>
+        <v>0.0008676877344849324</v>
       </c>
       <c r="V2">
-        <v>3.027624893836859E-2</v>
+        <v>0.03027624893836859</v>
       </c>
       <c r="W2">
-        <v>7.7024075856815689E-3</v>
+        <v>0.007702407585681569</v>
       </c>
       <c r="X2">
-        <v>4.0196551782004243E-2</v>
+        <v>0.04019655178200424</v>
       </c>
       <c r="Y2">
-        <v>3.027624893836859E-2</v>
+        <v>0.03027624893836859</v>
       </c>
       <c r="Z2">
-        <v>7.7024075856815689E-3</v>
+        <v>0.007702407585681569</v>
       </c>
       <c r="AA2">
-        <v>4.0196551782004243E-2</v>
+        <v>0.04019655178200424</v>
       </c>
       <c r="AB2">
-        <v>3.0275399102604302E-2</v>
+        <v>0.0302753991026043</v>
       </c>
       <c r="AC2">
-        <v>7.7021913838181627E-3</v>
+        <v>0.007702191383818163</v>
       </c>
       <c r="AD2">
-        <v>4.0195423489415058E-2</v>
+        <v>0.04019542348941506</v>
       </c>
       <c r="AE2">
-        <v>2.2074853379121009E-4</v>
+        <v>0.0002207485337912101</v>
       </c>
       <c r="AF2">
-        <v>1.34664196455369E-2</v>
+        <v>0.0134664196455369</v>
       </c>
       <c r="AG2">
-        <v>3.7856025156535167E-4</v>
+        <v>0.0003785602515653517</v>
       </c>
       <c r="AH2">
-        <v>2.2074853379121009E-4</v>
+        <v>0.0002207485337912101</v>
       </c>
       <c r="AI2">
-        <v>1.34664196455369E-2</v>
+        <v>0.0134664196455369</v>
       </c>
       <c r="AJ2">
-        <v>3.7856025156535167E-4</v>
+        <v>0.0003785602515653517</v>
       </c>
       <c r="AK2">
-        <v>5.5864826740810729E-4</v>
+        <v>0.0005586482674081073</v>
       </c>
       <c r="AL2">
-        <v>1.4540901986604231E-2</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="AM2">
-        <v>8.6768773448493242E-4</v>
+        <v>0.0008676877344849324</v>
       </c>
       <c r="AN2">
-        <v>3.3903076874678339E-4</v>
+        <v>0.0003390307687467834</v>
       </c>
       <c r="AO2">
-        <v>1.5385183508216219E-2</v>
+        <v>0.01538518350821622</v>
       </c>
       <c r="AP2">
-        <v>4.3655621541607089E-4</v>
+        <v>0.0004365562154160709</v>
       </c>
       <c r="AQ2">
-        <v>3.3903076874678339E-4</v>
+        <v>0.0003390307687467834</v>
       </c>
       <c r="AR2">
-        <v>1.5385183508216219E-2</v>
+        <v>0.01538518350821622</v>
       </c>
       <c r="AS2">
-        <v>4.3655621541607089E-4</v>
+        <v>0.0004365562154160709</v>
       </c>
       <c r="AT2">
-        <v>2.2074853379121009E-4</v>
+        <v>0.0002207485337912101</v>
       </c>
       <c r="AU2">
-        <v>1.34664196455369E-2</v>
+        <v>0.0134664196455369</v>
       </c>
       <c r="AV2">
-        <v>3.7856025156535167E-4</v>
+        <v>0.0003785602515653517</v>
       </c>
       <c r="AW2">
-        <v>2.2074853379121009E-4</v>
+        <v>0.0002207485337912101</v>
       </c>
       <c r="AX2">
-        <v>1.34664196455369E-2</v>
+        <v>0.0134664196455369</v>
       </c>
       <c r="AY2">
-        <v>3.7856025156535167E-4</v>
+        <v>0.0003785602515653517</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51">
       <c r="A3">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="B3">
-        <v>0.22635979242130261</v>
+        <v>0.2263597924213026</v>
       </c>
       <c r="C3">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="D3">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="E3">
-        <v>0.22635979242130261</v>
+        <v>0.2263597924213026</v>
       </c>
       <c r="F3">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="G3">
-        <v>9.076573040146127E-2</v>
+        <v>0.09076573040146127</v>
       </c>
       <c r="H3">
         <v>0.2105704306917219</v>
       </c>
       <c r="I3">
-        <v>0.14097655998524841</v>
+        <v>0.1409765599852484</v>
       </c>
       <c r="J3">
-        <v>2.6848141865304379E-2</v>
+        <v>0.02684814186530438</v>
       </c>
       <c r="K3">
-        <v>4.0916750876948918E-2</v>
+        <v>0.04091675087694892</v>
       </c>
       <c r="L3">
-        <v>4.1014820977209668E-2</v>
+        <v>0.04101482097720967</v>
       </c>
       <c r="M3">
-        <v>9.076573040146127E-2</v>
+        <v>0.09076573040146127</v>
       </c>
       <c r="N3">
         <v>0.2105704306917219</v>
       </c>
       <c r="O3">
-        <v>0.14097655998524841</v>
+        <v>0.1409765599852484</v>
       </c>
       <c r="P3">
-        <v>9.076573040146127E-2</v>
+        <v>0.09076573040146127</v>
       </c>
       <c r="Q3">
         <v>0.2105704306917219</v>
       </c>
       <c r="R3">
-        <v>0.14097655998524841</v>
+        <v>0.1409765599852484</v>
       </c>
       <c r="S3">
         <v>0.1325050224731904</v>
       </c>
       <c r="T3">
-        <v>2.6238275402749485E-2</v>
+        <v>0.02623887634839434</v>
       </c>
       <c r="U3">
-        <v>0.20580567320304041</v>
+        <v>0.2058056732030404</v>
       </c>
       <c r="V3">
-        <v>0.15011984134085329</v>
+        <v>0.1501198413408533</v>
       </c>
       <c r="W3">
-        <v>0.19883148133748241</v>
+        <v>0.1988314813374824</v>
       </c>
       <c r="X3">
-        <v>0.19930804467381369</v>
+        <v>0.1993080446738137</v>
       </c>
       <c r="Y3">
-        <v>0.15011984134085329</v>
+        <v>0.1501198413408533</v>
       </c>
       <c r="Z3">
-        <v>0.19883148133748241</v>
+        <v>0.1988314813374824</v>
       </c>
       <c r="AA3">
-        <v>0.19930804467381369</v>
+        <v>0.1993080446738137</v>
       </c>
       <c r="AB3">
-        <v>0.15011562756885141</v>
+        <v>0.1501156275688514</v>
       </c>
       <c r="AC3">
         <v>0.1988259002595803</v>
@@ -816,7 +754,7 @@
         <v>0.189123442380528</v>
       </c>
       <c r="AG3">
-        <v>0.18820104037224189</v>
+        <v>0.1882010403722419</v>
       </c>
       <c r="AH3">
         <v>0.1097450235421261</v>
@@ -825,34 +763,34 @@
         <v>0.189123442380528</v>
       </c>
       <c r="AJ3">
-        <v>0.18820104037224189</v>
+        <v>0.1882010403722419</v>
       </c>
       <c r="AK3">
         <v>0.1325050224731904</v>
       </c>
       <c r="AL3">
-        <v>1.4540901986604231E-2</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="AM3">
-        <v>0.20580567320304041</v>
+        <v>0.2058056732030404</v>
       </c>
       <c r="AN3">
-        <v>0.14144991040144761</v>
+        <v>0.1414499104014476</v>
       </c>
       <c r="AO3">
-        <v>0.21607071094760699</v>
+        <v>0.216070710947607</v>
       </c>
       <c r="AP3">
-        <v>0.18213933143607669</v>
+        <v>0.1821393314360767</v>
       </c>
       <c r="AQ3">
-        <v>0.14144991040144761</v>
+        <v>0.1414499104014476</v>
       </c>
       <c r="AR3">
-        <v>0.21607071094760699</v>
+        <v>0.216070710947607</v>
       </c>
       <c r="AS3">
-        <v>0.18213933143607669</v>
+        <v>0.1821393314360767</v>
       </c>
       <c r="AT3">
         <v>0.1097450235421261</v>
@@ -861,7 +799,7 @@
         <v>0.189123442380528</v>
       </c>
       <c r="AV3">
-        <v>0.18820104037224189</v>
+        <v>0.1882010403722419</v>
       </c>
       <c r="AW3">
         <v>0.1097450235421261</v>
@@ -870,30 +808,30 @@
         <v>0.189123442380528</v>
       </c>
       <c r="AY3">
-        <v>0.18820104037224189</v>
+        <v>0.1882010403722419</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51">
       <c r="A4">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="B4">
-        <v>0.22409796236541021</v>
+        <v>0.2240979623654102</v>
       </c>
       <c r="C4">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="D4">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="E4">
-        <v>0.22409796236541021</v>
+        <v>0.2240979623654102</v>
       </c>
       <c r="F4">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="G4">
-        <v>7.298818546593154E-2</v>
+        <v>0.07298818546593154</v>
       </c>
       <c r="H4">
         <v>0.2084663709383259</v>
@@ -902,16 +840,16 @@
         <v>0.1133646284896383</v>
       </c>
       <c r="J4">
-        <v>1.087073643375785E-2</v>
+        <v>0.01087073643375785</v>
       </c>
       <c r="K4">
-        <v>4.0493611660579687E-2</v>
+        <v>0.04049361166057969</v>
       </c>
       <c r="L4">
-        <v>1.6606784594549229E-2</v>
+        <v>0.01660678459454923</v>
       </c>
       <c r="M4">
-        <v>7.298818546593154E-2</v>
+        <v>0.07298818546593154</v>
       </c>
       <c r="N4">
         <v>0.2084663709383259</v>
@@ -920,7 +858,7 @@
         <v>0.1133646284896383</v>
       </c>
       <c r="P4">
-        <v>7.298818546593154E-2</v>
+        <v>0.07298818546593154</v>
       </c>
       <c r="Q4">
         <v>0.2084663709383259</v>
@@ -929,1033 +867,1033 @@
         <v>0.1133646284896383</v>
       </c>
       <c r="S4">
-        <v>7.2401354595038783E-2</v>
+        <v>0.07240135459503878</v>
       </c>
       <c r="T4">
-        <v>0.16905002841257127</v>
+        <v>0.1690547412033029</v>
       </c>
       <c r="U4">
-        <v>0.11245316777527301</v>
+        <v>0.112453167775273</v>
       </c>
       <c r="V4">
-        <v>6.0783097649035799E-2</v>
+        <v>0.0607830976490358</v>
       </c>
       <c r="W4">
-        <v>0.19677527219576199</v>
+        <v>0.196775272195762</v>
       </c>
       <c r="X4">
-        <v>8.0699261559570926E-2</v>
+        <v>0.08069926155957093</v>
       </c>
       <c r="Y4">
-        <v>6.0783097649035799E-2</v>
+        <v>0.0607830976490358</v>
       </c>
       <c r="Z4">
-        <v>0.19677527219576199</v>
+        <v>0.196775272195762</v>
       </c>
       <c r="AA4">
-        <v>8.0699261559570926E-2</v>
+        <v>0.08069926155957093</v>
       </c>
       <c r="AB4">
-        <v>6.0781391504712859E-2</v>
+        <v>0.06078139150471286</v>
       </c>
       <c r="AC4">
-        <v>0.19676974883439119</v>
+        <v>0.1967697488343912</v>
       </c>
       <c r="AD4">
-        <v>8.0696996380725139E-2</v>
+        <v>0.08069699638072514</v>
       </c>
       <c r="AE4">
-        <v>5.8708077211763743E-2</v>
+        <v>0.05870807721176374</v>
       </c>
       <c r="AF4">
-        <v>0.18723368500942231</v>
+        <v>0.1872336850094223</v>
       </c>
       <c r="AG4">
         <v>0.1006781068780459</v>
       </c>
       <c r="AH4">
-        <v>5.8708077211763743E-2</v>
+        <v>0.05870807721176374</v>
       </c>
       <c r="AI4">
-        <v>0.18723368500942231</v>
+        <v>0.1872336850094223</v>
       </c>
       <c r="AJ4">
         <v>0.1006781068780459</v>
       </c>
       <c r="AK4">
-        <v>7.2401354595038783E-2</v>
+        <v>0.07240135459503878</v>
       </c>
       <c r="AL4">
-        <v>6.4787130329130305E-2</v>
+        <v>0.0647871303291303</v>
       </c>
       <c r="AM4">
-        <v>0.11245316777527301</v>
+        <v>0.112453167775273</v>
       </c>
       <c r="AN4">
         <v>0.1112871408980786</v>
       </c>
       <c r="AO4">
-        <v>0.21391169134880059</v>
+        <v>0.2139116913488006</v>
       </c>
       <c r="AP4">
-        <v>0.14329995249258959</v>
+        <v>0.1432999524925896</v>
       </c>
       <c r="AQ4">
         <v>0.1112871408980786</v>
       </c>
       <c r="AR4">
-        <v>0.21391169134880059</v>
+        <v>0.2139116913488006</v>
       </c>
       <c r="AS4">
-        <v>0.14329995249258959</v>
+        <v>0.1432999524925896</v>
       </c>
       <c r="AT4">
-        <v>5.8708077211763743E-2</v>
+        <v>0.05870807721176374</v>
       </c>
       <c r="AU4">
-        <v>0.18723368500942231</v>
+        <v>0.1872336850094223</v>
       </c>
       <c r="AV4">
         <v>0.1006781068780459</v>
       </c>
       <c r="AW4">
-        <v>5.8708077211763743E-2</v>
+        <v>0.05870807721176374</v>
       </c>
       <c r="AX4">
-        <v>0.18723368500942231</v>
+        <v>0.1872336850094223</v>
       </c>
       <c r="AY4">
         <v>0.1006781068780459</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51">
       <c r="A5">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="B5">
-        <v>9.653105386736166E-2</v>
+        <v>0.09653105386736166</v>
       </c>
       <c r="C5">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="D5">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="E5">
-        <v>9.653105386736166E-2</v>
+        <v>0.09653105386736166</v>
       </c>
       <c r="F5">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="G5">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="H5">
-        <v>8.9797686110897973E-2</v>
+        <v>0.08979768611089797</v>
       </c>
       <c r="I5">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="J5">
-        <v>3.7948247542115591E-3</v>
+        <v>0.003794824754211559</v>
       </c>
       <c r="K5">
-        <v>1.6628617225702289E-2</v>
+        <v>0.01662861722570229</v>
       </c>
       <c r="L5">
-        <v>5.7972003691997842E-3</v>
+        <v>0.005797200369199784</v>
       </c>
       <c r="M5">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="N5">
-        <v>8.9797686110897973E-2</v>
+        <v>0.08979768611089797</v>
       </c>
       <c r="O5">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="P5">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="Q5">
-        <v>8.9797686110897973E-2</v>
+        <v>0.08979768611089797</v>
       </c>
       <c r="R5">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="S5">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="T5">
-        <v>0.19504265042326546</v>
+        <v>0.1950474781872779</v>
       </c>
       <c r="U5">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="V5">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="W5">
-        <v>8.0805355379354224E-2</v>
+        <v>0.08080535537935422</v>
       </c>
       <c r="X5">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="Y5">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="Z5">
-        <v>8.0805355379354224E-2</v>
+        <v>0.08080535537935422</v>
       </c>
       <c r="AA5">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="AB5">
-        <v>2.121794880071198E-2</v>
+        <v>0.02121794880071198</v>
       </c>
       <c r="AC5">
-        <v>8.0803087222519915E-2</v>
+        <v>0.08080308722251991</v>
       </c>
       <c r="AD5">
-        <v>2.8170212875838881E-2</v>
+        <v>0.02817021287583888</v>
       </c>
       <c r="AE5">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AF5">
-        <v>8.065162548849171E-2</v>
+        <v>0.08065162548849171</v>
       </c>
       <c r="AG5">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AH5">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AI5">
-        <v>8.065162548849171E-2</v>
+        <v>0.08065162548849171</v>
       </c>
       <c r="AJ5">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AK5">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="AL5">
-        <v>0.24834049582135209</v>
+        <v>0.2483404958213521</v>
       </c>
       <c r="AM5">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="AN5">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AO5">
-        <v>9.2143278691572489E-2</v>
+        <v>0.09214327869157249</v>
       </c>
       <c r="AP5">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AQ5">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AR5">
-        <v>9.2143278691572489E-2</v>
+        <v>0.09214327869157249</v>
       </c>
       <c r="AS5">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AT5">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AU5">
-        <v>8.065162548849171E-2</v>
+        <v>0.08065162548849171</v>
       </c>
       <c r="AV5">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AW5">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AX5">
-        <v>8.065162548849171E-2</v>
+        <v>0.08065162548849171</v>
       </c>
       <c r="AY5">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51">
       <c r="A6">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="B6">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="C6">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="D6">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="E6">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="F6">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="G6">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="H6">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="I6">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="J6">
-        <v>3.7948247542115591E-3</v>
+        <v>0.003794824754211559</v>
       </c>
       <c r="K6">
-        <v>9.1232782183906184E-3</v>
+        <v>0.009123278218390618</v>
       </c>
       <c r="L6">
-        <v>5.7972003691997842E-3</v>
+        <v>0.005797200369199784</v>
       </c>
       <c r="M6">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="N6">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="O6">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="P6">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="Q6">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="R6">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="S6">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="T6">
-        <v>0.15611659276390244</v>
+        <v>0.1561194814131179</v>
       </c>
       <c r="U6">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="V6">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="W6">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="X6">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="Y6">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="Z6">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="AA6">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="AB6">
-        <v>2.121794880071198E-2</v>
+        <v>0.02121794880071198</v>
       </c>
       <c r="AC6">
-        <v>4.4332552468432873E-2</v>
+        <v>0.04433255246843287</v>
       </c>
       <c r="AD6">
-        <v>2.8170212875838881E-2</v>
+        <v>0.02817021287583888</v>
       </c>
       <c r="AE6">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AF6">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AG6">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AH6">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AI6">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AJ6">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AK6">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="AL6">
-        <v>0.16034481276636189</v>
+        <v>0.1603448127663619</v>
       </c>
       <c r="AM6">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="AN6">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AO6">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AP6">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AQ6">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AR6">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AS6">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AT6">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AU6">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AV6">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AW6">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AX6">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AY6">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51">
       <c r="A7">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="B7">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="C7">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="D7">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="E7">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="F7">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="G7">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="H7">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="I7">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="J7">
-        <v>3.7948247542115591E-3</v>
+        <v>0.003794824754211559</v>
       </c>
       <c r="K7">
-        <v>9.1232782183906184E-3</v>
+        <v>0.009123278218390618</v>
       </c>
       <c r="L7">
-        <v>5.7972003691997842E-3</v>
+        <v>0.005797200369199784</v>
       </c>
       <c r="M7">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="N7">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="O7">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="P7">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="Q7">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="R7">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="S7">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="T7">
-        <v>0.10617299893863949</v>
+        <v>0.1061744027167735</v>
       </c>
       <c r="U7">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="V7">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="W7">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="X7">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="Y7">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="Z7">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="AA7">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="AB7">
-        <v>2.121794880071198E-2</v>
+        <v>0.02121794880071198</v>
       </c>
       <c r="AC7">
-        <v>4.4332552468432873E-2</v>
+        <v>0.04433255246843287</v>
       </c>
       <c r="AD7">
-        <v>2.8170212875838881E-2</v>
+        <v>0.02817021287583888</v>
       </c>
       <c r="AE7">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AF7">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AG7">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AH7">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AI7">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AJ7">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AK7">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="AL7">
-        <v>5.0893156953114797E-2</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="AM7">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="AN7">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AO7">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AP7">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AQ7">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AR7">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AS7">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AT7">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AU7">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AV7">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AW7">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AX7">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AY7">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51">
       <c r="A8">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="B8">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="C8">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="D8">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="E8">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="F8">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="G8">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="H8">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="I8">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="J8">
-        <v>3.7948247542115591E-3</v>
+        <v>0.003794824754211559</v>
       </c>
       <c r="K8">
-        <v>9.1232782183906184E-3</v>
+        <v>0.009123278218390618</v>
       </c>
       <c r="L8">
-        <v>5.7972003691997842E-3</v>
+        <v>0.005797200369199784</v>
       </c>
       <c r="M8">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="N8">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="O8">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="P8">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="Q8">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="R8">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="S8">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="T8">
-        <v>6.1919466480956781E-2</v>
+        <v>0.06192078408795966</v>
       </c>
       <c r="U8">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="V8">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="W8">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="X8">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="Y8">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="Z8">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="AA8">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="AB8">
-        <v>2.121794880071198E-2</v>
+        <v>0.02121794880071198</v>
       </c>
       <c r="AC8">
-        <v>4.4332552468432873E-2</v>
+        <v>0.04433255246843287</v>
       </c>
       <c r="AD8">
-        <v>2.8170212875838881E-2</v>
+        <v>0.02817021287583888</v>
       </c>
       <c r="AE8">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AF8">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AG8">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AH8">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AI8">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AJ8">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AK8">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="AL8">
-        <v>5.0893156953114797E-2</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="AM8">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="AN8">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AO8">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AP8">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AQ8">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AR8">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AS8">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AT8">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AU8">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AV8">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AW8">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AX8">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AY8">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51">
       <c r="A9">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="B9">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="C9">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="D9">
-        <v>1.7282873614216911E-2</v>
+        <v>0.01728287361421691</v>
       </c>
       <c r="E9">
-        <v>5.641233953012615E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="F9">
-        <v>2.156314273909956E-2</v>
+        <v>0.02156314273909956</v>
       </c>
       <c r="G9">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="H9">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="I9">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="J9">
-        <v>3.7948247542115591E-3</v>
+        <v>0.003794824754211559</v>
       </c>
       <c r="K9">
-        <v>9.1232782183906184E-3</v>
+        <v>0.009123278218390618</v>
       </c>
       <c r="L9">
-        <v>5.7972003691997842E-3</v>
+        <v>0.005797200369199784</v>
       </c>
       <c r="M9">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="N9">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="O9">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="P9">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="Q9">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="R9">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="S9">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="T9">
-        <v>6.1919466480956781E-2</v>
+        <v>0.06192078408795966</v>
       </c>
       <c r="U9">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="V9">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="W9">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="X9">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="Y9">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="Z9">
-        <v>4.4333796890958288E-2</v>
+        <v>0.04433379689095829</v>
       </c>
       <c r="AA9">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="AB9">
-        <v>2.121794880071198E-2</v>
+        <v>0.02121794880071198</v>
       </c>
       <c r="AC9">
-        <v>4.4332552468432873E-2</v>
+        <v>0.04433255246843287</v>
       </c>
       <c r="AD9">
-        <v>2.8170212875838881E-2</v>
+        <v>0.02817021287583888</v>
       </c>
       <c r="AE9">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AF9">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AG9">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AH9">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AI9">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AJ9">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AK9">
-        <v>1.7994462413373071E-2</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="AL9">
-        <v>5.0893156953114797E-2</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="AM9">
-        <v>2.7948845876090089E-2</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="AN9">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AO9">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AP9">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AQ9">
-        <v>2.2087278766677831E-2</v>
+        <v>0.02208727876667783</v>
       </c>
       <c r="AR9">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AS9">
-        <v>2.8440895977858351E-2</v>
+        <v>0.02844089597785835</v>
       </c>
       <c r="AT9">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AU9">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AV9">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
       <c r="AW9">
-        <v>1.4589371389502351E-2</v>
+        <v>0.01458937138950235</v>
       </c>
       <c r="AX9">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AY9">
-        <v>2.501921987221041E-2</v>
+        <v>0.02501921987221041</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51">
       <c r="A10">
-        <v>2.3879560197959209E-2</v>
+        <v>0.02387956019795921</v>
       </c>
       <c r="B10">
-        <v>3.3948097693559776E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="C10">
-        <v>2.97935619150708E-2</v>
+        <v>0.0297935619150708</v>
       </c>
       <c r="D10">
-        <v>2.3879560197959209E-2</v>
+        <v>0.02387956019795921</v>
       </c>
       <c r="E10">
-        <v>3.3948097693559776E-2</v>
+        <v>0.05641233953012615</v>
       </c>
       <c r="F10">
-        <v>2.97935619150708E-2</v>
+        <v>0.0297935619150708</v>
       </c>
       <c r="G10">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="H10">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="I10">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="J10">
-        <v>3.7948247542115591E-3</v>
+        <v>0.003794824754211559</v>
       </c>
       <c r="K10">
-        <v>2.485595926756648E-2</v>
+        <v>0.02485595926756648</v>
       </c>
       <c r="L10">
-        <v>5.7972003691997842E-3</v>
+        <v>0.005797200369199784</v>
       </c>
       <c r="M10">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="N10">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="O10">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="P10">
-        <v>1.8581293284265839E-2</v>
+        <v>0.01858129328426584</v>
       </c>
       <c r="Q10">
-        <v>5.2477387897040713E-2</v>
+        <v>0.05247738789704071</v>
       </c>
       <c r="R10">
-        <v>2.8860306590455451E-2</v>
+        <v>0.02886030659045545</v>
       </c>
       <c r="S10">
-        <v>2.4842262226883429E-2</v>
+        <v>0.02484226222688343</v>
       </c>
       <c r="T10">
-        <v>1.9706174528261178E-3</v>
+        <v>0.06192078408795966</v>
       </c>
       <c r="U10">
-        <v>3.858479026728702E-2</v>
+        <v>0.03858479026728702</v>
       </c>
       <c r="V10">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="W10">
-        <v>0.12078542639167859</v>
+        <v>0.1207854263916786</v>
       </c>
       <c r="X10">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="Y10">
-        <v>2.1218544392257271E-2</v>
+        <v>0.02121854439225727</v>
       </c>
       <c r="Z10">
-        <v>0.12078542639167859</v>
+        <v>0.1207854263916786</v>
       </c>
       <c r="AA10">
-        <v>2.8171003618656449E-2</v>
+        <v>0.02817100361865645</v>
       </c>
       <c r="AB10">
-        <v>2.121794880071198E-2</v>
+        <v>0.02121794880071198</v>
       </c>
       <c r="AC10">
         <v>0.1207820360187377</v>
       </c>
       <c r="AD10">
-        <v>2.8170212875838881E-2</v>
+        <v>0.02817021287583888</v>
       </c>
       <c r="AE10">
-        <v>2.014096224549702E-2</v>
+        <v>0.02014096224549702</v>
       </c>
       <c r="AF10">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AG10">
-        <v>3.4539607595469361E-2</v>
+        <v>0.03453960759546936</v>
       </c>
       <c r="AH10">
-        <v>2.014096224549702E-2</v>
+        <v>0.02014096224549702</v>
       </c>
       <c r="AI10">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AJ10">
-        <v>3.4539607595469361E-2</v>
+        <v>0.03453960759546936</v>
       </c>
       <c r="AK10">
-        <v>2.4842262226883429E-2</v>
+        <v>0.02484226222688343</v>
       </c>
       <c r="AL10">
-        <v>5.0893156953114797E-2</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="AM10">
-        <v>3.858479026728702E-2</v>
+        <v>0.03858479026728702</v>
       </c>
       <c r="AN10">
-        <v>3.4563604879611229E-2</v>
+        <v>0.03456360487961123</v>
       </c>
       <c r="AO10">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AP10">
-        <v>4.450615675136322E-2</v>
+        <v>0.04450615675136322</v>
       </c>
       <c r="AQ10">
-        <v>3.4563604879611229E-2</v>
+        <v>0.03456360487961123</v>
       </c>
       <c r="AR10">
-        <v>5.3848142278756783E-2</v>
+        <v>0.05384814227875678</v>
       </c>
       <c r="AS10">
-        <v>4.450615675136322E-2</v>
+        <v>0.04450615675136322</v>
       </c>
       <c r="AT10">
-        <v>2.014096224549702E-2</v>
+        <v>0.02014096224549702</v>
       </c>
       <c r="AU10">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AV10">
-        <v>3.4539607595469361E-2</v>
+        <v>0.03453960759546936</v>
       </c>
       <c r="AW10">
-        <v>2.014096224549702E-2</v>
+        <v>0.02014096224549702</v>
       </c>
       <c r="AX10">
-        <v>4.7132468759379161E-2</v>
+        <v>0.04713246875937916</v>
       </c>
       <c r="AY10">
-        <v>3.4539607595469361E-2</v>
+        <v>0.03453960759546936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set lentils, faba and chickpeas to have same stubble inputs as lupins. No porift change due to those landuses not being selected.
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -366,40 +366,40 @@
         <v>0.2129671871315134</v>
       </c>
       <c r="G1">
-        <v>0.01297240195222021</v>
+        <v>0.00614513094148918</v>
       </c>
       <c r="H1">
-        <v>0.1649289333906994</v>
+        <v>0.1599499218526465</v>
       </c>
       <c r="I1">
-        <v>0.02014862430876756</v>
+        <v>0.009544565079334256</v>
       </c>
       <c r="J1">
-        <v>0.002648605191673075</v>
+        <v>0.09505056148880539</v>
       </c>
       <c r="K1">
-        <v>0.01743553079410204</v>
+        <v>0.06354486258187295</v>
       </c>
       <c r="L1">
-        <v>0.004046167080045251</v>
+        <v>0.145204900316941</v>
       </c>
       <c r="M1">
-        <v>0.01297240195222021</v>
+        <v>0.00614513094148918</v>
       </c>
       <c r="N1">
-        <v>0.1649289333906994</v>
+        <v>0.1599499218526465</v>
       </c>
       <c r="O1">
-        <v>0.02014862430876756</v>
+        <v>0.009544565079334256</v>
       </c>
       <c r="P1">
-        <v>0.01297240195222021</v>
+        <v>0.00614513094148918</v>
       </c>
       <c r="Q1">
-        <v>0.1649289333906994</v>
+        <v>0.1599499218526465</v>
       </c>
       <c r="R1">
-        <v>0.02014862430876756</v>
+        <v>0.009544565079334256</v>
       </c>
       <c r="S1">
         <v>0.00614513094148918</v>
@@ -411,31 +411,31 @@
         <v>0.009544565079334256</v>
       </c>
       <c r="V1">
-        <v>0.01480952362153405</v>
+        <v>0.1458254340789792</v>
       </c>
       <c r="W1">
         <v>0.08472648344249727</v>
       </c>
       <c r="X1">
-        <v>0.01966200582944095</v>
+        <v>0.1936065337559213</v>
       </c>
       <c r="Y1">
-        <v>0.01480952362153405</v>
+        <v>0.1458254340789792</v>
       </c>
       <c r="Z1">
         <v>0.08472648344249727</v>
       </c>
       <c r="AA1">
-        <v>0.01966200582944095</v>
+        <v>0.1936065337559213</v>
       </c>
       <c r="AB1">
-        <v>0.01480910792727644</v>
+        <v>0.1458213408483589</v>
       </c>
       <c r="AC1">
         <v>0.0847241052219998</v>
       </c>
       <c r="AD1">
-        <v>0.01966145392897978</v>
+        <v>0.1936010993390977</v>
       </c>
       <c r="AE1">
         <v>0.002428233871703311</v>
@@ -521,40 +521,40 @@
         <v>0.04358803637417383</v>
       </c>
       <c r="G2">
-        <v>0.04736591307435725</v>
+        <v>0.0005586482674081073</v>
       </c>
       <c r="H2">
-        <v>0.01499353939915449</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="I2">
-        <v>0.07356833307293784</v>
+        <v>0.0008676877344849324</v>
       </c>
       <c r="J2">
-        <v>0.005414747440353047</v>
+        <v>0.01945401724727308</v>
       </c>
       <c r="K2">
-        <v>0.001585048254009276</v>
+        <v>0.005776805689261176</v>
       </c>
       <c r="L2">
-        <v>0.008271890770581887</v>
+        <v>0.02971911570966397</v>
       </c>
       <c r="M2">
-        <v>0.04736591307435725</v>
+        <v>0.0005586482674081073</v>
       </c>
       <c r="N2">
-        <v>0.01499353939915449</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="O2">
-        <v>0.07356833307293784</v>
+        <v>0.0008676877344849324</v>
       </c>
       <c r="P2">
-        <v>0.04736591307435725</v>
+        <v>0.0005586482674081073</v>
       </c>
       <c r="Q2">
-        <v>0.01499353939915449</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="R2">
-        <v>0.07356833307293784</v>
+        <v>0.0008676877344849324</v>
       </c>
       <c r="S2">
         <v>0.0005586482674081073</v>
@@ -566,31 +566,31 @@
         <v>0.0008676877344849324</v>
       </c>
       <c r="V2">
-        <v>0.03027624893836859</v>
+        <v>0.029846120477654</v>
       </c>
       <c r="W2">
         <v>0.007702407585681569</v>
       </c>
       <c r="X2">
-        <v>0.04019655178200424</v>
+        <v>0.0396254876128853</v>
       </c>
       <c r="Y2">
-        <v>0.03027624893836859</v>
+        <v>0.029846120477654</v>
       </c>
       <c r="Z2">
         <v>0.007702407585681569</v>
       </c>
       <c r="AA2">
-        <v>0.04019655178200424</v>
+        <v>0.0396254876128853</v>
       </c>
       <c r="AB2">
-        <v>0.0302753991026043</v>
+        <v>0.02984528271533216</v>
       </c>
       <c r="AC2">
         <v>0.007702191383818163</v>
       </c>
       <c r="AD2">
-        <v>0.04019542348941506</v>
+        <v>0.03962437534971758</v>
       </c>
       <c r="AE2">
         <v>0.0002207485337912101</v>
@@ -676,40 +676,40 @@
         <v>0.02156314273909956</v>
       </c>
       <c r="G3">
-        <v>0.09076573040146127</v>
+        <v>0.1325050224731904</v>
       </c>
       <c r="H3">
-        <v>0.2105704306917219</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="I3">
-        <v>0.1409765599852484</v>
+        <v>0.2058056732030404</v>
       </c>
       <c r="J3">
-        <v>0.02684814186530438</v>
+        <v>0.009623965327339321</v>
       </c>
       <c r="K3">
-        <v>0.04091675087694892</v>
+        <v>0.1491236110031118</v>
       </c>
       <c r="L3">
-        <v>0.04101482097720967</v>
+        <v>0.01470214277665879</v>
       </c>
       <c r="M3">
-        <v>0.09076573040146127</v>
+        <v>0.1325050224731904</v>
       </c>
       <c r="N3">
-        <v>0.2105704306917219</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="O3">
-        <v>0.1409765599852484</v>
+        <v>0.2058056732030404</v>
       </c>
       <c r="P3">
-        <v>0.09076573040146127</v>
+        <v>0.1325050224731904</v>
       </c>
       <c r="Q3">
-        <v>0.2105704306917219</v>
+        <v>0.01454090198660423</v>
       </c>
       <c r="R3">
-        <v>0.1409765599852484</v>
+        <v>0.2058056732030404</v>
       </c>
       <c r="S3">
         <v>0.1325050224731904</v>
@@ -721,31 +721,31 @@
         <v>0.2058056732030404</v>
       </c>
       <c r="V3">
-        <v>0.1501198413408533</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="W3">
         <v>0.1988314813374824</v>
       </c>
       <c r="X3">
-        <v>0.1993080446738137</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="Y3">
-        <v>0.1501198413408533</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="Z3">
         <v>0.1988314813374824</v>
       </c>
       <c r="AA3">
-        <v>0.1993080446738137</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="AB3">
-        <v>0.1501156275688514</v>
+        <v>0.0147645580029111</v>
       </c>
       <c r="AC3">
         <v>0.1988259002595803</v>
       </c>
       <c r="AD3">
-        <v>0.1993024502190707</v>
+        <v>0.01960230679535431</v>
       </c>
       <c r="AE3">
         <v>0.1097450235421261</v>
@@ -831,40 +831,40 @@
         <v>0.02156314273909956</v>
       </c>
       <c r="G4">
-        <v>0.07298818546593154</v>
+        <v>0.07240135459503878</v>
       </c>
       <c r="H4">
-        <v>0.2084663709383259</v>
+        <v>0.0647871303291303</v>
       </c>
       <c r="I4">
-        <v>0.1133646284896383</v>
+        <v>0.112453167775273</v>
       </c>
       <c r="J4">
-        <v>0.01087073643375785</v>
+        <v>0.009623965327339321</v>
       </c>
       <c r="K4">
-        <v>0.04049361166057969</v>
+        <v>0.1475814541468215</v>
       </c>
       <c r="L4">
-        <v>0.01660678459454923</v>
+        <v>0.01470214277665879</v>
       </c>
       <c r="M4">
-        <v>0.07298818546593154</v>
+        <v>0.07240135459503878</v>
       </c>
       <c r="N4">
-        <v>0.2084663709383259</v>
+        <v>0.0647871303291303</v>
       </c>
       <c r="O4">
-        <v>0.1133646284896383</v>
+        <v>0.112453167775273</v>
       </c>
       <c r="P4">
-        <v>0.07298818546593154</v>
+        <v>0.07240135459503878</v>
       </c>
       <c r="Q4">
-        <v>0.2084663709383259</v>
+        <v>0.0647871303291303</v>
       </c>
       <c r="R4">
-        <v>0.1133646284896383</v>
+        <v>0.112453167775273</v>
       </c>
       <c r="S4">
         <v>0.07240135459503878</v>
@@ -876,31 +876,31 @@
         <v>0.112453167775273</v>
       </c>
       <c r="V4">
-        <v>0.0607830976490358</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="W4">
         <v>0.196775272195762</v>
       </c>
       <c r="X4">
-        <v>0.08069926155957093</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="Y4">
-        <v>0.0607830976490358</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="Z4">
         <v>0.196775272195762</v>
       </c>
       <c r="AA4">
-        <v>0.08069926155957093</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="AB4">
-        <v>0.06078139150471286</v>
+        <v>0.0147645580029111</v>
       </c>
       <c r="AC4">
         <v>0.1967697488343912</v>
       </c>
       <c r="AD4">
-        <v>0.08069699638072514</v>
+        <v>0.01960230679535431</v>
       </c>
       <c r="AE4">
         <v>0.05870807721176374</v>
@@ -986,40 +986,40 @@
         <v>0.02156314273909956</v>
       </c>
       <c r="G5">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="H5">
-        <v>0.08979768611089797</v>
+        <v>0.2483404958213521</v>
       </c>
       <c r="I5">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="J5">
-        <v>0.003794824754211559</v>
+        <v>0.009623965327339321</v>
       </c>
       <c r="K5">
-        <v>0.01662861722570229</v>
+        <v>0.06060401653451566</v>
       </c>
       <c r="L5">
-        <v>0.005797200369199784</v>
+        <v>0.01470214277665879</v>
       </c>
       <c r="M5">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="N5">
-        <v>0.08979768611089797</v>
+        <v>0.2483404958213521</v>
       </c>
       <c r="O5">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="P5">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="Q5">
-        <v>0.08979768611089797</v>
+        <v>0.2483404958213521</v>
       </c>
       <c r="R5">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="S5">
         <v>0.01799446241337307</v>
@@ -1031,31 +1031,31 @@
         <v>0.02794884587609009</v>
       </c>
       <c r="V5">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="W5">
         <v>0.08080535537935422</v>
       </c>
       <c r="X5">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="Y5">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="Z5">
         <v>0.08080535537935422</v>
       </c>
       <c r="AA5">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="AB5">
-        <v>0.02121794880071198</v>
+        <v>0.0147645580029111</v>
       </c>
       <c r="AC5">
         <v>0.08080308722251991</v>
       </c>
       <c r="AD5">
-        <v>0.02817021287583888</v>
+        <v>0.01960230679535431</v>
       </c>
       <c r="AE5">
         <v>0.01458937138950235</v>
@@ -1141,40 +1141,40 @@
         <v>0.02156314273909956</v>
       </c>
       <c r="G6">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="H6">
-        <v>0.05247738789704071</v>
+        <v>0.1603448127663619</v>
       </c>
       <c r="I6">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="J6">
-        <v>0.003794824754211559</v>
+        <v>0.009623965327339321</v>
       </c>
       <c r="K6">
-        <v>0.009123278218390618</v>
+        <v>0.03325034766821872</v>
       </c>
       <c r="L6">
-        <v>0.005797200369199784</v>
+        <v>0.01470214277665879</v>
       </c>
       <c r="M6">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="N6">
-        <v>0.05247738789704071</v>
+        <v>0.1603448127663619</v>
       </c>
       <c r="O6">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="P6">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="Q6">
-        <v>0.05247738789704071</v>
+        <v>0.1603448127663619</v>
       </c>
       <c r="R6">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="S6">
         <v>0.01799446241337307</v>
@@ -1186,31 +1186,31 @@
         <v>0.02794884587609009</v>
       </c>
       <c r="V6">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="W6">
         <v>0.04433379689095829</v>
       </c>
       <c r="X6">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="Y6">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="Z6">
         <v>0.04433379689095829</v>
       </c>
       <c r="AA6">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="AB6">
-        <v>0.02121794880071198</v>
+        <v>0.0147645580029111</v>
       </c>
       <c r="AC6">
         <v>0.04433255246843287</v>
       </c>
       <c r="AD6">
-        <v>0.02817021287583888</v>
+        <v>0.01960230679535431</v>
       </c>
       <c r="AE6">
         <v>0.01458937138950235</v>
@@ -1296,40 +1296,40 @@
         <v>0.02156314273909956</v>
       </c>
       <c r="G7">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="H7">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="I7">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="J7">
-        <v>0.003794824754211559</v>
+        <v>0.009623965327339321</v>
       </c>
       <c r="K7">
-        <v>0.009123278218390618</v>
+        <v>0.03325034766821872</v>
       </c>
       <c r="L7">
-        <v>0.005797200369199784</v>
+        <v>0.01470214277665879</v>
       </c>
       <c r="M7">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="N7">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="O7">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="P7">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="Q7">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="R7">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="S7">
         <v>0.01799446241337307</v>
@@ -1341,31 +1341,31 @@
         <v>0.02794884587609009</v>
       </c>
       <c r="V7">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="W7">
         <v>0.04433379689095829</v>
       </c>
       <c r="X7">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="Y7">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="Z7">
         <v>0.04433379689095829</v>
       </c>
       <c r="AA7">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="AB7">
-        <v>0.02121794880071198</v>
+        <v>0.0147645580029111</v>
       </c>
       <c r="AC7">
         <v>0.04433255246843287</v>
       </c>
       <c r="AD7">
-        <v>0.02817021287583888</v>
+        <v>0.01960230679535431</v>
       </c>
       <c r="AE7">
         <v>0.01458937138950235</v>
@@ -1451,40 +1451,40 @@
         <v>0.02156314273909956</v>
       </c>
       <c r="G8">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="H8">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="I8">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="J8">
-        <v>0.003794824754211559</v>
+        <v>0.009623965327339321</v>
       </c>
       <c r="K8">
-        <v>0.009123278218390618</v>
+        <v>0.03325034766821872</v>
       </c>
       <c r="L8">
-        <v>0.005797200369199784</v>
+        <v>0.01470214277665879</v>
       </c>
       <c r="M8">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="N8">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="O8">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="P8">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="Q8">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="R8">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="S8">
         <v>0.01799446241337307</v>
@@ -1496,31 +1496,31 @@
         <v>0.02794884587609009</v>
       </c>
       <c r="V8">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="W8">
         <v>0.04433379689095829</v>
       </c>
       <c r="X8">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="Y8">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="Z8">
         <v>0.04433379689095829</v>
       </c>
       <c r="AA8">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="AB8">
-        <v>0.02121794880071198</v>
+        <v>0.0147645580029111</v>
       </c>
       <c r="AC8">
         <v>0.04433255246843287</v>
       </c>
       <c r="AD8">
-        <v>0.02817021287583888</v>
+        <v>0.01960230679535431</v>
       </c>
       <c r="AE8">
         <v>0.01458937138950235</v>
@@ -1606,40 +1606,40 @@
         <v>0.02156314273909956</v>
       </c>
       <c r="G9">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="H9">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="I9">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="J9">
-        <v>0.003794824754211559</v>
+        <v>0.009623965327339321</v>
       </c>
       <c r="K9">
-        <v>0.009123278218390618</v>
+        <v>0.03325034766821872</v>
       </c>
       <c r="L9">
-        <v>0.005797200369199784</v>
+        <v>0.01470214277665879</v>
       </c>
       <c r="M9">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="N9">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="O9">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="P9">
-        <v>0.01858129328426584</v>
+        <v>0.01799446241337307</v>
       </c>
       <c r="Q9">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="R9">
-        <v>0.02886030659045545</v>
+        <v>0.02794884587609009</v>
       </c>
       <c r="S9">
         <v>0.01799446241337307</v>
@@ -1651,31 +1651,31 @@
         <v>0.02794884587609009</v>
       </c>
       <c r="V9">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="W9">
         <v>0.04433379689095829</v>
       </c>
       <c r="X9">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="Y9">
-        <v>0.02121854439225727</v>
+        <v>0.01476497244664452</v>
       </c>
       <c r="Z9">
         <v>0.04433379689095829</v>
       </c>
       <c r="AA9">
-        <v>0.02817100361865645</v>
+        <v>0.01960285703554505</v>
       </c>
       <c r="AB9">
-        <v>0.02121794880071198</v>
+        <v>0.0147645580029111</v>
       </c>
       <c r="AC9">
         <v>0.04433255246843287</v>
       </c>
       <c r="AD9">
-        <v>0.02817021287583888</v>
+        <v>0.01960230679535431</v>
       </c>
       <c r="AE9">
         <v>0.01458937138950235</v>
@@ -1761,40 +1761,40 @@
         <v>0.0297935619150708</v>
       </c>
       <c r="G10">
-        <v>0.01858129328426584</v>
+        <v>0.02484226222688343</v>
       </c>
       <c r="H10">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="I10">
-        <v>0.02886030659045545</v>
+        <v>0.03858479026728702</v>
       </c>
       <c r="J10">
-        <v>0.003794824754211559</v>
+        <v>0.01329732916569063</v>
       </c>
       <c r="K10">
-        <v>0.02485595926756648</v>
+        <v>0.09058906979375894</v>
       </c>
       <c r="L10">
-        <v>0.005797200369199784</v>
+        <v>0.020313792214821</v>
       </c>
       <c r="M10">
-        <v>0.01858129328426584</v>
+        <v>0.02484226222688343</v>
       </c>
       <c r="N10">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="O10">
-        <v>0.02886030659045545</v>
+        <v>0.03858479026728702</v>
       </c>
       <c r="P10">
-        <v>0.01858129328426584</v>
+        <v>0.02484226222688343</v>
       </c>
       <c r="Q10">
-        <v>0.05247738789704071</v>
+        <v>0.0508931569531148</v>
       </c>
       <c r="R10">
-        <v>0.02886030659045545</v>
+        <v>0.03858479026728702</v>
       </c>
       <c r="S10">
         <v>0.02484226222688343</v>
@@ -1806,31 +1806,31 @@
         <v>0.03858479026728702</v>
       </c>
       <c r="V10">
-        <v>0.02121854439225727</v>
+        <v>0.02040060329266212</v>
       </c>
       <c r="W10">
         <v>0.1207854263916786</v>
       </c>
       <c r="X10">
-        <v>0.02817100361865645</v>
+        <v>0.027085056286428</v>
       </c>
       <c r="Y10">
-        <v>0.02121854439225727</v>
+        <v>0.02040060329266212</v>
       </c>
       <c r="Z10">
         <v>0.1207854263916786</v>
       </c>
       <c r="AA10">
-        <v>0.02817100361865645</v>
+        <v>0.027085056286428</v>
       </c>
       <c r="AB10">
-        <v>0.02121794880071198</v>
+        <v>0.02040003066022254</v>
       </c>
       <c r="AC10">
         <v>0.1207820360187377</v>
       </c>
       <c r="AD10">
-        <v>0.02817021287583888</v>
+        <v>0.02708429602548693</v>
       </c>
       <c r="AE10">
         <v>0.02014096224549702</v>

</xml_diff>

<commit_message>
Altered the Murdoch yields to line up with the yield estimated from consumption Change the quadratic parameters to be EBG rather than LWC Fixed error that stubble intake was based on PI rather than intake of forage Changed stubble deterioration calculation - could be further improved Changed calculation of LWC in the trial to the derivative of the equation Profit -87K (seems a bit extreme)
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.1706933457568406</v>
+        <v>0.07481643318340227</v>
       </c>
       <c r="B1">
-        <v>0.1772959242375393</v>
+        <v>0.5474071423077128</v>
       </c>
       <c r="C1">
-        <v>0.2129671871315134</v>
+        <v>0.09334543918882358</v>
       </c>
       <c r="D1">
-        <v>0.1706933457568406</v>
+        <v>0.07481643318340227</v>
       </c>
       <c r="E1">
-        <v>0.1772959242375393</v>
+        <v>0.5474071423077128</v>
       </c>
       <c r="F1">
-        <v>0.2129671871315134</v>
+        <v>0.09334543918882358</v>
       </c>
       <c r="G1">
-        <v>0.00614513094148918</v>
+        <v>0.0365855211770075</v>
       </c>
       <c r="H1">
-        <v>0.1599499218526465</v>
+        <v>0.000135</v>
       </c>
       <c r="I1">
-        <v>0.009544565079334256</v>
+        <v>0.05682432012599037</v>
       </c>
       <c r="J1">
-        <v>0.09505056148880539</v>
+        <v>0.0001837462737624004</v>
       </c>
       <c r="K1">
-        <v>0.06354486258187295</v>
+        <v>0.2405867043872038</v>
       </c>
       <c r="L1">
-        <v>0.145204900316941</v>
+        <v>0.0002807017543859648</v>
       </c>
       <c r="M1">
-        <v>0.00614513094148918</v>
+        <v>0.0365855211770075</v>
       </c>
       <c r="N1">
-        <v>0.1599499218526465</v>
+        <v>0.000135</v>
       </c>
       <c r="O1">
-        <v>0.009544565079334256</v>
+        <v>0.05682432012599037</v>
       </c>
       <c r="P1">
-        <v>0.00614513094148918</v>
+        <v>0.0365855211770075</v>
       </c>
       <c r="Q1">
-        <v>0.1599499218526465</v>
+        <v>0.000135</v>
       </c>
       <c r="R1">
-        <v>0.009544565079334256</v>
+        <v>0.05682432012599037</v>
       </c>
       <c r="S1">
-        <v>0.00614513094148918</v>
+        <v>0.0365855211770075</v>
       </c>
       <c r="T1">
-        <v>0.1892714792784908</v>
+        <v>0.0001366250148829625</v>
       </c>
       <c r="U1">
-        <v>0.009544565079334256</v>
+        <v>0.05682432012599037</v>
       </c>
       <c r="V1">
-        <v>0.1458254340789792</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="W1">
-        <v>0.08472648344249727</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X1">
-        <v>0.1936065337559213</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="Y1">
-        <v>0.1458254340789792</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="Z1">
-        <v>0.08472648344249727</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.1936065337559213</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="AB1">
-        <v>0.1458213408483589</v>
+        <v>0.0002114200663013328</v>
       </c>
       <c r="AC1">
-        <v>0.0847241052219998</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.1936010993390977</v>
+        <v>0.0002806938752596418</v>
       </c>
       <c r="AE1">
-        <v>0.002428233871703311</v>
+        <v>0.02971398364396932</v>
       </c>
       <c r="AF1">
-        <v>0.1481306161009059</v>
+        <v>0.4573582703426234</v>
       </c>
       <c r="AG1">
-        <v>0.00416416276721887</v>
+        <v>0.05095632088731759</v>
       </c>
       <c r="AH1">
-        <v>0.002428233871703311</v>
+        <v>0.02971398364396932</v>
       </c>
       <c r="AI1">
-        <v>0.1481306161009059</v>
+        <v>0.4573582703426234</v>
       </c>
       <c r="AJ1">
-        <v>0.00416416276721887</v>
+        <v>0.05095632088731759</v>
       </c>
       <c r="AK1">
-        <v>0.00614513094148918</v>
+        <v>0.0365855211770075</v>
       </c>
       <c r="AL1">
-        <v>0.1599499218526465</v>
+        <v>0.000135</v>
       </c>
       <c r="AM1">
-        <v>0.009544565079334256</v>
+        <v>0.05682432012599037</v>
       </c>
       <c r="AN1">
-        <v>0.003729338456214618</v>
+        <v>0.03494142061142295</v>
       </c>
       <c r="AO1">
-        <v>0.1692370185903785</v>
+        <v>0.522524999475544</v>
       </c>
       <c r="AP1">
-        <v>0.00480211836957678</v>
+        <v>0.04499265479581525</v>
       </c>
       <c r="AQ1">
-        <v>0.003729338456214618</v>
+        <v>0.03494142061142295</v>
       </c>
       <c r="AR1">
-        <v>0.1692370185903785</v>
+        <v>0.522524999475544</v>
       </c>
       <c r="AS1">
-        <v>0.00480211836957678</v>
+        <v>0.04499265479581525</v>
       </c>
       <c r="AT1">
-        <v>0.002428233871703311</v>
+        <v>0.02971398364396932</v>
       </c>
       <c r="AU1">
-        <v>0.1481306161009059</v>
+        <v>0.4573582703426234</v>
       </c>
       <c r="AV1">
-        <v>0.00416416276721887</v>
+        <v>0.05095632088731759</v>
       </c>
       <c r="AW1">
-        <v>0.002428233871703311</v>
+        <v>0.02971398364396932</v>
       </c>
       <c r="AX1">
-        <v>0.1481306161009059</v>
+        <v>0.4573582703426234</v>
       </c>
       <c r="AY1">
-        <v>0.00416416276721887</v>
+        <v>0.05095632088731759</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.03493584088653087</v>
+        <v>0.02074513396302448</v>
       </c>
       <c r="B2">
-        <v>0.01611781129432176</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C2">
-        <v>0.04358803637417383</v>
+        <v>0.02588286501259054</v>
       </c>
       <c r="D2">
-        <v>0.03493584088653087</v>
+        <v>0.02074513396302448</v>
       </c>
       <c r="E2">
-        <v>0.01611781129432176</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F2">
-        <v>0.04358803637417383</v>
+        <v>0.02588286501259054</v>
       </c>
       <c r="G2">
-        <v>0.0005586482674081073</v>
+        <v>0.01557936253929122</v>
       </c>
       <c r="H2">
-        <v>0.01454090198660423</v>
+        <v>0.4418362766619532</v>
       </c>
       <c r="I2">
-        <v>0.0008676877344849324</v>
+        <v>0.02419773330570764</v>
       </c>
       <c r="J2">
-        <v>0.01945401724727308</v>
+        <v>0.03759198692472752</v>
       </c>
       <c r="K2">
-        <v>0.005776805689261176</v>
+        <v>0.007205758283786679</v>
       </c>
       <c r="L2">
-        <v>0.02971911570966397</v>
+        <v>0.05742775874883905</v>
       </c>
       <c r="M2">
-        <v>0.0005586482674081073</v>
+        <v>0.01557936253929122</v>
       </c>
       <c r="N2">
-        <v>0.01454090198660423</v>
+        <v>0.4418362766619532</v>
       </c>
       <c r="O2">
-        <v>0.0008676877344849324</v>
+        <v>0.02419773330570764</v>
       </c>
       <c r="P2">
-        <v>0.0005586482674081073</v>
+        <v>0.01557936253929122</v>
       </c>
       <c r="Q2">
-        <v>0.01454090198660423</v>
+        <v>0.4418362766619532</v>
       </c>
       <c r="R2">
-        <v>0.0008676877344849324</v>
+        <v>0.02419773330570764</v>
       </c>
       <c r="S2">
-        <v>0.0005586482674081073</v>
+        <v>0.01557936253929122</v>
       </c>
       <c r="T2">
-        <v>0.03230281627140072</v>
+        <v>0.2444988935154161</v>
       </c>
       <c r="U2">
-        <v>0.0008676877344849324</v>
+        <v>0.02419773330570764</v>
       </c>
       <c r="V2">
-        <v>0.029846120477654</v>
+        <v>0.04325488239095251</v>
       </c>
       <c r="W2">
-        <v>0.007702407585681569</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.0396254876128853</v>
+        <v>0.05742775874883906</v>
       </c>
       <c r="Y2">
-        <v>0.029846120477654</v>
+        <v>0.04325488239095251</v>
       </c>
       <c r="Z2">
-        <v>0.007702407585681569</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.0396254876128853</v>
+        <v>0.05742775874883906</v>
       </c>
       <c r="AB2">
-        <v>0.02984528271533216</v>
+        <v>0.04325366825289628</v>
       </c>
       <c r="AC2">
-        <v>0.007702191383818163</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.03962437534971758</v>
+        <v>0.05742614678682399</v>
       </c>
       <c r="AE2">
-        <v>0.0002207485337912101</v>
+        <v>0.006319131266078181</v>
       </c>
       <c r="AF2">
-        <v>0.0134664196455369</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG2">
-        <v>0.0003785602515653517</v>
+        <v>0.01083663787331705</v>
       </c>
       <c r="AH2">
-        <v>0.0002207485337912101</v>
+        <v>0.006319131266078181</v>
       </c>
       <c r="AI2">
-        <v>0.0134664196455369</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ2">
-        <v>0.0003785602515653517</v>
+        <v>0.01083663787331705</v>
       </c>
       <c r="AK2">
-        <v>0.0005586482674081073</v>
+        <v>0.01557936253929122</v>
       </c>
       <c r="AL2">
-        <v>0.01454090198660423</v>
+        <v>0.4418362766619532</v>
       </c>
       <c r="AM2">
-        <v>0.0008676877344849324</v>
+        <v>0.02419773330570764</v>
       </c>
       <c r="AN2">
-        <v>0.0003390307687467834</v>
+        <v>0.006420380730502855</v>
       </c>
       <c r="AO2">
-        <v>0.01538518350821622</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP2">
-        <v>0.0004365562154160709</v>
+        <v>0.008267264719362398</v>
       </c>
       <c r="AQ2">
-        <v>0.0003390307687467834</v>
+        <v>0.006420380730502855</v>
       </c>
       <c r="AR2">
-        <v>0.01538518350821622</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS2">
-        <v>0.0004365562154160709</v>
+        <v>0.008267264719362398</v>
       </c>
       <c r="AT2">
-        <v>0.0002207485337912101</v>
+        <v>0.006319131266078181</v>
       </c>
       <c r="AU2">
-        <v>0.0134664196455369</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV2">
-        <v>0.0003785602515653517</v>
+        <v>0.01083663787331705</v>
       </c>
       <c r="AW2">
-        <v>0.0002207485337912101</v>
+        <v>0.006319131266078181</v>
       </c>
       <c r="AX2">
-        <v>0.0134664196455369</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY2">
-        <v>0.0003785602515653517</v>
+        <v>0.01083663787331705</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.01728287361421691</v>
+        <v>0.0214142361471025</v>
       </c>
       <c r="B3">
-        <v>0.2263597924213026</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C3">
-        <v>0.02156314273909956</v>
+        <v>0.02671767675885298</v>
       </c>
       <c r="D3">
-        <v>0.01728287361421691</v>
+        <v>0.0214142361471025</v>
       </c>
       <c r="E3">
-        <v>0.2263597924213026</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F3">
-        <v>0.02156314273909956</v>
+        <v>0.02671767675885298</v>
       </c>
       <c r="G3">
-        <v>0.1325050224731904</v>
+        <v>0.009430148722876983</v>
       </c>
       <c r="H3">
-        <v>0.01454090198660423</v>
+        <v>0.000135</v>
       </c>
       <c r="I3">
-        <v>0.2058056732030404</v>
+        <v>0.01464682673978765</v>
       </c>
       <c r="J3">
-        <v>0.009623965327339321</v>
+        <v>0.08268335115742874</v>
       </c>
       <c r="K3">
-        <v>0.1491236110031118</v>
+        <v>0.006508077731613697</v>
       </c>
       <c r="L3">
-        <v>0.01470214277665879</v>
+        <v>0.1263120130447528</v>
       </c>
       <c r="M3">
-        <v>0.1325050224731904</v>
+        <v>0.009430148722876983</v>
       </c>
       <c r="N3">
-        <v>0.01454090198660423</v>
+        <v>0.000135</v>
       </c>
       <c r="O3">
-        <v>0.2058056732030404</v>
+        <v>0.01464682673978765</v>
       </c>
       <c r="P3">
-        <v>0.1325050224731904</v>
+        <v>0.009430148722876983</v>
       </c>
       <c r="Q3">
-        <v>0.01454090198660423</v>
+        <v>0.000135</v>
       </c>
       <c r="R3">
-        <v>0.2058056732030404</v>
+        <v>0.01464682673978765</v>
       </c>
       <c r="S3">
-        <v>0.1325050224731904</v>
+        <v>0.009430148722876983</v>
       </c>
       <c r="T3">
-        <v>0.02623887634839434</v>
+        <v>0.3853733253599455</v>
       </c>
       <c r="U3">
-        <v>0.2058056732030404</v>
+        <v>0.01464682673978765</v>
       </c>
       <c r="V3">
-        <v>0.01476497244664452</v>
+        <v>0.09513885597922091</v>
       </c>
       <c r="W3">
-        <v>0.1988314813374824</v>
+        <v>0.6421694420890247</v>
       </c>
       <c r="X3">
-        <v>0.01960285703554505</v>
+        <v>0.1263120130447528</v>
       </c>
       <c r="Y3">
-        <v>0.01476497244664452</v>
+        <v>0.09513885597922091</v>
       </c>
       <c r="Z3">
-        <v>0.1988314813374824</v>
+        <v>0.6421694420890247</v>
       </c>
       <c r="AA3">
-        <v>0.01960285703554505</v>
+        <v>0.1263120130447528</v>
       </c>
       <c r="AB3">
-        <v>0.0147645580029111</v>
+        <v>0.09513618548980364</v>
       </c>
       <c r="AC3">
-        <v>0.1988259002595803</v>
+        <v>0.6421694420890247</v>
       </c>
       <c r="AD3">
-        <v>0.01960230679535431</v>
+        <v>0.1263084675439095</v>
       </c>
       <c r="AE3">
-        <v>0.1097450235421261</v>
+        <v>0.005727558998846923</v>
       </c>
       <c r="AF3">
-        <v>0.189123442380528</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG3">
-        <v>0.1882010403722419</v>
+        <v>0.009822154368235362</v>
       </c>
       <c r="AH3">
-        <v>0.1097450235421261</v>
+        <v>0.005727558998846923</v>
       </c>
       <c r="AI3">
-        <v>0.189123442380528</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ3">
-        <v>0.1882010403722419</v>
+        <v>0.009822154368235362</v>
       </c>
       <c r="AK3">
-        <v>0.1325050224731904</v>
+        <v>0.009430148722876983</v>
       </c>
       <c r="AL3">
-        <v>0.01454090198660423</v>
+        <v>0.000135</v>
       </c>
       <c r="AM3">
-        <v>0.2058056732030404</v>
+        <v>0.01464682673978765</v>
       </c>
       <c r="AN3">
-        <v>0.1414499104014476</v>
+        <v>0.008736829405631983</v>
       </c>
       <c r="AO3">
-        <v>0.216070710947607</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP3">
-        <v>0.1821393314360767</v>
+        <v>0.01125006203465633</v>
       </c>
       <c r="AQ3">
-        <v>0.1414499104014476</v>
+        <v>0.008736829405631983</v>
       </c>
       <c r="AR3">
-        <v>0.216070710947607</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS3">
-        <v>0.1821393314360767</v>
+        <v>0.01125006203465633</v>
       </c>
       <c r="AT3">
-        <v>0.1097450235421261</v>
+        <v>0.005727558998846923</v>
       </c>
       <c r="AU3">
-        <v>0.189123442380528</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV3">
-        <v>0.1882010403722419</v>
+        <v>0.009822154368235362</v>
       </c>
       <c r="AW3">
-        <v>0.1097450235421261</v>
+        <v>0.005727558998846923</v>
       </c>
       <c r="AX3">
-        <v>0.189123442380528</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY3">
-        <v>0.1882010403722419</v>
+        <v>0.009822154368235362</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.01728287361421691</v>
+        <v>0.01678115108026678</v>
       </c>
       <c r="B4">
-        <v>0.2240979623654102</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C4">
-        <v>0.02156314273909956</v>
+        <v>0.0209371638158903</v>
       </c>
       <c r="D4">
-        <v>0.01728287361421691</v>
+        <v>0.01678115108026678</v>
       </c>
       <c r="E4">
-        <v>0.2240979623654102</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F4">
-        <v>0.02156314273909956</v>
+        <v>0.0209371638158903</v>
       </c>
       <c r="G4">
-        <v>0.07240135459503878</v>
+        <v>0.01481009862646186</v>
       </c>
       <c r="H4">
-        <v>0.0647871303291303</v>
+        <v>0.000135</v>
       </c>
       <c r="I4">
-        <v>0.112453167775273</v>
+        <v>0.02300291914322799</v>
       </c>
       <c r="J4">
-        <v>0.009623965327339321</v>
+        <v>0.02887524959080777</v>
       </c>
       <c r="K4">
-        <v>0.1475814541468215</v>
+        <v>0.005810397811065906</v>
       </c>
       <c r="L4">
-        <v>0.01470214277665879</v>
+        <v>0.04411155150255314</v>
       </c>
       <c r="M4">
-        <v>0.07240135459503878</v>
+        <v>0.01481009862646186</v>
       </c>
       <c r="N4">
-        <v>0.0647871303291303</v>
+        <v>0.000135</v>
       </c>
       <c r="O4">
-        <v>0.112453167775273</v>
+        <v>0.02300291914322799</v>
       </c>
       <c r="P4">
-        <v>0.07240135459503878</v>
+        <v>0.01481009862646186</v>
       </c>
       <c r="Q4">
-        <v>0.0647871303291303</v>
+        <v>0.000135</v>
       </c>
       <c r="R4">
-        <v>0.112453167775273</v>
+        <v>0.02300291914322799</v>
       </c>
       <c r="S4">
-        <v>0.07240135459503878</v>
+        <v>0.01481009862646186</v>
       </c>
       <c r="T4">
-        <v>0.1690547412033029</v>
+        <v>0.1634663400102297</v>
       </c>
       <c r="U4">
-        <v>0.112453167775273</v>
+        <v>0.02300291914322799</v>
       </c>
       <c r="V4">
-        <v>0.01476497244664452</v>
+        <v>0.03322504680480767</v>
       </c>
       <c r="W4">
-        <v>0.196775272195762</v>
+        <v>0.2475150943455892</v>
       </c>
       <c r="X4">
-        <v>0.01960285703554505</v>
+        <v>0.04411155150255315</v>
       </c>
       <c r="Y4">
-        <v>0.01476497244664452</v>
+        <v>0.03322504680480767</v>
       </c>
       <c r="Z4">
-        <v>0.196775272195762</v>
+        <v>0.2475150943455892</v>
       </c>
       <c r="AA4">
-        <v>0.01960285703554505</v>
+        <v>0.04411155150255315</v>
       </c>
       <c r="AB4">
-        <v>0.0147645580029111</v>
+        <v>0.03322411419809333</v>
       </c>
       <c r="AC4">
-        <v>0.1967697488343912</v>
+        <v>0.2475150943455892</v>
       </c>
       <c r="AD4">
-        <v>0.01960230679535431</v>
+        <v>0.04411031331831965</v>
       </c>
       <c r="AE4">
-        <v>0.05870807721176374</v>
+        <v>0.005129906868375536</v>
       </c>
       <c r="AF4">
-        <v>0.1872336850094223</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG4">
-        <v>0.1006781068780459</v>
+        <v>0.008797244544490813</v>
       </c>
       <c r="AH4">
-        <v>0.05870807721176374</v>
+        <v>0.005129906868375536</v>
       </c>
       <c r="AI4">
-        <v>0.1872336850094223</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ4">
-        <v>0.1006781068780459</v>
+        <v>0.008797244544490813</v>
       </c>
       <c r="AK4">
-        <v>0.07240135459503878</v>
+        <v>0.01481009862646186</v>
       </c>
       <c r="AL4">
-        <v>0.0647871303291303</v>
+        <v>0.000135</v>
       </c>
       <c r="AM4">
-        <v>0.112453167775273</v>
+        <v>0.02300291914322799</v>
       </c>
       <c r="AN4">
-        <v>0.1112871408980786</v>
+        <v>0.005234508466137469</v>
       </c>
       <c r="AO4">
-        <v>0.2139116913488006</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP4">
-        <v>0.1432999524925896</v>
+        <v>0.006740264944056161</v>
       </c>
       <c r="AQ4">
-        <v>0.1112871408980786</v>
+        <v>0.005234508466137469</v>
       </c>
       <c r="AR4">
-        <v>0.2139116913488006</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS4">
-        <v>0.1432999524925896</v>
+        <v>0.006740264944056161</v>
       </c>
       <c r="AT4">
-        <v>0.05870807721176374</v>
+        <v>0.005129906868375536</v>
       </c>
       <c r="AU4">
-        <v>0.1872336850094223</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV4">
-        <v>0.1006781068780459</v>
+        <v>0.008797244544490813</v>
       </c>
       <c r="AW4">
-        <v>0.05870807721176374</v>
+        <v>0.005129906868375536</v>
       </c>
       <c r="AX4">
-        <v>0.1872336850094223</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY4">
-        <v>0.1006781068780459</v>
+        <v>0.008797244544490813</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.01728287361421691</v>
+        <v>0.01059325058413792</v>
       </c>
       <c r="B5">
-        <v>0.09653105386736166</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C5">
-        <v>0.02156314273909956</v>
+        <v>0.0132167705160393</v>
       </c>
       <c r="D5">
-        <v>0.01728287361421691</v>
+        <v>0.01059325058413792</v>
       </c>
       <c r="E5">
-        <v>0.09653105386736166</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F5">
-        <v>0.02156314273909956</v>
+        <v>0.0132167705160393</v>
       </c>
       <c r="G5">
-        <v>0.01799446241337307</v>
+        <v>0.01310050362190602</v>
       </c>
       <c r="H5">
-        <v>0.2483404958213521</v>
+        <v>0.000135</v>
       </c>
       <c r="I5">
-        <v>0.02794884587609009</v>
+        <v>0.02034759073189658</v>
       </c>
       <c r="J5">
-        <v>0.009623965327339321</v>
+        <v>0.0001837462737624004</v>
       </c>
       <c r="K5">
-        <v>0.06060401653451566</v>
+        <v>0.005112717890518113</v>
       </c>
       <c r="L5">
-        <v>0.01470214277665879</v>
+        <v>0.0002807017543859648</v>
       </c>
       <c r="M5">
-        <v>0.01799446241337307</v>
+        <v>0.01310050362190602</v>
       </c>
       <c r="N5">
-        <v>0.2483404958213521</v>
+        <v>0.000135</v>
       </c>
       <c r="O5">
-        <v>0.02794884587609009</v>
+        <v>0.02034759073189658</v>
       </c>
       <c r="P5">
-        <v>0.01799446241337307</v>
+        <v>0.01310050362190602</v>
       </c>
       <c r="Q5">
-        <v>0.2483404958213521</v>
+        <v>0.000135</v>
       </c>
       <c r="R5">
-        <v>0.02794884587609009</v>
+        <v>0.02034759073189658</v>
       </c>
       <c r="S5">
-        <v>0.01799446241337307</v>
+        <v>0.01310050362190602</v>
       </c>
       <c r="T5">
-        <v>0.1950474781872779</v>
+        <v>0.1508261135893549</v>
       </c>
       <c r="U5">
-        <v>0.02794884587609009</v>
+        <v>0.02034759073189658</v>
       </c>
       <c r="V5">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="W5">
-        <v>0.08080535537935422</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X5">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="Y5">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="Z5">
-        <v>0.08080535537935422</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA5">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="AB5">
-        <v>0.0147645580029111</v>
+        <v>0.0002114200663013328</v>
       </c>
       <c r="AC5">
-        <v>0.08080308722251991</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD5">
-        <v>0.01960230679535431</v>
+        <v>0.0002806938752596418</v>
       </c>
       <c r="AE5">
-        <v>0.01458937138950235</v>
+        <v>0.006043667133304243</v>
       </c>
       <c r="AF5">
-        <v>0.08065162548849171</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG5">
-        <v>0.02501921987221041</v>
+        <v>0.01036424619030472</v>
       </c>
       <c r="AH5">
-        <v>0.01458937138950235</v>
+        <v>0.006043667133304243</v>
       </c>
       <c r="AI5">
-        <v>0.08065162548849171</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ5">
-        <v>0.02501921987221041</v>
+        <v>0.01036424619030472</v>
       </c>
       <c r="AK5">
-        <v>0.01799446241337307</v>
+        <v>0.01310050362190602</v>
       </c>
       <c r="AL5">
-        <v>0.2483404958213521</v>
+        <v>0.000135</v>
       </c>
       <c r="AM5">
-        <v>0.02794884587609009</v>
+        <v>0.02034759073189658</v>
       </c>
       <c r="AN5">
-        <v>0.02208727876667783</v>
+        <v>0.004615573909869783</v>
       </c>
       <c r="AO5">
-        <v>0.09214327869157249</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP5">
-        <v>0.02844089597785835</v>
+        <v>0.005943287936708921</v>
       </c>
       <c r="AQ5">
-        <v>0.02208727876667783</v>
+        <v>0.004615573909869783</v>
       </c>
       <c r="AR5">
-        <v>0.09214327869157249</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS5">
-        <v>0.02844089597785835</v>
+        <v>0.005943287936708921</v>
       </c>
       <c r="AT5">
-        <v>0.01458937138950235</v>
+        <v>0.006043667133304243</v>
       </c>
       <c r="AU5">
-        <v>0.08065162548849171</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV5">
-        <v>0.02501921987221041</v>
+        <v>0.01036424619030472</v>
       </c>
       <c r="AW5">
-        <v>0.01458937138950235</v>
+        <v>0.006043667133304243</v>
       </c>
       <c r="AX5">
-        <v>0.08065162548849171</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY5">
-        <v>0.02501921987221041</v>
+        <v>0.01036424619030472</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.01728287361421691</v>
+        <v>0.007339850875162974</v>
       </c>
       <c r="B6">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C6">
-        <v>0.02156314273909956</v>
+        <v>0.009157635219565035</v>
       </c>
       <c r="D6">
-        <v>0.01728287361421691</v>
+        <v>0.007339850875162974</v>
       </c>
       <c r="E6">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F6">
-        <v>0.02156314273909956</v>
+        <v>0.009157635219565035</v>
       </c>
       <c r="G6">
-        <v>0.01799446241337307</v>
+        <v>0.008097861394374184</v>
       </c>
       <c r="H6">
-        <v>0.1603448127663619</v>
+        <v>0.000135</v>
       </c>
       <c r="I6">
-        <v>0.02794884587609009</v>
+        <v>0.01257752939977267</v>
       </c>
       <c r="J6">
-        <v>0.009623965327339321</v>
+        <v>0.0001837462737624004</v>
       </c>
       <c r="K6">
-        <v>0.03325034766821872</v>
+        <v>0.00442795584919</v>
       </c>
       <c r="L6">
-        <v>0.01470214277665879</v>
+        <v>0.0002807017543859648</v>
       </c>
       <c r="M6">
-        <v>0.01799446241337307</v>
+        <v>0.008097861394374184</v>
       </c>
       <c r="N6">
-        <v>0.1603448127663619</v>
+        <v>0.000135</v>
       </c>
       <c r="O6">
-        <v>0.02794884587609009</v>
+        <v>0.01257752939977267</v>
       </c>
       <c r="P6">
-        <v>0.01799446241337307</v>
+        <v>0.008097861394374184</v>
       </c>
       <c r="Q6">
-        <v>0.1603448127663619</v>
+        <v>0.000135</v>
       </c>
       <c r="R6">
-        <v>0.02794884587609009</v>
+        <v>0.01257752939977267</v>
       </c>
       <c r="S6">
-        <v>0.01799446241337307</v>
+        <v>0.008097861394374184</v>
       </c>
       <c r="T6">
-        <v>0.1561194814131179</v>
+        <v>0.03765077739103105</v>
       </c>
       <c r="U6">
-        <v>0.02794884587609009</v>
+        <v>0.01257752939977267</v>
       </c>
       <c r="V6">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="W6">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X6">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="Y6">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="Z6">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA6">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="AB6">
-        <v>0.0147645580029111</v>
+        <v>0.0002114200663013328</v>
       </c>
       <c r="AC6">
-        <v>0.04433255246843287</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD6">
-        <v>0.01960230679535431</v>
+        <v>0.0002806938752596418</v>
       </c>
       <c r="AE6">
-        <v>0.01458937138950235</v>
+        <v>0.005235176159642189</v>
       </c>
       <c r="AF6">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG6">
-        <v>0.02501921987221041</v>
+        <v>0.008977770180152351</v>
       </c>
       <c r="AH6">
-        <v>0.01458937138950235</v>
+        <v>0.005235176159642189</v>
       </c>
       <c r="AI6">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ6">
-        <v>0.02501921987221041</v>
+        <v>0.008977770180152351</v>
       </c>
       <c r="AK6">
-        <v>0.01799446241337307</v>
+        <v>0.008097861394374184</v>
       </c>
       <c r="AL6">
-        <v>0.1603448127663619</v>
+        <v>0.000135</v>
       </c>
       <c r="AM6">
-        <v>0.02794884587609009</v>
+        <v>0.01257752939977267</v>
       </c>
       <c r="AN6">
-        <v>0.02208727876667783</v>
+        <v>0.008009085077043631</v>
       </c>
       <c r="AO6">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP6">
-        <v>0.02844089597785835</v>
+        <v>0.01031297508218469</v>
       </c>
       <c r="AQ6">
-        <v>0.02208727876667783</v>
+        <v>0.008009085077043631</v>
       </c>
       <c r="AR6">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS6">
-        <v>0.02844089597785835</v>
+        <v>0.01031297508218469</v>
       </c>
       <c r="AT6">
-        <v>0.01458937138950235</v>
+        <v>0.005235176159642189</v>
       </c>
       <c r="AU6">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV6">
-        <v>0.02501921987221041</v>
+        <v>0.008977770180152351</v>
       </c>
       <c r="AW6">
-        <v>0.01458937138950235</v>
+        <v>0.005235176159642189</v>
       </c>
       <c r="AX6">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY6">
-        <v>0.02501921987221041</v>
+        <v>0.008977770180152351</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.01728287361421691</v>
+        <v>0.004686293227412809</v>
       </c>
       <c r="B7">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C7">
-        <v>0.02156314273909956</v>
+        <v>0.005846898613946534</v>
       </c>
       <c r="D7">
-        <v>0.01728287361421691</v>
+        <v>0.004686293227412809</v>
       </c>
       <c r="E7">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F7">
-        <v>0.02156314273909956</v>
+        <v>0.005846898613946534</v>
       </c>
       <c r="G7">
-        <v>0.01799446241337307</v>
+        <v>0.005450622479346398</v>
       </c>
       <c r="H7">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="I7">
-        <v>0.02794884587609009</v>
+        <v>0.008465860446644404</v>
       </c>
       <c r="J7">
-        <v>0.009623965327339321</v>
+        <v>0.0001837462737624004</v>
       </c>
       <c r="K7">
-        <v>0.03325034766821872</v>
+        <v>0.003720867464563825</v>
       </c>
       <c r="L7">
-        <v>0.01470214277665879</v>
+        <v>0.0002807017543859648</v>
       </c>
       <c r="M7">
-        <v>0.01799446241337307</v>
+        <v>0.005450622479346398</v>
       </c>
       <c r="N7">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="O7">
-        <v>0.02794884587609009</v>
+        <v>0.008465860446644404</v>
       </c>
       <c r="P7">
-        <v>0.01799446241337307</v>
+        <v>0.005450622479346398</v>
       </c>
       <c r="Q7">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="R7">
-        <v>0.02794884587609009</v>
+        <v>0.008465860446644404</v>
       </c>
       <c r="S7">
-        <v>0.01799446241337307</v>
+        <v>0.005450622479346398</v>
       </c>
       <c r="T7">
-        <v>0.1061744027167735</v>
+        <v>0.01763805007449084</v>
       </c>
       <c r="U7">
-        <v>0.02794884587609009</v>
+        <v>0.008465860446644404</v>
       </c>
       <c r="V7">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="W7">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X7">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="Y7">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="Z7">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="AB7">
-        <v>0.0147645580029111</v>
+        <v>0.0002114200663013328</v>
       </c>
       <c r="AC7">
-        <v>0.04433255246843287</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.01960230679535431</v>
+        <v>0.0002806938752596418</v>
       </c>
       <c r="AE7">
-        <v>0.01458937138950235</v>
+        <v>0.003311588045193456</v>
       </c>
       <c r="AF7">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG7">
-        <v>0.02501921987221041</v>
+        <v>0.005679021200906224</v>
       </c>
       <c r="AH7">
-        <v>0.01458937138950235</v>
+        <v>0.003311588045193456</v>
       </c>
       <c r="AI7">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ7">
-        <v>0.02501921987221041</v>
+        <v>0.005679021200906224</v>
       </c>
       <c r="AK7">
-        <v>0.01799446241337307</v>
+        <v>0.005450622479346398</v>
       </c>
       <c r="AL7">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="AM7">
-        <v>0.02794884587609009</v>
+        <v>0.008465860446644404</v>
       </c>
       <c r="AN7">
-        <v>0.02208727876667783</v>
+        <v>0.003384832146672472</v>
       </c>
       <c r="AO7">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP7">
-        <v>0.02844089597785835</v>
+        <v>0.004358511521630169</v>
       </c>
       <c r="AQ7">
-        <v>0.02208727876667783</v>
+        <v>0.003384832146672472</v>
       </c>
       <c r="AR7">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS7">
-        <v>0.02844089597785835</v>
+        <v>0.004358511521630169</v>
       </c>
       <c r="AT7">
-        <v>0.01458937138950235</v>
+        <v>0.003311588045193456</v>
       </c>
       <c r="AU7">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV7">
-        <v>0.02501921987221041</v>
+        <v>0.005679021200906224</v>
       </c>
       <c r="AW7">
-        <v>0.01458937138950235</v>
+        <v>0.003311588045193456</v>
       </c>
       <c r="AX7">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY7">
-        <v>0.02501921987221041</v>
+        <v>0.005679021200906224</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.01728287361421691</v>
+        <v>0.002591972155190214</v>
       </c>
       <c r="B8">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C8">
-        <v>0.02156314273909956</v>
+        <v>0.003233898876177747</v>
       </c>
       <c r="D8">
-        <v>0.01728287361421691</v>
+        <v>0.002591972155190214</v>
       </c>
       <c r="E8">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F8">
-        <v>0.02156314273909956</v>
+        <v>0.003233898876177747</v>
       </c>
       <c r="G8">
-        <v>0.01799446241337307</v>
+        <v>0.003301119589459739</v>
       </c>
       <c r="H8">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="I8">
-        <v>0.02794884587609009</v>
+        <v>0.005127270851714063</v>
       </c>
       <c r="J8">
-        <v>0.009623965327339321</v>
+        <v>0.0001837462737624004</v>
       </c>
       <c r="K8">
-        <v>0.03325034766821872</v>
+        <v>0.00301377907993765</v>
       </c>
       <c r="L8">
-        <v>0.01470214277665879</v>
+        <v>0.0002807017543859648</v>
       </c>
       <c r="M8">
-        <v>0.01799446241337307</v>
+        <v>0.003301119589459739</v>
       </c>
       <c r="N8">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="O8">
-        <v>0.02794884587609009</v>
+        <v>0.005127270851714063</v>
       </c>
       <c r="P8">
-        <v>0.01799446241337307</v>
+        <v>0.003301119589459739</v>
       </c>
       <c r="Q8">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="R8">
-        <v>0.02794884587609009</v>
+        <v>0.005127270851714063</v>
       </c>
       <c r="S8">
-        <v>0.01799446241337307</v>
+        <v>0.003301119589459739</v>
       </c>
       <c r="T8">
-        <v>0.06192078408795966</v>
+        <v>0.0001366250148829625</v>
       </c>
       <c r="U8">
-        <v>0.02794884587609009</v>
+        <v>0.005127270851714063</v>
       </c>
       <c r="V8">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="W8">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X8">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="Y8">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="Z8">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="AB8">
-        <v>0.0147645580029111</v>
+        <v>0.0002114200663013328</v>
       </c>
       <c r="AC8">
-        <v>0.04433255246843287</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.01960230679535431</v>
+        <v>0.0002806938752596418</v>
       </c>
       <c r="AE8">
-        <v>0.01458937138950235</v>
+        <v>0.001793375720001218</v>
       </c>
       <c r="AF8">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG8">
-        <v>0.02501921987221041</v>
+        <v>0.003075448575151025</v>
       </c>
       <c r="AH8">
-        <v>0.01458937138950235</v>
+        <v>0.001793375720001218</v>
       </c>
       <c r="AI8">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ8">
-        <v>0.02501921987221041</v>
+        <v>0.003075448575151025</v>
       </c>
       <c r="AK8">
-        <v>0.01799446241337307</v>
+        <v>0.003301119589459739</v>
       </c>
       <c r="AL8">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="AM8">
-        <v>0.02794884587609009</v>
+        <v>0.005127270851714063</v>
       </c>
       <c r="AN8">
-        <v>0.02208727876667783</v>
+        <v>0.002757219114174816</v>
       </c>
       <c r="AO8">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP8">
-        <v>0.02844089597785835</v>
+        <v>0.003550359591273614</v>
       </c>
       <c r="AQ8">
-        <v>0.02208727876667783</v>
+        <v>0.002757219114174816</v>
       </c>
       <c r="AR8">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS8">
-        <v>0.02844089597785835</v>
+        <v>0.003550359591273614</v>
       </c>
       <c r="AT8">
-        <v>0.01458937138950235</v>
+        <v>0.001793375720001218</v>
       </c>
       <c r="AU8">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV8">
-        <v>0.02501921987221041</v>
+        <v>0.003075448575151025</v>
       </c>
       <c r="AW8">
-        <v>0.01458937138950235</v>
+        <v>0.001793375720001218</v>
       </c>
       <c r="AX8">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY8">
-        <v>0.02501921987221041</v>
+        <v>0.003075448575151025</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.01728287361421691</v>
+        <v>0.00195336743855223</v>
       </c>
       <c r="B9">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C9">
-        <v>0.02156314273909956</v>
+        <v>0.002437137587163889</v>
       </c>
       <c r="D9">
-        <v>0.01728287361421691</v>
+        <v>0.00195336743855223</v>
       </c>
       <c r="E9">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F9">
-        <v>0.02156314273909956</v>
+        <v>0.002437137587163889</v>
       </c>
       <c r="G9">
-        <v>0.01799446241337307</v>
+        <v>0.001663813030250955</v>
       </c>
       <c r="H9">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="I9">
-        <v>0.02794884587609009</v>
+        <v>0.002584220238474888</v>
       </c>
       <c r="J9">
-        <v>0.009623965327339321</v>
+        <v>0.0001837462737624004</v>
       </c>
       <c r="K9">
-        <v>0.03325034766821872</v>
+        <v>0.002306690695311473</v>
       </c>
       <c r="L9">
-        <v>0.01470214277665879</v>
+        <v>0.0002807017543859648</v>
       </c>
       <c r="M9">
-        <v>0.01799446241337307</v>
+        <v>0.001663813030250955</v>
       </c>
       <c r="N9">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="O9">
-        <v>0.02794884587609009</v>
+        <v>0.002584220238474888</v>
       </c>
       <c r="P9">
-        <v>0.01799446241337307</v>
+        <v>0.001663813030250955</v>
       </c>
       <c r="Q9">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="R9">
-        <v>0.02794884587609009</v>
+        <v>0.002584220238474888</v>
       </c>
       <c r="S9">
-        <v>0.01799446241337307</v>
+        <v>0.001663813030250955</v>
       </c>
       <c r="T9">
-        <v>0.06192078408795966</v>
+        <v>0.0001366250148829625</v>
       </c>
       <c r="U9">
-        <v>0.02794884587609009</v>
+        <v>0.002584220238474888</v>
       </c>
       <c r="V9">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="W9">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X9">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="Y9">
-        <v>0.01476497244664452</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="Z9">
-        <v>0.04433379689095829</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.01960285703554505</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="AB9">
-        <v>0.0147645580029111</v>
+        <v>0.0002114200663013328</v>
       </c>
       <c r="AC9">
-        <v>0.04433255246843287</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.01960230679535431</v>
+        <v>0.0002806938752596418</v>
       </c>
       <c r="AE9">
-        <v>0.01458937138950235</v>
+        <v>0.0006852096282698977</v>
       </c>
       <c r="AF9">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG9">
-        <v>0.02501921987221041</v>
+        <v>0.001175061617841569</v>
       </c>
       <c r="AH9">
-        <v>0.01458937138950235</v>
+        <v>0.0006852096282698977</v>
       </c>
       <c r="AI9">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ9">
-        <v>0.02501921987221041</v>
+        <v>0.001175061617841569</v>
       </c>
       <c r="AK9">
-        <v>0.01799446241337307</v>
+        <v>0.001663813030250955</v>
       </c>
       <c r="AL9">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="AM9">
-        <v>0.02794884587609009</v>
+        <v>0.002584220238474888</v>
       </c>
       <c r="AN9">
-        <v>0.02208727876667783</v>
+        <v>0.001064803180778029</v>
       </c>
       <c r="AO9">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP9">
-        <v>0.02844089597785835</v>
+        <v>0.0013711040106529</v>
       </c>
       <c r="AQ9">
-        <v>0.02208727876667783</v>
+        <v>0.001064803180778029</v>
       </c>
       <c r="AR9">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS9">
-        <v>0.02844089597785835</v>
+        <v>0.0013711040106529</v>
       </c>
       <c r="AT9">
-        <v>0.01458937138950235</v>
+        <v>0.0006852096282698977</v>
       </c>
       <c r="AU9">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV9">
-        <v>0.02501921987221041</v>
+        <v>0.001175061617841569</v>
       </c>
       <c r="AW9">
-        <v>0.01458937138950235</v>
+        <v>0.0006852096282698977</v>
       </c>
       <c r="AX9">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY9">
-        <v>0.02501921987221041</v>
+        <v>0.001175061617841569</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.02387956019795921</v>
+        <v>0.001314762983047944</v>
       </c>
       <c r="B10">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="C10">
-        <v>0.0297935619150708</v>
+        <v>0.001640376623955987</v>
       </c>
       <c r="D10">
-        <v>0.02387956019795921</v>
+        <v>0.001314762983047944</v>
       </c>
       <c r="E10">
-        <v>0.05641233953012615</v>
+        <v>0.0001451228070175439</v>
       </c>
       <c r="F10">
-        <v>0.0297935619150708</v>
+        <v>0.001640376623955987</v>
       </c>
       <c r="G10">
-        <v>0.02484226222688343</v>
+        <v>0.006717157373719678</v>
       </c>
       <c r="H10">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="I10">
-        <v>0.03858479026728702</v>
+        <v>0.01043303166556461</v>
       </c>
       <c r="J10">
-        <v>0.01329732916569063</v>
+        <v>0.0001837462737624004</v>
       </c>
       <c r="K10">
-        <v>0.09058906979375894</v>
+        <v>0.03723341099470157</v>
       </c>
       <c r="L10">
-        <v>0.020313792214821</v>
+        <v>0.0002807017543859648</v>
       </c>
       <c r="M10">
-        <v>0.02484226222688343</v>
+        <v>0.006717157373719678</v>
       </c>
       <c r="N10">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="O10">
-        <v>0.03858479026728702</v>
+        <v>0.01043303166556461</v>
       </c>
       <c r="P10">
-        <v>0.02484226222688343</v>
+        <v>0.006717157373719678</v>
       </c>
       <c r="Q10">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="R10">
-        <v>0.03858479026728702</v>
+        <v>0.01043303166556461</v>
       </c>
       <c r="S10">
-        <v>0.02484226222688343</v>
+        <v>0.006717157373719678</v>
       </c>
       <c r="T10">
-        <v>0.06192078408795966</v>
+        <v>0.0001366250148829625</v>
       </c>
       <c r="U10">
-        <v>0.03858479026728702</v>
+        <v>0.01043303166556461</v>
       </c>
       <c r="V10">
-        <v>0.02040060329266212</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="W10">
-        <v>0.1207854263916786</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X10">
-        <v>0.027085056286428</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="Y10">
-        <v>0.02040060329266212</v>
+        <v>0.0002114260008996851</v>
       </c>
       <c r="Z10">
-        <v>0.1207854263916786</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.027085056286428</v>
+        <v>0.0002807017543859649</v>
       </c>
       <c r="AB10">
-        <v>0.02040003066022254</v>
+        <v>0.0002114200663013328</v>
       </c>
       <c r="AC10">
-        <v>0.1207820360187377</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.02708429602548693</v>
+        <v>0.0002806938752596418</v>
       </c>
       <c r="AE10">
-        <v>0.02014096224549702</v>
+        <v>0.01249907355974344</v>
       </c>
       <c r="AF10">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AG10">
-        <v>0.03453960759546936</v>
+        <v>0.02143458146628344</v>
       </c>
       <c r="AH10">
-        <v>0.02014096224549702</v>
+        <v>0.01249907355974344</v>
       </c>
       <c r="AI10">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AJ10">
-        <v>0.03453960759546936</v>
+        <v>0.02143458146628344</v>
       </c>
       <c r="AK10">
-        <v>0.02484226222688343</v>
+        <v>0.006717157373719678</v>
       </c>
       <c r="AL10">
-        <v>0.0508931569531148</v>
+        <v>0.000135</v>
       </c>
       <c r="AM10">
-        <v>0.03858479026728702</v>
+        <v>0.01043303166556461</v>
       </c>
       <c r="AN10">
-        <v>0.03456360487961123</v>
+        <v>0.02512224446964371</v>
       </c>
       <c r="AO10">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AP10">
-        <v>0.04450615675136322</v>
+        <v>0.03234889862346461</v>
       </c>
       <c r="AQ10">
-        <v>0.03456360487961123</v>
+        <v>0.02512224446964371</v>
       </c>
       <c r="AR10">
-        <v>0.05384814227875678</v>
+        <v>0.0001385263157894737</v>
       </c>
       <c r="AS10">
-        <v>0.04450615675136322</v>
+        <v>0.03234889862346461</v>
       </c>
       <c r="AT10">
-        <v>0.02014096224549702</v>
+        <v>0.01249907355974344</v>
       </c>
       <c r="AU10">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AV10">
-        <v>0.03453960759546936</v>
+        <v>0.02143458146628344</v>
       </c>
       <c r="AW10">
-        <v>0.02014096224549702</v>
+        <v>0.01249907355974344</v>
       </c>
       <c r="AX10">
-        <v>0.04713246875937916</v>
+        <v>0.00012125</v>
       </c>
       <c r="AY10">
-        <v>0.03453960759546936</v>
+        <v>0.02143458146628344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix error in the calculation of the starting LW in the calibration. It erroneously included an astype(int) in calculation of GD. Reduced profit by $500
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,31 +348,31 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.07481643318340227</v>
+        <v>0.07731728653101365</v>
       </c>
       <c r="B1">
         <v>0.5474071423077128</v>
       </c>
       <c r="C1">
-        <v>0.09334543918882358</v>
+        <v>0.09646565281231148</v>
       </c>
       <c r="D1">
-        <v>0.07481643318340227</v>
+        <v>0.07731728653101365</v>
       </c>
       <c r="E1">
         <v>0.5474071423077128</v>
       </c>
       <c r="F1">
-        <v>0.09334543918882358</v>
+        <v>0.09646565281231148</v>
       </c>
       <c r="G1">
-        <v>0.0365855211770075</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="H1">
         <v>0.000135</v>
       </c>
       <c r="I1">
-        <v>0.05682432012599037</v>
+        <v>0.05677620409395327</v>
       </c>
       <c r="J1">
         <v>0.0001837462737624004</v>
@@ -384,31 +384,31 @@
         <v>0.0002807017543859648</v>
       </c>
       <c r="M1">
-        <v>0.0365855211770075</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="N1">
         <v>0.000135</v>
       </c>
       <c r="O1">
-        <v>0.05682432012599037</v>
+        <v>0.05677620409395327</v>
       </c>
       <c r="P1">
-        <v>0.0365855211770075</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="Q1">
         <v>0.000135</v>
       </c>
       <c r="R1">
-        <v>0.05682432012599037</v>
+        <v>0.05677620409395327</v>
       </c>
       <c r="S1">
-        <v>0.0365855211770075</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="T1">
-        <v>0.0001366250148829625</v>
+        <v>0.0001365484945264078</v>
       </c>
       <c r="U1">
-        <v>0.05682432012599037</v>
+        <v>0.05677620409395327</v>
       </c>
       <c r="V1">
         <v>0.0002114260008996851</v>
@@ -438,406 +438,406 @@
         <v>0.0002806938752596418</v>
       </c>
       <c r="AE1">
-        <v>0.02971398364396932</v>
+        <v>0.02968570863698958</v>
       </c>
       <c r="AF1">
         <v>0.4573582703426234</v>
       </c>
       <c r="AG1">
-        <v>0.05095632088731759</v>
+        <v>0.0509078322583268</v>
       </c>
       <c r="AH1">
-        <v>0.02971398364396932</v>
+        <v>0.02968570863698958</v>
       </c>
       <c r="AI1">
         <v>0.4573582703426234</v>
       </c>
       <c r="AJ1">
-        <v>0.05095632088731759</v>
+        <v>0.0509078322583268</v>
       </c>
       <c r="AK1">
-        <v>0.0365855211770075</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="AL1">
         <v>0.000135</v>
       </c>
       <c r="AM1">
-        <v>0.05682432012599037</v>
+        <v>0.05677620409395327</v>
       </c>
       <c r="AN1">
-        <v>0.03494142061142295</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AO1">
         <v>0.522524999475544</v>
       </c>
       <c r="AP1">
-        <v>0.04499265479581525</v>
+        <v>0.04499318019128809</v>
       </c>
       <c r="AQ1">
-        <v>0.03494142061142295</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AR1">
         <v>0.522524999475544</v>
       </c>
       <c r="AS1">
-        <v>0.04499265479581525</v>
+        <v>0.04499318019128809</v>
       </c>
       <c r="AT1">
-        <v>0.02971398364396932</v>
+        <v>0.02968570863698958</v>
       </c>
       <c r="AU1">
         <v>0.4573582703426234</v>
       </c>
       <c r="AV1">
-        <v>0.05095632088731759</v>
+        <v>0.0509078322583268</v>
       </c>
       <c r="AW1">
-        <v>0.02971398364396932</v>
+        <v>0.02968570863698958</v>
       </c>
       <c r="AX1">
         <v>0.4573582703426234</v>
       </c>
       <c r="AY1">
-        <v>0.05095632088731759</v>
+        <v>0.0509078322583268</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.02074513396302448</v>
+        <v>0.01755041759985082</v>
       </c>
       <c r="B2">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C2">
-        <v>0.02588286501259054</v>
+        <v>0.02189694655436707</v>
       </c>
       <c r="D2">
-        <v>0.02074513396302448</v>
+        <v>0.01755041759985082</v>
       </c>
       <c r="E2">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F2">
-        <v>0.02588286501259054</v>
+        <v>0.02189694655436707</v>
       </c>
       <c r="G2">
-        <v>0.01557936253929122</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="H2">
-        <v>0.4418362766619532</v>
+        <v>0.4421718524041087</v>
       </c>
       <c r="I2">
-        <v>0.02419773330570764</v>
+        <v>0.02415587596617826</v>
       </c>
       <c r="J2">
-        <v>0.03759198692472752</v>
+        <v>0.03757302089152036</v>
       </c>
       <c r="K2">
         <v>0.007205758283786679</v>
       </c>
       <c r="L2">
-        <v>0.05742775874883905</v>
+        <v>0.05739878510662045</v>
       </c>
       <c r="M2">
-        <v>0.01557936253929122</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="N2">
-        <v>0.4418362766619532</v>
+        <v>0.4421718524041087</v>
       </c>
       <c r="O2">
-        <v>0.02419773330570764</v>
+        <v>0.02415587596617826</v>
       </c>
       <c r="P2">
-        <v>0.01557936253929122</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="Q2">
-        <v>0.4418362766619532</v>
+        <v>0.4421718524041087</v>
       </c>
       <c r="R2">
-        <v>0.02419773330570764</v>
+        <v>0.02415587596617826</v>
       </c>
       <c r="S2">
-        <v>0.01557936253929122</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="T2">
-        <v>0.2444988935154161</v>
+        <v>0.2489153681311922</v>
       </c>
       <c r="U2">
-        <v>0.02419773330570764</v>
+        <v>0.02415587596617826</v>
       </c>
       <c r="V2">
-        <v>0.04325488239095251</v>
+        <v>0.04323305929505068</v>
       </c>
       <c r="W2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.05742775874883906</v>
+        <v>0.05739878510662046</v>
       </c>
       <c r="Y2">
-        <v>0.04325488239095251</v>
+        <v>0.04323305929505068</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.05742775874883906</v>
+        <v>0.05739878510662046</v>
       </c>
       <c r="AB2">
-        <v>0.04325366825289628</v>
+        <v>0.04323184576955539</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.05742614678682399</v>
+        <v>0.05739717395787778</v>
       </c>
       <c r="AE2">
-        <v>0.006319131266078181</v>
+        <v>0.008408329871366324</v>
       </c>
       <c r="AF2">
         <v>0.00012125</v>
       </c>
       <c r="AG2">
-        <v>0.01083663787331705</v>
+        <v>0.01441939122621544</v>
       </c>
       <c r="AH2">
-        <v>0.006319131266078181</v>
+        <v>0.008408329871366324</v>
       </c>
       <c r="AI2">
         <v>0.00012125</v>
       </c>
       <c r="AJ2">
-        <v>0.01083663787331705</v>
+        <v>0.01441939122621544</v>
       </c>
       <c r="AK2">
-        <v>0.01557936253929122</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="AL2">
-        <v>0.4418362766619532</v>
+        <v>0.4421718524041087</v>
       </c>
       <c r="AM2">
-        <v>0.02419773330570764</v>
+        <v>0.02415587596617826</v>
       </c>
       <c r="AN2">
-        <v>0.006420380730502855</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AO2">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP2">
-        <v>0.008267264719362398</v>
+        <v>0.0124013764768583</v>
       </c>
       <c r="AQ2">
-        <v>0.006420380730502855</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AR2">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS2">
-        <v>0.008267264719362398</v>
+        <v>0.0124013764768583</v>
       </c>
       <c r="AT2">
-        <v>0.006319131266078181</v>
+        <v>0.008408329871366324</v>
       </c>
       <c r="AU2">
         <v>0.00012125</v>
       </c>
       <c r="AV2">
-        <v>0.01083663787331705</v>
+        <v>0.01441939122621544</v>
       </c>
       <c r="AW2">
-        <v>0.006319131266078181</v>
+        <v>0.008408329871366324</v>
       </c>
       <c r="AX2">
         <v>0.00012125</v>
       </c>
       <c r="AY2">
-        <v>0.01083663787331705</v>
+        <v>0.01441939122621544</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.0214142361471025</v>
+        <v>0.02119267433551551</v>
       </c>
       <c r="B3">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C3">
-        <v>0.02671767675885298</v>
+        <v>0.02644124304328999</v>
       </c>
       <c r="D3">
-        <v>0.0214142361471025</v>
+        <v>0.02119267433551551</v>
       </c>
       <c r="E3">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F3">
-        <v>0.02671767675885298</v>
+        <v>0.02644124304328999</v>
       </c>
       <c r="G3">
-        <v>0.009430148722876983</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="H3">
         <v>0.000135</v>
       </c>
       <c r="I3">
-        <v>0.01464682673978765</v>
+        <v>0.0146300794477108</v>
       </c>
       <c r="J3">
-        <v>0.08268335115742874</v>
+        <v>0.08267466301563467</v>
       </c>
       <c r="K3">
         <v>0.006508077731613697</v>
       </c>
       <c r="L3">
-        <v>0.1263120130447528</v>
+        <v>0.1262987405217567</v>
       </c>
       <c r="M3">
-        <v>0.009430148722876983</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="N3">
         <v>0.000135</v>
       </c>
       <c r="O3">
-        <v>0.01464682673978765</v>
+        <v>0.0146300794477108</v>
       </c>
       <c r="P3">
-        <v>0.009430148722876983</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="Q3">
         <v>0.000135</v>
       </c>
       <c r="R3">
-        <v>0.01464682673978765</v>
+        <v>0.0146300794477108</v>
       </c>
       <c r="S3">
-        <v>0.009430148722876983</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="T3">
-        <v>0.3853733253599455</v>
+        <v>0.3816241081381909</v>
       </c>
       <c r="U3">
-        <v>0.01464682673978765</v>
+        <v>0.0146300794477108</v>
       </c>
       <c r="V3">
-        <v>0.09513885597922091</v>
+        <v>0.09512885904683606</v>
       </c>
       <c r="W3">
-        <v>0.6421694420890247</v>
+        <v>0.6495506920745807</v>
       </c>
       <c r="X3">
-        <v>0.1263120130447528</v>
+        <v>0.1262987405217568</v>
       </c>
       <c r="Y3">
-        <v>0.09513885597922091</v>
+        <v>0.09512885904683606</v>
       </c>
       <c r="Z3">
-        <v>0.6421694420890247</v>
+        <v>0.6495506920745807</v>
       </c>
       <c r="AA3">
-        <v>0.1263120130447528</v>
+        <v>0.1262987405217568</v>
       </c>
       <c r="AB3">
-        <v>0.09513618548980364</v>
+        <v>0.09512618883802657</v>
       </c>
       <c r="AC3">
-        <v>0.6421694420890247</v>
+        <v>0.6495506920745807</v>
       </c>
       <c r="AD3">
-        <v>0.1263084675439095</v>
+        <v>0.126295195393465</v>
       </c>
       <c r="AE3">
-        <v>0.005727558998846923</v>
+        <v>0.003807786292626348</v>
       </c>
       <c r="AF3">
         <v>0.00012125</v>
       </c>
       <c r="AG3">
-        <v>0.009822154368235362</v>
+        <v>0.006529948408206034</v>
       </c>
       <c r="AH3">
-        <v>0.005727558998846923</v>
+        <v>0.003807786292626348</v>
       </c>
       <c r="AI3">
         <v>0.00012125</v>
       </c>
       <c r="AJ3">
-        <v>0.009822154368235362</v>
+        <v>0.006529948408206034</v>
       </c>
       <c r="AK3">
-        <v>0.009430148722876983</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="AL3">
         <v>0.000135</v>
       </c>
       <c r="AM3">
-        <v>0.01464682673978765</v>
+        <v>0.0146300794477108</v>
       </c>
       <c r="AN3">
-        <v>0.008736829405631983</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AO3">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP3">
-        <v>0.01125006203465633</v>
+        <v>0.007508842428978549</v>
       </c>
       <c r="AQ3">
-        <v>0.008736829405631983</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AR3">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS3">
-        <v>0.01125006203465633</v>
+        <v>0.007508842428978549</v>
       </c>
       <c r="AT3">
-        <v>0.005727558998846923</v>
+        <v>0.003807786292626348</v>
       </c>
       <c r="AU3">
         <v>0.00012125</v>
       </c>
       <c r="AV3">
-        <v>0.009822154368235362</v>
+        <v>0.006529948408206034</v>
       </c>
       <c r="AW3">
-        <v>0.005727558998846923</v>
+        <v>0.003807786292626348</v>
       </c>
       <c r="AX3">
         <v>0.00012125</v>
       </c>
       <c r="AY3">
-        <v>0.009822154368235362</v>
+        <v>0.006529948408206034</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.01678115108026678</v>
+        <v>0.01439149236759607</v>
       </c>
       <c r="B4">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C4">
-        <v>0.0209371638158903</v>
+        <v>0.0179556832433156</v>
       </c>
       <c r="D4">
-        <v>0.01678115108026678</v>
+        <v>0.01439149236759607</v>
       </c>
       <c r="E4">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F4">
-        <v>0.0209371638158903</v>
+        <v>0.0179556832433156</v>
       </c>
       <c r="G4">
-        <v>0.01481009862646186</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="H4">
         <v>0.000135</v>
       </c>
       <c r="I4">
-        <v>0.02300291914322799</v>
+        <v>0.02299555475793542</v>
       </c>
       <c r="J4">
         <v>0.02887524959080777</v>
@@ -849,37 +849,37 @@
         <v>0.04411155150255314</v>
       </c>
       <c r="M4">
-        <v>0.01481009862646186</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="N4">
         <v>0.000135</v>
       </c>
       <c r="O4">
-        <v>0.02300291914322799</v>
+        <v>0.02299555475793542</v>
       </c>
       <c r="P4">
-        <v>0.01481009862646186</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="Q4">
         <v>0.000135</v>
       </c>
       <c r="R4">
-        <v>0.02300291914322799</v>
+        <v>0.02299555475793542</v>
       </c>
       <c r="S4">
-        <v>0.01481009862646186</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="T4">
-        <v>0.1634663400102297</v>
+        <v>0.1634062351202291</v>
       </c>
       <c r="U4">
-        <v>0.02300291914322799</v>
+        <v>0.02299555475793542</v>
       </c>
       <c r="V4">
         <v>0.03322504680480767</v>
       </c>
       <c r="W4">
-        <v>0.2475150943455892</v>
+        <v>0.2414632182751259</v>
       </c>
       <c r="X4">
         <v>0.04411155150255315</v>
@@ -888,7 +888,7 @@
         <v>0.03322504680480767</v>
       </c>
       <c r="Z4">
-        <v>0.2475150943455892</v>
+        <v>0.2414632182751259</v>
       </c>
       <c r="AA4">
         <v>0.04411155150255315</v>
@@ -897,102 +897,102 @@
         <v>0.03322411419809333</v>
       </c>
       <c r="AC4">
-        <v>0.2475150943455892</v>
+        <v>0.2414632182751259</v>
       </c>
       <c r="AD4">
         <v>0.04411031331831965</v>
       </c>
       <c r="AE4">
-        <v>0.005129906868375536</v>
+        <v>0.006830537398357178</v>
       </c>
       <c r="AF4">
         <v>0.00012125</v>
       </c>
       <c r="AG4">
-        <v>0.008797244544490813</v>
+        <v>0.01171364498526784</v>
       </c>
       <c r="AH4">
-        <v>0.005129906868375536</v>
+        <v>0.006830537398357178</v>
       </c>
       <c r="AI4">
         <v>0.00012125</v>
       </c>
       <c r="AJ4">
-        <v>0.008797244544490813</v>
+        <v>0.01171364498526784</v>
       </c>
       <c r="AK4">
-        <v>0.01481009862646186</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="AL4">
         <v>0.000135</v>
       </c>
       <c r="AM4">
-        <v>0.02300291914322799</v>
+        <v>0.02299555475793542</v>
       </c>
       <c r="AN4">
-        <v>0.005234508466137469</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AO4">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP4">
-        <v>0.006740264944056161</v>
+        <v>0.006739114170875077</v>
       </c>
       <c r="AQ4">
-        <v>0.005234508466137469</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AR4">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS4">
-        <v>0.006740264944056161</v>
+        <v>0.006739114170875077</v>
       </c>
       <c r="AT4">
-        <v>0.005129906868375536</v>
+        <v>0.006830537398357178</v>
       </c>
       <c r="AU4">
         <v>0.00012125</v>
       </c>
       <c r="AV4">
-        <v>0.008797244544490813</v>
+        <v>0.01171364498526784</v>
       </c>
       <c r="AW4">
-        <v>0.005129906868375536</v>
+        <v>0.006830537398357178</v>
       </c>
       <c r="AX4">
         <v>0.00012125</v>
       </c>
       <c r="AY4">
-        <v>0.008797244544490813</v>
+        <v>0.01171364498526784</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.01059325058413792</v>
+        <v>0.01074853299647219</v>
       </c>
       <c r="B5">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C5">
-        <v>0.0132167705160393</v>
+        <v>0.01341051010453466</v>
       </c>
       <c r="D5">
-        <v>0.01059325058413792</v>
+        <v>0.01074853299647219</v>
       </c>
       <c r="E5">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F5">
-        <v>0.0132167705160393</v>
+        <v>0.01341051010453466</v>
       </c>
       <c r="G5">
-        <v>0.01310050362190602</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="H5">
         <v>0.000135</v>
       </c>
       <c r="I5">
-        <v>0.02034759073189658</v>
+        <v>0.01743604713253146</v>
       </c>
       <c r="J5">
         <v>0.0001837462737624004</v>
@@ -1004,31 +1004,31 @@
         <v>0.0002807017543859648</v>
       </c>
       <c r="M5">
-        <v>0.01310050362190602</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="N5">
         <v>0.000135</v>
       </c>
       <c r="O5">
-        <v>0.02034759073189658</v>
+        <v>0.01743604713253146</v>
       </c>
       <c r="P5">
-        <v>0.01310050362190602</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="Q5">
         <v>0.000135</v>
       </c>
       <c r="R5">
-        <v>0.02034759073189658</v>
+        <v>0.01743604713253146</v>
       </c>
       <c r="S5">
-        <v>0.01310050362190602</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="T5">
-        <v>0.1508261135893549</v>
+        <v>0.1475644697343298</v>
       </c>
       <c r="U5">
-        <v>0.02034759073189658</v>
+        <v>0.01743604713253146</v>
       </c>
       <c r="V5">
         <v>0.0002114260008996851</v>
@@ -1058,96 +1058,96 @@
         <v>0.0002806938752596418</v>
       </c>
       <c r="AE5">
-        <v>0.006043667133304243</v>
+        <v>0.004525899389334496</v>
       </c>
       <c r="AF5">
         <v>0.00012125</v>
       </c>
       <c r="AG5">
-        <v>0.01036424619030472</v>
+        <v>0.00776143597405022</v>
       </c>
       <c r="AH5">
-        <v>0.006043667133304243</v>
+        <v>0.004525899389334496</v>
       </c>
       <c r="AI5">
         <v>0.00012125</v>
       </c>
       <c r="AJ5">
-        <v>0.01036424619030472</v>
+        <v>0.00776143597405022</v>
       </c>
       <c r="AK5">
-        <v>0.01310050362190602</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="AL5">
         <v>0.000135</v>
       </c>
       <c r="AM5">
-        <v>0.02034759073189658</v>
+        <v>0.01743604713253146</v>
       </c>
       <c r="AN5">
-        <v>0.004615573909869783</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AO5">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP5">
-        <v>0.005943287936708921</v>
+        <v>0.008913410739905316</v>
       </c>
       <c r="AQ5">
-        <v>0.004615573909869783</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AR5">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS5">
-        <v>0.005943287936708921</v>
+        <v>0.008913410739905316</v>
       </c>
       <c r="AT5">
-        <v>0.006043667133304243</v>
+        <v>0.004525899389334496</v>
       </c>
       <c r="AU5">
         <v>0.00012125</v>
       </c>
       <c r="AV5">
-        <v>0.01036424619030472</v>
+        <v>0.00776143597405022</v>
       </c>
       <c r="AW5">
-        <v>0.006043667133304243</v>
+        <v>0.004525899389334496</v>
       </c>
       <c r="AX5">
         <v>0.00012125</v>
       </c>
       <c r="AY5">
-        <v>0.01036424619030472</v>
+        <v>0.00776143597405022</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.007339850875162974</v>
+        <v>0.007604888653009554</v>
       </c>
       <c r="B6">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C6">
-        <v>0.009157635219565035</v>
+        <v>0.009488312140691069</v>
       </c>
       <c r="D6">
-        <v>0.007339850875162974</v>
+        <v>0.007604888653009554</v>
       </c>
       <c r="E6">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F6">
-        <v>0.009157635219565035</v>
+        <v>0.009488312140691069</v>
       </c>
       <c r="G6">
-        <v>0.008097861394374184</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="H6">
         <v>0.000135</v>
       </c>
       <c r="I6">
-        <v>0.01257752939977267</v>
+        <v>0.01258161109759086</v>
       </c>
       <c r="J6">
         <v>0.0001837462737624004</v>
@@ -1159,31 +1159,31 @@
         <v>0.0002807017543859648</v>
       </c>
       <c r="M6">
-        <v>0.008097861394374184</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="N6">
         <v>0.000135</v>
       </c>
       <c r="O6">
-        <v>0.01257752939977267</v>
+        <v>0.01258161109759086</v>
       </c>
       <c r="P6">
-        <v>0.008097861394374184</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="Q6">
         <v>0.000135</v>
       </c>
       <c r="R6">
-        <v>0.01257752939977267</v>
+        <v>0.01258161109759086</v>
       </c>
       <c r="S6">
-        <v>0.008097861394374184</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="T6">
-        <v>0.03765077739103105</v>
+        <v>0.04031362834701079</v>
       </c>
       <c r="U6">
-        <v>0.01257752939977267</v>
+        <v>0.01258161109759086</v>
       </c>
       <c r="V6">
         <v>0.0002114260008996851</v>
@@ -1213,96 +1213,96 @@
         <v>0.0002806938752596418</v>
       </c>
       <c r="AE6">
-        <v>0.005235176159642189</v>
+        <v>0.005228291075369343</v>
       </c>
       <c r="AF6">
         <v>0.00012125</v>
       </c>
       <c r="AG6">
-        <v>0.008977770180152351</v>
+        <v>0.008965962993080192</v>
       </c>
       <c r="AH6">
-        <v>0.005235176159642189</v>
+        <v>0.005228291075369343</v>
       </c>
       <c r="AI6">
         <v>0.00012125</v>
       </c>
       <c r="AJ6">
-        <v>0.008977770180152351</v>
+        <v>0.008965962993080192</v>
       </c>
       <c r="AK6">
-        <v>0.008097861394374184</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="AL6">
         <v>0.000135</v>
       </c>
       <c r="AM6">
-        <v>0.01257752939977267</v>
+        <v>0.01258161109759086</v>
       </c>
       <c r="AN6">
-        <v>0.008009085077043631</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AO6">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP6">
-        <v>0.01031297508218469</v>
+        <v>0.007739104680945521</v>
       </c>
       <c r="AQ6">
-        <v>0.008009085077043631</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AR6">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS6">
-        <v>0.01031297508218469</v>
+        <v>0.007739104680945521</v>
       </c>
       <c r="AT6">
-        <v>0.005235176159642189</v>
+        <v>0.005228291075369343</v>
       </c>
       <c r="AU6">
         <v>0.00012125</v>
       </c>
       <c r="AV6">
-        <v>0.008977770180152351</v>
+        <v>0.008965962993080192</v>
       </c>
       <c r="AW6">
-        <v>0.005235176159642189</v>
+        <v>0.005228291075369343</v>
       </c>
       <c r="AX6">
         <v>0.00012125</v>
       </c>
       <c r="AY6">
-        <v>0.008977770180152351</v>
+        <v>0.008965962993080192</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.004686293227412809</v>
+        <v>0.004772845845953531</v>
       </c>
       <c r="B7">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C7">
-        <v>0.005846898613946534</v>
+        <v>0.005954886817164148</v>
       </c>
       <c r="D7">
-        <v>0.004686293227412809</v>
+        <v>0.004772845845953531</v>
       </c>
       <c r="E7">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F7">
-        <v>0.005846898613946534</v>
+        <v>0.005954886817164148</v>
       </c>
       <c r="G7">
-        <v>0.005450622479346398</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="H7">
         <v>0.000135</v>
       </c>
       <c r="I7">
-        <v>0.008465860446644404</v>
+        <v>0.008465953554413931</v>
       </c>
       <c r="J7">
         <v>0.0001837462737624004</v>
@@ -1314,31 +1314,31 @@
         <v>0.0002807017543859648</v>
       </c>
       <c r="M7">
-        <v>0.005450622479346398</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="N7">
         <v>0.000135</v>
       </c>
       <c r="O7">
-        <v>0.008465860446644404</v>
+        <v>0.008465953554413931</v>
       </c>
       <c r="P7">
-        <v>0.005450622479346398</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="Q7">
         <v>0.000135</v>
       </c>
       <c r="R7">
-        <v>0.008465860446644404</v>
+        <v>0.008465953554413931</v>
       </c>
       <c r="S7">
-        <v>0.005450622479346398</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="T7">
-        <v>0.01763805007449084</v>
+        <v>0.01762999655094151</v>
       </c>
       <c r="U7">
-        <v>0.008465860446644404</v>
+        <v>0.008465953554413931</v>
       </c>
       <c r="V7">
         <v>0.0002114260008996851</v>
@@ -1368,96 +1368,96 @@
         <v>0.0002806938752596418</v>
       </c>
       <c r="AE7">
-        <v>0.003311588045193456</v>
+        <v>0.002205253767146671</v>
       </c>
       <c r="AF7">
         <v>0.00012125</v>
       </c>
       <c r="AG7">
-        <v>0.005679021200906224</v>
+        <v>0.003781775609191951</v>
       </c>
       <c r="AH7">
-        <v>0.003311588045193456</v>
+        <v>0.002205253767146671</v>
       </c>
       <c r="AI7">
         <v>0.00012125</v>
       </c>
       <c r="AJ7">
-        <v>0.005679021200906224</v>
+        <v>0.003781775609191951</v>
       </c>
       <c r="AK7">
-        <v>0.005450622479346398</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="AL7">
         <v>0.000135</v>
       </c>
       <c r="AM7">
-        <v>0.008465860446644404</v>
+        <v>0.008465953554413931</v>
       </c>
       <c r="AN7">
-        <v>0.003384832146672472</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AO7">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP7">
-        <v>0.004358511521630169</v>
+        <v>0.004358279431280953</v>
       </c>
       <c r="AQ7">
-        <v>0.003384832146672472</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AR7">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS7">
-        <v>0.004358511521630169</v>
+        <v>0.004358279431280953</v>
       </c>
       <c r="AT7">
-        <v>0.003311588045193456</v>
+        <v>0.002205253767146671</v>
       </c>
       <c r="AU7">
         <v>0.00012125</v>
       </c>
       <c r="AV7">
-        <v>0.005679021200906224</v>
+        <v>0.003781775609191951</v>
       </c>
       <c r="AW7">
-        <v>0.003311588045193456</v>
+        <v>0.002205253767146671</v>
       </c>
       <c r="AX7">
         <v>0.00012125</v>
       </c>
       <c r="AY7">
-        <v>0.005679021200906224</v>
+        <v>0.003781775609191951</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.002591972155190214</v>
+        <v>0.003991392245221766</v>
       </c>
       <c r="B8">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C8">
-        <v>0.003233898876177747</v>
+        <v>0.004979898750208604</v>
       </c>
       <c r="D8">
-        <v>0.002591972155190214</v>
+        <v>0.003991392245221766</v>
       </c>
       <c r="E8">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F8">
-        <v>0.003233898876177747</v>
+        <v>0.004979898750208604</v>
       </c>
       <c r="G8">
-        <v>0.003301119589459739</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="H8">
         <v>0.000135</v>
       </c>
       <c r="I8">
-        <v>0.005127270851714063</v>
+        <v>0.005128934512910387</v>
       </c>
       <c r="J8">
         <v>0.0001837462737624004</v>
@@ -1469,31 +1469,31 @@
         <v>0.0002807017543859648</v>
       </c>
       <c r="M8">
-        <v>0.003301119589459739</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="N8">
         <v>0.000135</v>
       </c>
       <c r="O8">
-        <v>0.005127270851714063</v>
+        <v>0.005128934512910387</v>
       </c>
       <c r="P8">
-        <v>0.003301119589459739</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="Q8">
         <v>0.000135</v>
       </c>
       <c r="R8">
-        <v>0.005127270851714063</v>
+        <v>0.005128934512910387</v>
       </c>
       <c r="S8">
-        <v>0.003301119589459739</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="T8">
-        <v>0.0001366250148829625</v>
+        <v>0.0001365484945264078</v>
       </c>
       <c r="U8">
-        <v>0.005127270851714063</v>
+        <v>0.005128934512910387</v>
       </c>
       <c r="V8">
         <v>0.0002114260008996851</v>
@@ -1523,96 +1523,96 @@
         <v>0.0002806938752596418</v>
       </c>
       <c r="AE8">
-        <v>0.001793375720001218</v>
+        <v>0.002687051978199552</v>
       </c>
       <c r="AF8">
         <v>0.00012125</v>
       </c>
       <c r="AG8">
-        <v>0.003075448575151025</v>
+        <v>0.004608008286018807</v>
       </c>
       <c r="AH8">
-        <v>0.001793375720001218</v>
+        <v>0.002687051978199552</v>
       </c>
       <c r="AI8">
         <v>0.00012125</v>
       </c>
       <c r="AJ8">
-        <v>0.003075448575151025</v>
+        <v>0.004608008286018807</v>
       </c>
       <c r="AK8">
-        <v>0.003301119589459739</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="AL8">
         <v>0.000135</v>
       </c>
       <c r="AM8">
-        <v>0.005127270851714063</v>
+        <v>0.005128934512910387</v>
       </c>
       <c r="AN8">
-        <v>0.002757219114174816</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AO8">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP8">
-        <v>0.003550359591273614</v>
+        <v>0.003550170747573319</v>
       </c>
       <c r="AQ8">
-        <v>0.002757219114174816</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AR8">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS8">
-        <v>0.003550359591273614</v>
+        <v>0.003550170747573319</v>
       </c>
       <c r="AT8">
-        <v>0.001793375720001218</v>
+        <v>0.002687051978199552</v>
       </c>
       <c r="AU8">
         <v>0.00012125</v>
       </c>
       <c r="AV8">
-        <v>0.003075448575151025</v>
+        <v>0.004608008286018807</v>
       </c>
       <c r="AW8">
-        <v>0.001793375720001218</v>
+        <v>0.002687051978199552</v>
       </c>
       <c r="AX8">
         <v>0.00012125</v>
       </c>
       <c r="AY8">
-        <v>0.003075448575151025</v>
+        <v>0.004608008286018807</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.00195336743855223</v>
+        <v>0.002005334436762057</v>
       </c>
       <c r="B9">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C9">
-        <v>0.002437137587163889</v>
+        <v>0.002501974710036744</v>
       </c>
       <c r="D9">
-        <v>0.00195336743855223</v>
+        <v>0.002005334436762057</v>
       </c>
       <c r="E9">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F9">
-        <v>0.002437137587163889</v>
+        <v>0.002501974710036744</v>
       </c>
       <c r="G9">
-        <v>0.001663813030250955</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="H9">
         <v>0.000135</v>
       </c>
       <c r="I9">
-        <v>0.002584220238474888</v>
+        <v>0.002594667384101244</v>
       </c>
       <c r="J9">
         <v>0.0001837462737624004</v>
@@ -1624,31 +1624,31 @@
         <v>0.0002807017543859648</v>
       </c>
       <c r="M9">
-        <v>0.001663813030250955</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="N9">
         <v>0.000135</v>
       </c>
       <c r="O9">
-        <v>0.002584220238474888</v>
+        <v>0.002594667384101244</v>
       </c>
       <c r="P9">
-        <v>0.001663813030250955</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="Q9">
         <v>0.000135</v>
       </c>
       <c r="R9">
-        <v>0.002584220238474888</v>
+        <v>0.002594667384101244</v>
       </c>
       <c r="S9">
-        <v>0.001663813030250955</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="T9">
-        <v>0.0001366250148829625</v>
+        <v>0.0001365484945264078</v>
       </c>
       <c r="U9">
-        <v>0.002584220238474888</v>
+        <v>0.002594667384101244</v>
       </c>
       <c r="V9">
         <v>0.0002114260008996851</v>
@@ -1678,96 +1678,96 @@
         <v>0.0002806938752596418</v>
       </c>
       <c r="AE9">
-        <v>0.0006852096282698977</v>
+        <v>0.0006846436056344724</v>
       </c>
       <c r="AF9">
         <v>0.00012125</v>
       </c>
       <c r="AG9">
-        <v>0.001175061617841569</v>
+        <v>0.001174090949236989</v>
       </c>
       <c r="AH9">
-        <v>0.0006852096282698977</v>
+        <v>0.0006846436056344724</v>
       </c>
       <c r="AI9">
         <v>0.00012125</v>
       </c>
       <c r="AJ9">
-        <v>0.001175061617841569</v>
+        <v>0.001174090949236989</v>
       </c>
       <c r="AK9">
-        <v>0.001663813030250955</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="AL9">
         <v>0.000135</v>
       </c>
       <c r="AM9">
-        <v>0.002584220238474888</v>
+        <v>0.002594667384101244</v>
       </c>
       <c r="AN9">
-        <v>0.001064803180778029</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AO9">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP9">
-        <v>0.0013711040106529</v>
+        <v>0.001371030941835658</v>
       </c>
       <c r="AQ9">
-        <v>0.001064803180778029</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AR9">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS9">
-        <v>0.0013711040106529</v>
+        <v>0.001371030941835658</v>
       </c>
       <c r="AT9">
-        <v>0.0006852096282698977</v>
+        <v>0.0006846436056344724</v>
       </c>
       <c r="AU9">
         <v>0.00012125</v>
       </c>
       <c r="AV9">
-        <v>0.001175061617841569</v>
+        <v>0.001174090949236989</v>
       </c>
       <c r="AW9">
-        <v>0.0006852096282698977</v>
+        <v>0.0006846436056344724</v>
       </c>
       <c r="AX9">
         <v>0.00012125</v>
       </c>
       <c r="AY9">
-        <v>0.001175061617841569</v>
+        <v>0.001174090949236989</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.001314762983047944</v>
+        <v>0.001349740535953804</v>
       </c>
       <c r="B10">
         <v>0.0001451228070175439</v>
       </c>
       <c r="C10">
-        <v>0.001640376623955987</v>
+        <v>0.001684016702730448</v>
       </c>
       <c r="D10">
-        <v>0.001314762983047944</v>
+        <v>0.001349740535953804</v>
       </c>
       <c r="E10">
         <v>0.0001451228070175439</v>
       </c>
       <c r="F10">
-        <v>0.001640376623955987</v>
+        <v>0.001684016702730448</v>
       </c>
       <c r="G10">
-        <v>0.006717157373719678</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="H10">
         <v>0.000135</v>
       </c>
       <c r="I10">
-        <v>0.01043303166556461</v>
+        <v>0.01131567667817344</v>
       </c>
       <c r="J10">
         <v>0.0001837462737624004</v>
@@ -1779,31 +1779,31 @@
         <v>0.0002807017543859648</v>
       </c>
       <c r="M10">
-        <v>0.006717157373719678</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="N10">
         <v>0.000135</v>
       </c>
       <c r="O10">
-        <v>0.01043303166556461</v>
+        <v>0.01131567667817344</v>
       </c>
       <c r="P10">
-        <v>0.006717157373719678</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="Q10">
         <v>0.000135</v>
       </c>
       <c r="R10">
-        <v>0.01043303166556461</v>
+        <v>0.01131567667817344</v>
       </c>
       <c r="S10">
-        <v>0.006717157373719678</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="T10">
-        <v>0.0001366250148829625</v>
+        <v>0.0001365484945264078</v>
       </c>
       <c r="U10">
-        <v>0.01043303166556461</v>
+        <v>0.01131567667817344</v>
       </c>
       <c r="V10">
         <v>0.0002114260008996851</v>
@@ -1833,67 +1833,67 @@
         <v>0.0002806938752596418</v>
       </c>
       <c r="AE10">
-        <v>0.01249907355974344</v>
+        <v>0.0124887484612893</v>
       </c>
       <c r="AF10">
         <v>0.00012125</v>
       </c>
       <c r="AG10">
-        <v>0.02143458146628344</v>
+        <v>0.0214168750208493</v>
       </c>
       <c r="AH10">
-        <v>0.01249907355974344</v>
+        <v>0.0124887484612893</v>
       </c>
       <c r="AI10">
         <v>0.00012125</v>
       </c>
       <c r="AJ10">
-        <v>0.02143458146628344</v>
+        <v>0.0214168750208493</v>
       </c>
       <c r="AK10">
-        <v>0.006717157373719678</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="AL10">
         <v>0.000135</v>
       </c>
       <c r="AM10">
-        <v>0.01043303166556461</v>
+        <v>0.01131567667817344</v>
       </c>
       <c r="AN10">
-        <v>0.02512224446964371</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AO10">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AP10">
-        <v>0.03234889862346461</v>
+        <v>0.03234717552329418</v>
       </c>
       <c r="AQ10">
-        <v>0.02512224446964371</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AR10">
         <v>0.0001385263157894737</v>
       </c>
       <c r="AS10">
-        <v>0.03234889862346461</v>
+        <v>0.03234717552329418</v>
       </c>
       <c r="AT10">
-        <v>0.01249907355974344</v>
+        <v>0.0124887484612893</v>
       </c>
       <c r="AU10">
         <v>0.00012125</v>
       </c>
       <c r="AV10">
-        <v>0.02143458146628344</v>
+        <v>0.0214168750208493</v>
       </c>
       <c r="AW10">
-        <v>0.01249907355974344</v>
+        <v>0.0124887484612893</v>
       </c>
       <c r="AX10">
         <v>0.00012125</v>
       </c>
       <c r="AY10">
-        <v>0.02143458146628344</v>
+        <v>0.0214168750208493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update stubble sim structure so that we can handle more trials easily. No profit change
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -351,154 +351,154 @@
         <v>0.07731728653101365</v>
       </c>
       <c r="B1">
-        <v>0.5474071423077128</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="C1">
-        <v>0.09646565281231148</v>
+        <v>0.07731728653101365</v>
       </c>
       <c r="D1">
         <v>0.07731728653101365</v>
       </c>
       <c r="E1">
-        <v>0.5474071423077128</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="F1">
-        <v>0.09646565281231148</v>
+        <v>0.07731728653101365</v>
       </c>
       <c r="G1">
         <v>0.03655454236186033</v>
       </c>
       <c r="H1">
-        <v>0.000135</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="I1">
-        <v>0.05677620409395327</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="J1">
-        <v>0.0001837462737624004</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="K1">
-        <v>0.2405867043872038</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="L1">
-        <v>0.0002807017543859648</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="M1">
         <v>0.03655454236186033</v>
       </c>
       <c r="N1">
-        <v>0.000135</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="O1">
-        <v>0.05677620409395327</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="P1">
         <v>0.03655454236186033</v>
       </c>
       <c r="Q1">
-        <v>0.000135</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="R1">
-        <v>0.05677620409395327</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="S1">
         <v>0.03655454236186033</v>
       </c>
       <c r="T1">
-        <v>0.0001365484945264078</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="U1">
-        <v>0.05677620409395327</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="V1">
-        <v>0.0002114260008996851</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="W1">
-        <v>0.0001146235521235521</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="X1">
-        <v>0.0002807017543859649</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="Y1">
-        <v>0.0002114260008996851</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="Z1">
-        <v>0.0001146235521235521</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AA1">
-        <v>0.0002807017543859649</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="AB1">
-        <v>0.0002114200663013328</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="AC1">
-        <v>0.0001146235521235521</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AD1">
-        <v>0.0002806938752596418</v>
+        <v>0.05612955758300964</v>
       </c>
       <c r="AE1">
         <v>0.02968570863698958</v>
       </c>
       <c r="AF1">
-        <v>0.4573582703426234</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AG1">
-        <v>0.0509078322583268</v>
+        <v>0.02968570863698958</v>
       </c>
       <c r="AH1">
         <v>0.02968570863698958</v>
       </c>
       <c r="AI1">
-        <v>0.4573582703426234</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AJ1">
-        <v>0.0509078322583268</v>
+        <v>0.02968570863698958</v>
       </c>
       <c r="AK1">
         <v>0.03655454236186033</v>
       </c>
       <c r="AL1">
-        <v>0.000135</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AM1">
-        <v>0.05677620409395327</v>
+        <v>0.03655454236186033</v>
       </c>
       <c r="AN1">
         <v>0.03494182863500563</v>
       </c>
       <c r="AO1">
-        <v>0.522524999475544</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AP1">
-        <v>0.04499318019128809</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AQ1">
         <v>0.03494182863500563</v>
       </c>
       <c r="AR1">
-        <v>0.522524999475544</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AS1">
-        <v>0.04499318019128809</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AT1">
         <v>0.02968570863698958</v>
       </c>
       <c r="AU1">
-        <v>0.4573582703426234</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AV1">
-        <v>0.0509078322583268</v>
+        <v>0.02968570863698958</v>
       </c>
       <c r="AW1">
         <v>0.02968570863698958</v>
       </c>
       <c r="AX1">
-        <v>0.4573582703426234</v>
+        <v>0.03494182863500563</v>
       </c>
       <c r="AY1">
-        <v>0.0509078322583268</v>
+        <v>0.02968570863698958</v>
       </c>
     </row>
     <row r="2" spans="1:51">
@@ -506,154 +506,154 @@
         <v>0.01755041759985082</v>
       </c>
       <c r="B2">
-        <v>0.0001451228070175439</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="C2">
-        <v>0.02189694655436707</v>
+        <v>0.01755041759985082</v>
       </c>
       <c r="D2">
         <v>0.01755041759985082</v>
       </c>
       <c r="E2">
-        <v>0.0001451228070175439</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="F2">
-        <v>0.02189694655436707</v>
+        <v>0.01755041759985082</v>
       </c>
       <c r="G2">
         <v>0.01555241329329285</v>
       </c>
       <c r="H2">
-        <v>0.4421718524041087</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="I2">
-        <v>0.02415587596617826</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="J2">
-        <v>0.03757302089152036</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="K2">
-        <v>0.007205758283786679</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="L2">
-        <v>0.05739878510662045</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="M2">
         <v>0.01555241329329285</v>
       </c>
       <c r="N2">
-        <v>0.4421718524041087</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="O2">
-        <v>0.02415587596617826</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="P2">
         <v>0.01555241329329285</v>
       </c>
       <c r="Q2">
-        <v>0.4421718524041087</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="R2">
-        <v>0.02415587596617826</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="S2">
         <v>0.01555241329329285</v>
       </c>
       <c r="T2">
-        <v>0.2489153681311922</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="U2">
-        <v>0.02415587596617826</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="V2">
-        <v>0.04323305929505068</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="W2">
-        <v>0.0001146235521235521</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="X2">
-        <v>0.05739878510662046</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="Y2">
-        <v>0.04323305929505068</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="Z2">
-        <v>0.0001146235521235521</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AA2">
-        <v>0.05739878510662046</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="AB2">
-        <v>0.04323184576955539</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="AC2">
-        <v>0.0001146235521235521</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AD2">
-        <v>0.05739717395787778</v>
+        <v>0.01359068049863939</v>
       </c>
       <c r="AE2">
         <v>0.008408329871366324</v>
       </c>
       <c r="AF2">
-        <v>0.00012125</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AG2">
-        <v>0.01441939122621544</v>
+        <v>0.008408329871366324</v>
       </c>
       <c r="AH2">
         <v>0.008408329871366324</v>
       </c>
       <c r="AI2">
-        <v>0.00012125</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AJ2">
-        <v>0.01441939122621544</v>
+        <v>0.008408329871366324</v>
       </c>
       <c r="AK2">
         <v>0.01555241329329285</v>
       </c>
       <c r="AL2">
-        <v>0.4421718524041087</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AM2">
-        <v>0.02415587596617826</v>
+        <v>0.01555241329329285</v>
       </c>
       <c r="AN2">
         <v>0.009630943397427958</v>
       </c>
       <c r="AO2">
-        <v>0.0001385263157894737</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AP2">
-        <v>0.0124013764768583</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AQ2">
         <v>0.009630943397427958</v>
       </c>
       <c r="AR2">
-        <v>0.0001385263157894737</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AS2">
-        <v>0.0124013764768583</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AT2">
         <v>0.008408329871366324</v>
       </c>
       <c r="AU2">
-        <v>0.00012125</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AV2">
-        <v>0.01441939122621544</v>
+        <v>0.008408329871366324</v>
       </c>
       <c r="AW2">
         <v>0.008408329871366324</v>
       </c>
       <c r="AX2">
-        <v>0.00012125</v>
+        <v>0.009630943397427958</v>
       </c>
       <c r="AY2">
-        <v>0.01441939122621544</v>
+        <v>0.008408329871366324</v>
       </c>
     </row>
     <row r="3" spans="1:51">
@@ -661,154 +661,154 @@
         <v>0.02119267433551551</v>
       </c>
       <c r="B3">
-        <v>0.0001451228070175439</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="C3">
-        <v>0.02644124304328999</v>
+        <v>0.02119267433551551</v>
       </c>
       <c r="D3">
         <v>0.02119267433551551</v>
       </c>
       <c r="E3">
-        <v>0.0001451228070175439</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="F3">
-        <v>0.02644124304328999</v>
+        <v>0.02119267433551551</v>
       </c>
       <c r="G3">
         <v>0.00941936621975901</v>
       </c>
       <c r="H3">
-        <v>0.000135</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="I3">
-        <v>0.0146300794477108</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="J3">
-        <v>0.08267466301563467</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="K3">
-        <v>0.006508077731613697</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="L3">
-        <v>0.1262987405217567</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="M3">
         <v>0.00941936621975901</v>
       </c>
       <c r="N3">
-        <v>0.000135</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="O3">
-        <v>0.0146300794477108</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="P3">
         <v>0.00941936621975901</v>
       </c>
       <c r="Q3">
-        <v>0.000135</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="R3">
-        <v>0.0146300794477108</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="S3">
         <v>0.00941936621975901</v>
       </c>
       <c r="T3">
-        <v>0.3816241081381909</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="U3">
-        <v>0.0146300794477108</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="V3">
-        <v>0.09512885904683606</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="W3">
-        <v>0.6495506920745807</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="X3">
-        <v>0.1262987405217568</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="Y3">
-        <v>0.09512885904683606</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="Z3">
-        <v>0.6495506920745807</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AA3">
-        <v>0.1262987405217568</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="AB3">
-        <v>0.09512618883802657</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="AC3">
-        <v>0.6495506920745807</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AD3">
-        <v>0.126295195393465</v>
+        <v>0.01351203110498505</v>
       </c>
       <c r="AE3">
         <v>0.003807786292626348</v>
       </c>
       <c r="AF3">
-        <v>0.00012125</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AG3">
-        <v>0.006529948408206034</v>
+        <v>0.003807786292626348</v>
       </c>
       <c r="AH3">
         <v>0.003807786292626348</v>
       </c>
       <c r="AI3">
-        <v>0.00012125</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AJ3">
-        <v>0.006529948408206034</v>
+        <v>0.003807786292626348</v>
       </c>
       <c r="AK3">
         <v>0.00941936621975901</v>
       </c>
       <c r="AL3">
-        <v>0.000135</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AM3">
-        <v>0.0146300794477108</v>
+        <v>0.00941936621975901</v>
       </c>
       <c r="AN3">
         <v>0.005831387874454591</v>
       </c>
       <c r="AO3">
-        <v>0.0001385263157894737</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AP3">
-        <v>0.007508842428978549</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AQ3">
         <v>0.005831387874454591</v>
       </c>
       <c r="AR3">
-        <v>0.0001385263157894737</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AS3">
-        <v>0.007508842428978549</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AT3">
         <v>0.003807786292626348</v>
       </c>
       <c r="AU3">
-        <v>0.00012125</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AV3">
-        <v>0.006529948408206034</v>
+        <v>0.003807786292626348</v>
       </c>
       <c r="AW3">
         <v>0.003807786292626348</v>
       </c>
       <c r="AX3">
-        <v>0.00012125</v>
+        <v>0.005831387874454591</v>
       </c>
       <c r="AY3">
-        <v>0.006529948408206034</v>
+        <v>0.003807786292626348</v>
       </c>
     </row>
     <row r="4" spans="1:51">
@@ -816,154 +816,154 @@
         <v>0.01439149236759607</v>
       </c>
       <c r="B4">
-        <v>0.0001451228070175439</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="C4">
-        <v>0.0179556832433156</v>
+        <v>0.01439149236759607</v>
       </c>
       <c r="D4">
         <v>0.01439149236759607</v>
       </c>
       <c r="E4">
-        <v>0.0001451228070175439</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="F4">
-        <v>0.0179556832433156</v>
+        <v>0.01439149236759607</v>
       </c>
       <c r="G4">
         <v>0.01480535717291733</v>
       </c>
       <c r="H4">
-        <v>0.000135</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="I4">
-        <v>0.02299555475793542</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="J4">
-        <v>0.02887524959080777</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="K4">
-        <v>0.005810397811065906</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="L4">
-        <v>0.04411155150255314</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="M4">
         <v>0.01480535717291733</v>
       </c>
       <c r="N4">
-        <v>0.000135</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="O4">
-        <v>0.02299555475793542</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="P4">
         <v>0.01480535717291733</v>
       </c>
       <c r="Q4">
-        <v>0.000135</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="R4">
-        <v>0.02299555475793542</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="S4">
         <v>0.01480535717291733</v>
       </c>
       <c r="T4">
-        <v>0.1634062351202291</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="U4">
-        <v>0.02299555475793542</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="V4">
-        <v>0.03322504680480767</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="W4">
-        <v>0.2414632182751259</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="X4">
-        <v>0.04411155150255315</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="Y4">
-        <v>0.03322504680480767</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="Z4">
-        <v>0.2414632182751259</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AA4">
-        <v>0.04411155150255315</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="AB4">
-        <v>0.03322411419809333</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="AC4">
-        <v>0.2414632182751259</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AD4">
-        <v>0.04411031331831965</v>
+        <v>0.009812553570043313</v>
       </c>
       <c r="AE4">
         <v>0.006830537398357178</v>
       </c>
       <c r="AF4">
-        <v>0.00012125</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AG4">
-        <v>0.01171364498526784</v>
+        <v>0.006830537398357178</v>
       </c>
       <c r="AH4">
         <v>0.006830537398357178</v>
       </c>
       <c r="AI4">
-        <v>0.00012125</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AJ4">
-        <v>0.01171364498526784</v>
+        <v>0.006830537398357178</v>
       </c>
       <c r="AK4">
         <v>0.01480535717291733</v>
       </c>
       <c r="AL4">
-        <v>0.000135</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AM4">
-        <v>0.02299555475793542</v>
+        <v>0.01480535717291733</v>
       </c>
       <c r="AN4">
         <v>0.00523361477249056</v>
       </c>
       <c r="AO4">
-        <v>0.0001385263157894737</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AP4">
-        <v>0.006739114170875077</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AQ4">
         <v>0.00523361477249056</v>
       </c>
       <c r="AR4">
-        <v>0.0001385263157894737</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AS4">
-        <v>0.006739114170875077</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AT4">
         <v>0.006830537398357178</v>
       </c>
       <c r="AU4">
-        <v>0.00012125</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AV4">
-        <v>0.01171364498526784</v>
+        <v>0.006830537398357178</v>
       </c>
       <c r="AW4">
         <v>0.006830537398357178</v>
       </c>
       <c r="AX4">
-        <v>0.00012125</v>
+        <v>0.00523361477249056</v>
       </c>
       <c r="AY4">
-        <v>0.01171364498526784</v>
+        <v>0.006830537398357178</v>
       </c>
     </row>
     <row r="5" spans="1:51">
@@ -971,154 +971,154 @@
         <v>0.01074853299647219</v>
       </c>
       <c r="B5">
-        <v>0.0001451228070175439</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="C5">
-        <v>0.01341051010453466</v>
+        <v>0.01074853299647219</v>
       </c>
       <c r="D5">
         <v>0.01074853299647219</v>
       </c>
       <c r="E5">
-        <v>0.0001451228070175439</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="F5">
-        <v>0.01341051010453466</v>
+        <v>0.01074853299647219</v>
       </c>
       <c r="G5">
         <v>0.01122594815382163</v>
       </c>
       <c r="H5">
-        <v>0.000135</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="I5">
-        <v>0.01743604713253146</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="J5">
-        <v>0.0001837462737624004</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="K5">
-        <v>0.005112717890518113</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="L5">
-        <v>0.0002807017543859648</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="M5">
         <v>0.01122594815382163</v>
       </c>
       <c r="N5">
-        <v>0.000135</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="O5">
-        <v>0.01743604713253146</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="P5">
         <v>0.01122594815382163</v>
       </c>
       <c r="Q5">
-        <v>0.000135</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="R5">
-        <v>0.01743604713253146</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="S5">
         <v>0.01122594815382163</v>
       </c>
       <c r="T5">
-        <v>0.1475644697343298</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="U5">
-        <v>0.01743604713253146</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="V5">
-        <v>0.0002114260008996851</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="W5">
-        <v>0.0001146235521235521</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="X5">
-        <v>0.0002807017543859649</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="Y5">
-        <v>0.0002114260008996851</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="Z5">
-        <v>0.0001146235521235521</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AA5">
-        <v>0.0002807017543859649</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="AB5">
-        <v>0.0002114200663013328</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="AC5">
-        <v>0.0001146235521235521</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AD5">
-        <v>0.0002806938752596418</v>
+        <v>0.008835356260096223</v>
       </c>
       <c r="AE5">
         <v>0.004525899389334496</v>
       </c>
       <c r="AF5">
-        <v>0.00012125</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AG5">
-        <v>0.00776143597405022</v>
+        <v>0.004525899389334496</v>
       </c>
       <c r="AH5">
         <v>0.004525899389334496</v>
       </c>
       <c r="AI5">
-        <v>0.00012125</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AJ5">
-        <v>0.00776143597405022</v>
+        <v>0.004525899389334496</v>
       </c>
       <c r="AK5">
         <v>0.01122594815382163</v>
       </c>
       <c r="AL5">
-        <v>0.000135</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AM5">
-        <v>0.01743604713253146</v>
+        <v>0.01122594815382163</v>
       </c>
       <c r="AN5">
         <v>0.006922179523720256</v>
       </c>
       <c r="AO5">
-        <v>0.0001385263157894737</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AP5">
-        <v>0.008913410739905316</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AQ5">
         <v>0.006922179523720256</v>
       </c>
       <c r="AR5">
-        <v>0.0001385263157894737</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AS5">
-        <v>0.008913410739905316</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AT5">
         <v>0.004525899389334496</v>
       </c>
       <c r="AU5">
-        <v>0.00012125</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AV5">
-        <v>0.00776143597405022</v>
+        <v>0.004525899389334496</v>
       </c>
       <c r="AW5">
         <v>0.004525899389334496</v>
       </c>
       <c r="AX5">
-        <v>0.00012125</v>
+        <v>0.006922179523720256</v>
       </c>
       <c r="AY5">
-        <v>0.00776143597405022</v>
+        <v>0.004525899389334496</v>
       </c>
     </row>
     <row r="6" spans="1:51">
@@ -1126,154 +1126,154 @@
         <v>0.007604888653009554</v>
       </c>
       <c r="B6">
-        <v>0.0001451228070175439</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="C6">
-        <v>0.009488312140691069</v>
+        <v>0.007604888653009554</v>
       </c>
       <c r="D6">
         <v>0.007604888653009554</v>
       </c>
       <c r="E6">
-        <v>0.0001451228070175439</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="F6">
-        <v>0.009488312140691069</v>
+        <v>0.007604888653009554</v>
       </c>
       <c r="G6">
         <v>0.008100489336805078</v>
       </c>
       <c r="H6">
-        <v>0.000135</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="I6">
-        <v>0.01258161109759086</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="J6">
-        <v>0.0001837462737624004</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="K6">
-        <v>0.00442795584919</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="L6">
-        <v>0.0002807017543859648</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="M6">
         <v>0.008100489336805078</v>
       </c>
       <c r="N6">
-        <v>0.000135</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="O6">
-        <v>0.01258161109759086</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="P6">
         <v>0.008100489336805078</v>
       </c>
       <c r="Q6">
-        <v>0.000135</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="R6">
-        <v>0.01258161109759086</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="S6">
         <v>0.008100489336805078</v>
       </c>
       <c r="T6">
-        <v>0.04031362834701079</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="U6">
-        <v>0.01258161109759086</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="V6">
-        <v>0.0002114260008996851</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="W6">
-        <v>0.0001146235521235521</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="X6">
-        <v>0.0002807017543859649</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="Y6">
-        <v>0.0002114260008996851</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="Z6">
-        <v>0.0001146235521235521</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AA6">
-        <v>0.0002807017543859649</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="AB6">
-        <v>0.0002114200663013328</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="AC6">
-        <v>0.0001146235521235521</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AD6">
-        <v>0.0002806938752596418</v>
+        <v>0.006807549415768157</v>
       </c>
       <c r="AE6">
         <v>0.005228291075369343</v>
       </c>
       <c r="AF6">
-        <v>0.00012125</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AG6">
-        <v>0.008965962993080192</v>
+        <v>0.005228291075369343</v>
       </c>
       <c r="AH6">
         <v>0.005228291075369343</v>
       </c>
       <c r="AI6">
-        <v>0.00012125</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AJ6">
-        <v>0.008965962993080192</v>
+        <v>0.005228291075369343</v>
       </c>
       <c r="AK6">
         <v>0.008100489336805078</v>
       </c>
       <c r="AL6">
-        <v>0.000135</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AM6">
-        <v>0.01258161109759086</v>
+        <v>0.008100489336805078</v>
       </c>
       <c r="AN6">
         <v>0.00601021017852676</v>
       </c>
       <c r="AO6">
-        <v>0.0001385263157894737</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AP6">
-        <v>0.007739104680945521</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AQ6">
         <v>0.00601021017852676</v>
       </c>
       <c r="AR6">
-        <v>0.0001385263157894737</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AS6">
-        <v>0.007739104680945521</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AT6">
         <v>0.005228291075369343</v>
       </c>
       <c r="AU6">
-        <v>0.00012125</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AV6">
-        <v>0.008965962993080192</v>
+        <v>0.005228291075369343</v>
       </c>
       <c r="AW6">
         <v>0.005228291075369343</v>
       </c>
       <c r="AX6">
-        <v>0.00012125</v>
+        <v>0.00601021017852676</v>
       </c>
       <c r="AY6">
-        <v>0.008965962993080192</v>
+        <v>0.005228291075369343</v>
       </c>
     </row>
     <row r="7" spans="1:51">
@@ -1281,154 +1281,154 @@
         <v>0.004772845845953531</v>
       </c>
       <c r="B7">
-        <v>0.0001451228070175439</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="C7">
-        <v>0.005954886817164148</v>
+        <v>0.004772845845953531</v>
       </c>
       <c r="D7">
         <v>0.004772845845953531</v>
       </c>
       <c r="E7">
-        <v>0.0001451228070175439</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="F7">
-        <v>0.005954886817164148</v>
+        <v>0.004772845845953531</v>
       </c>
       <c r="G7">
         <v>0.005450682425444587</v>
       </c>
       <c r="H7">
-        <v>0.000135</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="I7">
-        <v>0.008465953554413931</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="J7">
-        <v>0.0001837462737624004</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="K7">
-        <v>0.003720867464563825</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="L7">
-        <v>0.0002807017543859648</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="M7">
         <v>0.005450682425444587</v>
       </c>
       <c r="N7">
-        <v>0.000135</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="O7">
-        <v>0.008465953554413931</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="P7">
         <v>0.005450682425444587</v>
       </c>
       <c r="Q7">
-        <v>0.000135</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="R7">
-        <v>0.008465953554413931</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="S7">
         <v>0.005450682425444587</v>
       </c>
       <c r="T7">
-        <v>0.01762999655094151</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="U7">
-        <v>0.008465953554413931</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="V7">
-        <v>0.0002114260008996851</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="W7">
-        <v>0.0001146235521235521</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="X7">
-        <v>0.0002807017543859649</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="Y7">
-        <v>0.0002114260008996851</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="Z7">
-        <v>0.0001146235521235521</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AA7">
-        <v>0.0002807017543859649</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="AB7">
-        <v>0.0002114200663013328</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="AC7">
-        <v>0.0001146235521235521</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AD7">
-        <v>0.0002806938752596418</v>
+        <v>0.004078748875308266</v>
       </c>
       <c r="AE7">
         <v>0.002205253767146671</v>
       </c>
       <c r="AF7">
-        <v>0.00012125</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AG7">
-        <v>0.003781775609191951</v>
+        <v>0.002205253767146671</v>
       </c>
       <c r="AH7">
         <v>0.002205253767146671</v>
       </c>
       <c r="AI7">
-        <v>0.00012125</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AJ7">
-        <v>0.003781775609191951</v>
+        <v>0.002205253767146671</v>
       </c>
       <c r="AK7">
         <v>0.005450682425444587</v>
       </c>
       <c r="AL7">
-        <v>0.000135</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AM7">
-        <v>0.008465953554413931</v>
+        <v>0.005450682425444587</v>
       </c>
       <c r="AN7">
         <v>0.003384651904663001</v>
       </c>
       <c r="AO7">
-        <v>0.0001385263157894737</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AP7">
-        <v>0.004358279431280953</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AQ7">
         <v>0.003384651904663001</v>
       </c>
       <c r="AR7">
-        <v>0.0001385263157894737</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AS7">
-        <v>0.004358279431280953</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AT7">
         <v>0.002205253767146671</v>
       </c>
       <c r="AU7">
-        <v>0.00012125</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AV7">
-        <v>0.003781775609191951</v>
+        <v>0.002205253767146671</v>
       </c>
       <c r="AW7">
         <v>0.002205253767146671</v>
       </c>
       <c r="AX7">
-        <v>0.00012125</v>
+        <v>0.003384651904663001</v>
       </c>
       <c r="AY7">
-        <v>0.003781775609191951</v>
+        <v>0.002205253767146671</v>
       </c>
     </row>
     <row r="8" spans="1:51">
@@ -1436,154 +1436,154 @@
         <v>0.003991392245221766</v>
       </c>
       <c r="B8">
-        <v>0.0001451228070175439</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="C8">
-        <v>0.004979898750208604</v>
+        <v>0.003991392245221766</v>
       </c>
       <c r="D8">
         <v>0.003991392245221766</v>
       </c>
       <c r="E8">
-        <v>0.0001451228070175439</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="F8">
-        <v>0.004979898750208604</v>
+        <v>0.003991392245221766</v>
       </c>
       <c r="G8">
         <v>0.00330219071379162</v>
       </c>
       <c r="H8">
-        <v>0.000135</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="I8">
-        <v>0.005128934512910387</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="J8">
-        <v>0.0001837462737624004</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="K8">
-        <v>0.00301377907993765</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="L8">
-        <v>0.0002807017543859648</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="M8">
         <v>0.00330219071379162</v>
       </c>
       <c r="N8">
-        <v>0.000135</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="O8">
-        <v>0.005128934512910387</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="P8">
         <v>0.00330219071379162</v>
       </c>
       <c r="Q8">
-        <v>0.000135</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="R8">
-        <v>0.005128934512910387</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="S8">
         <v>0.00330219071379162</v>
       </c>
       <c r="T8">
-        <v>0.0001365484945264078</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="U8">
-        <v>0.005128934512910387</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="V8">
-        <v>0.0002114260008996851</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="W8">
-        <v>0.0001146235521235521</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="X8">
-        <v>0.0002807017543859649</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="Y8">
-        <v>0.0002114260008996851</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="Z8">
-        <v>0.0001146235521235521</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AA8">
-        <v>0.0002807017543859649</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="AB8">
-        <v>0.0002114200663013328</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="AC8">
-        <v>0.0001146235521235521</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AD8">
-        <v>0.0002806938752596418</v>
+        <v>0.003374232351427357</v>
       </c>
       <c r="AE8">
         <v>0.002687051978199552</v>
       </c>
       <c r="AF8">
-        <v>0.00012125</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AG8">
-        <v>0.004608008286018807</v>
+        <v>0.002687051978199552</v>
       </c>
       <c r="AH8">
         <v>0.002687051978199552</v>
       </c>
       <c r="AI8">
-        <v>0.00012125</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AJ8">
-        <v>0.004608008286018807</v>
+        <v>0.002687051978199552</v>
       </c>
       <c r="AK8">
         <v>0.00330219071379162</v>
       </c>
       <c r="AL8">
-        <v>0.000135</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AM8">
-        <v>0.005128934512910387</v>
+        <v>0.00330219071379162</v>
       </c>
       <c r="AN8">
         <v>0.002757072457632948</v>
       </c>
       <c r="AO8">
-        <v>0.0001385263157894737</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AP8">
-        <v>0.003550170747573319</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AQ8">
         <v>0.002757072457632948</v>
       </c>
       <c r="AR8">
-        <v>0.0001385263157894737</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AS8">
-        <v>0.003550170747573319</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AT8">
         <v>0.002687051978199552</v>
       </c>
       <c r="AU8">
-        <v>0.00012125</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AV8">
-        <v>0.004608008286018807</v>
+        <v>0.002687051978199552</v>
       </c>
       <c r="AW8">
         <v>0.002687051978199552</v>
       </c>
       <c r="AX8">
-        <v>0.00012125</v>
+        <v>0.002757072457632948</v>
       </c>
       <c r="AY8">
-        <v>0.004608008286018807</v>
+        <v>0.002687051978199552</v>
       </c>
     </row>
     <row r="9" spans="1:51">
@@ -1591,154 +1591,154 @@
         <v>0.002005334436762057</v>
       </c>
       <c r="B9">
-        <v>0.0001451228070175439</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="C9">
-        <v>0.002501974710036744</v>
+        <v>0.002005334436762057</v>
       </c>
       <c r="D9">
         <v>0.002005334436762057</v>
       </c>
       <c r="E9">
-        <v>0.0001451228070175439</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="F9">
-        <v>0.002501974710036744</v>
+        <v>0.002005334436762057</v>
       </c>
       <c r="G9">
         <v>0.001670539274695322</v>
       </c>
       <c r="H9">
-        <v>0.000135</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="I9">
-        <v>0.002594667384101244</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="J9">
-        <v>0.0001837462737624004</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="K9">
-        <v>0.002306690695311473</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="L9">
-        <v>0.0002807017543859648</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="M9">
         <v>0.001670539274695322</v>
       </c>
       <c r="N9">
-        <v>0.000135</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="O9">
-        <v>0.002594667384101244</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="P9">
         <v>0.001670539274695322</v>
       </c>
       <c r="Q9">
-        <v>0.000135</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="R9">
-        <v>0.002594667384101244</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="S9">
         <v>0.001670539274695322</v>
       </c>
       <c r="T9">
-        <v>0.0001365484945264078</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="U9">
-        <v>0.002594667384101244</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="V9">
-        <v>0.0002114260008996851</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="W9">
-        <v>0.0001146235521235521</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="X9">
-        <v>0.0002807017543859649</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="Y9">
-        <v>0.0002114260008996851</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="Z9">
-        <v>0.0001146235521235521</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AA9">
-        <v>0.0002807017543859649</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="AB9">
-        <v>0.0002114200663013328</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="AC9">
-        <v>0.0001146235521235521</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AD9">
-        <v>0.0002806938752596418</v>
+        <v>0.00153504043604689</v>
       </c>
       <c r="AE9">
         <v>0.0006846436056344724</v>
       </c>
       <c r="AF9">
-        <v>0.00012125</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AG9">
-        <v>0.001174090949236989</v>
+        <v>0.0006846436056344724</v>
       </c>
       <c r="AH9">
         <v>0.0006846436056344724</v>
       </c>
       <c r="AI9">
-        <v>0.00012125</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AJ9">
-        <v>0.001174090949236989</v>
+        <v>0.0006846436056344724</v>
       </c>
       <c r="AK9">
         <v>0.001670539274695322</v>
       </c>
       <c r="AL9">
-        <v>0.000135</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AM9">
-        <v>0.002594667384101244</v>
+        <v>0.001670539274695322</v>
       </c>
       <c r="AN9">
         <v>0.001064746435331724</v>
       </c>
       <c r="AO9">
-        <v>0.0001385263157894737</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AP9">
-        <v>0.001371030941835658</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AQ9">
         <v>0.001064746435331724</v>
       </c>
       <c r="AR9">
-        <v>0.0001385263157894737</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AS9">
-        <v>0.001371030941835658</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AT9">
         <v>0.0006846436056344724</v>
       </c>
       <c r="AU9">
-        <v>0.00012125</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AV9">
-        <v>0.001174090949236989</v>
+        <v>0.0006846436056344724</v>
       </c>
       <c r="AW9">
         <v>0.0006846436056344724</v>
       </c>
       <c r="AX9">
-        <v>0.00012125</v>
+        <v>0.001064746435331724</v>
       </c>
       <c r="AY9">
-        <v>0.001174090949236989</v>
+        <v>0.0006846436056344724</v>
       </c>
     </row>
     <row r="10" spans="1:51">
@@ -1746,154 +1746,154 @@
         <v>0.001349740535953804</v>
       </c>
       <c r="B10">
-        <v>0.0001451228070175439</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="C10">
-        <v>0.001684016702730448</v>
+        <v>0.001349740535953804</v>
       </c>
       <c r="D10">
         <v>0.001349740535953804</v>
       </c>
       <c r="E10">
-        <v>0.0001451228070175439</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="F10">
-        <v>0.001684016702730448</v>
+        <v>0.001349740535953804</v>
       </c>
       <c r="G10">
         <v>0.007285435669508927</v>
       </c>
       <c r="H10">
-        <v>0.000135</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="I10">
-        <v>0.01131567667817344</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="J10">
-        <v>0.0001837462737624004</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="K10">
-        <v>0.03723341099470157</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="L10">
-        <v>0.0002807017543859648</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="M10">
         <v>0.007285435669508927</v>
       </c>
       <c r="N10">
-        <v>0.000135</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="O10">
-        <v>0.01131567667817344</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="P10">
         <v>0.007285435669508927</v>
       </c>
       <c r="Q10">
-        <v>0.000135</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="R10">
-        <v>0.01131567667817344</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="S10">
         <v>0.007285435669508927</v>
       </c>
       <c r="T10">
-        <v>0.0001365484945264078</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="U10">
-        <v>0.01131567667817344</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="V10">
-        <v>0.0002114260008996851</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="W10">
-        <v>0.0001146235521235521</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="X10">
-        <v>0.0002807017543859649</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="Y10">
-        <v>0.0002114260008996851</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="Z10">
-        <v>0.0001146235521235521</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AA10">
-        <v>0.0002807017543859649</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="AB10">
-        <v>0.0002114200663013328</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="AC10">
-        <v>0.0001146235521235521</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AD10">
-        <v>0.0002806938752596418</v>
+        <v>0.01323532342061096</v>
       </c>
       <c r="AE10">
         <v>0.0124887484612893</v>
       </c>
       <c r="AF10">
-        <v>0.00012125</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AG10">
-        <v>0.0214168750208493</v>
+        <v>0.0124887484612893</v>
       </c>
       <c r="AH10">
         <v>0.0124887484612893</v>
       </c>
       <c r="AI10">
-        <v>0.00012125</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AJ10">
-        <v>0.0214168750208493</v>
+        <v>0.0124887484612893</v>
       </c>
       <c r="AK10">
         <v>0.007285435669508927</v>
       </c>
       <c r="AL10">
-        <v>0.000135</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AM10">
-        <v>0.01131567667817344</v>
+        <v>0.007285435669508927</v>
       </c>
       <c r="AN10">
         <v>0.02512090630526812</v>
       </c>
       <c r="AO10">
-        <v>0.0001385263157894737</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AP10">
-        <v>0.03234717552329418</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AQ10">
         <v>0.02512090630526812</v>
       </c>
       <c r="AR10">
-        <v>0.0001385263157894737</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AS10">
-        <v>0.03234717552329418</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AT10">
         <v>0.0124887484612893</v>
       </c>
       <c r="AU10">
-        <v>0.00012125</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AV10">
-        <v>0.0214168750208493</v>
+        <v>0.0124887484612893</v>
       </c>
       <c r="AW10">
         <v>0.0124887484612893</v>
       </c>
       <c r="AX10">
-        <v>0.00012125</v>
+        <v>0.02512090630526812</v>
       </c>
       <c r="AY10">
-        <v>0.0214168750208493</v>
+        <v>0.0124887484612893</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the sim inputs for each trial seperatly. slight profit reduce.
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.07731728653101365</v>
+        <v>0.06367969960706951</v>
       </c>
       <c r="B1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.07731728653101365</v>
+        <v>0.06367969960706951</v>
       </c>
       <c r="D1">
-        <v>0.07731728653101365</v>
+        <v>0.06367969960706951</v>
       </c>
       <c r="E1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.07731728653101365</v>
+        <v>0.06367969960706951</v>
       </c>
       <c r="G1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="H1">
-        <v>0.03494182863500563</v>
+        <v>0.02645332309889065</v>
       </c>
       <c r="I1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="J1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="K1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="M1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="N1">
-        <v>0.03494182863500563</v>
+        <v>0.02645332309889065</v>
       </c>
       <c r="O1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="P1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="Q1">
-        <v>0.03494182863500563</v>
+        <v>0.02645332309889065</v>
       </c>
       <c r="R1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="S1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="T1">
-        <v>0.03494182863500563</v>
+        <v>0.02645332309889065</v>
       </c>
       <c r="U1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="V1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="W1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="Y1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="Z1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="AB1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="AC1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.05612955758300964</v>
+        <v>0.05847353881583695</v>
       </c>
       <c r="AE1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
       <c r="AF1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
       <c r="AH1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
       <c r="AI1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
       <c r="AK1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="AL1">
-        <v>0.03494182863500563</v>
+        <v>0.02645332309889065</v>
       </c>
       <c r="AM1">
-        <v>0.03655454236186033</v>
+        <v>0.04452719281900871</v>
       </c>
       <c r="AN1">
-        <v>0.03494182863500563</v>
+        <v>0.05673815188542608</v>
       </c>
       <c r="AO1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP1">
-        <v>0.03494182863500563</v>
+        <v>0.05673815188542608</v>
       </c>
       <c r="AQ1">
-        <v>0.03494182863500563</v>
+        <v>0.05673815188542608</v>
       </c>
       <c r="AR1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.03494182863500563</v>
+        <v>0.05673815188542608</v>
       </c>
       <c r="AT1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
       <c r="AU1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
       <c r="AW1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
       <c r="AX1">
-        <v>0.03494182863500563</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.02968570863698958</v>
+        <v>0.03252494619613576</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.01755041759985082</v>
+        <v>0.01025330033830534</v>
       </c>
       <c r="B2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.01755041759985082</v>
+        <v>0.01025330033830534</v>
       </c>
       <c r="D2">
-        <v>0.01755041759985082</v>
+        <v>0.01025330033830534</v>
       </c>
       <c r="E2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.01755041759985082</v>
+        <v>0.01025330033830534</v>
       </c>
       <c r="G2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="H2">
-        <v>0.009630943397427958</v>
+        <v>0.355566172325769</v>
       </c>
       <c r="I2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="J2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="K2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="M2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="N2">
-        <v>0.009630943397427958</v>
+        <v>0.355566172325769</v>
       </c>
       <c r="O2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="P2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="Q2">
-        <v>0.009630943397427958</v>
+        <v>0.355566172325769</v>
       </c>
       <c r="R2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="S2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="T2">
-        <v>0.009630943397427958</v>
+        <v>0.355566172325769</v>
       </c>
       <c r="U2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="V2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="W2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="Y2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="Z2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="AB2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="AC2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.01359068049863939</v>
+        <v>0.008598109140940398</v>
       </c>
       <c r="AE2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
       <c r="AF2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
       <c r="AH2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
       <c r="AI2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
       <c r="AK2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="AL2">
-        <v>0.009630943397427958</v>
+        <v>0.355566172325769</v>
       </c>
       <c r="AM2">
-        <v>0.01555241329329285</v>
+        <v>0.01023589746068457</v>
       </c>
       <c r="AN2">
-        <v>0.009630943397427958</v>
+        <v>0.008046378741818749</v>
       </c>
       <c r="AO2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.009630943397427958</v>
+        <v>0.008046378741818749</v>
       </c>
       <c r="AQ2">
-        <v>0.009630943397427958</v>
+        <v>0.008046378741818749</v>
       </c>
       <c r="AR2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.009630943397427958</v>
+        <v>0.008046378741818749</v>
       </c>
       <c r="AT2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
       <c r="AU2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
       <c r="AW2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
       <c r="AX2">
-        <v>0.009630943397427958</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.008408329871366324</v>
+        <v>0.007188277216068179</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.02119267433551551</v>
+        <v>0.009293911769232208</v>
       </c>
       <c r="B3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="C3">
-        <v>0.02119267433551551</v>
+        <v>0.009293911769232208</v>
       </c>
       <c r="D3">
-        <v>0.02119267433551551</v>
+        <v>0.009293911769232208</v>
       </c>
       <c r="E3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="F3">
-        <v>0.02119267433551551</v>
+        <v>0.009293911769232208</v>
       </c>
       <c r="G3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="H3">
-        <v>0.005831387874454591</v>
+        <v>0.2919178348084053</v>
       </c>
       <c r="I3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="J3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="K3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="L3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="M3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="N3">
-        <v>0.005831387874454591</v>
+        <v>0.2919178348084053</v>
       </c>
       <c r="O3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="P3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="Q3">
-        <v>0.005831387874454591</v>
+        <v>0.2919178348084053</v>
       </c>
       <c r="R3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="S3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="T3">
-        <v>0.005831387874454591</v>
+        <v>0.2919178348084053</v>
       </c>
       <c r="U3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="V3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="W3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="X3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="Y3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="Z3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AA3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="AB3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="AC3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AD3">
-        <v>0.01351203110498505</v>
+        <v>0.008672413242674874</v>
       </c>
       <c r="AE3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
       <c r="AF3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AG3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
       <c r="AH3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
       <c r="AI3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AJ3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
       <c r="AK3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="AL3">
-        <v>0.005831387874454591</v>
+        <v>0.2919178348084053</v>
       </c>
       <c r="AM3">
-        <v>0.00941936621975901</v>
+        <v>0.01162448032571289</v>
       </c>
       <c r="AN3">
-        <v>0.005831387874454591</v>
+        <v>0.008465247067155761</v>
       </c>
       <c r="AO3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AP3">
-        <v>0.005831387874454591</v>
+        <v>0.008465247067155761</v>
       </c>
       <c r="AQ3">
-        <v>0.005831387874454591</v>
+        <v>0.008465247067155761</v>
       </c>
       <c r="AR3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AS3">
-        <v>0.005831387874454591</v>
+        <v>0.008465247067155761</v>
       </c>
       <c r="AT3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
       <c r="AU3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AV3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
       <c r="AW3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
       <c r="AX3">
-        <v>0.005831387874454591</v>
+        <v>0.6005669028436544</v>
       </c>
       <c r="AY3">
-        <v>0.003807786292626348</v>
+        <v>0.006351370514127526</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.01439149236759607</v>
+        <v>0.005547967643471884</v>
       </c>
       <c r="B4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="C4">
-        <v>0.01439149236759607</v>
+        <v>0.005547967643471884</v>
       </c>
       <c r="D4">
-        <v>0.01439149236759607</v>
+        <v>0.005547967643471884</v>
       </c>
       <c r="E4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="F4">
-        <v>0.01439149236759607</v>
+        <v>0.005547967643471884</v>
       </c>
       <c r="G4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="H4">
-        <v>0.00523361477249056</v>
+        <v>0.1596580675690371</v>
       </c>
       <c r="I4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="J4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="K4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="L4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="M4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="N4">
-        <v>0.00523361477249056</v>
+        <v>0.1596580675690371</v>
       </c>
       <c r="O4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="P4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="Q4">
-        <v>0.00523361477249056</v>
+        <v>0.1596580675690371</v>
       </c>
       <c r="R4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="S4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="T4">
-        <v>0.00523361477249056</v>
+        <v>0.1596580675690371</v>
       </c>
       <c r="U4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="V4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="W4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="X4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="Y4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="Z4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AA4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="AB4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="AC4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AD4">
-        <v>0.009812553570043313</v>
+        <v>0.008831150671660506</v>
       </c>
       <c r="AE4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
       <c r="AF4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AG4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
       <c r="AH4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
       <c r="AI4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AJ4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
       <c r="AK4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="AL4">
-        <v>0.00523361477249056</v>
+        <v>0.1596580675690371</v>
       </c>
       <c r="AM4">
-        <v>0.01480535717291733</v>
+        <v>0.01251778709856828</v>
       </c>
       <c r="AN4">
-        <v>0.00523361477249056</v>
+        <v>0.009925545014390046</v>
       </c>
       <c r="AO4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AP4">
-        <v>0.00523361477249056</v>
+        <v>0.009925545014390046</v>
       </c>
       <c r="AQ4">
-        <v>0.00523361477249056</v>
+        <v>0.009925545014390046</v>
       </c>
       <c r="AR4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AS4">
-        <v>0.00523361477249056</v>
+        <v>0.009925545014390046</v>
       </c>
       <c r="AT4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
       <c r="AU4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AV4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
       <c r="AW4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
       <c r="AX4">
-        <v>0.00523361477249056</v>
+        <v>0.2802132262183178</v>
       </c>
       <c r="AY4">
-        <v>0.006830537398357178</v>
+        <v>0.006517876462149508</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.01074853299647219</v>
+        <v>0.004896836875254575</v>
       </c>
       <c r="B5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C5">
-        <v>0.01074853299647219</v>
+        <v>0.004896836875254575</v>
       </c>
       <c r="D5">
-        <v>0.01074853299647219</v>
+        <v>0.004896836875254575</v>
       </c>
       <c r="E5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F5">
-        <v>0.01074853299647219</v>
+        <v>0.004896836875254575</v>
       </c>
       <c r="G5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="H5">
-        <v>0.006922179523720256</v>
+        <v>0.1104532511443694</v>
       </c>
       <c r="I5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="J5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="K5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="M5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="N5">
-        <v>0.006922179523720256</v>
+        <v>0.1104532511443694</v>
       </c>
       <c r="O5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="P5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="Q5">
-        <v>0.006922179523720256</v>
+        <v>0.1104532511443694</v>
       </c>
       <c r="R5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="S5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="T5">
-        <v>0.006922179523720256</v>
+        <v>0.1104532511443694</v>
       </c>
       <c r="U5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="V5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="W5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="Y5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="Z5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="AB5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="AC5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD5">
-        <v>0.008835356260096223</v>
+        <v>0.007778777372740387</v>
       </c>
       <c r="AE5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
       <c r="AF5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
       <c r="AH5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
       <c r="AI5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
       <c r="AK5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="AL5">
-        <v>0.006922179523720256</v>
+        <v>0.1104532511443694</v>
       </c>
       <c r="AM5">
-        <v>0.01122594815382163</v>
+        <v>0.01106770690415737</v>
       </c>
       <c r="AN5">
-        <v>0.006922179523720256</v>
+        <v>0.008739424205235657</v>
       </c>
       <c r="AO5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP5">
-        <v>0.006922179523720256</v>
+        <v>0.008739424205235657</v>
       </c>
       <c r="AQ5">
-        <v>0.006922179523720256</v>
+        <v>0.008739424205235657</v>
       </c>
       <c r="AR5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS5">
-        <v>0.006922179523720256</v>
+        <v>0.008739424205235657</v>
       </c>
       <c r="AT5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
       <c r="AU5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
       <c r="AW5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
       <c r="AX5">
-        <v>0.006922179523720256</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY5">
-        <v>0.004525899389334496</v>
+        <v>0.005240283941084238</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.007604888653009554</v>
+        <v>0.004247439599807374</v>
       </c>
       <c r="B6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C6">
-        <v>0.007604888653009554</v>
+        <v>0.004247439599807374</v>
       </c>
       <c r="D6">
-        <v>0.007604888653009554</v>
+        <v>0.004247439599807374</v>
       </c>
       <c r="E6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F6">
-        <v>0.007604888653009554</v>
+        <v>0.004247439599807374</v>
       </c>
       <c r="G6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="H6">
-        <v>0.00601021017852676</v>
+        <v>0.0344086061921234</v>
       </c>
       <c r="I6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="J6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="K6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="M6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="N6">
-        <v>0.00601021017852676</v>
+        <v>0.0344086061921234</v>
       </c>
       <c r="O6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="P6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="Q6">
-        <v>0.00601021017852676</v>
+        <v>0.0344086061921234</v>
       </c>
       <c r="R6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="S6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="T6">
-        <v>0.00601021017852676</v>
+        <v>0.0344086061921234</v>
       </c>
       <c r="U6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="V6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="W6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="Y6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="Z6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="AB6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="AC6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD6">
-        <v>0.006807549415768157</v>
+        <v>0.005002015415800676</v>
       </c>
       <c r="AE6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
       <c r="AF6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
       <c r="AH6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
       <c r="AI6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
       <c r="AK6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="AL6">
-        <v>0.00601021017852676</v>
+        <v>0.0344086061921234</v>
       </c>
       <c r="AM6">
-        <v>0.008100489336805078</v>
+        <v>0.00797963806751387</v>
       </c>
       <c r="AN6">
-        <v>0.00601021017852676</v>
+        <v>0.005253540687798442</v>
       </c>
       <c r="AO6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP6">
-        <v>0.00601021017852676</v>
+        <v>0.005253540687798442</v>
       </c>
       <c r="AQ6">
-        <v>0.00601021017852676</v>
+        <v>0.005253540687798442</v>
       </c>
       <c r="AR6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS6">
-        <v>0.00601021017852676</v>
+        <v>0.005253540687798442</v>
       </c>
       <c r="AT6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
       <c r="AU6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
       <c r="AW6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
       <c r="AX6">
-        <v>0.00601021017852676</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY6">
-        <v>0.005228291075369343</v>
+        <v>0.004020988077555074</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.004772845845953531</v>
+        <v>0.00179556533161163</v>
       </c>
       <c r="B7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.004772845845953531</v>
+        <v>0.00179556533161163</v>
       </c>
       <c r="D7">
-        <v>0.004772845845953531</v>
+        <v>0.00179556533161163</v>
       </c>
       <c r="E7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.004772845845953531</v>
+        <v>0.00179556533161163</v>
       </c>
       <c r="G7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="H7">
-        <v>0.003384651904663001</v>
+        <v>0.01953017441316452</v>
       </c>
       <c r="I7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="J7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="K7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="M7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="N7">
-        <v>0.003384651904663001</v>
+        <v>0.01953017441316452</v>
       </c>
       <c r="O7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="P7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="Q7">
-        <v>0.003384651904663001</v>
+        <v>0.01953017441316452</v>
       </c>
       <c r="R7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="S7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="T7">
-        <v>0.003384651904663001</v>
+        <v>0.01953017441316452</v>
       </c>
       <c r="U7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="V7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="W7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="Y7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="Z7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="AB7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="AC7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.004078748875308266</v>
+        <v>0.003065713775538204</v>
       </c>
       <c r="AE7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
       <c r="AF7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
       <c r="AH7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
       <c r="AI7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
       <c r="AK7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="AL7">
-        <v>0.003384651904663001</v>
+        <v>0.01953017441316452</v>
       </c>
       <c r="AM7">
-        <v>0.005450682425444587</v>
+        <v>0.005371047128878667</v>
       </c>
       <c r="AN7">
-        <v>0.003384651904663001</v>
+        <v>0.003489096590180395</v>
       </c>
       <c r="AO7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.003384651904663001</v>
+        <v>0.003489096590180395</v>
       </c>
       <c r="AQ7">
-        <v>0.003384651904663001</v>
+        <v>0.003489096590180395</v>
       </c>
       <c r="AR7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.003384651904663001</v>
+        <v>0.003489096590180395</v>
       </c>
       <c r="AT7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
       <c r="AU7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
       <c r="AW7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
       <c r="AX7">
-        <v>0.003384651904663001</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.002205253767146671</v>
+        <v>0.002925344336363591</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.003991392245221766</v>
+        <v>0.001466544116934519</v>
       </c>
       <c r="B8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.003991392245221766</v>
+        <v>0.001466544116934519</v>
       </c>
       <c r="D8">
-        <v>0.003991392245221766</v>
+        <v>0.001466544116934519</v>
       </c>
       <c r="E8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.003991392245221766</v>
+        <v>0.001466544116934519</v>
       </c>
       <c r="G8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="H8">
-        <v>0.002757072457632948</v>
+        <v>0.001749940937478829</v>
       </c>
       <c r="I8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="J8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="K8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="M8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="N8">
-        <v>0.002757072457632948</v>
+        <v>0.001749940937478829</v>
       </c>
       <c r="O8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="P8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="Q8">
-        <v>0.002757072457632948</v>
+        <v>0.001749940937478829</v>
       </c>
       <c r="R8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="S8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="T8">
-        <v>0.002757072457632948</v>
+        <v>0.001749940937478829</v>
       </c>
       <c r="U8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="V8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="W8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="Y8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="Z8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="AB8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="AC8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.003374232351427357</v>
+        <v>0.002060177720505365</v>
       </c>
       <c r="AE8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
       <c r="AF8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
       <c r="AH8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
       <c r="AI8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
       <c r="AK8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="AL8">
-        <v>0.002757072457632948</v>
+        <v>0.001749940937478829</v>
       </c>
       <c r="AM8">
-        <v>0.00330219071379162</v>
+        <v>0.002168617090675048</v>
       </c>
       <c r="AN8">
-        <v>0.002757072457632948</v>
+        <v>0.002258055588362314</v>
       </c>
       <c r="AO8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP8">
-        <v>0.002757072457632948</v>
+        <v>0.002258055588362314</v>
       </c>
       <c r="AQ8">
-        <v>0.002757072457632948</v>
+        <v>0.002258055588362314</v>
       </c>
       <c r="AR8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002757072457632948</v>
+        <v>0.002258055588362314</v>
       </c>
       <c r="AT8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
       <c r="AU8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
       <c r="AW8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
       <c r="AX8">
-        <v>0.002757072457632948</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.002687051978199552</v>
+        <v>0.001615403696625696</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.002005334436762057</v>
+        <v>0.001137523008674775</v>
       </c>
       <c r="B9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.002005334436762057</v>
+        <v>0.001137523008674775</v>
       </c>
       <c r="D9">
-        <v>0.002005334436762057</v>
+        <v>0.001137523008674775</v>
       </c>
       <c r="E9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.002005334436762057</v>
+        <v>0.001137523008674775</v>
       </c>
       <c r="G9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="H9">
-        <v>0.001064746435331724</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="I9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="J9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="K9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="M9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="N9">
-        <v>0.001064746435331724</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="O9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="P9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="Q9">
-        <v>0.001064746435331724</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="R9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="S9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="T9">
-        <v>0.001064746435331724</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="U9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="V9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="W9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="Y9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="Z9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="AB9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="AC9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.00153504043604689</v>
+        <v>0.001139027750111053</v>
       </c>
       <c r="AE9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
       <c r="AF9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
       <c r="AH9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
       <c r="AI9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
       <c r="AK9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="AL9">
-        <v>0.001064746435331724</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="AM9">
-        <v>0.001670539274695322</v>
+        <v>0.001645616507591864</v>
       </c>
       <c r="AN9">
-        <v>0.001064746435331724</v>
+        <v>0.001139529330589813</v>
       </c>
       <c r="AO9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP9">
-        <v>0.001064746435331724</v>
+        <v>0.001139529330589813</v>
       </c>
       <c r="AQ9">
-        <v>0.001064746435331724</v>
+        <v>0.001139529330589813</v>
       </c>
       <c r="AR9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001064746435331724</v>
+        <v>0.001139529330589813</v>
       </c>
       <c r="AT9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
       <c r="AU9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
       <c r="AW9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
       <c r="AX9">
-        <v>0.001064746435331724</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.0006846436056344724</v>
+        <v>0.0009252817338288512</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.001349740535953804</v>
+        <v>0.02837565107795857</v>
       </c>
       <c r="B10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.001349740535953804</v>
+        <v>0.02837565107795857</v>
       </c>
       <c r="D10">
-        <v>0.001349740535953804</v>
+        <v>0.02837565107795857</v>
       </c>
       <c r="E10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.001349740535953804</v>
+        <v>0.02837565107795857</v>
       </c>
       <c r="G10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="H10">
-        <v>0.02512090630526812</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="I10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="J10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="K10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="M10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="N10">
-        <v>0.02512090630526812</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="O10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="P10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="Q10">
-        <v>0.02512090630526812</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="R10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="S10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="T10">
-        <v>0.02512090630526812</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="U10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="V10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="W10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="X10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="Y10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="Z10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="AB10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="AC10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.01323532342061096</v>
+        <v>0.01823733023305132</v>
       </c>
       <c r="AE10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
       <c r="AF10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
       <c r="AH10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
       <c r="AI10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
       <c r="AK10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="AL10">
-        <v>0.02512090630526812</v>
+        <v>0.000131314755380893</v>
       </c>
       <c r="AM10">
-        <v>0.007285435669508927</v>
+        <v>0.007176744350673809</v>
       </c>
       <c r="AN10">
-        <v>0.02512090630526812</v>
+        <v>0.01485788995141557</v>
       </c>
       <c r="AO10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AP10">
-        <v>0.02512090630526812</v>
+        <v>0.01485788995141557</v>
       </c>
       <c r="AQ10">
-        <v>0.02512090630526812</v>
+        <v>0.01485788995141557</v>
       </c>
       <c r="AR10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.02512090630526812</v>
+        <v>0.01485788995141557</v>
       </c>
       <c r="AT10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
       <c r="AU10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
       <c r="AW10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
       <c r="AX10">
-        <v>0.02512090630526812</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.0124887484612893</v>
+        <v>0.008777638535301927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update stubble sim foo to be consistent (increase foo for eds trials). small profit reduce
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,22 +348,22 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.06367969960706951</v>
+        <v>0.06363819708708202</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.06367969960706951</v>
+        <v>0.06363819708708202</v>
       </c>
       <c r="D1">
-        <v>0.06367969960706951</v>
+        <v>0.06363819708708202</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.06367969960706951</v>
+        <v>0.06363819708708202</v>
       </c>
       <c r="G1">
         <v>0.04452719281900871</v>
@@ -375,13 +375,13 @@
         <v>0.04452719281900871</v>
       </c>
       <c r="J1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="M1">
         <v>0.04452719281900871</v>
@@ -411,49 +411,49 @@
         <v>0.04452719281900871</v>
       </c>
       <c r="V1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="W1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="Y1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="Z1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="AB1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.05847353881583695</v>
+        <v>0.05846248942234432</v>
       </c>
       <c r="AE1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
       <c r="AH1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
       <c r="AK1">
         <v>0.04452719281900871</v>
@@ -465,60 +465,60 @@
         <v>0.04452719281900871</v>
       </c>
       <c r="AN1">
-        <v>0.05673815188542608</v>
+        <v>0.05673725353409841</v>
       </c>
       <c r="AO1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP1">
-        <v>0.05673815188542608</v>
+        <v>0.05673725353409841</v>
       </c>
       <c r="AQ1">
-        <v>0.05673815188542608</v>
+        <v>0.05673725353409841</v>
       </c>
       <c r="AR1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.05673815188542608</v>
+        <v>0.05673725353409841</v>
       </c>
       <c r="AT1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
       <c r="AW1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.03252494619613576</v>
+        <v>0.03251997651482077</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.01025330033830534</v>
+        <v>0.01023604765218303</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.01025330033830534</v>
+        <v>0.01023604765218303</v>
       </c>
       <c r="D2">
-        <v>0.01025330033830534</v>
+        <v>0.01023604765218303</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.01025330033830534</v>
+        <v>0.01023604765218303</v>
       </c>
       <c r="G2">
         <v>0.01023589746068457</v>
@@ -530,13 +530,13 @@
         <v>0.01023589746068457</v>
       </c>
       <c r="J2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="M2">
         <v>0.01023589746068457</v>
@@ -566,49 +566,49 @@
         <v>0.01023589746068457</v>
       </c>
       <c r="V2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="W2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="Y2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="AB2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.008598109140940398</v>
+        <v>0.008592710578368684</v>
       </c>
       <c r="AE2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
       <c r="AH2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
       <c r="AK2">
         <v>0.01023589746068457</v>
@@ -620,60 +620,60 @@
         <v>0.01023589746068457</v>
       </c>
       <c r="AN2">
-        <v>0.008046378741818749</v>
+        <v>0.008044931553763901</v>
       </c>
       <c r="AO2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.008046378741818749</v>
+        <v>0.008044931553763901</v>
       </c>
       <c r="AQ2">
-        <v>0.008046378741818749</v>
+        <v>0.008044931553763901</v>
       </c>
       <c r="AR2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.008046378741818749</v>
+        <v>0.008044931553763901</v>
       </c>
       <c r="AT2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
       <c r="AW2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.007188277216068179</v>
+        <v>0.00718430115432968</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.009293911769232208</v>
+        <v>0.009273507682533707</v>
       </c>
       <c r="B3">
         <v>0.6005669028436544</v>
       </c>
       <c r="C3">
-        <v>0.009293911769232208</v>
+        <v>0.009273507682533707</v>
       </c>
       <c r="D3">
-        <v>0.009293911769232208</v>
+        <v>0.009273507682533707</v>
       </c>
       <c r="E3">
         <v>0.6005669028436544</v>
       </c>
       <c r="F3">
-        <v>0.009293911769232208</v>
+        <v>0.009273507682533707</v>
       </c>
       <c r="G3">
         <v>0.01162448032571289</v>
@@ -685,13 +685,13 @@
         <v>0.01162448032571289</v>
       </c>
       <c r="J3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="K3">
         <v>0.6005669028436544</v>
       </c>
       <c r="L3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="M3">
         <v>0.01162448032571289</v>
@@ -721,49 +721,49 @@
         <v>0.01162448032571289</v>
       </c>
       <c r="V3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="W3">
         <v>0.6005669028436544</v>
       </c>
       <c r="X3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="Y3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="Z3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AA3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="AB3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="AC3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AD3">
-        <v>0.008672413242674874</v>
+        <v>0.008666288540442961</v>
       </c>
       <c r="AE3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
       <c r="AF3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AG3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
       <c r="AH3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
       <c r="AI3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AJ3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
       <c r="AK3">
         <v>0.01162448032571289</v>
@@ -775,60 +775,60 @@
         <v>0.01162448032571289</v>
       </c>
       <c r="AN3">
-        <v>0.008465247067155761</v>
+        <v>0.008463882159746045</v>
       </c>
       <c r="AO3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AP3">
-        <v>0.008465247067155761</v>
+        <v>0.008463882159746045</v>
       </c>
       <c r="AQ3">
-        <v>0.008465247067155761</v>
+        <v>0.008463882159746045</v>
       </c>
       <c r="AR3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AS3">
-        <v>0.008465247067155761</v>
+        <v>0.008463882159746045</v>
       </c>
       <c r="AT3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
       <c r="AU3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AV3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
       <c r="AW3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
       <c r="AX3">
         <v>0.6005669028436544</v>
       </c>
       <c r="AY3">
-        <v>0.006351370514127526</v>
+        <v>0.00559480427302851</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.005547967643471884</v>
+        <v>0.005534367540043079</v>
       </c>
       <c r="B4">
         <v>0.2802132262183178</v>
       </c>
       <c r="C4">
-        <v>0.005547967643471884</v>
+        <v>0.005534367540043079</v>
       </c>
       <c r="D4">
-        <v>0.005547967643471884</v>
+        <v>0.005534367540043079</v>
       </c>
       <c r="E4">
         <v>0.2802132262183178</v>
       </c>
       <c r="F4">
-        <v>0.005547967643471884</v>
+        <v>0.005534367540043079</v>
       </c>
       <c r="G4">
         <v>0.01251778709856828</v>
@@ -840,13 +840,13 @@
         <v>0.01251778709856828</v>
       </c>
       <c r="J4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="K4">
         <v>0.2802132262183178</v>
       </c>
       <c r="L4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="M4">
         <v>0.01251778709856828</v>
@@ -876,49 +876,49 @@
         <v>0.01251778709856828</v>
       </c>
       <c r="V4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="W4">
         <v>0.2802132262183178</v>
       </c>
       <c r="X4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="Y4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="Z4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AA4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="AB4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="AC4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AD4">
-        <v>0.008831150671660506</v>
+        <v>0.008824762978372612</v>
       </c>
       <c r="AE4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
       <c r="AF4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AG4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
       <c r="AH4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
       <c r="AI4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AJ4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
       <c r="AK4">
         <v>0.01251778709856828</v>
@@ -930,60 +930,60 @@
         <v>0.01251778709856828</v>
       </c>
       <c r="AN4">
-        <v>0.009925545014390046</v>
+        <v>0.009921561457815788</v>
       </c>
       <c r="AO4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AP4">
-        <v>0.009925545014390046</v>
+        <v>0.009921561457815788</v>
       </c>
       <c r="AQ4">
-        <v>0.009925545014390046</v>
+        <v>0.009921561457815788</v>
       </c>
       <c r="AR4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AS4">
-        <v>0.009925545014390046</v>
+        <v>0.009921561457815788</v>
       </c>
       <c r="AT4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
       <c r="AU4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AV4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
       <c r="AW4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
       <c r="AX4">
         <v>0.2802132262183178</v>
       </c>
       <c r="AY4">
-        <v>0.006517876462149508</v>
+        <v>0.005738609312496817</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.004896836875254575</v>
+        <v>0.004884832742452431</v>
       </c>
       <c r="B5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C5">
-        <v>0.004896836875254575</v>
+        <v>0.004884832742452431</v>
       </c>
       <c r="D5">
-        <v>0.004896836875254575</v>
+        <v>0.004884832742452431</v>
       </c>
       <c r="E5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F5">
-        <v>0.004896836875254575</v>
+        <v>0.004884832742452431</v>
       </c>
       <c r="G5">
         <v>0.01106770690415737</v>
@@ -995,13 +995,13 @@
         <v>0.01106770690415737</v>
       </c>
       <c r="J5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="K5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="M5">
         <v>0.01106770690415737</v>
@@ -1031,49 +1031,49 @@
         <v>0.01106770690415737</v>
       </c>
       <c r="V5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="W5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="Y5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="Z5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="AB5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="AC5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD5">
-        <v>0.007778777372740387</v>
+        <v>0.006844333466138565</v>
       </c>
       <c r="AE5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
       <c r="AF5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
       <c r="AH5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
       <c r="AI5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
       <c r="AK5">
         <v>0.01106770690415737</v>
@@ -1085,60 +1085,60 @@
         <v>0.01106770690415737</v>
       </c>
       <c r="AN5">
-        <v>0.008739424205235657</v>
+        <v>0.007497500374033943</v>
       </c>
       <c r="AO5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP5">
-        <v>0.008739424205235657</v>
+        <v>0.007497500374033943</v>
       </c>
       <c r="AQ5">
-        <v>0.008739424205235657</v>
+        <v>0.007497500374033943</v>
       </c>
       <c r="AR5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS5">
-        <v>0.008739424205235657</v>
+        <v>0.007497500374033943</v>
       </c>
       <c r="AT5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
       <c r="AU5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
       <c r="AW5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
       <c r="AX5">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY5">
-        <v>0.005240283941084238</v>
+        <v>0.00584237822529203</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.004247439599807374</v>
+        <v>0.00211764917937729</v>
       </c>
       <c r="B6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C6">
-        <v>0.004247439599807374</v>
+        <v>0.00211764917937729</v>
       </c>
       <c r="D6">
-        <v>0.004247439599807374</v>
+        <v>0.00211764917937729</v>
       </c>
       <c r="E6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F6">
-        <v>0.004247439599807374</v>
+        <v>0.00211764917937729</v>
       </c>
       <c r="G6">
         <v>0.00797963806751387</v>
@@ -1150,13 +1150,13 @@
         <v>0.00797963806751387</v>
       </c>
       <c r="J6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="K6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="M6">
         <v>0.00797963806751387</v>
@@ -1186,49 +1186,49 @@
         <v>0.00797963806751387</v>
       </c>
       <c r="V6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="W6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="Y6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="Z6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="AB6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="AC6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD6">
-        <v>0.005002015415800676</v>
+        <v>0.004988701160627227</v>
       </c>
       <c r="AE6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
       <c r="AF6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
       <c r="AH6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
       <c r="AI6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
       <c r="AK6">
         <v>0.00797963806751387</v>
@@ -1240,60 +1240,60 @@
         <v>0.00797963806751387</v>
       </c>
       <c r="AN6">
-        <v>0.005253540687798442</v>
+        <v>0.005945718487710539</v>
       </c>
       <c r="AO6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP6">
-        <v>0.005253540687798442</v>
+        <v>0.005945718487710539</v>
       </c>
       <c r="AQ6">
-        <v>0.005253540687798442</v>
+        <v>0.005945718487710539</v>
       </c>
       <c r="AR6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS6">
-        <v>0.005253540687798442</v>
+        <v>0.005945718487710539</v>
       </c>
       <c r="AT6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
       <c r="AU6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
       <c r="AW6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
       <c r="AX6">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY6">
-        <v>0.004020988077555074</v>
+        <v>0.00345019153248999</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.00179556533161163</v>
+        <v>0.003579756775059508</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.00179556533161163</v>
+        <v>0.003579756775059508</v>
       </c>
       <c r="D7">
-        <v>0.00179556533161163</v>
+        <v>0.003579756775059508</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.00179556533161163</v>
+        <v>0.003579756775059508</v>
       </c>
       <c r="G7">
         <v>0.005371047128878667</v>
@@ -1305,13 +1305,13 @@
         <v>0.005371047128878667</v>
       </c>
       <c r="J7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="M7">
         <v>0.005371047128878667</v>
@@ -1341,49 +1341,49 @@
         <v>0.005371047128878667</v>
       </c>
       <c r="V7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="W7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="Y7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="Z7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="AB7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.003065713775538204</v>
+        <v>0.003238919119006539</v>
       </c>
       <c r="AE7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
       <c r="AH7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
       <c r="AK7">
         <v>0.005371047128878667</v>
@@ -1395,60 +1395,60 @@
         <v>0.005371047128878667</v>
       </c>
       <c r="AN7">
-        <v>0.003489096590180395</v>
+        <v>0.003125306566988882</v>
       </c>
       <c r="AO7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.003489096590180395</v>
+        <v>0.003125306566988882</v>
       </c>
       <c r="AQ7">
-        <v>0.003489096590180395</v>
+        <v>0.003125306566988882</v>
       </c>
       <c r="AR7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.003489096590180395</v>
+        <v>0.003125306566988882</v>
       </c>
       <c r="AT7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
       <c r="AW7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.002925344336363591</v>
+        <v>0.003382532191177788</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.001466544116934519</v>
+        <v>0.001461899318125731</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.001466544116934519</v>
+        <v>0.001461899318125731</v>
       </c>
       <c r="D8">
-        <v>0.001466544116934519</v>
+        <v>0.001461899318125731</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.001466544116934519</v>
+        <v>0.001461899318125731</v>
       </c>
       <c r="G8">
         <v>0.002168617090675048</v>
@@ -1460,13 +1460,13 @@
         <v>0.002168617090675048</v>
       </c>
       <c r="J8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="M8">
         <v>0.002168617090675048</v>
@@ -1496,49 +1496,49 @@
         <v>0.002168617090675048</v>
       </c>
       <c r="V8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="W8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="Y8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="Z8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="AB8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.002060177720505365</v>
+        <v>0.002265933693025022</v>
       </c>
       <c r="AE8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
       <c r="AH8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
       <c r="AK8">
         <v>0.002168617090675048</v>
@@ -1550,60 +1550,60 @@
         <v>0.002168617090675048</v>
       </c>
       <c r="AN8">
-        <v>0.002258055588362314</v>
+        <v>0.002533945151324786</v>
       </c>
       <c r="AO8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP8">
-        <v>0.002258055588362314</v>
+        <v>0.002533945151324786</v>
       </c>
       <c r="AQ8">
-        <v>0.002258055588362314</v>
+        <v>0.002533945151324786</v>
       </c>
       <c r="AR8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002258055588362314</v>
+        <v>0.002533945151324786</v>
       </c>
       <c r="AT8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
       <c r="AW8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.001615403696625696</v>
+        <v>0.001614580524199471</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.001137523008674775</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="B9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.001137523008674775</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="D9">
-        <v>0.001137523008674775</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="E9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.001137523008674775</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="G9">
         <v>0.001645616507591864</v>
@@ -1615,13 +1615,13 @@
         <v>0.001645616507591864</v>
       </c>
       <c r="J9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="K9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="M9">
         <v>0.001645616507591864</v>
@@ -1651,49 +1651,49 @@
         <v>0.001645616507591864</v>
       </c>
       <c r="V9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="W9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="Y9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="Z9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="AB9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="AC9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.001139027750111053</v>
+        <v>0.0009142763819375917</v>
       </c>
       <c r="AE9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
       <c r="AH9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
       <c r="AK9">
         <v>0.001645616507591864</v>
@@ -1705,60 +1705,60 @@
         <v>0.001645616507591864</v>
       </c>
       <c r="AN9">
-        <v>0.001139529330589813</v>
+        <v>0.001140666220330917</v>
       </c>
       <c r="AO9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP9">
-        <v>0.001139529330589813</v>
+        <v>0.001140666220330917</v>
       </c>
       <c r="AQ9">
-        <v>0.001139529330589813</v>
+        <v>0.001140666220330917</v>
       </c>
       <c r="AR9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001139529330589813</v>
+        <v>0.001140666220330917</v>
       </c>
       <c r="AT9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
       <c r="AW9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.0009252817338288512</v>
+        <v>0.001244229571702852</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.02837565107795857</v>
+        <v>0.02919563830989572</v>
       </c>
       <c r="B10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.02837565107795857</v>
+        <v>0.02919563830989572</v>
       </c>
       <c r="D10">
-        <v>0.02837565107795857</v>
+        <v>0.02919563830989572</v>
       </c>
       <c r="E10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.02837565107795857</v>
+        <v>0.02919563830989572</v>
       </c>
       <c r="G10">
         <v>0.007176744350673809</v>
@@ -1770,13 +1770,13 @@
         <v>0.007176744350673809</v>
       </c>
       <c r="J10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="K10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="M10">
         <v>0.007176744350673809</v>
@@ -1806,49 +1806,49 @@
         <v>0.007176744350673809</v>
       </c>
       <c r="V10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="W10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="Y10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="Z10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="AB10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="AC10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.01823733023305132</v>
+        <v>0.01854423993040142</v>
       </c>
       <c r="AE10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
       <c r="AH10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
       <c r="AK10">
         <v>0.007176744350673809</v>
@@ -1860,40 +1860,40 @@
         <v>0.007176744350673809</v>
       </c>
       <c r="AN10">
-        <v>0.01485788995141557</v>
+        <v>0.01499377380390331</v>
       </c>
       <c r="AO10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP10">
-        <v>0.01485788995141557</v>
+        <v>0.01499377380390331</v>
       </c>
       <c r="AQ10">
-        <v>0.01485788995141557</v>
+        <v>0.01499377380390331</v>
       </c>
       <c r="AR10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.01485788995141557</v>
+        <v>0.01499377380390331</v>
       </c>
       <c r="AT10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
       <c r="AW10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.008777638535301927</v>
+        <v>0.008770730412966141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Halve the rate of stubble quality and quantity decay. Increase profit 14k
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.06363819708708202</v>
+        <v>0.06306780474039508</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.06363819708708202</v>
+        <v>0.06306780474039508</v>
       </c>
       <c r="D1">
-        <v>0.06363819708708202</v>
+        <v>0.06306780474039508</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.06363819708708202</v>
+        <v>0.06306780474039508</v>
       </c>
       <c r="G1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="H1">
-        <v>0.02645332309889065</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="I1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="J1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="M1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="N1">
-        <v>0.02645332309889065</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="O1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="P1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="Q1">
-        <v>0.02645332309889065</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="R1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="S1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="T1">
-        <v>0.02645332309889065</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="U1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="V1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="W1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="Y1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="Z1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="AB1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.05846248942234432</v>
+        <v>0.04926191676111156</v>
       </c>
       <c r="AE1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
       <c r="AH1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
       <c r="AK1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="AL1">
-        <v>0.02645332309889065</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="AM1">
-        <v>0.04452719281900871</v>
+        <v>0.03558111393175733</v>
       </c>
       <c r="AN1">
-        <v>0.05673725353409841</v>
+        <v>0.04465995410135038</v>
       </c>
       <c r="AO1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP1">
-        <v>0.05673725353409841</v>
+        <v>0.04465995410135038</v>
       </c>
       <c r="AQ1">
-        <v>0.05673725353409841</v>
+        <v>0.04465995410135038</v>
       </c>
       <c r="AR1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.05673725353409841</v>
+        <v>0.04465995410135038</v>
       </c>
       <c r="AT1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
       <c r="AW1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.03251997651482077</v>
+        <v>0.02849738243999362</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.01023604765218303</v>
+        <v>0.006714450648976265</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.01023604765218303</v>
+        <v>0.006714450648976265</v>
       </c>
       <c r="D2">
-        <v>0.01023604765218303</v>
+        <v>0.006714450648976265</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.01023604765218303</v>
+        <v>0.006714450648976265</v>
       </c>
       <c r="G2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="H2">
-        <v>0.355566172325769</v>
+        <v>0.2244740956086487</v>
       </c>
       <c r="I2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="J2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="M2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="N2">
-        <v>0.355566172325769</v>
+        <v>0.2244740956086487</v>
       </c>
       <c r="O2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="P2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="Q2">
-        <v>0.355566172325769</v>
+        <v>0.2244740956086487</v>
       </c>
       <c r="R2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="S2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="T2">
-        <v>0.355566172325769</v>
+        <v>0.2244740956086487</v>
       </c>
       <c r="U2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="V2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="W2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="Y2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="AB2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.008592710578368684</v>
+        <v>0.01016740849419035</v>
       </c>
       <c r="AE2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
       <c r="AH2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
       <c r="AK2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="AL2">
-        <v>0.355566172325769</v>
+        <v>0.2244740956086487</v>
       </c>
       <c r="AM2">
-        <v>0.01023589746068457</v>
+        <v>0.01253565421970539</v>
       </c>
       <c r="AN2">
-        <v>0.008044931553763901</v>
+        <v>0.01131839444259504</v>
       </c>
       <c r="AO2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.008044931553763901</v>
+        <v>0.01131839444259504</v>
       </c>
       <c r="AQ2">
-        <v>0.008044931553763901</v>
+        <v>0.01131839444259504</v>
       </c>
       <c r="AR2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.008044931553763901</v>
+        <v>0.01131839444259504</v>
       </c>
       <c r="AT2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
       <c r="AW2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.00718430115432968</v>
+        <v>0.00698792195454436</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.009273507682533707</v>
+        <v>0.009109237672534635</v>
       </c>
       <c r="B3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="C3">
-        <v>0.009273507682533707</v>
+        <v>0.009109237672534635</v>
       </c>
       <c r="D3">
-        <v>0.009273507682533707</v>
+        <v>0.009109237672534635</v>
       </c>
       <c r="E3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="F3">
-        <v>0.009273507682533707</v>
+        <v>0.009109237672534635</v>
       </c>
       <c r="G3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="H3">
-        <v>0.2919178348084053</v>
+        <v>0.3423722353179456</v>
       </c>
       <c r="I3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="J3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="K3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="L3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="M3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="N3">
-        <v>0.2919178348084053</v>
+        <v>0.3423722353179456</v>
       </c>
       <c r="O3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="P3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="Q3">
-        <v>0.2919178348084053</v>
+        <v>0.3423722353179456</v>
       </c>
       <c r="R3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="S3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="T3">
-        <v>0.2919178348084053</v>
+        <v>0.3423722353179456</v>
       </c>
       <c r="U3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="V3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="W3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="X3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="Y3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="Z3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AA3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="AB3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="AC3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AD3">
-        <v>0.008666288540442961</v>
+        <v>0.005867219464591533</v>
       </c>
       <c r="AE3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
       <c r="AF3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AG3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
       <c r="AH3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
       <c r="AI3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AJ3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
       <c r="AK3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="AL3">
-        <v>0.2919178348084053</v>
+        <v>0.3423722353179456</v>
       </c>
       <c r="AM3">
-        <v>0.01162448032571289</v>
+        <v>0.009093518520982672</v>
       </c>
       <c r="AN3">
-        <v>0.008463882159746045</v>
+        <v>0.004786546728610497</v>
       </c>
       <c r="AO3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AP3">
-        <v>0.008463882159746045</v>
+        <v>0.004786546728610497</v>
       </c>
       <c r="AQ3">
-        <v>0.008463882159746045</v>
+        <v>0.004786546728610497</v>
       </c>
       <c r="AR3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AS3">
-        <v>0.008463882159746045</v>
+        <v>0.004786546728610497</v>
       </c>
       <c r="AT3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
       <c r="AU3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AV3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
       <c r="AW3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
       <c r="AX3">
-        <v>0.6005669028436544</v>
+        <v>0.2668534846590581</v>
       </c>
       <c r="AY3">
-        <v>0.00559480427302851</v>
+        <v>0.007171566937359345</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.005534367540043079</v>
+        <v>0.005420519449361357</v>
       </c>
       <c r="B4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="C4">
-        <v>0.005534367540043079</v>
+        <v>0.005420519449361357</v>
       </c>
       <c r="D4">
-        <v>0.005534367540043079</v>
+        <v>0.005420519449361357</v>
       </c>
       <c r="E4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="F4">
-        <v>0.005534367540043079</v>
+        <v>0.005420519449361357</v>
       </c>
       <c r="G4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="H4">
-        <v>0.1596580675690371</v>
+        <v>0.1261746369158506</v>
       </c>
       <c r="I4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="J4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="K4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="L4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="M4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="N4">
-        <v>0.1596580675690371</v>
+        <v>0.1261746369158506</v>
       </c>
       <c r="O4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="P4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="Q4">
-        <v>0.1596580675690371</v>
+        <v>0.1261746369158506</v>
       </c>
       <c r="R4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="S4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="T4">
-        <v>0.1596580675690371</v>
+        <v>0.1261746369158506</v>
       </c>
       <c r="U4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="V4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="W4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="X4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="Y4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="Z4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AA4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="AB4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="AC4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AD4">
-        <v>0.008824762978372612</v>
+        <v>0.007877263386645909</v>
       </c>
       <c r="AE4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
       <c r="AF4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AG4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
       <c r="AH4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
       <c r="AI4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AJ4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
       <c r="AK4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="AL4">
-        <v>0.1596580675690371</v>
+        <v>0.1261746369158506</v>
       </c>
       <c r="AM4">
-        <v>0.01251778709856828</v>
+        <v>0.0102019374725316</v>
       </c>
       <c r="AN4">
-        <v>0.009921561457815788</v>
+        <v>0.008696178032407426</v>
       </c>
       <c r="AO4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AP4">
-        <v>0.009921561457815788</v>
+        <v>0.008696178032407426</v>
       </c>
       <c r="AQ4">
-        <v>0.009921561457815788</v>
+        <v>0.008696178032407426</v>
       </c>
       <c r="AR4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AS4">
-        <v>0.009921561457815788</v>
+        <v>0.008696178032407426</v>
       </c>
       <c r="AT4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
       <c r="AU4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AV4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
       <c r="AW4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
       <c r="AX4">
-        <v>0.2802132262183178</v>
+        <v>0.2781158972827227</v>
       </c>
       <c r="AY4">
-        <v>0.005738609312496817</v>
+        <v>0.005590661190567116</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.004884832742452431</v>
+        <v>0.004793462679244488</v>
       </c>
       <c r="B5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="C5">
-        <v>0.004884832742452431</v>
+        <v>0.004793462679244488</v>
       </c>
       <c r="D5">
-        <v>0.004884832742452431</v>
+        <v>0.004793462679244488</v>
       </c>
       <c r="E5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="F5">
-        <v>0.004884832742452431</v>
+        <v>0.004793462679244488</v>
       </c>
       <c r="G5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="H5">
-        <v>0.1104532511443694</v>
+        <v>0.1156952150243516</v>
       </c>
       <c r="I5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="J5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="K5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="L5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="M5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="N5">
-        <v>0.1104532511443694</v>
+        <v>0.1156952150243516</v>
       </c>
       <c r="O5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="P5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="Q5">
-        <v>0.1104532511443694</v>
+        <v>0.1156952150243516</v>
       </c>
       <c r="R5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="S5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="T5">
-        <v>0.1104532511443694</v>
+        <v>0.1156952150243516</v>
       </c>
       <c r="U5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="V5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="W5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="X5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="Y5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="Z5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AA5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="AB5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="AC5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AD5">
-        <v>0.006844333466138565</v>
+        <v>0.008303999007486009</v>
       </c>
       <c r="AE5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
       <c r="AF5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AG5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
       <c r="AH5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
       <c r="AI5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AJ5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
       <c r="AK5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="AL5">
-        <v>0.1104532511443694</v>
+        <v>0.1156952150243516</v>
       </c>
       <c r="AM5">
-        <v>0.01106770690415737</v>
+        <v>0.01264891185818256</v>
       </c>
       <c r="AN5">
-        <v>0.007497500374033943</v>
+        <v>0.009474177783566516</v>
       </c>
       <c r="AO5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AP5">
-        <v>0.007497500374033943</v>
+        <v>0.009474177783566516</v>
       </c>
       <c r="AQ5">
-        <v>0.007497500374033943</v>
+        <v>0.009474177783566516</v>
       </c>
       <c r="AR5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AS5">
-        <v>0.007497500374033943</v>
+        <v>0.009474177783566516</v>
       </c>
       <c r="AT5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
       <c r="AU5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AV5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
       <c r="AW5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
       <c r="AX5">
-        <v>0.0001146235521235521</v>
+        <v>0.1443880420814829</v>
       </c>
       <c r="AY5">
-        <v>0.00584237822529203</v>
+        <v>0.005110596849404262</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.00211764917937729</v>
+        <v>0.004166405517841728</v>
       </c>
       <c r="B6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="C6">
-        <v>0.00211764917937729</v>
+        <v>0.004166405517841728</v>
       </c>
       <c r="D6">
-        <v>0.00211764917937729</v>
+        <v>0.004166405517841728</v>
       </c>
       <c r="E6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="F6">
-        <v>0.00211764917937729</v>
+        <v>0.004166405517841728</v>
       </c>
       <c r="G6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="H6">
-        <v>0.0344086061921234</v>
+        <v>0.1350192605204197</v>
       </c>
       <c r="I6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="J6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="K6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="L6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="M6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="N6">
-        <v>0.0344086061921234</v>
+        <v>0.1350192605204197</v>
       </c>
       <c r="O6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="P6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="Q6">
-        <v>0.0344086061921234</v>
+        <v>0.1350192605204197</v>
       </c>
       <c r="R6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="S6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="T6">
-        <v>0.0344086061921234</v>
+        <v>0.1350192605204197</v>
       </c>
       <c r="U6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="V6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="W6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="X6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="Y6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="Z6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AA6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="AB6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="AC6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AD6">
-        <v>0.004988701160627227</v>
+        <v>0.005528819024960711</v>
       </c>
       <c r="AE6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
       <c r="AF6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AG6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
       <c r="AH6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
       <c r="AI6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AJ6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
       <c r="AK6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="AL6">
-        <v>0.0344086061921234</v>
+        <v>0.1350192605204197</v>
       </c>
       <c r="AM6">
-        <v>0.00797963806751387</v>
+        <v>0.007855676172478693</v>
       </c>
       <c r="AN6">
-        <v>0.005945718487710539</v>
+        <v>0.00598295686066704</v>
       </c>
       <c r="AO6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AP6">
-        <v>0.005945718487710539</v>
+        <v>0.00598295686066704</v>
       </c>
       <c r="AQ6">
-        <v>0.005945718487710539</v>
+        <v>0.00598295686066704</v>
       </c>
       <c r="AR6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AS6">
-        <v>0.005945718487710539</v>
+        <v>0.00598295686066704</v>
       </c>
       <c r="AT6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
       <c r="AU6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AV6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
       <c r="AW6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
       <c r="AX6">
-        <v>0.0001146235521235521</v>
+        <v>0.08512536239498097</v>
       </c>
       <c r="AY6">
-        <v>0.00345019153248999</v>
+        <v>0.004524209450964819</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.003579756775059508</v>
+        <v>0.001757814719276604</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.003579756775059508</v>
+        <v>0.001757814719276604</v>
       </c>
       <c r="D7">
-        <v>0.003579756775059508</v>
+        <v>0.001757814719276604</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.003579756775059508</v>
+        <v>0.001757814719276604</v>
       </c>
       <c r="G7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="H7">
-        <v>0.01953017441316452</v>
+        <v>0.0316895400158389</v>
       </c>
       <c r="I7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="J7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="M7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="N7">
-        <v>0.01953017441316452</v>
+        <v>0.0316895400158389</v>
       </c>
       <c r="O7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="P7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="Q7">
-        <v>0.01953017441316452</v>
+        <v>0.0316895400158389</v>
       </c>
       <c r="R7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="S7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="T7">
-        <v>0.01953017441316452</v>
+        <v>0.0316895400158389</v>
       </c>
       <c r="U7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="V7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="W7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="Y7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="Z7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="AB7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.003238919119006539</v>
+        <v>0.004231664473843333</v>
       </c>
       <c r="AE7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
       <c r="AH7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
       <c r="AK7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="AL7">
-        <v>0.01953017441316452</v>
+        <v>0.0316895400158389</v>
       </c>
       <c r="AM7">
-        <v>0.005371047128878667</v>
+        <v>0.005324837346308348</v>
       </c>
       <c r="AN7">
-        <v>0.003125306566988882</v>
+        <v>0.00505628105869891</v>
       </c>
       <c r="AO7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.003125306566988882</v>
+        <v>0.00505628105869891</v>
       </c>
       <c r="AQ7">
-        <v>0.003125306566988882</v>
+        <v>0.00505628105869891</v>
       </c>
       <c r="AR7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.003125306566988882</v>
+        <v>0.00505628105869891</v>
       </c>
       <c r="AT7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
       <c r="AW7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.003382532191177788</v>
+        <v>0.002396989158289127</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.001461899318125731</v>
+        <v>0.001444689175807819</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.001461899318125731</v>
+        <v>0.001444689175807819</v>
       </c>
       <c r="D8">
-        <v>0.001461899318125731</v>
+        <v>0.001444689175807819</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.001461899318125731</v>
+        <v>0.001444689175807819</v>
       </c>
       <c r="G8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="H8">
-        <v>0.001749940937478829</v>
+        <v>0.01972328970670128</v>
       </c>
       <c r="I8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="J8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="M8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="N8">
-        <v>0.001749940937478829</v>
+        <v>0.01972328970670128</v>
       </c>
       <c r="O8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="P8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="Q8">
-        <v>0.001749940937478829</v>
+        <v>0.01972328970670128</v>
       </c>
       <c r="R8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="S8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="T8">
-        <v>0.001749940937478829</v>
+        <v>0.01972328970670128</v>
       </c>
       <c r="U8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="V8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="W8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="Y8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="Z8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="AB8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.002265933693025022</v>
+        <v>0.002487410389947549</v>
       </c>
       <c r="AE8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
       <c r="AH8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
       <c r="AK8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="AL8">
-        <v>0.001749940937478829</v>
+        <v>0.01972328970670128</v>
       </c>
       <c r="AM8">
-        <v>0.002168617090675048</v>
+        <v>0.004358992832131712</v>
       </c>
       <c r="AN8">
-        <v>0.002533945151324786</v>
+        <v>0.002834984127994126</v>
       </c>
       <c r="AO8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP8">
-        <v>0.002533945151324786</v>
+        <v>0.002834984127994126</v>
       </c>
       <c r="AQ8">
-        <v>0.002533945151324786</v>
+        <v>0.002834984127994126</v>
       </c>
       <c r="AR8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002533945151324786</v>
+        <v>0.002834984127994126</v>
       </c>
       <c r="AT8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
       <c r="AW8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.001614580524199471</v>
+        <v>0.00239479929688068</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.000235106866757617</v>
+        <v>0.001131563533137037</v>
       </c>
       <c r="B9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.000235106866757617</v>
+        <v>0.001131563533137037</v>
       </c>
       <c r="D9">
-        <v>0.000235106866757617</v>
+        <v>0.001131563533137037</v>
       </c>
       <c r="E9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.000235106866757617</v>
+        <v>0.001131563533137037</v>
       </c>
       <c r="G9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="H9">
-        <v>0.000131314755380893</v>
+        <v>0.004556281085100681</v>
       </c>
       <c r="I9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="J9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="K9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="M9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="N9">
-        <v>0.000131314755380893</v>
+        <v>0.004556281085100681</v>
       </c>
       <c r="O9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="P9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="Q9">
-        <v>0.000131314755380893</v>
+        <v>0.004556281085100681</v>
       </c>
       <c r="R9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="S9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="T9">
-        <v>0.000131314755380893</v>
+        <v>0.004556281085100681</v>
       </c>
       <c r="U9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="V9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="W9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="Y9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="Z9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="AB9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="AC9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.0009142763819375917</v>
+        <v>0.001459289167070384</v>
       </c>
       <c r="AE9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
       <c r="AH9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
       <c r="AK9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="AL9">
-        <v>0.000131314755380893</v>
+        <v>0.004556281085100681</v>
       </c>
       <c r="AM9">
-        <v>0.001645616507591864</v>
+        <v>0.001693993878494935</v>
       </c>
       <c r="AN9">
-        <v>0.001140666220330917</v>
+        <v>0.001568531045048166</v>
       </c>
       <c r="AO9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP9">
-        <v>0.001140666220330917</v>
+        <v>0.001568531045048166</v>
       </c>
       <c r="AQ9">
-        <v>0.001140666220330917</v>
+        <v>0.001568531045048166</v>
       </c>
       <c r="AR9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001140666220330917</v>
+        <v>0.001568531045048166</v>
       </c>
       <c r="AT9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
       <c r="AW9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.001244229571702852</v>
+        <v>0.001262150404563678</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.02919563830989572</v>
+        <v>0.03050653266836716</v>
       </c>
       <c r="B10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.02919563830989572</v>
+        <v>0.03050653266836716</v>
       </c>
       <c r="D10">
-        <v>0.02919563830989572</v>
+        <v>0.03050653266836716</v>
       </c>
       <c r="E10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.02919563830989572</v>
+        <v>0.03050653266836716</v>
       </c>
       <c r="G10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="H10">
-        <v>0.000131314755380893</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="I10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="J10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="K10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="M10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="N10">
-        <v>0.000131314755380893</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="O10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="P10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="Q10">
-        <v>0.000131314755380893</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="R10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="S10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="T10">
-        <v>0.000131314755380893</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="U10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="V10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="W10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="Y10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="Z10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="AB10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="AC10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.01854423993040142</v>
+        <v>0.02100146363922594</v>
       </c>
       <c r="AE10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
       <c r="AH10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
       <c r="AK10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="AL10">
-        <v>0.000131314755380893</v>
+        <v>0.0001477229025714423</v>
       </c>
       <c r="AM10">
-        <v>0.007176744350673809</v>
+        <v>0.008385022273839802</v>
       </c>
       <c r="AN10">
-        <v>0.01499377380390331</v>
+        <v>0.01783310729617886</v>
       </c>
       <c r="AO10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP10">
-        <v>0.01499377380390331</v>
+        <v>0.01783310729617886</v>
       </c>
       <c r="AQ10">
-        <v>0.01499377380390331</v>
+        <v>0.01783310729617886</v>
       </c>
       <c r="AR10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.01499377380390331</v>
+        <v>0.01783310729617886</v>
       </c>
       <c r="AT10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
       <c r="AW10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.008770730412966141</v>
+        <v>0.009458563785318296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sup to eds trials
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,22 +348,22 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.06306780474039508</v>
+        <v>0.04665226629368208</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.06306780474039508</v>
+        <v>0.04665226629368208</v>
       </c>
       <c r="D1">
-        <v>0.06306780474039508</v>
+        <v>0.04665226629368208</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.06306780474039508</v>
+        <v>0.04665226629368208</v>
       </c>
       <c r="G1">
         <v>0.03558111393175733</v>
@@ -375,13 +375,13 @@
         <v>0.03558111393175733</v>
       </c>
       <c r="J1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="M1">
         <v>0.03558111393175733</v>
@@ -411,49 +411,49 @@
         <v>0.03558111393175733</v>
       </c>
       <c r="V1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="W1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="Y1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="Z1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="AB1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.04926191676111156</v>
+        <v>0.03735598459240319</v>
       </c>
       <c r="AE1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
       <c r="AH1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
       <c r="AK1">
         <v>0.03558111393175733</v>
@@ -465,60 +465,60 @@
         <v>0.03558111393175733</v>
       </c>
       <c r="AN1">
-        <v>0.04465995410135038</v>
+        <v>0.03425722402531023</v>
       </c>
       <c r="AO1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP1">
-        <v>0.04465995410135038</v>
+        <v>0.03425722402531023</v>
       </c>
       <c r="AQ1">
-        <v>0.04465995410135038</v>
+        <v>0.03425722402531023</v>
       </c>
       <c r="AR1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.04465995410135038</v>
+        <v>0.03425722402531023</v>
       </c>
       <c r="AT1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
       <c r="AW1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.02849738243999362</v>
+        <v>0.02110766726064944</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.006714450648976265</v>
+        <v>0.002610490556715228</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.006714450648976265</v>
+        <v>0.002610490556715228</v>
       </c>
       <c r="D2">
-        <v>0.006714450648976265</v>
+        <v>0.002610490556715228</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.006714450648976265</v>
+        <v>0.002610490556715228</v>
       </c>
       <c r="G2">
         <v>0.01253565421970539</v>
@@ -530,13 +530,13 @@
         <v>0.01253565421970539</v>
       </c>
       <c r="J2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="M2">
         <v>0.01253565421970539</v>
@@ -566,49 +566,49 @@
         <v>0.01253565421970539</v>
       </c>
       <c r="V2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="W2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="Y2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="AB2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.01016740849419035</v>
+        <v>0.006482358909336725</v>
       </c>
       <c r="AE2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
       <c r="AH2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
       <c r="AK2">
         <v>0.01253565421970539</v>
@@ -620,60 +620,60 @@
         <v>0.01253565421970539</v>
       </c>
       <c r="AN2">
-        <v>0.01131839444259504</v>
+        <v>0.007772981693543889</v>
       </c>
       <c r="AO2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.01131839444259504</v>
+        <v>0.007772981693543889</v>
       </c>
       <c r="AQ2">
-        <v>0.01131839444259504</v>
+        <v>0.007772981693543889</v>
       </c>
       <c r="AR2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.01131839444259504</v>
+        <v>0.007772981693543889</v>
       </c>
       <c r="AT2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
       <c r="AW2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.00698792195454436</v>
+        <v>0.004332799637236224</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.009109237672534635</v>
+        <v>0.004731886036200379</v>
       </c>
       <c r="B3">
         <v>0.2668534846590581</v>
       </c>
       <c r="C3">
-        <v>0.009109237672534635</v>
+        <v>0.004731886036200379</v>
       </c>
       <c r="D3">
-        <v>0.009109237672534635</v>
+        <v>0.004731886036200379</v>
       </c>
       <c r="E3">
         <v>0.2668534846590581</v>
       </c>
       <c r="F3">
-        <v>0.009109237672534635</v>
+        <v>0.004731886036200379</v>
       </c>
       <c r="G3">
         <v>0.009093518520982672</v>
@@ -685,13 +685,13 @@
         <v>0.009093518520982672</v>
       </c>
       <c r="J3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="K3">
         <v>0.2668534846590581</v>
       </c>
       <c r="L3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="M3">
         <v>0.009093518520982672</v>
@@ -721,49 +721,49 @@
         <v>0.009093518520982672</v>
       </c>
       <c r="V3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="W3">
         <v>0.2668534846590581</v>
       </c>
       <c r="X3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="Y3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="Z3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AA3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="AB3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="AC3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AD3">
-        <v>0.005867219464591533</v>
+        <v>0.004650448319821364</v>
       </c>
       <c r="AE3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
       <c r="AF3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AG3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
       <c r="AH3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
       <c r="AI3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AJ3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
       <c r="AK3">
         <v>0.009093518520982672</v>
@@ -775,60 +775,60 @@
         <v>0.009093518520982672</v>
       </c>
       <c r="AN3">
-        <v>0.004786546728610497</v>
+        <v>0.004623302414361691</v>
       </c>
       <c r="AO3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AP3">
-        <v>0.004786546728610497</v>
+        <v>0.004623302414361691</v>
       </c>
       <c r="AQ3">
-        <v>0.004786546728610497</v>
+        <v>0.004623302414361691</v>
       </c>
       <c r="AR3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AS3">
-        <v>0.004786546728610497</v>
+        <v>0.004623302414361691</v>
       </c>
       <c r="AT3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
       <c r="AU3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AV3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
       <c r="AW3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
       <c r="AX3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AY3">
-        <v>0.007171566937359345</v>
+        <v>0.003922127044429769</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.005420519449361357</v>
+        <v>0.004242790958970301</v>
       </c>
       <c r="B4">
         <v>0.2781158972827227</v>
       </c>
       <c r="C4">
-        <v>0.005420519449361357</v>
+        <v>0.004242790958970301</v>
       </c>
       <c r="D4">
-        <v>0.005420519449361357</v>
+        <v>0.004242790958970301</v>
       </c>
       <c r="E4">
         <v>0.2781158972827227</v>
       </c>
       <c r="F4">
-        <v>0.005420519449361357</v>
+        <v>0.004242790958970301</v>
       </c>
       <c r="G4">
         <v>0.0102019374725316</v>
@@ -840,13 +840,13 @@
         <v>0.0102019374725316</v>
       </c>
       <c r="J4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="K4">
         <v>0.2781158972827227</v>
       </c>
       <c r="L4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="M4">
         <v>0.0102019374725316</v>
@@ -876,49 +876,49 @@
         <v>0.0102019374725316</v>
       </c>
       <c r="V4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="W4">
         <v>0.2781158972827227</v>
       </c>
       <c r="X4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="Y4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="Z4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AA4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="AB4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="AC4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AD4">
-        <v>0.007877263386645909</v>
+        <v>0.004526771924218011</v>
       </c>
       <c r="AE4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
       <c r="AF4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AG4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
       <c r="AH4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
       <c r="AI4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AJ4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
       <c r="AK4">
         <v>0.0102019374725316</v>
@@ -930,60 +930,60 @@
         <v>0.0102019374725316</v>
       </c>
       <c r="AN4">
-        <v>0.008696178032407426</v>
+        <v>0.004621432245967247</v>
       </c>
       <c r="AO4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AP4">
-        <v>0.008696178032407426</v>
+        <v>0.004621432245967247</v>
       </c>
       <c r="AQ4">
-        <v>0.008696178032407426</v>
+        <v>0.004621432245967247</v>
       </c>
       <c r="AR4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AS4">
-        <v>0.008696178032407426</v>
+        <v>0.004621432245967247</v>
       </c>
       <c r="AT4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
       <c r="AU4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AV4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
       <c r="AW4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
       <c r="AX4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AY4">
-        <v>0.005590661190567116</v>
+        <v>0.002864940877222379</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.004793462679244488</v>
+        <v>0.003700807392733978</v>
       </c>
       <c r="B5">
         <v>0.1443880420814829</v>
       </c>
       <c r="C5">
-        <v>0.004793462679244488</v>
+        <v>0.003700807392733978</v>
       </c>
       <c r="D5">
-        <v>0.004793462679244488</v>
+        <v>0.003700807392733978</v>
       </c>
       <c r="E5">
         <v>0.1443880420814829</v>
       </c>
       <c r="F5">
-        <v>0.004793462679244488</v>
+        <v>0.003700807392733978</v>
       </c>
       <c r="G5">
         <v>0.01264891185818256</v>
@@ -995,13 +995,13 @@
         <v>0.01264891185818256</v>
       </c>
       <c r="J5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="K5">
         <v>0.1443880420814829</v>
       </c>
       <c r="L5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="M5">
         <v>0.01264891185818256</v>
@@ -1031,49 +1031,49 @@
         <v>0.01264891185818256</v>
       </c>
       <c r="V5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="W5">
         <v>0.1443880420814829</v>
       </c>
       <c r="X5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="Y5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="Z5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AA5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="AB5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="AC5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AD5">
-        <v>0.008303999007486009</v>
+        <v>0.004770686745860708</v>
       </c>
       <c r="AE5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
       <c r="AF5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AG5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
       <c r="AH5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
       <c r="AI5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AJ5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
       <c r="AK5">
         <v>0.01264891185818256</v>
@@ -1085,60 +1085,60 @@
         <v>0.01264891185818256</v>
       </c>
       <c r="AN5">
-        <v>0.009474177783566516</v>
+        <v>0.005127313196902951</v>
       </c>
       <c r="AO5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AP5">
-        <v>0.009474177783566516</v>
+        <v>0.005127313196902951</v>
       </c>
       <c r="AQ5">
-        <v>0.009474177783566516</v>
+        <v>0.005127313196902951</v>
       </c>
       <c r="AR5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AS5">
-        <v>0.009474177783566516</v>
+        <v>0.005127313196902951</v>
       </c>
       <c r="AT5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
       <c r="AU5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AV5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
       <c r="AW5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
       <c r="AX5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AY5">
-        <v>0.005110596849404262</v>
+        <v>0.00288359076064733</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.004166405517841728</v>
+        <v>0.001608342994589428</v>
       </c>
       <c r="B6">
         <v>0.08512536239498097</v>
       </c>
       <c r="C6">
-        <v>0.004166405517841728</v>
+        <v>0.001608342994589428</v>
       </c>
       <c r="D6">
-        <v>0.004166405517841728</v>
+        <v>0.001608342994589428</v>
       </c>
       <c r="E6">
         <v>0.08512536239498097</v>
       </c>
       <c r="F6">
-        <v>0.004166405517841728</v>
+        <v>0.001608342994589428</v>
       </c>
       <c r="G6">
         <v>0.007855676172478693</v>
@@ -1150,13 +1150,13 @@
         <v>0.007855676172478693</v>
       </c>
       <c r="J6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="K6">
         <v>0.08512536239498097</v>
       </c>
       <c r="L6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="M6">
         <v>0.007855676172478693</v>
@@ -1186,49 +1186,49 @@
         <v>0.007855676172478693</v>
       </c>
       <c r="V6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="W6">
         <v>0.08512536239498097</v>
       </c>
       <c r="X6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="Y6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="Z6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AA6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="AB6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="AC6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AD6">
-        <v>0.005528819024960711</v>
+        <v>0.003984875587610923</v>
       </c>
       <c r="AE6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
       <c r="AF6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AG6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
       <c r="AH6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
       <c r="AI6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AJ6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
       <c r="AK6">
         <v>0.007855676172478693</v>
@@ -1240,60 +1240,60 @@
         <v>0.007855676172478693</v>
       </c>
       <c r="AN6">
-        <v>0.00598295686066704</v>
+        <v>0.004777053118618087</v>
       </c>
       <c r="AO6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AP6">
-        <v>0.00598295686066704</v>
+        <v>0.004777053118618087</v>
       </c>
       <c r="AQ6">
-        <v>0.00598295686066704</v>
+        <v>0.004777053118618087</v>
       </c>
       <c r="AR6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AS6">
-        <v>0.00598295686066704</v>
+        <v>0.004777053118618087</v>
       </c>
       <c r="AT6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
       <c r="AU6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AV6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
       <c r="AW6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
       <c r="AX6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AY6">
-        <v>0.004524209450964819</v>
+        <v>0.002204241333530696</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.001757814719276604</v>
+        <v>0.001366282390633341</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.001757814719276604</v>
+        <v>0.001366282390633341</v>
       </c>
       <c r="D7">
-        <v>0.001757814719276604</v>
+        <v>0.001366282390633341</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.001757814719276604</v>
+        <v>0.001366282390633341</v>
       </c>
       <c r="G7">
         <v>0.005324837346308348</v>
@@ -1305,13 +1305,13 @@
         <v>0.005324837346308348</v>
       </c>
       <c r="J7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="M7">
         <v>0.005324837346308348</v>
@@ -1341,49 +1341,49 @@
         <v>0.005324837346308348</v>
       </c>
       <c r="V7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="W7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="Y7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="Z7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="AB7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.004231664473843333</v>
+        <v>0.002587467028897387</v>
       </c>
       <c r="AE7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
       <c r="AH7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
       <c r="AK7">
         <v>0.005324837346308348</v>
@@ -1395,60 +1395,60 @@
         <v>0.005324837346308348</v>
       </c>
       <c r="AN7">
-        <v>0.00505628105869891</v>
+        <v>0.002994528574985402</v>
       </c>
       <c r="AO7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.00505628105869891</v>
+        <v>0.002994528574985402</v>
       </c>
       <c r="AQ7">
-        <v>0.00505628105869891</v>
+        <v>0.002994528574985402</v>
       </c>
       <c r="AR7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.00505628105869891</v>
+        <v>0.002994528574985402</v>
       </c>
       <c r="AT7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
       <c r="AW7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.002396989158289127</v>
+        <v>0.002313762597583816</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.001444689175807819</v>
+        <v>0.001124221786677254</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.001444689175807819</v>
+        <v>0.001124221786677254</v>
       </c>
       <c r="D8">
-        <v>0.001444689175807819</v>
+        <v>0.001124221786677254</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.001444689175807819</v>
+        <v>0.001124221786677254</v>
       </c>
       <c r="G8">
         <v>0.004358992832131712</v>
@@ -1460,13 +1460,13 @@
         <v>0.004358992832131712</v>
       </c>
       <c r="J8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="M8">
         <v>0.004358992832131712</v>
@@ -1496,49 +1496,49 @@
         <v>0.004358992832131712</v>
       </c>
       <c r="V8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="W8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="Y8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="Z8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="AB8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.002487410389947549</v>
+        <v>0.002115154515154888</v>
       </c>
       <c r="AE8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
       <c r="AH8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
       <c r="AK8">
         <v>0.004358992832131712</v>
@@ -1550,60 +1550,60 @@
         <v>0.004358992832131712</v>
       </c>
       <c r="AN8">
-        <v>0.002834984127994126</v>
+        <v>0.002445465424647433</v>
       </c>
       <c r="AO8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP8">
-        <v>0.002834984127994126</v>
+        <v>0.002445465424647433</v>
       </c>
       <c r="AQ8">
-        <v>0.002834984127994126</v>
+        <v>0.002445465424647433</v>
       </c>
       <c r="AR8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002834984127994126</v>
+        <v>0.002445465424647433</v>
       </c>
       <c r="AT8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
       <c r="AW8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.00239479929688068</v>
+        <v>0.001272307867092222</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.001131563533137037</v>
+        <v>0.0008821610848996937</v>
       </c>
       <c r="B9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.001131563533137037</v>
+        <v>0.0008821610848996937</v>
       </c>
       <c r="D9">
-        <v>0.001131563533137037</v>
+        <v>0.0008821610848996937</v>
       </c>
       <c r="E9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.001131563533137037</v>
+        <v>0.0008821610848996937</v>
       </c>
       <c r="G9">
         <v>0.001693993878494935</v>
@@ -1615,13 +1615,13 @@
         <v>0.001693993878494935</v>
       </c>
       <c r="J9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="K9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="M9">
         <v>0.001693993878494935</v>
@@ -1651,49 +1651,49 @@
         <v>0.001693993878494935</v>
       </c>
       <c r="V9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="W9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="Y9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="Z9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="AB9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="AC9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.001459289167070384</v>
+        <v>0.001235512084227121</v>
       </c>
       <c r="AE9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
       <c r="AH9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
       <c r="AK9">
         <v>0.001693993878494935</v>
@@ -1705,60 +1705,60 @@
         <v>0.001693993878494935</v>
       </c>
       <c r="AN9">
-        <v>0.001568531045048166</v>
+        <v>0.001353295750669597</v>
       </c>
       <c r="AO9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP9">
-        <v>0.001568531045048166</v>
+        <v>0.001353295750669597</v>
       </c>
       <c r="AQ9">
-        <v>0.001568531045048166</v>
+        <v>0.001353295750669597</v>
       </c>
       <c r="AR9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001568531045048166</v>
+        <v>0.001353295750669597</v>
       </c>
       <c r="AT9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
       <c r="AW9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.001262150404563678</v>
+        <v>0.0007733584508437914</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.03050653266836716</v>
+        <v>0.02599160768826621</v>
       </c>
       <c r="B10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.03050653266836716</v>
+        <v>0.02599160768826621</v>
       </c>
       <c r="D10">
-        <v>0.03050653266836716</v>
+        <v>0.02599160768826621</v>
       </c>
       <c r="E10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.03050653266836716</v>
+        <v>0.02599160768826621</v>
       </c>
       <c r="G10">
         <v>0.008385022273839802</v>
@@ -1770,13 +1770,13 @@
         <v>0.008385022273839802</v>
       </c>
       <c r="J10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="K10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="M10">
         <v>0.008385022273839802</v>
@@ -1806,49 +1806,49 @@
         <v>0.008385022273839802</v>
       </c>
       <c r="V10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="W10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="Y10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="Z10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="AB10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="AC10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.02100146363922594</v>
+        <v>0.02078459270982999</v>
       </c>
       <c r="AE10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
       <c r="AH10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
       <c r="AK10">
         <v>0.008385022273839802</v>
@@ -1860,40 +1860,40 @@
         <v>0.008385022273839802</v>
       </c>
       <c r="AN10">
-        <v>0.01783310729617886</v>
+        <v>0.01904892105035125</v>
       </c>
       <c r="AO10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP10">
-        <v>0.01783310729617886</v>
+        <v>0.01904892105035125</v>
       </c>
       <c r="AQ10">
-        <v>0.01783310729617886</v>
+        <v>0.01904892105035125</v>
       </c>
       <c r="AR10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.01783310729617886</v>
+        <v>0.01904892105035125</v>
       </c>
       <c r="AT10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
       <c r="AW10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.009458563785318296</v>
+        <v>0.01091272794100258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update a,b,c coefficients for the CropResidue trials including scaling for EBG. Reduced profit by $2000
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.04665226629368208</v>
+        <v>0.04883906362401351</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.04665226629368208</v>
+        <v>0.04883906362401351</v>
       </c>
       <c r="D1">
-        <v>0.04665226629368208</v>
+        <v>0.04883906362401351</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.04665226629368208</v>
+        <v>0.04883906362401351</v>
       </c>
       <c r="G1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="H1">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="I1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="J1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="M1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="N1">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="O1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="P1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="Q1">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="R1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="S1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="T1">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="U1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="V1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="W1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="Y1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="Z1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="AB1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.03735598459240319</v>
+        <v>0.03383218409982959</v>
       </c>
       <c r="AE1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
       <c r="AH1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
       <c r="AK1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="AL1">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="AM1">
-        <v>0.03558111393175733</v>
+        <v>0.0276819434970707</v>
       </c>
       <c r="AN1">
-        <v>0.03425722402531023</v>
+        <v>0.02882989092510162</v>
       </c>
       <c r="AO1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP1">
-        <v>0.03425722402531023</v>
+        <v>0.02882989092510162</v>
       </c>
       <c r="AQ1">
-        <v>0.03425722402531023</v>
+        <v>0.02882989092510162</v>
       </c>
       <c r="AR1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.03425722402531023</v>
+        <v>0.02882989092510162</v>
       </c>
       <c r="AT1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
       <c r="AW1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.02110766726064944</v>
+        <v>0.01387135483210843</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.002610490556715228</v>
+        <v>0.006711500336291474</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.002610490556715228</v>
+        <v>0.006711500336291474</v>
       </c>
       <c r="D2">
-        <v>0.002610490556715228</v>
+        <v>0.006711500336291474</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.002610490556715228</v>
+        <v>0.006711500336291474</v>
       </c>
       <c r="G2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="H2">
-        <v>0.2244740956086487</v>
+        <v>0.1343675673028482</v>
       </c>
       <c r="I2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="J2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="M2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="N2">
-        <v>0.2244740956086487</v>
+        <v>0.1343675673028482</v>
       </c>
       <c r="O2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="P2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="Q2">
-        <v>0.2244740956086487</v>
+        <v>0.1343675673028482</v>
       </c>
       <c r="R2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="S2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="T2">
-        <v>0.2244740956086487</v>
+        <v>0.1343675673028482</v>
       </c>
       <c r="U2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="V2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="W2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="Y2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="AB2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.006482358909336725</v>
+        <v>0.007523242975825024</v>
       </c>
       <c r="AE2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
       <c r="AH2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
       <c r="AK2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="AL2">
-        <v>0.2244740956086487</v>
+        <v>0.1343675673028482</v>
       </c>
       <c r="AM2">
-        <v>0.01253565421970539</v>
+        <v>0.01522376636419349</v>
       </c>
       <c r="AN2">
-        <v>0.007772981693543889</v>
+        <v>0.007793823855669541</v>
       </c>
       <c r="AO2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.007772981693543889</v>
+        <v>0.007793823855669541</v>
       </c>
       <c r="AQ2">
-        <v>0.007772981693543889</v>
+        <v>0.007793823855669541</v>
       </c>
       <c r="AR2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.007772981693543889</v>
+        <v>0.007793823855669541</v>
       </c>
       <c r="AT2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
       <c r="AW2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.004332799637236224</v>
+        <v>0.007860302061988761</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.004731886036200379</v>
+        <v>0.006015769247113818</v>
       </c>
       <c r="B3">
         <v>0.2668534846590581</v>
       </c>
       <c r="C3">
-        <v>0.004731886036200379</v>
+        <v>0.006015769247113818</v>
       </c>
       <c r="D3">
-        <v>0.004731886036200379</v>
+        <v>0.006015769247113818</v>
       </c>
       <c r="E3">
         <v>0.2668534846590581</v>
       </c>
       <c r="F3">
-        <v>0.004731886036200379</v>
+        <v>0.006015769247113818</v>
       </c>
       <c r="G3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="H3">
-        <v>0.3423722353179456</v>
+        <v>0.341024247652797</v>
       </c>
       <c r="I3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="J3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="K3">
         <v>0.2668534846590581</v>
       </c>
       <c r="L3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="M3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="N3">
-        <v>0.3423722353179456</v>
+        <v>0.341024247652797</v>
       </c>
       <c r="O3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="P3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="Q3">
-        <v>0.3423722353179456</v>
+        <v>0.341024247652797</v>
       </c>
       <c r="R3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="S3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="T3">
-        <v>0.3423722353179456</v>
+        <v>0.341024247652797</v>
       </c>
       <c r="U3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="V3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="W3">
         <v>0.2668534846590581</v>
       </c>
       <c r="X3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="Y3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="Z3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AA3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="AB3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="AC3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AD3">
-        <v>0.004650448319821364</v>
+        <v>0.00680289948498498</v>
       </c>
       <c r="AE3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
       <c r="AF3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AG3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
       <c r="AH3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
       <c r="AI3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AJ3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
       <c r="AK3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="AL3">
-        <v>0.3423722353179456</v>
+        <v>0.341024247652797</v>
       </c>
       <c r="AM3">
-        <v>0.009093518520982672</v>
+        <v>0.01151661934628936</v>
       </c>
       <c r="AN3">
-        <v>0.004623302414361691</v>
+        <v>0.007065276230942035</v>
       </c>
       <c r="AO3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AP3">
-        <v>0.004623302414361691</v>
+        <v>0.007065276230942035</v>
       </c>
       <c r="AQ3">
-        <v>0.004623302414361691</v>
+        <v>0.007065276230942035</v>
       </c>
       <c r="AR3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AS3">
-        <v>0.004623302414361691</v>
+        <v>0.007065276230942035</v>
       </c>
       <c r="AT3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
       <c r="AU3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AV3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
       <c r="AW3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
       <c r="AX3">
         <v>0.2668534846590581</v>
       </c>
       <c r="AY3">
-        <v>0.003922127044429769</v>
+        <v>0.004966213843244637</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.004242790958970301</v>
+        <v>0.005393970066814792</v>
       </c>
       <c r="B4">
         <v>0.2781158972827227</v>
       </c>
       <c r="C4">
-        <v>0.004242790958970301</v>
+        <v>0.005393970066814792</v>
       </c>
       <c r="D4">
-        <v>0.004242790958970301</v>
+        <v>0.005393970066814792</v>
       </c>
       <c r="E4">
         <v>0.2781158972827227</v>
       </c>
       <c r="F4">
-        <v>0.004242790958970301</v>
+        <v>0.005393970066814792</v>
       </c>
       <c r="G4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="H4">
-        <v>0.1261746369158506</v>
+        <v>0.181346755414095</v>
       </c>
       <c r="I4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="J4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="K4">
         <v>0.2781158972827227</v>
       </c>
       <c r="L4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="M4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="N4">
-        <v>0.1261746369158506</v>
+        <v>0.181346755414095</v>
       </c>
       <c r="O4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="P4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="Q4">
-        <v>0.1261746369158506</v>
+        <v>0.181346755414095</v>
       </c>
       <c r="R4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="S4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="T4">
-        <v>0.1261746369158506</v>
+        <v>0.181346755414095</v>
       </c>
       <c r="U4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="V4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="W4">
         <v>0.2781158972827227</v>
       </c>
       <c r="X4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="Y4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="Z4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AA4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="AB4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="AC4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AD4">
-        <v>0.004526771924218011</v>
+        <v>0.004858428566768769</v>
       </c>
       <c r="AE4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
       <c r="AF4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AG4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
       <c r="AH4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
       <c r="AI4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AJ4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
       <c r="AK4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="AL4">
-        <v>0.1261746369158506</v>
+        <v>0.181346755414095</v>
       </c>
       <c r="AM4">
-        <v>0.0102019374725316</v>
+        <v>0.0103460619953366</v>
       </c>
       <c r="AN4">
-        <v>0.004621432245967247</v>
+        <v>0.004679914733420094</v>
       </c>
       <c r="AO4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AP4">
-        <v>0.004621432245967247</v>
+        <v>0.004679914733420094</v>
       </c>
       <c r="AQ4">
-        <v>0.004621432245967247</v>
+        <v>0.004679914733420094</v>
       </c>
       <c r="AR4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AS4">
-        <v>0.004621432245967247</v>
+        <v>0.004679914733420094</v>
       </c>
       <c r="AT4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
       <c r="AU4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AV4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
       <c r="AW4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
       <c r="AX4">
         <v>0.2781158972827227</v>
       </c>
       <c r="AY4">
-        <v>0.002864940877222379</v>
+        <v>0.003829583257226451</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.003700807392733978</v>
+        <v>0.004772170886515766</v>
       </c>
       <c r="B5">
         <v>0.1443880420814829</v>
       </c>
       <c r="C5">
-        <v>0.003700807392733978</v>
+        <v>0.004772170886515766</v>
       </c>
       <c r="D5">
-        <v>0.003700807392733978</v>
+        <v>0.004772170886515766</v>
       </c>
       <c r="E5">
         <v>0.1443880420814829</v>
       </c>
       <c r="F5">
-        <v>0.003700807392733978</v>
+        <v>0.004772170886515766</v>
       </c>
       <c r="G5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="H5">
-        <v>0.1156952150243516</v>
+        <v>0.1286560934306459</v>
       </c>
       <c r="I5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="J5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="K5">
         <v>0.1443880420814829</v>
       </c>
       <c r="L5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="M5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="N5">
-        <v>0.1156952150243516</v>
+        <v>0.1286560934306459</v>
       </c>
       <c r="O5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="P5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="Q5">
-        <v>0.1156952150243516</v>
+        <v>0.1286560934306459</v>
       </c>
       <c r="R5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="S5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="T5">
-        <v>0.1156952150243516</v>
+        <v>0.1286560934306459</v>
       </c>
       <c r="U5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="V5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="W5">
         <v>0.1443880420814829</v>
       </c>
       <c r="X5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="Y5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="Z5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AA5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="AB5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="AC5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AD5">
-        <v>0.004770686745860708</v>
+        <v>0.004803100762577241</v>
       </c>
       <c r="AE5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
       <c r="AF5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AG5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
       <c r="AH5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
       <c r="AI5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AJ5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
       <c r="AK5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="AL5">
-        <v>0.1156952150243516</v>
+        <v>0.1286560934306459</v>
       </c>
       <c r="AM5">
-        <v>0.01264891185818256</v>
+        <v>0.01099006671890949</v>
       </c>
       <c r="AN5">
-        <v>0.005127313196902951</v>
+        <v>0.0048134107212644</v>
       </c>
       <c r="AO5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AP5">
-        <v>0.005127313196902951</v>
+        <v>0.0048134107212644</v>
       </c>
       <c r="AQ5">
-        <v>0.005127313196902951</v>
+        <v>0.0048134107212644</v>
       </c>
       <c r="AR5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AS5">
-        <v>0.005127313196902951</v>
+        <v>0.0048134107212644</v>
       </c>
       <c r="AT5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
       <c r="AU5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AV5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
       <c r="AW5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
       <c r="AX5">
         <v>0.1443880420814829</v>
       </c>
       <c r="AY5">
-        <v>0.00288359076064733</v>
+        <v>0.002809028538015816</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.001608342994589428</v>
+        <v>0.004098910266749983</v>
       </c>
       <c r="B6">
         <v>0.08512536239498097</v>
       </c>
       <c r="C6">
-        <v>0.001608342994589428</v>
+        <v>0.004098910266749983</v>
       </c>
       <c r="D6">
-        <v>0.001608342994589428</v>
+        <v>0.004098910266749983</v>
       </c>
       <c r="E6">
         <v>0.08512536239498097</v>
       </c>
       <c r="F6">
-        <v>0.001608342994589428</v>
+        <v>0.004098910266749983</v>
       </c>
       <c r="G6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="H6">
-        <v>0.1350192605204197</v>
+        <v>0.1474189210845402</v>
       </c>
       <c r="I6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="J6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="K6">
         <v>0.08512536239498097</v>
       </c>
       <c r="L6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="M6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="N6">
-        <v>0.1350192605204197</v>
+        <v>0.1474189210845402</v>
       </c>
       <c r="O6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="P6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="Q6">
-        <v>0.1350192605204197</v>
+        <v>0.1474189210845402</v>
       </c>
       <c r="R6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="S6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="T6">
-        <v>0.1350192605204197</v>
+        <v>0.1474189210845402</v>
       </c>
       <c r="U6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="V6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="W6">
         <v>0.08512536239498097</v>
       </c>
       <c r="X6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="Y6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="Z6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AA6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="AB6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="AC6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AD6">
-        <v>0.003984875587610923</v>
+        <v>0.004219910365570005</v>
       </c>
       <c r="AE6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
       <c r="AF6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AG6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
       <c r="AH6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
       <c r="AI6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AJ6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
       <c r="AK6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="AL6">
-        <v>0.1350192605204197</v>
+        <v>0.1474189210845402</v>
       </c>
       <c r="AM6">
-        <v>0.007855676172478693</v>
+        <v>0.009554676093535362</v>
       </c>
       <c r="AN6">
-        <v>0.004777053118618087</v>
+        <v>0.004260243731843346</v>
       </c>
       <c r="AO6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AP6">
-        <v>0.004777053118618087</v>
+        <v>0.004260243731843346</v>
       </c>
       <c r="AQ6">
-        <v>0.004777053118618087</v>
+        <v>0.004260243731843346</v>
       </c>
       <c r="AR6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AS6">
-        <v>0.004777053118618087</v>
+        <v>0.004260243731843346</v>
       </c>
       <c r="AT6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
       <c r="AU6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AV6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
       <c r="AW6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
       <c r="AX6">
         <v>0.08512536239498097</v>
       </c>
       <c r="AY6">
-        <v>0.002204241333530696</v>
+        <v>0.003410378847863681</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.001366282390633341</v>
+        <v>0.003482011278369164</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.001366282390633341</v>
+        <v>0.003482011278369164</v>
       </c>
       <c r="D7">
-        <v>0.001366282390633341</v>
+        <v>0.003482011278369164</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.001366282390633341</v>
+        <v>0.003482011278369164</v>
       </c>
       <c r="G7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="H7">
-        <v>0.0316895400158389</v>
+        <v>0.04242186275106314</v>
       </c>
       <c r="I7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="J7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="M7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="N7">
-        <v>0.0316895400158389</v>
+        <v>0.04242186275106314</v>
       </c>
       <c r="O7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="P7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="Q7">
-        <v>0.0316895400158389</v>
+        <v>0.04242186275106314</v>
       </c>
       <c r="R7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="S7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="T7">
-        <v>0.0316895400158389</v>
+        <v>0.04242186275106314</v>
       </c>
       <c r="U7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="V7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="W7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="Y7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="Z7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="AB7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.002587467028897387</v>
+        <v>0.004173793603937087</v>
       </c>
       <c r="AE7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
       <c r="AH7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
       <c r="AK7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="AL7">
-        <v>0.0316895400158389</v>
+        <v>0.04242186275106314</v>
       </c>
       <c r="AM7">
-        <v>0.005324837346308348</v>
+        <v>0.00675040158951316</v>
       </c>
       <c r="AN7">
-        <v>0.002994528574985402</v>
+        <v>0.004404387712459728</v>
       </c>
       <c r="AO7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.002994528574985402</v>
+        <v>0.004404387712459728</v>
       </c>
       <c r="AQ7">
-        <v>0.002994528574985402</v>
+        <v>0.004404387712459728</v>
       </c>
       <c r="AR7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.002994528574985402</v>
+        <v>0.004404387712459728</v>
       </c>
       <c r="AT7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
       <c r="AW7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.002313762597583816</v>
+        <v>0.00249368869746697</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.001124221786677254</v>
+        <v>0.001432556340637118</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.001124221786677254</v>
+        <v>0.001432556340637118</v>
       </c>
       <c r="D8">
-        <v>0.001124221786677254</v>
+        <v>0.001432556340637118</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.001124221786677254</v>
+        <v>0.001432556340637118</v>
       </c>
       <c r="G8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="H8">
-        <v>0.01972328970670128</v>
+        <v>0.02430331561935923</v>
       </c>
       <c r="I8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="J8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="M8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="N8">
-        <v>0.01972328970670128</v>
+        <v>0.02430331561935923</v>
       </c>
       <c r="O8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="P8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="Q8">
-        <v>0.01972328970670128</v>
+        <v>0.02430331561935923</v>
       </c>
       <c r="R8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="S8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="T8">
-        <v>0.01972328970670128</v>
+        <v>0.02430331561935923</v>
       </c>
       <c r="U8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="V8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="W8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="Y8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="Z8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="AB8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.002115154515154888</v>
+        <v>0.00221549462029774</v>
       </c>
       <c r="AE8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
       <c r="AH8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
       <c r="AK8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="AL8">
-        <v>0.01972328970670128</v>
+        <v>0.02430331561935923</v>
       </c>
       <c r="AM8">
-        <v>0.004358992832131712</v>
+        <v>0.003315803075463913</v>
       </c>
       <c r="AN8">
-        <v>0.002445465424647433</v>
+        <v>0.002476474046851281</v>
       </c>
       <c r="AO8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP8">
-        <v>0.002445465424647433</v>
+        <v>0.002476474046851281</v>
       </c>
       <c r="AQ8">
-        <v>0.002445465424647433</v>
+        <v>0.002476474046851281</v>
       </c>
       <c r="AR8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002445465424647433</v>
+        <v>0.002476474046851281</v>
       </c>
       <c r="AT8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
       <c r="AW8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.001272307867092222</v>
+        <v>0.001738885179379683</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.0008821610848996937</v>
+        <v>0.001124106944268181</v>
       </c>
       <c r="B9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.0008821610848996937</v>
+        <v>0.001124106944268181</v>
       </c>
       <c r="D9">
-        <v>0.0008821610848996937</v>
+        <v>0.001124106944268181</v>
       </c>
       <c r="E9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.0008821610848996937</v>
+        <v>0.001124106944268181</v>
       </c>
       <c r="G9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="H9">
-        <v>0.004556281085100681</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="I9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="J9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="K9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="M9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="N9">
-        <v>0.004556281085100681</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="O9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="P9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="Q9">
-        <v>0.004556281085100681</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="R9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="S9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="T9">
-        <v>0.004556281085100681</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="U9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="V9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="W9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="Y9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="Z9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="AB9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="AC9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.001235512084227121</v>
+        <v>0.00131163292374832</v>
       </c>
       <c r="AE9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
       <c r="AH9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
       <c r="AK9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="AL9">
-        <v>0.004556281085100681</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="AM9">
-        <v>0.001693993878494935</v>
+        <v>0.002577177890623237</v>
       </c>
       <c r="AN9">
-        <v>0.001353295750669597</v>
+        <v>0.001374141583575033</v>
       </c>
       <c r="AO9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP9">
-        <v>0.001353295750669597</v>
+        <v>0.001374141583575033</v>
       </c>
       <c r="AQ9">
-        <v>0.001353295750669597</v>
+        <v>0.001374141583575033</v>
       </c>
       <c r="AR9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001353295750669597</v>
+        <v>0.001374141583575033</v>
       </c>
       <c r="AT9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
       <c r="AW9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.0007733584508437914</v>
+        <v>0.001075465919238414</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.02599160768826621</v>
+        <v>0.03241998865556998</v>
       </c>
       <c r="B10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.02599160768826621</v>
+        <v>0.03241998865556998</v>
       </c>
       <c r="D10">
-        <v>0.02599160768826621</v>
+        <v>0.03241998865556998</v>
       </c>
       <c r="E10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.02599160768826621</v>
+        <v>0.03241998865556998</v>
       </c>
       <c r="G10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="H10">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="I10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="J10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="K10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="M10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="N10">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="O10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="P10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="Q10">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="R10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="S10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="T10">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="U10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="V10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="W10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="Y10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="Z10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="AB10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="AC10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.02078459270982999</v>
+        <v>0.02282290081881093</v>
       </c>
       <c r="AE10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
       <c r="AH10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
       <c r="AK10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="AL10">
-        <v>0.0001477229025714423</v>
+        <v>0.0001537455815503871</v>
       </c>
       <c r="AM10">
-        <v>0.008385022273839802</v>
+        <v>0.008504436229392088</v>
       </c>
       <c r="AN10">
-        <v>0.01904892105035125</v>
+        <v>0.01962387153989125</v>
       </c>
       <c r="AO10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP10">
-        <v>0.01904892105035125</v>
+        <v>0.01962387153989125</v>
       </c>
       <c r="AQ10">
-        <v>0.01904892105035125</v>
+        <v>0.01962387153989125</v>
       </c>
       <c r="AR10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.01904892105035125</v>
+        <v>0.01962387153989125</v>
       </c>
       <c r="AT10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
       <c r="AW10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.01091272794100258</v>
+        <v>0.01177686905883765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the estimated lupin stubble parameters to generate growth aligned closer with Ed's stubble including supp feeding as per Ed's trials No effect on profit because no lupins grown
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -366,13 +366,13 @@
         <v>0.04883906362401351</v>
       </c>
       <c r="G1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="H1">
         <v>0.0001537455815503871</v>
       </c>
       <c r="I1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="J1">
         <v>0.03383218409982959</v>
@@ -384,31 +384,31 @@
         <v>0.03383218409982959</v>
       </c>
       <c r="M1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="N1">
         <v>0.0001537455815503871</v>
       </c>
       <c r="O1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="P1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="Q1">
         <v>0.0001537455815503871</v>
       </c>
       <c r="R1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="S1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="T1">
         <v>0.0001537455815503871</v>
       </c>
       <c r="U1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="V1">
         <v>0.03383218409982959</v>
@@ -456,13 +456,13 @@
         <v>0.01387135483210843</v>
       </c>
       <c r="AK1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="AL1">
         <v>0.0001537455815503871</v>
       </c>
       <c r="AM1">
-        <v>0.0276819434970707</v>
+        <v>0.03528612143816936</v>
       </c>
       <c r="AN1">
         <v>0.02882989092510162</v>
@@ -521,13 +521,13 @@
         <v>0.006711500336291474</v>
       </c>
       <c r="G2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="H2">
         <v>0.1343675673028482</v>
       </c>
       <c r="I2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="J2">
         <v>0.007523242975825024</v>
@@ -539,31 +539,31 @@
         <v>0.007523242975825024</v>
       </c>
       <c r="M2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="N2">
         <v>0.1343675673028482</v>
       </c>
       <c r="O2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="P2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="Q2">
         <v>0.1343675673028482</v>
       </c>
       <c r="R2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="S2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="T2">
         <v>0.1343675673028482</v>
       </c>
       <c r="U2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="V2">
         <v>0.007523242975825024</v>
@@ -611,13 +611,13 @@
         <v>0.007860302061988761</v>
       </c>
       <c r="AK2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="AL2">
         <v>0.1343675673028482</v>
       </c>
       <c r="AM2">
-        <v>0.01522376636419349</v>
+        <v>0.006457780777315358</v>
       </c>
       <c r="AN2">
         <v>0.007793823855669541</v>
@@ -676,13 +676,13 @@
         <v>0.006015769247113818</v>
       </c>
       <c r="G3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="H3">
         <v>0.341024247652797</v>
       </c>
       <c r="I3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="J3">
         <v>0.00680289948498498</v>
@@ -694,31 +694,31 @@
         <v>0.00680289948498498</v>
       </c>
       <c r="M3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="N3">
         <v>0.341024247652797</v>
       </c>
       <c r="O3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="P3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="Q3">
         <v>0.341024247652797</v>
       </c>
       <c r="R3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="S3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="T3">
         <v>0.341024247652797</v>
       </c>
       <c r="U3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="V3">
         <v>0.00680289948498498</v>
@@ -766,13 +766,13 @@
         <v>0.004966213843244637</v>
       </c>
       <c r="AK3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="AL3">
         <v>0.341024247652797</v>
       </c>
       <c r="AM3">
-        <v>0.01151661934628936</v>
+        <v>0.00584934642747072</v>
       </c>
       <c r="AN3">
         <v>0.007065276230942035</v>
@@ -831,13 +831,13 @@
         <v>0.005393970066814792</v>
       </c>
       <c r="G4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="H4">
         <v>0.181346755414095</v>
       </c>
       <c r="I4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="J4">
         <v>0.004858428566768769</v>
@@ -849,31 +849,31 @@
         <v>0.004858428566768769</v>
       </c>
       <c r="M4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="N4">
         <v>0.181346755414095</v>
       </c>
       <c r="O4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="P4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="Q4">
         <v>0.181346755414095</v>
       </c>
       <c r="R4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="S4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="T4">
         <v>0.181346755414095</v>
       </c>
       <c r="U4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="V4">
         <v>0.004858428566768769</v>
@@ -921,13 +921,13 @@
         <v>0.003829583257226451</v>
       </c>
       <c r="AK4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="AL4">
         <v>0.181346755414095</v>
       </c>
       <c r="AM4">
-        <v>0.0103460619953366</v>
+        <v>0.005249676530928998</v>
       </c>
       <c r="AN4">
         <v>0.004679914733420094</v>
@@ -986,13 +986,13 @@
         <v>0.004772170886515766</v>
       </c>
       <c r="G5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="H5">
         <v>0.1286560934306459</v>
       </c>
       <c r="I5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="J5">
         <v>0.004803100762577241</v>
@@ -1004,31 +1004,31 @@
         <v>0.004803100762577241</v>
       </c>
       <c r="M5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="N5">
         <v>0.1286560934306459</v>
       </c>
       <c r="O5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="P5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="Q5">
         <v>0.1286560934306459</v>
       </c>
       <c r="R5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="S5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="T5">
         <v>0.1286560934306459</v>
       </c>
       <c r="U5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="V5">
         <v>0.004803100762577241</v>
@@ -1076,13 +1076,13 @@
         <v>0.002809028538015816</v>
       </c>
       <c r="AK5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="AL5">
         <v>0.1286560934306459</v>
       </c>
       <c r="AM5">
-        <v>0.01099006671890949</v>
+        <v>0.003092023956230371</v>
       </c>
       <c r="AN5">
         <v>0.0048134107212644</v>
@@ -1141,13 +1141,13 @@
         <v>0.004098910266749983</v>
       </c>
       <c r="G6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="H6">
         <v>0.1474189210845402</v>
       </c>
       <c r="I6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="J6">
         <v>0.004219910365570005</v>
@@ -1159,31 +1159,31 @@
         <v>0.004219910365570005</v>
       </c>
       <c r="M6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="N6">
         <v>0.1474189210845402</v>
       </c>
       <c r="O6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="P6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="Q6">
         <v>0.1474189210845402</v>
       </c>
       <c r="R6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="S6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="T6">
         <v>0.1474189210845402</v>
       </c>
       <c r="U6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="V6">
         <v>0.004219910365570005</v>
@@ -1231,13 +1231,13 @@
         <v>0.003410378847863681</v>
       </c>
       <c r="AK6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="AL6">
         <v>0.1474189210845402</v>
       </c>
       <c r="AM6">
-        <v>0.009554676093535362</v>
+        <v>0.005373854080857359</v>
       </c>
       <c r="AN6">
         <v>0.004260243731843346</v>
@@ -1296,13 +1296,13 @@
         <v>0.003482011278369164</v>
       </c>
       <c r="G7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="H7">
         <v>0.04242186275106314</v>
       </c>
       <c r="I7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="J7">
         <v>0.004173793603937087</v>
@@ -1314,31 +1314,31 @@
         <v>0.004173793603937087</v>
       </c>
       <c r="M7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="N7">
         <v>0.04242186275106314</v>
       </c>
       <c r="O7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="P7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="Q7">
         <v>0.04242186275106314</v>
       </c>
       <c r="R7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="S7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="T7">
         <v>0.04242186275106314</v>
       </c>
       <c r="U7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="V7">
         <v>0.004173793603937087</v>
@@ -1386,13 +1386,13 @@
         <v>0.00249368869746697</v>
       </c>
       <c r="AK7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="AL7">
         <v>0.04242186275106314</v>
       </c>
       <c r="AM7">
-        <v>0.00675040158951316</v>
+        <v>0.003418627722410212</v>
       </c>
       <c r="AN7">
         <v>0.004404387712459728</v>
@@ -1451,13 +1451,13 @@
         <v>0.001432556340637118</v>
       </c>
       <c r="G8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="H8">
         <v>0.02430331561935923</v>
       </c>
       <c r="I8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="J8">
         <v>0.00221549462029774</v>
@@ -1469,31 +1469,31 @@
         <v>0.00221549462029774</v>
       </c>
       <c r="M8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="N8">
         <v>0.02430331561935923</v>
       </c>
       <c r="O8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="P8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="Q8">
         <v>0.02430331561935923</v>
       </c>
       <c r="R8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="S8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="T8">
         <v>0.02430331561935923</v>
       </c>
       <c r="U8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="V8">
         <v>0.00221549462029774</v>
@@ -1541,13 +1541,13 @@
         <v>0.001738885179379683</v>
       </c>
       <c r="AK8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="AL8">
         <v>0.02430331561935923</v>
       </c>
       <c r="AM8">
-        <v>0.003315803075463913</v>
+        <v>0.001868579563410878</v>
       </c>
       <c r="AN8">
         <v>0.002476474046851281</v>
@@ -1606,13 +1606,13 @@
         <v>0.001124106944268181</v>
       </c>
       <c r="G9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="H9">
         <v>0.0001537455815503871</v>
       </c>
       <c r="I9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="J9">
         <v>0.00131163292374832</v>
@@ -1624,31 +1624,31 @@
         <v>0.00131163292374832</v>
       </c>
       <c r="M9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="N9">
         <v>0.0001537455815503871</v>
       </c>
       <c r="O9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="P9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="Q9">
         <v>0.0001537455815503871</v>
       </c>
       <c r="R9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="S9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="T9">
         <v>0.0001537455815503871</v>
       </c>
       <c r="U9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="V9">
         <v>0.00131163292374832</v>
@@ -1696,13 +1696,13 @@
         <v>0.001075465919238414</v>
       </c>
       <c r="AK9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="AL9">
         <v>0.0001537455815503871</v>
       </c>
       <c r="AM9">
-        <v>0.002577177890623237</v>
+        <v>0.001455408475076304</v>
       </c>
       <c r="AN9">
         <v>0.001374141583575033</v>
@@ -1761,13 +1761,13 @@
         <v>0.03241998865556998</v>
       </c>
       <c r="G10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="H10">
         <v>0.0001537455815503871</v>
       </c>
       <c r="I10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="J10">
         <v>0.02282290081881093</v>
@@ -1779,31 +1779,31 @@
         <v>0.02282290081881093</v>
       </c>
       <c r="M10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="N10">
         <v>0.0001537455815503871</v>
       </c>
       <c r="O10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="P10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="Q10">
         <v>0.0001537455815503871</v>
       </c>
       <c r="R10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="S10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="T10">
         <v>0.0001537455815503871</v>
       </c>
       <c r="U10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="V10">
         <v>0.02282290081881093</v>
@@ -1851,13 +1851,13 @@
         <v>0.01177686905883765</v>
       </c>
       <c r="AK10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="AL10">
         <v>0.0001537455815503871</v>
       </c>
       <c r="AM10">
-        <v>0.008504436229392088</v>
+        <v>0.01342174696481772</v>
       </c>
       <c r="AN10">
         <v>0.01962387153989125</v>

</xml_diff>

<commit_message>
re-run stubble sim. Profit increased by 1k (probs due to the changes dad made to sheep)
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1552 +348,1552 @@
   <sheetData>
     <row r="1" spans="1:51">
       <c r="A1">
-        <v>0.04883906362401351</v>
+        <v>0.04887908386567361</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.04883906362401351</v>
+        <v>0.04887908386567361</v>
       </c>
       <c r="D1">
-        <v>0.04883906362401351</v>
+        <v>0.04887908386567361</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.04883906362401351</v>
+        <v>0.04887908386567361</v>
       </c>
       <c r="G1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="H1">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="I1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="J1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="M1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="N1">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="O1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="P1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="Q1">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="R1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="S1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="T1">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="U1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="V1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="W1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="Y1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="Z1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="AB1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.03383218409982959</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="AE1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
       <c r="AH1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
       <c r="AK1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="AL1">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="AM1">
-        <v>0.03528612143816936</v>
+        <v>0.03528994484009806</v>
       </c>
       <c r="AN1">
-        <v>0.02882989092510162</v>
+        <v>0.03104662118617465</v>
       </c>
       <c r="AO1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP1">
-        <v>0.02882989092510162</v>
+        <v>0.03104662118617465</v>
       </c>
       <c r="AQ1">
-        <v>0.02882989092510162</v>
+        <v>0.03104662118617465</v>
       </c>
       <c r="AR1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.02882989092510162</v>
+        <v>0.03104662118617465</v>
       </c>
       <c r="AT1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
       <c r="AW1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.01387135483210843</v>
+        <v>0.01647340995996823</v>
       </c>
     </row>
     <row r="2" spans="1:51">
       <c r="A2">
-        <v>0.006711500336291474</v>
+        <v>0.006729471584568375</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.006711500336291474</v>
+        <v>0.006729471584568375</v>
       </c>
       <c r="D2">
-        <v>0.006711500336291474</v>
+        <v>0.006729471584568375</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.006711500336291474</v>
+        <v>0.006729471584568375</v>
       </c>
       <c r="G2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="H2">
-        <v>0.1343675673028482</v>
+        <v>0.1726507920312587</v>
       </c>
       <c r="I2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="J2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="M2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="N2">
-        <v>0.1343675673028482</v>
+        <v>0.1726507920312587</v>
       </c>
       <c r="O2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="P2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="Q2">
-        <v>0.1343675673028482</v>
+        <v>0.1726507920312587</v>
       </c>
       <c r="R2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="S2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="T2">
-        <v>0.1343675673028482</v>
+        <v>0.1726507920312587</v>
       </c>
       <c r="U2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="V2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="W2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="Y2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="AB2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.007523242975825024</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="AE2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
       <c r="AH2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
       <c r="AK2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="AL2">
-        <v>0.1343675673028482</v>
+        <v>0.1726507920312587</v>
       </c>
       <c r="AM2">
-        <v>0.006457780777315358</v>
+        <v>0.008613748025750392</v>
       </c>
       <c r="AN2">
-        <v>0.007793823855669541</v>
+        <v>0.008384905110307858</v>
       </c>
       <c r="AO2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.007793823855669541</v>
+        <v>0.008384905110307858</v>
       </c>
       <c r="AQ2">
-        <v>0.007793823855669541</v>
+        <v>0.008384905110307858</v>
       </c>
       <c r="AR2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.007793823855669541</v>
+        <v>0.008384905110307858</v>
       </c>
       <c r="AT2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
       <c r="AW2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.007860302061988761</v>
+        <v>0.007053385709507021</v>
       </c>
     </row>
     <row r="3" spans="1:51">
       <c r="A3">
-        <v>0.006015769247113818</v>
+        <v>0.0060372868083389</v>
       </c>
       <c r="B3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="C3">
-        <v>0.006015769247113818</v>
+        <v>0.0060372868083389</v>
       </c>
       <c r="D3">
-        <v>0.006015769247113818</v>
+        <v>0.0060372868083389</v>
       </c>
       <c r="E3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="F3">
-        <v>0.006015769247113818</v>
+        <v>0.0060372868083389</v>
       </c>
       <c r="G3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="H3">
-        <v>0.341024247652797</v>
+        <v>0.3338558167167581</v>
       </c>
       <c r="I3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="J3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="K3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="L3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="M3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="N3">
-        <v>0.341024247652797</v>
+        <v>0.3338558167167581</v>
       </c>
       <c r="O3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="P3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="Q3">
-        <v>0.341024247652797</v>
+        <v>0.3338558167167581</v>
       </c>
       <c r="R3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="S3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="T3">
-        <v>0.341024247652797</v>
+        <v>0.3338558167167581</v>
       </c>
       <c r="U3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="V3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="W3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="X3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="Y3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="Z3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AA3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="AB3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="AC3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AD3">
-        <v>0.00680289948498498</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="AE3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
       <c r="AF3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AG3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
       <c r="AH3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
       <c r="AI3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AJ3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
       <c r="AK3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="AL3">
-        <v>0.341024247652797</v>
+        <v>0.3338558167167581</v>
       </c>
       <c r="AM3">
-        <v>0.00584934642747072</v>
+        <v>0.005854187974434026</v>
       </c>
       <c r="AN3">
-        <v>0.007065276230942035</v>
+        <v>0.006578235638616182</v>
       </c>
       <c r="AO3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AP3">
-        <v>0.007065276230942035</v>
+        <v>0.006578235638616182</v>
       </c>
       <c r="AQ3">
-        <v>0.007065276230942035</v>
+        <v>0.006578235638616182</v>
       </c>
       <c r="AR3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AS3">
-        <v>0.007065276230942035</v>
+        <v>0.006578235638616182</v>
       </c>
       <c r="AT3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
       <c r="AU3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AV3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
       <c r="AW3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
       <c r="AX3">
-        <v>0.2668534846590581</v>
+        <v>0.3402453775823806</v>
       </c>
       <c r="AY3">
-        <v>0.004966213843244637</v>
+        <v>0.004272412788252482</v>
       </c>
     </row>
     <row r="4" spans="1:51">
       <c r="A4">
-        <v>0.005393970066814792</v>
+        <v>0.005413263642548172</v>
       </c>
       <c r="B4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="C4">
-        <v>0.005393970066814792</v>
+        <v>0.005413263642548172</v>
       </c>
       <c r="D4">
-        <v>0.005393970066814792</v>
+        <v>0.005413263642548172</v>
       </c>
       <c r="E4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="F4">
-        <v>0.005393970066814792</v>
+        <v>0.005413263642548172</v>
       </c>
       <c r="G4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="H4">
-        <v>0.181346755414095</v>
+        <v>0.1648490742215563</v>
       </c>
       <c r="I4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="J4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="K4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="L4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="M4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="N4">
-        <v>0.181346755414095</v>
+        <v>0.1648490742215563</v>
       </c>
       <c r="O4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="P4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="Q4">
-        <v>0.181346755414095</v>
+        <v>0.1648490742215563</v>
       </c>
       <c r="R4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="S4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="T4">
-        <v>0.181346755414095</v>
+        <v>0.1648490742215563</v>
       </c>
       <c r="U4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="V4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="W4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="X4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="Y4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="Z4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AA4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="AB4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="AC4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AD4">
-        <v>0.004858428566768769</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="AE4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
       <c r="AF4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AG4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
       <c r="AH4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
       <c r="AI4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AJ4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
       <c r="AK4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="AL4">
-        <v>0.181346755414095</v>
+        <v>0.1648490742215563</v>
       </c>
       <c r="AM4">
-        <v>0.005249676530928998</v>
+        <v>0.003498571737094966</v>
       </c>
       <c r="AN4">
-        <v>0.004679914733420094</v>
+        <v>0.003770201317777681</v>
       </c>
       <c r="AO4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AP4">
-        <v>0.004679914733420094</v>
+        <v>0.003770201317777681</v>
       </c>
       <c r="AQ4">
-        <v>0.004679914733420094</v>
+        <v>0.003770201317777681</v>
       </c>
       <c r="AR4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AS4">
-        <v>0.004679914733420094</v>
+        <v>0.003770201317777681</v>
       </c>
       <c r="AT4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
       <c r="AU4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AV4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
       <c r="AW4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
       <c r="AX4">
-        <v>0.2781158972827227</v>
+        <v>0.2180215461683213</v>
       </c>
       <c r="AY4">
-        <v>0.003829583257226451</v>
+        <v>0.003181174702858095</v>
       </c>
     </row>
     <row r="5" spans="1:51">
       <c r="A5">
-        <v>0.004772170886515766</v>
+        <v>0.004789240476757439</v>
       </c>
       <c r="B5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="C5">
-        <v>0.004772170886515766</v>
+        <v>0.004789240476757439</v>
       </c>
       <c r="D5">
-        <v>0.004772170886515766</v>
+        <v>0.004789240476757439</v>
       </c>
       <c r="E5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="F5">
-        <v>0.004772170886515766</v>
+        <v>0.004789240476757439</v>
       </c>
       <c r="G5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="H5">
-        <v>0.1286560934306459</v>
+        <v>0.1205545666743273</v>
       </c>
       <c r="I5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="J5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="K5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="L5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="M5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="N5">
-        <v>0.1286560934306459</v>
+        <v>0.1205545666743273</v>
       </c>
       <c r="O5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="P5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="Q5">
-        <v>0.1286560934306459</v>
+        <v>0.1205545666743273</v>
       </c>
       <c r="R5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="S5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="T5">
-        <v>0.1286560934306459</v>
+        <v>0.1205545666743273</v>
       </c>
       <c r="U5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="V5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="W5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="X5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="Y5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="Z5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AA5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="AB5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="AC5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AD5">
-        <v>0.004803100762577241</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="AE5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
       <c r="AF5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AG5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
       <c r="AH5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
       <c r="AI5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AJ5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
       <c r="AK5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="AL5">
-        <v>0.1286560934306459</v>
+        <v>0.1205545666743273</v>
       </c>
       <c r="AM5">
-        <v>0.003092023956230371</v>
+        <v>0.004636429019548354</v>
       </c>
       <c r="AN5">
-        <v>0.0048134107212644</v>
+        <v>0.004518170312306937</v>
       </c>
       <c r="AO5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AP5">
-        <v>0.0048134107212644</v>
+        <v>0.004518170312306937</v>
       </c>
       <c r="AQ5">
-        <v>0.0048134107212644</v>
+        <v>0.004518170312306937</v>
       </c>
       <c r="AR5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AS5">
-        <v>0.0048134107212644</v>
+        <v>0.004518170312306937</v>
       </c>
       <c r="AT5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
       <c r="AU5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AV5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
       <c r="AW5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
       <c r="AX5">
-        <v>0.1443880420814829</v>
+        <v>0.1548463323034465</v>
       </c>
       <c r="AY5">
-        <v>0.002809028538015816</v>
+        <v>0.00336429189201454</v>
       </c>
     </row>
     <row r="6" spans="1:51">
       <c r="A6">
-        <v>0.004098910266749983</v>
+        <v>0.004119109618312391</v>
       </c>
       <c r="B6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="C6">
-        <v>0.004098910266749983</v>
+        <v>0.004119109618312391</v>
       </c>
       <c r="D6">
-        <v>0.004098910266749983</v>
+        <v>0.004119109618312391</v>
       </c>
       <c r="E6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="F6">
-        <v>0.004098910266749983</v>
+        <v>0.004119109618312391</v>
       </c>
       <c r="G6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="H6">
-        <v>0.1474189210845402</v>
+        <v>0.1485869724678432</v>
       </c>
       <c r="I6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="J6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="K6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="L6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="M6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="N6">
-        <v>0.1474189210845402</v>
+        <v>0.1485869724678432</v>
       </c>
       <c r="O6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="P6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="Q6">
-        <v>0.1474189210845402</v>
+        <v>0.1485869724678432</v>
       </c>
       <c r="R6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="S6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="T6">
-        <v>0.1474189210845402</v>
+        <v>0.1485869724678432</v>
       </c>
       <c r="U6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="V6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="W6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="X6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="Y6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="Z6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AA6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="AB6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="AC6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AD6">
-        <v>0.004219910365570005</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="AE6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
       <c r="AF6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AG6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
       <c r="AH6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
       <c r="AI6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AJ6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
       <c r="AK6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="AL6">
-        <v>0.1474189210845402</v>
+        <v>0.1485869724678432</v>
       </c>
       <c r="AM6">
-        <v>0.005373854080857359</v>
+        <v>0.004031134973236498</v>
       </c>
       <c r="AN6">
-        <v>0.004260243731843346</v>
+        <v>0.004516253983688661</v>
       </c>
       <c r="AO6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AP6">
-        <v>0.004260243731843346</v>
+        <v>0.004516253983688661</v>
       </c>
       <c r="AQ6">
-        <v>0.004260243731843346</v>
+        <v>0.004516253983688661</v>
       </c>
       <c r="AR6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AS6">
-        <v>0.004260243731843346</v>
+        <v>0.004516253983688661</v>
       </c>
       <c r="AT6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
       <c r="AU6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AV6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
       <c r="AW6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
       <c r="AX6">
-        <v>0.08512536239498097</v>
+        <v>0.07167803657229711</v>
       </c>
       <c r="AY6">
-        <v>0.003410378847863681</v>
+        <v>0.00292715091194398</v>
       </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7">
-        <v>0.003482011278369164</v>
+        <v>0.00349917072984269</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.003482011278369164</v>
+        <v>0.00349917072984269</v>
       </c>
       <c r="D7">
-        <v>0.003482011278369164</v>
+        <v>0.00349917072984269</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.003482011278369164</v>
+        <v>0.00349917072984269</v>
       </c>
       <c r="G7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="H7">
-        <v>0.04242186275106314</v>
+        <v>0.03706360975065923</v>
       </c>
       <c r="I7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="J7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="M7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="N7">
-        <v>0.04242186275106314</v>
+        <v>0.03706360975065923</v>
       </c>
       <c r="O7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="P7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="Q7">
-        <v>0.04242186275106314</v>
+        <v>0.03706360975065923</v>
       </c>
       <c r="R7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="S7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="T7">
-        <v>0.04242186275106314</v>
+        <v>0.03706360975065923</v>
       </c>
       <c r="U7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="V7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="W7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="Y7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="Z7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="AB7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.004173793603937087</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="AE7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
       <c r="AH7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
       <c r="AK7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="AL7">
-        <v>0.04242186275106314</v>
+        <v>0.03706360975065923</v>
       </c>
       <c r="AM7">
-        <v>0.003418627722410212</v>
+        <v>0.00341847216176009</v>
       </c>
       <c r="AN7">
-        <v>0.004404387712459728</v>
+        <v>0.004403902541550681</v>
       </c>
       <c r="AO7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.004404387712459728</v>
+        <v>0.004403902541550681</v>
       </c>
       <c r="AQ7">
-        <v>0.004404387712459728</v>
+        <v>0.004403902541550681</v>
       </c>
       <c r="AR7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.004404387712459728</v>
+        <v>0.004403902541550681</v>
       </c>
       <c r="AT7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
       <c r="AW7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.00249368869746697</v>
+        <v>0.002915829553714546</v>
       </c>
     </row>
     <row r="8" spans="1:51">
       <c r="A8">
-        <v>0.001432556340637118</v>
+        <v>0.001439616018507967</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.001432556340637118</v>
+        <v>0.001439616018507967</v>
       </c>
       <c r="D8">
-        <v>0.001432556340637118</v>
+        <v>0.001439616018507967</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.001432556340637118</v>
+        <v>0.001439616018507967</v>
       </c>
       <c r="G8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="H8">
-        <v>0.02430331561935923</v>
+        <v>0.02198347762265828</v>
       </c>
       <c r="I8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="J8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="M8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="N8">
-        <v>0.02430331561935923</v>
+        <v>0.02198347762265828</v>
       </c>
       <c r="O8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="P8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="Q8">
-        <v>0.02430331561935923</v>
+        <v>0.02198347762265828</v>
       </c>
       <c r="R8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="S8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="T8">
-        <v>0.02430331561935923</v>
+        <v>0.02198347762265828</v>
       </c>
       <c r="U8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="V8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="W8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="Y8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="Z8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="AB8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.00221549462029774</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="AE8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
       <c r="AH8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
       <c r="AK8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="AL8">
-        <v>0.02430331561935923</v>
+        <v>0.02198347762265828</v>
       </c>
       <c r="AM8">
-        <v>0.001868579563410878</v>
+        <v>0.002802853103701819</v>
       </c>
       <c r="AN8">
-        <v>0.002476474046851281</v>
+        <v>0.002476187249861067</v>
       </c>
       <c r="AO8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP8">
-        <v>0.002476474046851281</v>
+        <v>0.002476187249861067</v>
       </c>
       <c r="AQ8">
-        <v>0.002476474046851281</v>
+        <v>0.002476187249861067</v>
       </c>
       <c r="AR8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002476474046851281</v>
+        <v>0.002476187249861067</v>
       </c>
       <c r="AT8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
       <c r="AW8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.001738885179379683</v>
+        <v>0.001724088426423199</v>
       </c>
     </row>
     <row r="9" spans="1:51">
       <c r="A9">
-        <v>0.001124106944268181</v>
+        <v>0.001129646574273117</v>
       </c>
       <c r="B9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.001124106944268181</v>
+        <v>0.001129646574273117</v>
       </c>
       <c r="D9">
-        <v>0.001124106944268181</v>
+        <v>0.001129646574273117</v>
       </c>
       <c r="E9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.001124106944268181</v>
+        <v>0.001129646574273117</v>
       </c>
       <c r="G9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="H9">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="I9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="J9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="K9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="M9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="N9">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="O9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="P9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="Q9">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="R9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="S9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="T9">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="U9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="V9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="W9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="Y9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="Z9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="AB9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="AC9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.00131163292374832</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="AE9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
       <c r="AH9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
       <c r="AK9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="AL9">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="AM9">
-        <v>0.001455408475076304</v>
+        <v>0.0007276711044972345</v>
       </c>
       <c r="AN9">
-        <v>0.001374141583575033</v>
+        <v>0.001234286783493983</v>
       </c>
       <c r="AO9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP9">
-        <v>0.001374141583575033</v>
+        <v>0.001234286783493983</v>
       </c>
       <c r="AQ9">
-        <v>0.001374141583575033</v>
+        <v>0.001234286783493983</v>
       </c>
       <c r="AR9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001374141583575033</v>
+        <v>0.001234286783493983</v>
       </c>
       <c r="AT9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
       <c r="AW9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.001075465919238414</v>
+        <v>0.0008077252184532221</v>
       </c>
     </row>
     <row r="10" spans="1:51">
       <c r="A10">
-        <v>0.03241998865556998</v>
+        <v>0.03239724877960055</v>
       </c>
       <c r="B10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.03241998865556998</v>
+        <v>0.03239724877960055</v>
       </c>
       <c r="D10">
-        <v>0.03241998865556998</v>
+        <v>0.03239724877960055</v>
       </c>
       <c r="E10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.03241998865556998</v>
+        <v>0.03239724877960055</v>
       </c>
       <c r="G10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="H10">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="I10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="J10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="K10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="M10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="N10">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="O10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="P10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="Q10">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="R10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="S10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="T10">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="U10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="V10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="W10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="X10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="Y10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="Z10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="AB10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="AC10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.02282290081881093</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="AE10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
       <c r="AH10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
       <c r="AK10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="AL10">
-        <v>0.0001537455815503871</v>
+        <v>0.0001518968383129674</v>
       </c>
       <c r="AM10">
-        <v>0.01342174696481772</v>
+        <v>0.01342113595031052</v>
       </c>
       <c r="AN10">
-        <v>0.01962387153989125</v>
+        <v>0.0194897758411525</v>
       </c>
       <c r="AO10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP10">
-        <v>0.01962387153989125</v>
+        <v>0.0194897758411525</v>
       </c>
       <c r="AQ10">
-        <v>0.01962387153989125</v>
+        <v>0.0194897758411525</v>
       </c>
       <c r="AR10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.01962387153989125</v>
+        <v>0.0194897758411525</v>
       </c>
       <c r="AT10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
       <c r="AW10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.01177686905883765</v>
+        <v>0.01177336119396915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add mixed species land use. This still needs to be calibrated. Currently it is turned off. No profit change.
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -340,13 +340,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY10"/>
+  <dimension ref="A1:BB10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:54">
       <c r="A1">
         <v>0.04887908386567361</v>
       </c>
@@ -411,13 +411,13 @@
         <v>0.03528994484009806</v>
       </c>
       <c r="V1">
-        <v>0.03550473685604939</v>
+        <v>0.03003653031203316</v>
       </c>
       <c r="W1">
-        <v>0.0001146235521235521</v>
+        <v>0.0001394724095831623</v>
       </c>
       <c r="X1">
-        <v>0.03550473685604939</v>
+        <v>0.03003653031203316</v>
       </c>
       <c r="Y1">
         <v>0.03550473685604939</v>
@@ -438,13 +438,13 @@
         <v>0.03550473685604939</v>
       </c>
       <c r="AE1">
-        <v>0.01647340995996823</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.01647340995996823</v>
+        <v>0.03550473685604939</v>
       </c>
       <c r="AH1">
         <v>0.01647340995996823</v>
@@ -456,22 +456,22 @@
         <v>0.01647340995996823</v>
       </c>
       <c r="AK1">
+        <v>0.01647340995996823</v>
+      </c>
+      <c r="AL1">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AM1">
+        <v>0.01647340995996823</v>
+      </c>
+      <c r="AN1">
         <v>0.03528994484009806</v>
       </c>
-      <c r="AL1">
+      <c r="AO1">
         <v>0.0001518968383129674</v>
       </c>
-      <c r="AM1">
+      <c r="AP1">
         <v>0.03528994484009806</v>
-      </c>
-      <c r="AN1">
-        <v>0.03104662118617465</v>
-      </c>
-      <c r="AO1">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AP1">
-        <v>0.03104662118617465</v>
       </c>
       <c r="AQ1">
         <v>0.03104662118617465</v>
@@ -483,13 +483,13 @@
         <v>0.03104662118617465</v>
       </c>
       <c r="AT1">
-        <v>0.01647340995996823</v>
+        <v>0.03104662118617465</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.01647340995996823</v>
+        <v>0.03104662118617465</v>
       </c>
       <c r="AW1">
         <v>0.01647340995996823</v>
@@ -500,8 +500,17 @@
       <c r="AY1">
         <v>0.01647340995996823</v>
       </c>
+      <c r="AZ1">
+        <v>0.01647340995996823</v>
+      </c>
+      <c r="BA1">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BB1">
+        <v>0.01647340995996823</v>
+      </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:54">
       <c r="A2">
         <v>0.006729471584568375</v>
       </c>
@@ -566,13 +575,13 @@
         <v>0.008613748025750392</v>
       </c>
       <c r="V2">
-        <v>0.007971046728872989</v>
+        <v>0.007800672337179483</v>
       </c>
       <c r="W2">
-        <v>0.0001146235521235521</v>
+        <v>0.115138735871547</v>
       </c>
       <c r="X2">
-        <v>0.007971046728872989</v>
+        <v>0.007800672337179483</v>
       </c>
       <c r="Y2">
         <v>0.007971046728872989</v>
@@ -593,13 +602,13 @@
         <v>0.007971046728872989</v>
       </c>
       <c r="AE2">
-        <v>0.007053385709507021</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.007053385709507021</v>
+        <v>0.007971046728872989</v>
       </c>
       <c r="AH2">
         <v>0.007053385709507021</v>
@@ -611,22 +620,22 @@
         <v>0.007053385709507021</v>
       </c>
       <c r="AK2">
+        <v>0.007053385709507021</v>
+      </c>
+      <c r="AL2">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AM2">
+        <v>0.007053385709507021</v>
+      </c>
+      <c r="AN2">
         <v>0.008613748025750392</v>
       </c>
-      <c r="AL2">
+      <c r="AO2">
         <v>0.1726507920312587</v>
       </c>
-      <c r="AM2">
+      <c r="AP2">
         <v>0.008613748025750392</v>
-      </c>
-      <c r="AN2">
-        <v>0.008384905110307858</v>
-      </c>
-      <c r="AO2">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AP2">
-        <v>0.008384905110307858</v>
       </c>
       <c r="AQ2">
         <v>0.008384905110307858</v>
@@ -638,13 +647,13 @@
         <v>0.008384905110307858</v>
       </c>
       <c r="AT2">
-        <v>0.007053385709507021</v>
+        <v>0.008384905110307858</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.007053385709507021</v>
+        <v>0.008384905110307858</v>
       </c>
       <c r="AW2">
         <v>0.007053385709507021</v>
@@ -655,8 +664,17 @@
       <c r="AY2">
         <v>0.007053385709507021</v>
       </c>
+      <c r="AZ2">
+        <v>0.007053385709507021</v>
+      </c>
+      <c r="BA2">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BB2">
+        <v>0.007053385709507021</v>
+      </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:54">
       <c r="A3">
         <v>0.0060372868083389</v>
       </c>
@@ -721,13 +739,13 @@
         <v>0.005854187974434026</v>
       </c>
       <c r="V3">
-        <v>0.006442998431046862</v>
+        <v>0.005738715325018062</v>
       </c>
       <c r="W3">
-        <v>0.3402453775823806</v>
+        <v>0.3359856703386322</v>
       </c>
       <c r="X3">
-        <v>0.006442998431046862</v>
+        <v>0.005738715325018062</v>
       </c>
       <c r="Y3">
         <v>0.006442998431046862</v>
@@ -748,13 +766,13 @@
         <v>0.006442998431046862</v>
       </c>
       <c r="AE3">
-        <v>0.004272412788252482</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="AF3">
         <v>0.3402453775823806</v>
       </c>
       <c r="AG3">
-        <v>0.004272412788252482</v>
+        <v>0.006442998431046862</v>
       </c>
       <c r="AH3">
         <v>0.004272412788252482</v>
@@ -766,22 +784,22 @@
         <v>0.004272412788252482</v>
       </c>
       <c r="AK3">
+        <v>0.004272412788252482</v>
+      </c>
+      <c r="AL3">
+        <v>0.3402453775823806</v>
+      </c>
+      <c r="AM3">
+        <v>0.004272412788252482</v>
+      </c>
+      <c r="AN3">
         <v>0.005854187974434026</v>
       </c>
-      <c r="AL3">
+      <c r="AO3">
         <v>0.3338558167167581</v>
       </c>
-      <c r="AM3">
+      <c r="AP3">
         <v>0.005854187974434026</v>
-      </c>
-      <c r="AN3">
-        <v>0.006578235638616182</v>
-      </c>
-      <c r="AO3">
-        <v>0.3402453775823806</v>
-      </c>
-      <c r="AP3">
-        <v>0.006578235638616182</v>
       </c>
       <c r="AQ3">
         <v>0.006578235638616182</v>
@@ -793,13 +811,13 @@
         <v>0.006578235638616182</v>
       </c>
       <c r="AT3">
-        <v>0.004272412788252482</v>
+        <v>0.006578235638616182</v>
       </c>
       <c r="AU3">
         <v>0.3402453775823806</v>
       </c>
       <c r="AV3">
-        <v>0.004272412788252482</v>
+        <v>0.006578235638616182</v>
       </c>
       <c r="AW3">
         <v>0.004272412788252482</v>
@@ -810,8 +828,17 @@
       <c r="AY3">
         <v>0.004272412788252482</v>
       </c>
+      <c r="AZ3">
+        <v>0.004272412788252482</v>
+      </c>
+      <c r="BA3">
+        <v>0.3402453775823806</v>
+      </c>
+      <c r="BB3">
+        <v>0.004272412788252482</v>
+      </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:54">
       <c r="A4">
         <v>0.005413263642548172</v>
       </c>
@@ -876,13 +903,13 @@
         <v>0.003498571737094966</v>
       </c>
       <c r="V4">
-        <v>0.004180966898970304</v>
+        <v>0.003797826962670339</v>
       </c>
       <c r="W4">
-        <v>0.2180215461683213</v>
+        <v>0.1825732315371447</v>
       </c>
       <c r="X4">
-        <v>0.004180966898970304</v>
+        <v>0.003797826962670339</v>
       </c>
       <c r="Y4">
         <v>0.004180966898970304</v>
@@ -903,13 +930,13 @@
         <v>0.004180966898970304</v>
       </c>
       <c r="AE4">
-        <v>0.003181174702858095</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="AF4">
         <v>0.2180215461683213</v>
       </c>
       <c r="AG4">
-        <v>0.003181174702858095</v>
+        <v>0.004180966898970304</v>
       </c>
       <c r="AH4">
         <v>0.003181174702858095</v>
@@ -921,22 +948,22 @@
         <v>0.003181174702858095</v>
       </c>
       <c r="AK4">
+        <v>0.003181174702858095</v>
+      </c>
+      <c r="AL4">
+        <v>0.2180215461683213</v>
+      </c>
+      <c r="AM4">
+        <v>0.003181174702858095</v>
+      </c>
+      <c r="AN4">
         <v>0.003498571737094966</v>
       </c>
-      <c r="AL4">
+      <c r="AO4">
         <v>0.1648490742215563</v>
       </c>
-      <c r="AM4">
+      <c r="AP4">
         <v>0.003498571737094966</v>
-      </c>
-      <c r="AN4">
-        <v>0.003770201317777681</v>
-      </c>
-      <c r="AO4">
-        <v>0.2180215461683213</v>
-      </c>
-      <c r="AP4">
-        <v>0.003770201317777681</v>
       </c>
       <c r="AQ4">
         <v>0.003770201317777681</v>
@@ -948,13 +975,13 @@
         <v>0.003770201317777681</v>
       </c>
       <c r="AT4">
-        <v>0.003181174702858095</v>
+        <v>0.003770201317777681</v>
       </c>
       <c r="AU4">
         <v>0.2180215461683213</v>
       </c>
       <c r="AV4">
-        <v>0.003181174702858095</v>
+        <v>0.003770201317777681</v>
       </c>
       <c r="AW4">
         <v>0.003181174702858095</v>
@@ -965,8 +992,17 @@
       <c r="AY4">
         <v>0.003181174702858095</v>
       </c>
+      <c r="AZ4">
+        <v>0.003181174702858095</v>
+      </c>
+      <c r="BA4">
+        <v>0.2180215461683213</v>
+      </c>
+      <c r="BB4">
+        <v>0.003181174702858095</v>
+      </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:54">
       <c r="A5">
         <v>0.004789240476757439</v>
       </c>
@@ -1031,13 +1067,13 @@
         <v>0.004636429019548354</v>
       </c>
       <c r="V5">
-        <v>0.004585937853419563</v>
+        <v>0.00424410917389367</v>
       </c>
       <c r="W5">
-        <v>0.1548463323034465</v>
+        <v>0.131985155217367</v>
       </c>
       <c r="X5">
-        <v>0.004585937853419563</v>
+        <v>0.00424410917389367</v>
       </c>
       <c r="Y5">
         <v>0.004585937853419563</v>
@@ -1058,13 +1094,13 @@
         <v>0.004585937853419563</v>
       </c>
       <c r="AE5">
-        <v>0.00336429189201454</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="AF5">
         <v>0.1548463323034465</v>
       </c>
       <c r="AG5">
-        <v>0.00336429189201454</v>
+        <v>0.004585937853419563</v>
       </c>
       <c r="AH5">
         <v>0.00336429189201454</v>
@@ -1076,22 +1112,22 @@
         <v>0.00336429189201454</v>
       </c>
       <c r="AK5">
+        <v>0.00336429189201454</v>
+      </c>
+      <c r="AL5">
+        <v>0.1548463323034465</v>
+      </c>
+      <c r="AM5">
+        <v>0.00336429189201454</v>
+      </c>
+      <c r="AN5">
         <v>0.004636429019548354</v>
       </c>
-      <c r="AL5">
+      <c r="AO5">
         <v>0.1205545666743273</v>
       </c>
-      <c r="AM5">
+      <c r="AP5">
         <v>0.004636429019548354</v>
-      </c>
-      <c r="AN5">
-        <v>0.004518170312306937</v>
-      </c>
-      <c r="AO5">
-        <v>0.1548463323034465</v>
-      </c>
-      <c r="AP5">
-        <v>0.004518170312306937</v>
       </c>
       <c r="AQ5">
         <v>0.004518170312306937</v>
@@ -1103,13 +1139,13 @@
         <v>0.004518170312306937</v>
       </c>
       <c r="AT5">
-        <v>0.00336429189201454</v>
+        <v>0.004518170312306937</v>
       </c>
       <c r="AU5">
         <v>0.1548463323034465</v>
       </c>
       <c r="AV5">
-        <v>0.00336429189201454</v>
+        <v>0.004518170312306937</v>
       </c>
       <c r="AW5">
         <v>0.00336429189201454</v>
@@ -1120,8 +1156,17 @@
       <c r="AY5">
         <v>0.00336429189201454</v>
       </c>
+      <c r="AZ5">
+        <v>0.00336429189201454</v>
+      </c>
+      <c r="BA5">
+        <v>0.1548463323034465</v>
+      </c>
+      <c r="BB5">
+        <v>0.00336429189201454</v>
+      </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:54">
       <c r="A6">
         <v>0.004119109618312391</v>
       </c>
@@ -1186,13 +1231,13 @@
         <v>0.004031134973236498</v>
       </c>
       <c r="V6">
-        <v>0.004416967892344595</v>
+        <v>0.003936186909500405</v>
       </c>
       <c r="W6">
-        <v>0.07167803657229711</v>
+        <v>0.1229506605026612</v>
       </c>
       <c r="X6">
-        <v>0.004416967892344595</v>
+        <v>0.003936186909500405</v>
       </c>
       <c r="Y6">
         <v>0.004416967892344595</v>
@@ -1213,13 +1258,13 @@
         <v>0.004416967892344595</v>
       </c>
       <c r="AE6">
-        <v>0.00292715091194398</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="AF6">
         <v>0.07167803657229711</v>
       </c>
       <c r="AG6">
-        <v>0.00292715091194398</v>
+        <v>0.004416967892344595</v>
       </c>
       <c r="AH6">
         <v>0.00292715091194398</v>
@@ -1231,22 +1276,22 @@
         <v>0.00292715091194398</v>
       </c>
       <c r="AK6">
+        <v>0.00292715091194398</v>
+      </c>
+      <c r="AL6">
+        <v>0.07167803657229711</v>
+      </c>
+      <c r="AM6">
+        <v>0.00292715091194398</v>
+      </c>
+      <c r="AN6">
         <v>0.004031134973236498</v>
       </c>
-      <c r="AL6">
+      <c r="AO6">
         <v>0.1485869724678432</v>
       </c>
-      <c r="AM6">
+      <c r="AP6">
         <v>0.004031134973236498</v>
-      </c>
-      <c r="AN6">
-        <v>0.004516253983688661</v>
-      </c>
-      <c r="AO6">
-        <v>0.07167803657229711</v>
-      </c>
-      <c r="AP6">
-        <v>0.004516253983688661</v>
       </c>
       <c r="AQ6">
         <v>0.004516253983688661</v>
@@ -1258,13 +1303,13 @@
         <v>0.004516253983688661</v>
       </c>
       <c r="AT6">
-        <v>0.00292715091194398</v>
+        <v>0.004516253983688661</v>
       </c>
       <c r="AU6">
         <v>0.07167803657229711</v>
       </c>
       <c r="AV6">
-        <v>0.00292715091194398</v>
+        <v>0.004516253983688661</v>
       </c>
       <c r="AW6">
         <v>0.00292715091194398</v>
@@ -1275,8 +1320,17 @@
       <c r="AY6">
         <v>0.00292715091194398</v>
       </c>
+      <c r="AZ6">
+        <v>0.00292715091194398</v>
+      </c>
+      <c r="BA6">
+        <v>0.07167803657229711</v>
+      </c>
+      <c r="BB6">
+        <v>0.00292715091194398</v>
+      </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:54">
       <c r="A7">
         <v>0.00349917072984269</v>
       </c>
@@ -1341,13 +1395,13 @@
         <v>0.00341847216176009</v>
       </c>
       <c r="V7">
-        <v>0.004177719588623684</v>
+        <v>0.003708715660526274</v>
       </c>
       <c r="W7">
-        <v>0.0001146235521235521</v>
+        <v>0.024747281017814</v>
       </c>
       <c r="X7">
-        <v>0.004177719588623684</v>
+        <v>0.003708715660526274</v>
       </c>
       <c r="Y7">
         <v>0.004177719588623684</v>
@@ -1368,13 +1422,13 @@
         <v>0.004177719588623684</v>
       </c>
       <c r="AE7">
-        <v>0.002915829553714546</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.002915829553714546</v>
+        <v>0.004177719588623684</v>
       </c>
       <c r="AH7">
         <v>0.002915829553714546</v>
@@ -1386,22 +1440,22 @@
         <v>0.002915829553714546</v>
       </c>
       <c r="AK7">
+        <v>0.002915829553714546</v>
+      </c>
+      <c r="AL7">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AM7">
+        <v>0.002915829553714546</v>
+      </c>
+      <c r="AN7">
         <v>0.00341847216176009</v>
       </c>
-      <c r="AL7">
+      <c r="AO7">
         <v>0.03706360975065923</v>
       </c>
-      <c r="AM7">
+      <c r="AP7">
         <v>0.00341847216176009</v>
-      </c>
-      <c r="AN7">
-        <v>0.004403902541550681</v>
-      </c>
-      <c r="AO7">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AP7">
-        <v>0.004403902541550681</v>
       </c>
       <c r="AQ7">
         <v>0.004403902541550681</v>
@@ -1413,13 +1467,13 @@
         <v>0.004403902541550681</v>
       </c>
       <c r="AT7">
-        <v>0.002915829553714546</v>
+        <v>0.004403902541550681</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.002915829553714546</v>
+        <v>0.004403902541550681</v>
       </c>
       <c r="AW7">
         <v>0.002915829553714546</v>
@@ -1430,8 +1484,17 @@
       <c r="AY7">
         <v>0.002915829553714546</v>
       </c>
+      <c r="AZ7">
+        <v>0.002915829553714546</v>
+      </c>
+      <c r="BA7">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BB7">
+        <v>0.002915829553714546</v>
+      </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:54">
       <c r="A8">
         <v>0.001439616018507967</v>
       </c>
@@ -1496,13 +1559,13 @@
         <v>0.002802853103701819</v>
       </c>
       <c r="V8">
-        <v>0.002217044442022792</v>
+        <v>0.002159886817805626</v>
       </c>
       <c r="W8">
-        <v>0.0001146235521235521</v>
+        <v>0.01469385959914671</v>
       </c>
       <c r="X8">
-        <v>0.002217044442022792</v>
+        <v>0.002159886817805626</v>
       </c>
       <c r="Y8">
         <v>0.002217044442022792</v>
@@ -1523,13 +1586,13 @@
         <v>0.002217044442022792</v>
       </c>
       <c r="AE8">
-        <v>0.001724088426423199</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.001724088426423199</v>
+        <v>0.002217044442022792</v>
       </c>
       <c r="AH8">
         <v>0.001724088426423199</v>
@@ -1541,22 +1604,22 @@
         <v>0.001724088426423199</v>
       </c>
       <c r="AK8">
+        <v>0.001724088426423199</v>
+      </c>
+      <c r="AL8">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AM8">
+        <v>0.001724088426423199</v>
+      </c>
+      <c r="AN8">
         <v>0.002802853103701819</v>
       </c>
-      <c r="AL8">
+      <c r="AO8">
         <v>0.02198347762265828</v>
       </c>
-      <c r="AM8">
+      <c r="AP8">
         <v>0.002802853103701819</v>
-      </c>
-      <c r="AN8">
-        <v>0.002476187249861067</v>
-      </c>
-      <c r="AO8">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AP8">
-        <v>0.002476187249861067</v>
       </c>
       <c r="AQ8">
         <v>0.002476187249861067</v>
@@ -1568,13 +1631,13 @@
         <v>0.002476187249861067</v>
       </c>
       <c r="AT8">
-        <v>0.001724088426423199</v>
+        <v>0.002476187249861067</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.001724088426423199</v>
+        <v>0.002476187249861067</v>
       </c>
       <c r="AW8">
         <v>0.001724088426423199</v>
@@ -1585,8 +1648,17 @@
       <c r="AY8">
         <v>0.001724088426423199</v>
       </c>
+      <c r="AZ8">
+        <v>0.001724088426423199</v>
+      </c>
+      <c r="BA8">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BB8">
+        <v>0.001724088426423199</v>
+      </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:54">
       <c r="A9">
         <v>0.001129646574273117</v>
       </c>
@@ -1651,13 +1723,13 @@
         <v>0.0007276711044972345</v>
       </c>
       <c r="V9">
-        <v>0.001208126731188766</v>
+        <v>0.00102508978087982</v>
       </c>
       <c r="W9">
-        <v>0.0001146235521235521</v>
+        <v>0.0001394724095831623</v>
       </c>
       <c r="X9">
-        <v>0.001208126731188766</v>
+        <v>0.00102508978087982</v>
       </c>
       <c r="Y9">
         <v>0.001208126731188766</v>
@@ -1678,13 +1750,13 @@
         <v>0.001208126731188766</v>
       </c>
       <c r="AE9">
-        <v>0.0008077252184532221</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.0008077252184532221</v>
+        <v>0.001208126731188766</v>
       </c>
       <c r="AH9">
         <v>0.0008077252184532221</v>
@@ -1696,22 +1768,22 @@
         <v>0.0008077252184532221</v>
       </c>
       <c r="AK9">
+        <v>0.0008077252184532221</v>
+      </c>
+      <c r="AL9">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AM9">
+        <v>0.0008077252184532221</v>
+      </c>
+      <c r="AN9">
         <v>0.0007276711044972345</v>
       </c>
-      <c r="AL9">
+      <c r="AO9">
         <v>0.0001518968383129674</v>
       </c>
-      <c r="AM9">
+      <c r="AP9">
         <v>0.0007276711044972345</v>
-      </c>
-      <c r="AN9">
-        <v>0.001234286783493983</v>
-      </c>
-      <c r="AO9">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AP9">
-        <v>0.001234286783493983</v>
       </c>
       <c r="AQ9">
         <v>0.001234286783493983</v>
@@ -1723,13 +1795,13 @@
         <v>0.001234286783493983</v>
       </c>
       <c r="AT9">
-        <v>0.0008077252184532221</v>
+        <v>0.001234286783493983</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.0008077252184532221</v>
+        <v>0.001234286783493983</v>
       </c>
       <c r="AW9">
         <v>0.0008077252184532221</v>
@@ -1740,8 +1812,17 @@
       <c r="AY9">
         <v>0.0008077252184532221</v>
       </c>
+      <c r="AZ9">
+        <v>0.0008077252184532221</v>
+      </c>
+      <c r="BA9">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BB9">
+        <v>0.0008077252184532221</v>
+      </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:54">
       <c r="A10">
         <v>0.03239724877960055</v>
       </c>
@@ -1806,13 +1887,13 @@
         <v>0.01342113595031052</v>
       </c>
       <c r="V10">
-        <v>0.02271664407576451</v>
+        <v>0.01826206209161527</v>
       </c>
       <c r="W10">
-        <v>0.0001146235521235521</v>
+        <v>0.0001394724095831623</v>
       </c>
       <c r="X10">
-        <v>0.02271664407576451</v>
+        <v>0.01826206209161527</v>
       </c>
       <c r="Y10">
         <v>0.02271664407576451</v>
@@ -1833,13 +1914,13 @@
         <v>0.02271664407576451</v>
       </c>
       <c r="AE10">
-        <v>0.01177336119396915</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.01177336119396915</v>
+        <v>0.02271664407576451</v>
       </c>
       <c r="AH10">
         <v>0.01177336119396915</v>
@@ -1851,22 +1932,22 @@
         <v>0.01177336119396915</v>
       </c>
       <c r="AK10">
+        <v>0.01177336119396915</v>
+      </c>
+      <c r="AL10">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AM10">
+        <v>0.01177336119396915</v>
+      </c>
+      <c r="AN10">
         <v>0.01342113595031052</v>
       </c>
-      <c r="AL10">
+      <c r="AO10">
         <v>0.0001518968383129674</v>
       </c>
-      <c r="AM10">
+      <c r="AP10">
         <v>0.01342113595031052</v>
-      </c>
-      <c r="AN10">
-        <v>0.0194897758411525</v>
-      </c>
-      <c r="AO10">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AP10">
-        <v>0.0194897758411525</v>
       </c>
       <c r="AQ10">
         <v>0.0194897758411525</v>
@@ -1878,13 +1959,13 @@
         <v>0.0194897758411525</v>
       </c>
       <c r="AT10">
-        <v>0.01177336119396915</v>
+        <v>0.0194897758411525</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.01177336119396915</v>
+        <v>0.0194897758411525</v>
       </c>
       <c r="AW10">
         <v>0.01177336119396915</v>
@@ -1893,6 +1974,15 @@
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
+        <v>0.01177336119396915</v>
+      </c>
+      <c r="AZ10">
+        <v>0.01177336119396915</v>
+      </c>
+      <c r="BA10">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BB10">
         <v>0.01177336119396915</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stubble sim for GEPEP feeding system and SR halved in Ed's trials
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1642 +348,1642 @@
   <sheetData>
     <row r="1" spans="1:54">
       <c r="A1">
-        <v>0.04887908386567361</v>
+        <v>0.00759462609864864</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.04887908386567361</v>
+        <v>0.00759462609864864</v>
       </c>
       <c r="D1">
-        <v>0.04887908386567361</v>
+        <v>0.00759462609864864</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.04887908386567361</v>
+        <v>0.00759462609864864</v>
       </c>
       <c r="G1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="I1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="M1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="O1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="R1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="U1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V1">
-        <v>0.03003653031203316</v>
+        <v>0.001264963354505144</v>
       </c>
       <c r="W1">
-        <v>0.0001394724095831623</v>
+        <v>0.0001465043978653304</v>
       </c>
       <c r="X1">
-        <v>0.03003653031203316</v>
+        <v>0.001264963354505144</v>
       </c>
       <c r="Y1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="Z1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="AB1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="AE1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.03550473685604939</v>
+        <v>0.002085041190888201</v>
       </c>
       <c r="AH1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AK1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AL1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AN1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AO1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="AP1">
-        <v>0.03528994484009806</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AQ1">
-        <v>0.03104662118617465</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AR1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.03104662118617465</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AT1">
-        <v>0.03104662118617465</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.03104662118617465</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AW1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AZ1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="BA1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
     </row>
     <row r="2" spans="1:54">
       <c r="A2">
-        <v>0.006729471584568375</v>
+        <v>0.02041368300311761</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.006729471584568375</v>
+        <v>0.02041368300311761</v>
       </c>
       <c r="D2">
-        <v>0.006729471584568375</v>
+        <v>0.02041368300311761</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.006729471584568375</v>
+        <v>0.02041368300311761</v>
       </c>
       <c r="G2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="H2">
-        <v>0.1726507920312587</v>
+        <v>0.07118276118399262</v>
       </c>
       <c r="I2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="J2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="M2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="N2">
-        <v>0.1726507920312587</v>
+        <v>0.07118276118399262</v>
       </c>
       <c r="O2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="P2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="Q2">
-        <v>0.1726507920312587</v>
+        <v>0.07118276118399262</v>
       </c>
       <c r="R2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="S2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="T2">
-        <v>0.1726507920312587</v>
+        <v>0.07118276118399262</v>
       </c>
       <c r="U2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="V2">
-        <v>0.007800672337179483</v>
+        <v>0.004612303486206622</v>
       </c>
       <c r="W2">
-        <v>0.115138735871547</v>
+        <v>0.04749338197336959</v>
       </c>
       <c r="X2">
-        <v>0.007800672337179483</v>
+        <v>0.004612303486206622</v>
       </c>
       <c r="Y2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="AB2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="AE2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.007971046728872989</v>
+        <v>0.00688612458702335</v>
       </c>
       <c r="AH2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
       <c r="AK2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
       <c r="AL2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
       <c r="AN2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="AO2">
-        <v>0.1726507920312587</v>
+        <v>0.07118276118399262</v>
       </c>
       <c r="AP2">
-        <v>0.008613748025750392</v>
+        <v>0.002149498247719897</v>
       </c>
       <c r="AQ2">
-        <v>0.008384905110307858</v>
+        <v>0.002376938448325265</v>
       </c>
       <c r="AR2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.008384905110307858</v>
+        <v>0.002376938448325265</v>
       </c>
       <c r="AT2">
-        <v>0.008384905110307858</v>
+        <v>0.002376938448325265</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.008384905110307858</v>
+        <v>0.002376938448325265</v>
       </c>
       <c r="AW2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
       <c r="AZ2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
       <c r="BA2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB2">
-        <v>0.007053385709507021</v>
+        <v>0.001296063903816529</v>
       </c>
     </row>
     <row r="3" spans="1:54">
       <c r="A3">
-        <v>0.0060372868083389</v>
+        <v>0.01057066614377407</v>
       </c>
       <c r="B3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="C3">
-        <v>0.0060372868083389</v>
+        <v>0.01057066614377407</v>
       </c>
       <c r="D3">
-        <v>0.0060372868083389</v>
+        <v>0.01057066614377407</v>
       </c>
       <c r="E3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="F3">
-        <v>0.0060372868083389</v>
+        <v>0.01057066614377407</v>
       </c>
       <c r="G3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="H3">
-        <v>0.3338558167167581</v>
+        <v>0.1697429054257266</v>
       </c>
       <c r="I3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="J3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="K3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="L3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="M3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="N3">
-        <v>0.3338558167167581</v>
+        <v>0.1697429054257266</v>
       </c>
       <c r="O3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="P3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="Q3">
-        <v>0.3338558167167581</v>
+        <v>0.1697429054257266</v>
       </c>
       <c r="R3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="S3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="T3">
-        <v>0.3338558167167581</v>
+        <v>0.1697429054257266</v>
       </c>
       <c r="U3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="V3">
-        <v>0.005738715325018062</v>
+        <v>0.01015205241744275</v>
       </c>
       <c r="W3">
-        <v>0.3359856703386322</v>
+        <v>0.1132001448011923</v>
       </c>
       <c r="X3">
-        <v>0.005738715325018062</v>
+        <v>0.01015205241744275</v>
       </c>
       <c r="Y3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="Z3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AA3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="AB3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="AC3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AD3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="AE3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="AF3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AG3">
-        <v>0.006442998431046862</v>
+        <v>0.01067099286858934</v>
       </c>
       <c r="AH3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
       <c r="AI3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AJ3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
       <c r="AK3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
       <c r="AL3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AM3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
       <c r="AN3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="AO3">
-        <v>0.3338558167167581</v>
+        <v>0.1697429054257266</v>
       </c>
       <c r="AP3">
-        <v>0.005854187974434026</v>
+        <v>0.01658794603533465</v>
       </c>
       <c r="AQ3">
-        <v>0.006578235638616182</v>
+        <v>0.01070443511019443</v>
       </c>
       <c r="AR3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AS3">
-        <v>0.006578235638616182</v>
+        <v>0.01070443511019443</v>
       </c>
       <c r="AT3">
-        <v>0.006578235638616182</v>
+        <v>0.01070443511019443</v>
       </c>
       <c r="AU3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AV3">
-        <v>0.006578235638616182</v>
+        <v>0.01070443511019443</v>
       </c>
       <c r="AW3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
       <c r="AX3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="AY3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
       <c r="AZ3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
       <c r="BA3">
-        <v>0.3402453775823806</v>
+        <v>0.0001146235521235521</v>
       </c>
       <c r="BB3">
-        <v>0.004272412788252482</v>
+        <v>0.005896224706203615</v>
       </c>
     </row>
     <row r="4" spans="1:54">
       <c r="A4">
-        <v>0.005413263642548172</v>
+        <v>0.009409580673869889</v>
       </c>
       <c r="B4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="C4">
-        <v>0.005413263642548172</v>
+        <v>0.009409580673869889</v>
       </c>
       <c r="D4">
-        <v>0.005413263642548172</v>
+        <v>0.009409580673869889</v>
       </c>
       <c r="E4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="F4">
-        <v>0.005413263642548172</v>
+        <v>0.009409580673869889</v>
       </c>
       <c r="G4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="H4">
-        <v>0.1648490742215563</v>
+        <v>0.3388185924116158</v>
       </c>
       <c r="I4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="J4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="K4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="L4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="M4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="N4">
-        <v>0.1648490742215563</v>
+        <v>0.3388185924116158</v>
       </c>
       <c r="O4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="P4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="Q4">
-        <v>0.1648490742215563</v>
+        <v>0.3388185924116158</v>
       </c>
       <c r="R4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="S4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="T4">
-        <v>0.1648490742215563</v>
+        <v>0.3388185924116158</v>
       </c>
       <c r="U4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="V4">
-        <v>0.003797826962670339</v>
+        <v>0.01001410428649459</v>
       </c>
       <c r="W4">
-        <v>0.1825732315371447</v>
+        <v>0.3656027125343897</v>
       </c>
       <c r="X4">
-        <v>0.003797826962670339</v>
+        <v>0.01001410428649459</v>
       </c>
       <c r="Y4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="Z4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AA4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="AB4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="AC4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AD4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="AE4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="AF4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AG4">
-        <v>0.004180966898970304</v>
+        <v>0.01191542503805678</v>
       </c>
       <c r="AH4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
       <c r="AI4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AJ4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
       <c r="AK4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
       <c r="AL4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AM4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
       <c r="AN4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="AO4">
-        <v>0.1648490742215563</v>
+        <v>0.3388185924116158</v>
       </c>
       <c r="AP4">
-        <v>0.003498571737094966</v>
+        <v>0.01141231700844677</v>
       </c>
       <c r="AQ4">
-        <v>0.003770201317777681</v>
+        <v>0.01275070649278574</v>
       </c>
       <c r="AR4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AS4">
-        <v>0.003770201317777681</v>
+        <v>0.01275070649278574</v>
       </c>
       <c r="AT4">
-        <v>0.003770201317777681</v>
+        <v>0.01275070649278574</v>
       </c>
       <c r="AU4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AV4">
-        <v>0.003770201317777681</v>
+        <v>0.01275070649278574</v>
       </c>
       <c r="AW4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
       <c r="AX4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="AY4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
       <c r="AZ4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
       <c r="BA4">
-        <v>0.2180215461683213</v>
+        <v>0.4191709527799375</v>
       </c>
       <c r="BB4">
-        <v>0.003181174702858095</v>
+        <v>0.005512356422394117</v>
       </c>
     </row>
     <row r="5" spans="1:54">
       <c r="A5">
-        <v>0.004789240476757439</v>
+        <v>0.004730266210747842</v>
       </c>
       <c r="B5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="C5">
-        <v>0.004789240476757439</v>
+        <v>0.004730266210747842</v>
       </c>
       <c r="D5">
-        <v>0.004789240476757439</v>
+        <v>0.004730266210747842</v>
       </c>
       <c r="E5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="F5">
-        <v>0.004789240476757439</v>
+        <v>0.004730266210747842</v>
       </c>
       <c r="G5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="H5">
-        <v>0.1205545666743273</v>
+        <v>0.1535027570230704</v>
       </c>
       <c r="I5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="J5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="K5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="L5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="M5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="N5">
-        <v>0.1205545666743273</v>
+        <v>0.1535027570230704</v>
       </c>
       <c r="O5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="P5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="Q5">
-        <v>0.1205545666743273</v>
+        <v>0.1535027570230704</v>
       </c>
       <c r="R5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="S5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="T5">
-        <v>0.1205545666743273</v>
+        <v>0.1535027570230704</v>
       </c>
       <c r="U5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="V5">
-        <v>0.00424410917389367</v>
+        <v>0.00753772381756907</v>
       </c>
       <c r="W5">
-        <v>0.131985155217367</v>
+        <v>0.1690100650517203</v>
       </c>
       <c r="X5">
-        <v>0.00424410917389367</v>
+        <v>0.00753772381756907</v>
       </c>
       <c r="Y5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="Z5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AA5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="AB5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="AC5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AD5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="AE5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="AF5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AG5">
-        <v>0.004585937853419563</v>
+        <v>0.007650147053398483</v>
       </c>
       <c r="AH5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
       <c r="AI5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AJ5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
       <c r="AK5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
       <c r="AL5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AM5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
       <c r="AN5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="AO5">
-        <v>0.1205545666743273</v>
+        <v>0.1535027570230704</v>
       </c>
       <c r="AP5">
-        <v>0.004636429019548354</v>
+        <v>0.008556719398943676</v>
       </c>
       <c r="AQ5">
-        <v>0.004518170312306937</v>
+        <v>0.008623440667615362</v>
       </c>
       <c r="AR5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AS5">
-        <v>0.004518170312306937</v>
+        <v>0.008623440667615362</v>
       </c>
       <c r="AT5">
-        <v>0.004518170312306937</v>
+        <v>0.008623440667615362</v>
       </c>
       <c r="AU5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AV5">
-        <v>0.004518170312306937</v>
+        <v>0.008623440667615362</v>
       </c>
       <c r="AW5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
       <c r="AX5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="AY5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
       <c r="AZ5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
       <c r="BA5">
-        <v>0.1548463323034465</v>
+        <v>0.20002468110902</v>
       </c>
       <c r="BB5">
-        <v>0.00336429189201454</v>
+        <v>0.006803379555222943</v>
       </c>
     </row>
     <row r="6" spans="1:54">
       <c r="A6">
-        <v>0.004119109618312391</v>
+        <v>0.006185850092295575</v>
       </c>
       <c r="B6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="C6">
-        <v>0.004119109618312391</v>
+        <v>0.006185850092295575</v>
       </c>
       <c r="D6">
-        <v>0.004119109618312391</v>
+        <v>0.006185850092295575</v>
       </c>
       <c r="E6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="F6">
-        <v>0.004119109618312391</v>
+        <v>0.006185850092295575</v>
       </c>
       <c r="G6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="H6">
-        <v>0.1485869724678432</v>
+        <v>0.1807878729936434</v>
       </c>
       <c r="I6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="J6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="K6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="L6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="M6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="N6">
-        <v>0.1485869724678432</v>
+        <v>0.1807878729936434</v>
       </c>
       <c r="O6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="P6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="Q6">
-        <v>0.1485869724678432</v>
+        <v>0.1807878729936434</v>
       </c>
       <c r="R6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="S6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="T6">
-        <v>0.1485869724678432</v>
+        <v>0.1807878729936434</v>
       </c>
       <c r="U6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="V6">
-        <v>0.003936186909500405</v>
+        <v>0.00570674854429134</v>
       </c>
       <c r="W6">
-        <v>0.1229506605026612</v>
+        <v>0.157841451771241</v>
       </c>
       <c r="X6">
-        <v>0.003936186909500405</v>
+        <v>0.00570674854429134</v>
       </c>
       <c r="Y6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="Z6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AA6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="AB6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="AC6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AD6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="AE6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="AF6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AG6">
-        <v>0.004416967892344595</v>
+        <v>0.006587655188362998</v>
       </c>
       <c r="AH6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
       <c r="AI6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AJ6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
       <c r="AK6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
       <c r="AL6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AM6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
       <c r="AN6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="AO6">
-        <v>0.1485869724678432</v>
+        <v>0.1807878729936434</v>
       </c>
       <c r="AP6">
-        <v>0.004031134973236498</v>
+        <v>0.004732336266869595</v>
       </c>
       <c r="AQ6">
-        <v>0.004516253983688661</v>
+        <v>0.006721590220385473</v>
       </c>
       <c r="AR6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AS6">
-        <v>0.004516253983688661</v>
+        <v>0.006721590220385473</v>
       </c>
       <c r="AT6">
-        <v>0.004516253983688661</v>
+        <v>0.006721590220385473</v>
       </c>
       <c r="AU6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AV6">
-        <v>0.004516253983688661</v>
+        <v>0.006721590220385473</v>
       </c>
       <c r="AW6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
       <c r="AX6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="AY6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
       <c r="AZ6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
       <c r="BA6">
-        <v>0.07167803657229711</v>
+        <v>0.1119486093264362</v>
       </c>
       <c r="BB6">
-        <v>0.00292715091194398</v>
+        <v>0.004432141394858894</v>
       </c>
     </row>
     <row r="7" spans="1:54">
       <c r="A7">
-        <v>0.00349917072984269</v>
+        <v>0.006141093498466928</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.00349917072984269</v>
+        <v>0.006141093498466928</v>
       </c>
       <c r="D7">
-        <v>0.00349917072984269</v>
+        <v>0.006141093498466928</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.00349917072984269</v>
+        <v>0.006141093498466928</v>
       </c>
       <c r="G7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="H7">
-        <v>0.03706360975065923</v>
+        <v>0.05751089640026903</v>
       </c>
       <c r="I7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="J7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="M7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="N7">
-        <v>0.03706360975065923</v>
+        <v>0.05751089640026903</v>
       </c>
       <c r="O7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="P7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="Q7">
-        <v>0.03706360975065923</v>
+        <v>0.05751089640026903</v>
       </c>
       <c r="R7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="S7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="T7">
-        <v>0.03706360975065923</v>
+        <v>0.05751089640026903</v>
       </c>
       <c r="U7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="V7">
-        <v>0.003708715660526274</v>
+        <v>0.00572792679572471</v>
       </c>
       <c r="W7">
-        <v>0.024747281017814</v>
+        <v>0.0383788054508872</v>
       </c>
       <c r="X7">
-        <v>0.003708715660526274</v>
+        <v>0.00572792679572471</v>
       </c>
       <c r="Y7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="Z7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="AB7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="AE7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.004177719588623684</v>
+        <v>0.006501067766784065</v>
       </c>
       <c r="AH7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
       <c r="AK7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
       <c r="AL7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
       <c r="AN7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="AO7">
-        <v>0.03706360975065923</v>
+        <v>0.05751089640026903</v>
       </c>
       <c r="AP7">
-        <v>0.00341847216176009</v>
+        <v>0.005726529599075309</v>
       </c>
       <c r="AQ7">
-        <v>0.004403902541550681</v>
+        <v>0.006621059189556445</v>
       </c>
       <c r="AR7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.004403902541550681</v>
+        <v>0.006621059189556445</v>
       </c>
       <c r="AT7">
-        <v>0.004403902541550681</v>
+        <v>0.006621059189556445</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.004403902541550681</v>
+        <v>0.006621059189556445</v>
       </c>
       <c r="AW7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
       <c r="AZ7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
       <c r="BA7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB7">
-        <v>0.002915829553714546</v>
+        <v>0.004182343451930697</v>
       </c>
     </row>
     <row r="8" spans="1:54">
       <c r="A8">
-        <v>0.001439616018507967</v>
+        <v>0.00364252475991092</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.001439616018507967</v>
+        <v>0.00364252475991092</v>
       </c>
       <c r="D8">
-        <v>0.001439616018507967</v>
+        <v>0.00364252475991092</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.001439616018507967</v>
+        <v>0.00364252475991092</v>
       </c>
       <c r="G8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="H8">
-        <v>0.02198347762265828</v>
+        <v>0.02324368150239949</v>
       </c>
       <c r="I8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="J8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="M8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="N8">
-        <v>0.02198347762265828</v>
+        <v>0.02324368150239949</v>
       </c>
       <c r="O8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="P8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="Q8">
-        <v>0.02198347762265828</v>
+        <v>0.02324368150239949</v>
       </c>
       <c r="R8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="S8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="T8">
-        <v>0.02198347762265828</v>
+        <v>0.02324368150239949</v>
       </c>
       <c r="U8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="V8">
-        <v>0.002159886817805626</v>
+        <v>0.003259040051800573</v>
       </c>
       <c r="W8">
-        <v>0.01469385959914671</v>
+        <v>0.01553399551897418</v>
       </c>
       <c r="X8">
-        <v>0.002159886817805626</v>
+        <v>0.003259040051800573</v>
       </c>
       <c r="Y8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="Z8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="AB8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="AE8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.002217044442022792</v>
+        <v>0.003803107096720129</v>
       </c>
       <c r="AH8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
       <c r="AK8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
       <c r="AL8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
       <c r="AN8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="AO8">
-        <v>0.02198347762265828</v>
+        <v>0.02324368150239949</v>
       </c>
       <c r="AP8">
-        <v>0.002802853103701819</v>
+        <v>0.001402276693471218</v>
       </c>
       <c r="AQ8">
-        <v>0.002476187249861067</v>
+        <v>0.0038566345423232</v>
       </c>
       <c r="AR8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002476187249861067</v>
+        <v>0.0038566345423232</v>
       </c>
       <c r="AT8">
-        <v>0.002476187249861067</v>
+        <v>0.0038566345423232</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.002476187249861067</v>
+        <v>0.0038566345423232</v>
       </c>
       <c r="AW8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
       <c r="AZ8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
       <c r="BA8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB8">
-        <v>0.001724088426423199</v>
+        <v>0.003099287641126138</v>
       </c>
     </row>
     <row r="9" spans="1:54">
       <c r="A9">
-        <v>0.001129646574273117</v>
+        <v>0.001715251307115534</v>
       </c>
       <c r="B9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.001129646574273117</v>
+        <v>0.001715251307115534</v>
       </c>
       <c r="D9">
-        <v>0.001129646574273117</v>
+        <v>0.001715251307115534</v>
       </c>
       <c r="E9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.001129646574273117</v>
+        <v>0.001715251307115534</v>
       </c>
       <c r="G9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H9">
-        <v>0.0001518968383129674</v>
+        <v>0.004885643417810262</v>
       </c>
       <c r="I9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="K9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="M9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N9">
-        <v>0.0001518968383129674</v>
+        <v>0.004885643417810262</v>
       </c>
       <c r="O9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q9">
-        <v>0.0001518968383129674</v>
+        <v>0.004885643417810262</v>
       </c>
       <c r="R9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T9">
-        <v>0.0001518968383129674</v>
+        <v>0.004885643417810262</v>
       </c>
       <c r="U9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V9">
-        <v>0.00102508978087982</v>
+        <v>0.001367094210241216</v>
       </c>
       <c r="W9">
-        <v>0.0001394724095831623</v>
+        <v>0.003295303462581358</v>
       </c>
       <c r="X9">
-        <v>0.00102508978087982</v>
+        <v>0.001367094210241216</v>
       </c>
       <c r="Y9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="Z9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="AB9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="AC9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="AE9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.001208126731188766</v>
+        <v>0.001747906564358462</v>
       </c>
       <c r="AH9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
       <c r="AK9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
       <c r="AL9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
       <c r="AN9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AO9">
-        <v>0.0001518968383129674</v>
+        <v>0.004885643417810262</v>
       </c>
       <c r="AP9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AQ9">
-        <v>0.001234286783493983</v>
+        <v>0.001758791650106104</v>
       </c>
       <c r="AR9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001234286783493983</v>
+        <v>0.001758791650106104</v>
       </c>
       <c r="AT9">
-        <v>0.001234286783493983</v>
+        <v>0.001758791650106104</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.001234286783493983</v>
+        <v>0.001758791650106104</v>
       </c>
       <c r="AW9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
       <c r="AZ9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
       <c r="BA9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB9">
-        <v>0.0008077252184532221</v>
+        <v>0.001196550853702675</v>
       </c>
     </row>
     <row r="10" spans="1:54">
       <c r="A10">
-        <v>0.03239724877960055</v>
+        <v>0.003324717093018974</v>
       </c>
       <c r="B10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.03239724877960055</v>
+        <v>0.003324717093018974</v>
       </c>
       <c r="D10">
-        <v>0.03239724877960055</v>
+        <v>0.003324717093018974</v>
       </c>
       <c r="E10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.03239724877960055</v>
+        <v>0.003324717093018974</v>
       </c>
       <c r="G10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="I10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="K10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="M10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="O10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="R10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="U10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V10">
-        <v>0.01826206209161527</v>
+        <v>0.0008766622095328988</v>
       </c>
       <c r="W10">
-        <v>0.0001394724095831623</v>
+        <v>0.0001465043978653304</v>
       </c>
       <c r="X10">
-        <v>0.01826206209161527</v>
+        <v>0.0008766622095328988</v>
       </c>
       <c r="Y10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="Z10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="AB10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="AC10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="AE10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.02271664407576451</v>
+        <v>0.001405514187186772</v>
       </c>
       <c r="AH10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AK10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AL10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AN10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AO10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001624448207362195</v>
       </c>
       <c r="AP10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AQ10">
-        <v>0.0194897758411525</v>
+        <v>0.0007657798852427053</v>
       </c>
       <c r="AR10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.0194897758411525</v>
+        <v>0.0007657798852427053</v>
       </c>
       <c r="AT10">
-        <v>0.0194897758411525</v>
+        <v>0.0007657798852427053</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.0194897758411525</v>
+        <v>0.0007657798852427053</v>
       </c>
       <c r="AW10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AZ10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="BA10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update stubble sim (bit different due to changes affecting sgen, i assume)
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,1642 +348,1642 @@
   <sheetData>
     <row r="1" spans="1:54">
       <c r="A1">
-        <v>0.04887908386567361</v>
+        <v>0.03545577386460821</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.04887908386567361</v>
+        <v>0.03545577386460821</v>
       </c>
       <c r="D1">
-        <v>0.04887908386567361</v>
+        <v>0.03545577386460821</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.04887908386567361</v>
+        <v>0.03545577386460821</v>
       </c>
       <c r="G1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="H1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="I1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="J1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="M1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="N1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="O1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="P1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="Q1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="R1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="S1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="T1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="U1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="V1">
-        <v>0.03003653031203316</v>
+        <v>0.006653353295715964</v>
       </c>
       <c r="W1">
-        <v>0.0001394724095831623</v>
+        <v>0.0001400348751304675</v>
       </c>
       <c r="X1">
-        <v>0.03003653031203316</v>
+        <v>0.006653353295715964</v>
       </c>
       <c r="Y1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="Z1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="AB1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="AE1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.03550473685604939</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="AH1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AK1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AL1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AN1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="AO1">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="AP1">
-        <v>0.03528994484009806</v>
+        <v>0.001175430265398609</v>
       </c>
       <c r="AQ1">
-        <v>0.03104662118617465</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AR1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS1">
-        <v>0.03104662118617465</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AT1">
-        <v>0.03104662118617465</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.03104662118617465</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AW1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AZ1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="BA1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB1">
-        <v>0.01647340995996823</v>
+        <v>0.0001648236055669436</v>
       </c>
     </row>
     <row r="2" spans="1:54">
       <c r="A2">
-        <v>0.006729471584568375</v>
+        <v>0.01331514114706135</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.006729471584568375</v>
+        <v>0.01331514114706135</v>
       </c>
       <c r="D2">
-        <v>0.006729471584568375</v>
+        <v>0.01331514114706135</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.006729471584568375</v>
+        <v>0.01331514114706135</v>
       </c>
       <c r="G2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="H2">
-        <v>0.1726507920312587</v>
+        <v>0.1512910435046977</v>
       </c>
       <c r="I2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="J2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="M2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="N2">
-        <v>0.1726507920312587</v>
+        <v>0.1512910435046977</v>
       </c>
       <c r="O2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="P2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="Q2">
-        <v>0.1726507920312587</v>
+        <v>0.1512910435046977</v>
       </c>
       <c r="R2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="S2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="T2">
-        <v>0.1726507920312587</v>
+        <v>0.1512910435046977</v>
       </c>
       <c r="U2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="V2">
-        <v>0.007800672337179483</v>
+        <v>0.01258396833395928</v>
       </c>
       <c r="W2">
-        <v>0.115138735871547</v>
+        <v>0.1008989035205063</v>
       </c>
       <c r="X2">
-        <v>0.007800672337179483</v>
+        <v>0.01258396833395928</v>
       </c>
       <c r="Y2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="Z2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="AB2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="AE2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.007971046728872989</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="AH2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
       <c r="AK2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
       <c r="AL2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
       <c r="AN2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="AO2">
-        <v>0.1726507920312587</v>
+        <v>0.1512910435046977</v>
       </c>
       <c r="AP2">
-        <v>0.008613748025750392</v>
+        <v>0.02262491053503307</v>
       </c>
       <c r="AQ2">
-        <v>0.008384905110307858</v>
+        <v>0.01306272931671001</v>
       </c>
       <c r="AR2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS2">
-        <v>0.008384905110307858</v>
+        <v>0.01306272931671001</v>
       </c>
       <c r="AT2">
-        <v>0.008384905110307858</v>
+        <v>0.01306272931671001</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.008384905110307858</v>
+        <v>0.01306272931671001</v>
       </c>
       <c r="AW2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
       <c r="AZ2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
       <c r="BA2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB2">
-        <v>0.007053385709507021</v>
+        <v>0.006479769352745266</v>
       </c>
     </row>
     <row r="3" spans="1:54">
       <c r="A3">
-        <v>0.0060372868083389</v>
+        <v>0.01051194564093447</v>
       </c>
       <c r="B3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="C3">
-        <v>0.0060372868083389</v>
+        <v>0.01051194564093447</v>
       </c>
       <c r="D3">
-        <v>0.0060372868083389</v>
+        <v>0.01051194564093447</v>
       </c>
       <c r="E3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="F3">
-        <v>0.0060372868083389</v>
+        <v>0.01051194564093447</v>
       </c>
       <c r="G3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="H3">
-        <v>0.3338558167167581</v>
+        <v>0.3311108033259505</v>
       </c>
       <c r="I3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="J3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="K3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="L3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="M3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="N3">
-        <v>0.3338558167167581</v>
+        <v>0.3311108033259505</v>
       </c>
       <c r="O3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="P3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="Q3">
-        <v>0.3338558167167581</v>
+        <v>0.3311108033259505</v>
       </c>
       <c r="R3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="S3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="T3">
-        <v>0.3338558167167581</v>
+        <v>0.3311108033259505</v>
       </c>
       <c r="U3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="V3">
-        <v>0.005738715325018062</v>
+        <v>0.01272778309089564</v>
       </c>
       <c r="W3">
-        <v>0.3359856703386322</v>
+        <v>0.3238510920252826</v>
       </c>
       <c r="X3">
-        <v>0.005738715325018062</v>
+        <v>0.01272778309089564</v>
       </c>
       <c r="Y3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="Z3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AA3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="AB3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="AC3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AD3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="AE3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="AF3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AG3">
-        <v>0.006442998431046862</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="AH3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
       <c r="AI3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AJ3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
       <c r="AK3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
       <c r="AL3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AM3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
       <c r="AN3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="AO3">
-        <v>0.3338558167167581</v>
+        <v>0.3311108033259505</v>
       </c>
       <c r="AP3">
-        <v>0.005854187974434026</v>
+        <v>0.01374566675163806</v>
       </c>
       <c r="AQ3">
-        <v>0.006578235638616182</v>
+        <v>0.01491526926391605</v>
       </c>
       <c r="AR3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AS3">
-        <v>0.006578235638616182</v>
+        <v>0.01491526926391605</v>
       </c>
       <c r="AT3">
-        <v>0.006578235638616182</v>
+        <v>0.01491526926391605</v>
       </c>
       <c r="AU3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AV3">
-        <v>0.006578235638616182</v>
+        <v>0.01491526926391605</v>
       </c>
       <c r="AW3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
       <c r="AX3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="AY3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
       <c r="AZ3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
       <c r="BA3">
-        <v>0.3402453775823806</v>
+        <v>0.309331669423947</v>
       </c>
       <c r="BB3">
-        <v>0.004272412788252482</v>
+        <v>0.01004553072597439</v>
       </c>
     </row>
     <row r="4" spans="1:54">
       <c r="A4">
-        <v>0.005413263642548172</v>
+        <v>0.01218671493848782</v>
       </c>
       <c r="B4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="C4">
-        <v>0.005413263642548172</v>
+        <v>0.01218671493848782</v>
       </c>
       <c r="D4">
-        <v>0.005413263642548172</v>
+        <v>0.01218671493848782</v>
       </c>
       <c r="E4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="F4">
-        <v>0.005413263642548172</v>
+        <v>0.01218671493848782</v>
       </c>
       <c r="G4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="H4">
-        <v>0.1648490742215563</v>
+        <v>0.1803031754725153</v>
       </c>
       <c r="I4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="J4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="K4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="L4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="M4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="N4">
-        <v>0.1648490742215563</v>
+        <v>0.1803031754725153</v>
       </c>
       <c r="O4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="P4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="Q4">
-        <v>0.1648490742215563</v>
+        <v>0.1803031754725153</v>
       </c>
       <c r="R4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="S4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="T4">
-        <v>0.1648490742215563</v>
+        <v>0.1803031754725153</v>
       </c>
       <c r="U4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="V4">
-        <v>0.003797826962670339</v>
+        <v>0.009587958428762032</v>
       </c>
       <c r="W4">
-        <v>0.1825732315371447</v>
+        <v>0.2002385385131124</v>
       </c>
       <c r="X4">
-        <v>0.003797826962670339</v>
+        <v>0.009587958428762032</v>
       </c>
       <c r="Y4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="Z4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AA4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="AB4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="AC4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AD4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="AE4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="AF4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AG4">
-        <v>0.004180966898970304</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="AH4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
       <c r="AI4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AJ4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
       <c r="AK4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
       <c r="AL4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AM4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
       <c r="AN4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="AO4">
-        <v>0.1648490742215563</v>
+        <v>0.1803031754725153</v>
       </c>
       <c r="AP4">
-        <v>0.003498571737094966</v>
+        <v>0.008830914452507423</v>
       </c>
       <c r="AQ4">
-        <v>0.003770201317777681</v>
+        <v>0.01002434804893105</v>
       </c>
       <c r="AR4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AS4">
-        <v>0.003770201317777681</v>
+        <v>0.01002434804893105</v>
       </c>
       <c r="AT4">
-        <v>0.003770201317777681</v>
+        <v>0.01002434804893105</v>
       </c>
       <c r="AU4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AV4">
-        <v>0.003770201317777681</v>
+        <v>0.01002434804893105</v>
       </c>
       <c r="AW4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
       <c r="AX4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="AY4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
       <c r="AZ4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
       <c r="BA4">
-        <v>0.2180215461683213</v>
+        <v>0.2401092645943063</v>
       </c>
       <c r="BB4">
-        <v>0.003181174702858095</v>
+        <v>0.008012517731772919</v>
       </c>
     </row>
     <row r="5" spans="1:54">
       <c r="A5">
-        <v>0.004789240476757439</v>
+        <v>0.009680657902577198</v>
       </c>
       <c r="B5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="C5">
-        <v>0.004789240476757439</v>
+        <v>0.009680657902577198</v>
       </c>
       <c r="D5">
-        <v>0.004789240476757439</v>
+        <v>0.009680657902577198</v>
       </c>
       <c r="E5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="F5">
-        <v>0.004789240476757439</v>
+        <v>0.009680657902577198</v>
       </c>
       <c r="G5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="H5">
-        <v>0.1205545666743273</v>
+        <v>0.1279935295394772</v>
       </c>
       <c r="I5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="J5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="K5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="L5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="M5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="N5">
-        <v>0.1205545666743273</v>
+        <v>0.1279935295394772</v>
       </c>
       <c r="O5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="P5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="Q5">
-        <v>0.1205545666743273</v>
+        <v>0.1279935295394772</v>
       </c>
       <c r="R5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="S5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="T5">
-        <v>0.1205545666743273</v>
+        <v>0.1279935295394772</v>
       </c>
       <c r="U5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="V5">
-        <v>0.00424410917389367</v>
+        <v>0.008955780224535791</v>
       </c>
       <c r="W5">
-        <v>0.131985155217367</v>
+        <v>0.1369294622163093</v>
       </c>
       <c r="X5">
-        <v>0.00424410917389367</v>
+        <v>0.008955780224535791</v>
       </c>
       <c r="Y5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="Z5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AA5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="AB5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="AC5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AD5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="AE5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="AF5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AG5">
-        <v>0.004585937853419563</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="AH5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
       <c r="AI5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AJ5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
       <c r="AK5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
       <c r="AL5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AM5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
       <c r="AN5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="AO5">
-        <v>0.1205545666743273</v>
+        <v>0.1279935295394772</v>
       </c>
       <c r="AP5">
-        <v>0.004636429019548354</v>
+        <v>0.009385874096320437</v>
       </c>
       <c r="AQ5">
-        <v>0.004518170312306937</v>
+        <v>0.01019874235380429</v>
       </c>
       <c r="AR5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AS5">
-        <v>0.004518170312306937</v>
+        <v>0.01019874235380429</v>
       </c>
       <c r="AT5">
-        <v>0.004518170312306937</v>
+        <v>0.01019874235380429</v>
       </c>
       <c r="AU5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AV5">
-        <v>0.004518170312306937</v>
+        <v>0.01019874235380429</v>
       </c>
       <c r="AW5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
       <c r="AX5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="AY5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
       <c r="AZ5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
       <c r="BA5">
-        <v>0.1548463323034465</v>
+        <v>0.1548013275699734</v>
       </c>
       <c r="BB5">
-        <v>0.00336429189201454</v>
+        <v>0.006513851255720016</v>
       </c>
     </row>
     <row r="6" spans="1:54">
       <c r="A6">
-        <v>0.004119109618312391</v>
+        <v>0.007503798698266477</v>
       </c>
       <c r="B6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="C6">
-        <v>0.004119109618312391</v>
+        <v>0.007503798698266477</v>
       </c>
       <c r="D6">
-        <v>0.004119109618312391</v>
+        <v>0.007503798698266477</v>
       </c>
       <c r="E6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="F6">
-        <v>0.004119109618312391</v>
+        <v>0.007503798698266477</v>
       </c>
       <c r="G6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="H6">
-        <v>0.1485869724678432</v>
+        <v>0.1494313824275443</v>
       </c>
       <c r="I6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="J6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="K6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="L6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="M6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="N6">
-        <v>0.1485869724678432</v>
+        <v>0.1494313824275443</v>
       </c>
       <c r="O6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="P6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="Q6">
-        <v>0.1485869724678432</v>
+        <v>0.1494313824275443</v>
       </c>
       <c r="R6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="S6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="T6">
-        <v>0.1485869724678432</v>
+        <v>0.1494313824275443</v>
       </c>
       <c r="U6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="V6">
-        <v>0.003936186909500405</v>
+        <v>0.007022701431492167</v>
       </c>
       <c r="W6">
-        <v>0.1229506605026612</v>
+        <v>0.125006887507649</v>
       </c>
       <c r="X6">
-        <v>0.003936186909500405</v>
+        <v>0.007022701431492167</v>
       </c>
       <c r="Y6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="Z6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AA6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="AB6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="AC6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AD6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="AE6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="AF6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AG6">
-        <v>0.004416967892344595</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="AH6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
       <c r="AI6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AJ6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
       <c r="AK6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
       <c r="AL6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AM6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
       <c r="AN6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="AO6">
-        <v>0.1485869724678432</v>
+        <v>0.1494313824275443</v>
       </c>
       <c r="AP6">
-        <v>0.004031134973236498</v>
+        <v>0.003394023396034468</v>
       </c>
       <c r="AQ6">
-        <v>0.004516253983688661</v>
+        <v>0.00826170616524438</v>
       </c>
       <c r="AR6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AS6">
-        <v>0.004516253983688661</v>
+        <v>0.00826170616524438</v>
       </c>
       <c r="AT6">
-        <v>0.004516253983688661</v>
+        <v>0.00826170616524438</v>
       </c>
       <c r="AU6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AV6">
-        <v>0.004516253983688661</v>
+        <v>0.00826170616524438</v>
       </c>
       <c r="AW6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
       <c r="AX6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="AY6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
       <c r="AZ6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
       <c r="BA6">
-        <v>0.07167803657229711</v>
+        <v>0.07615789766785841</v>
       </c>
       <c r="BB6">
-        <v>0.00292715091194398</v>
+        <v>0.006737984715205545</v>
       </c>
     </row>
     <row r="7" spans="1:54">
       <c r="A7">
-        <v>0.00349917072984269</v>
+        <v>0.004619230646090584</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.00349917072984269</v>
+        <v>0.004619230646090584</v>
       </c>
       <c r="D7">
-        <v>0.00349917072984269</v>
+        <v>0.004619230646090584</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.00349917072984269</v>
+        <v>0.004619230646090584</v>
       </c>
       <c r="G7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H7">
-        <v>0.03706360975065923</v>
+        <v>0.03729258762855925</v>
       </c>
       <c r="I7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="M7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N7">
-        <v>0.03706360975065923</v>
+        <v>0.03729258762855925</v>
       </c>
       <c r="O7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q7">
-        <v>0.03706360975065923</v>
+        <v>0.03729258762855925</v>
       </c>
       <c r="R7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T7">
-        <v>0.03706360975065923</v>
+        <v>0.03729258762855925</v>
       </c>
       <c r="U7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V7">
-        <v>0.003708715660526274</v>
+        <v>0.003249069490238883</v>
       </c>
       <c r="W7">
-        <v>0.024747281017814</v>
+        <v>0.02489993293641402</v>
       </c>
       <c r="X7">
-        <v>0.003708715660526274</v>
+        <v>0.003249069490238883</v>
       </c>
       <c r="Y7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="Z7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="AB7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="AE7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.004177719588623684</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="AH7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="AK7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="AL7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="AN7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AO7">
-        <v>0.03706360975065923</v>
+        <v>0.03729258762855925</v>
       </c>
       <c r="AP7">
-        <v>0.00341847216176009</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AQ7">
-        <v>0.004403902541550681</v>
+        <v>0.004977361601669884</v>
       </c>
       <c r="AR7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS7">
-        <v>0.004403902541550681</v>
+        <v>0.004977361601669884</v>
       </c>
       <c r="AT7">
-        <v>0.004403902541550681</v>
+        <v>0.004977361601669884</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.004403902541550681</v>
+        <v>0.004977361601669884</v>
       </c>
       <c r="AW7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="AZ7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="BA7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB7">
-        <v>0.002915829553714546</v>
+        <v>0.001503619736861317</v>
       </c>
     </row>
     <row r="8" spans="1:54">
       <c r="A8">
-        <v>0.001439616018507967</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.001439616018507967</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="D8">
-        <v>0.001439616018507967</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.001439616018507967</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="G8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H8">
-        <v>0.02198347762265828</v>
+        <v>0.02211925649135387</v>
       </c>
       <c r="I8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="M8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N8">
-        <v>0.02198347762265828</v>
+        <v>0.02211925649135387</v>
       </c>
       <c r="O8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q8">
-        <v>0.02198347762265828</v>
+        <v>0.02211925649135387</v>
       </c>
       <c r="R8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T8">
-        <v>0.02198347762265828</v>
+        <v>0.02211925649135387</v>
       </c>
       <c r="U8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V8">
-        <v>0.002159886817805626</v>
+        <v>0.0003698114948764792</v>
       </c>
       <c r="W8">
-        <v>0.01469385959914671</v>
+        <v>0.01478437884494376</v>
       </c>
       <c r="X8">
-        <v>0.002159886817805626</v>
+        <v>0.0003698114948764792</v>
       </c>
       <c r="Y8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="Z8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="AB8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="AE8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.002217044442022792</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="AH8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AK8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AL8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AN8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AO8">
-        <v>0.02198347762265828</v>
+        <v>0.02211925649135387</v>
       </c>
       <c r="AP8">
-        <v>0.002802853103701819</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AQ8">
-        <v>0.002476187249861067</v>
+        <v>0.0006129982931315117</v>
       </c>
       <c r="AR8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS8">
-        <v>0.002476187249861067</v>
+        <v>0.0006129982931315117</v>
       </c>
       <c r="AT8">
-        <v>0.002476187249861067</v>
+        <v>0.0006129982931315117</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.002476187249861067</v>
+        <v>0.0006129982931315117</v>
       </c>
       <c r="AW8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AZ8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="BA8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB8">
-        <v>0.001724088426423199</v>
+        <v>0.0001648236055669436</v>
       </c>
     </row>
     <row r="9" spans="1:54">
       <c r="A9">
-        <v>0.001129646574273117</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="B9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C9">
-        <v>0.001129646574273117</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="D9">
-        <v>0.001129646574273117</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="E9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F9">
-        <v>0.001129646574273117</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="G9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H9">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="I9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="K9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="M9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N9">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="O9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q9">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="R9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T9">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="U9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V9">
-        <v>0.00102508978087982</v>
+        <v>0.0002136034642349976</v>
       </c>
       <c r="W9">
-        <v>0.0001394724095831623</v>
+        <v>0.0001400348751304675</v>
       </c>
       <c r="X9">
-        <v>0.00102508978087982</v>
+        <v>0.0002136034642349976</v>
       </c>
       <c r="Y9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="Z9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AB9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AC9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AE9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AF9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG9">
-        <v>0.001208126731188766</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AH9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AK9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AL9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AN9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AO9">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="AP9">
-        <v>0.0007276711044972345</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AQ9">
-        <v>0.001234286783493983</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AR9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS9">
-        <v>0.001234286783493983</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AT9">
-        <v>0.001234286783493983</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AU9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV9">
-        <v>0.001234286783493983</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AW9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AZ9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="BA9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB9">
-        <v>0.0008077252184532221</v>
+        <v>0.0001648236055669436</v>
       </c>
     </row>
     <row r="10" spans="1:54">
       <c r="A10">
-        <v>0.03239724877960055</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="B10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C10">
-        <v>0.03239724877960055</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="D10">
-        <v>0.03239724877960055</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="E10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F10">
-        <v>0.03239724877960055</v>
+        <v>0.000235106866757617</v>
       </c>
       <c r="G10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="I10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="K10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="M10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="O10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="R10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="U10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V10">
-        <v>0.01826206209161527</v>
+        <v>0.0002136034642349976</v>
       </c>
       <c r="W10">
-        <v>0.0001394724095831623</v>
+        <v>0.0001400348751304675</v>
       </c>
       <c r="X10">
-        <v>0.01826206209161527</v>
+        <v>0.0002136034642349976</v>
       </c>
       <c r="Y10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="Z10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AA10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AB10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AC10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AE10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AF10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG10">
-        <v>0.02271664407576451</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AH10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AK10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AL10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AN10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AO10">
-        <v>0.0001518968383129674</v>
+        <v>0.0001527405366339252</v>
       </c>
       <c r="AP10">
-        <v>0.01342113595031052</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AQ10">
-        <v>0.0194897758411525</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AR10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AS10">
-        <v>0.0194897758411525</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AT10">
-        <v>0.0194897758411525</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AU10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV10">
-        <v>0.0194897758411525</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AW10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AZ10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="BA10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB10">
-        <v>0.01177336119396915</v>
+        <v>0.0001648236055669436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add legume fodder land use. No profit change because I didnt add any rotation.
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -340,13 +340,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB10"/>
+  <dimension ref="A1:BE10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:57">
       <c r="A1">
         <v>0.03545577386460821</v>
       </c>
@@ -411,22 +411,22 @@
         <v>0.001175430265398609</v>
       </c>
       <c r="V1">
+        <v>0.001175430265398609</v>
+      </c>
+      <c r="W1">
+        <v>0.0001527405366339252</v>
+      </c>
+      <c r="X1">
+        <v>0.001175430265398609</v>
+      </c>
+      <c r="Y1">
         <v>0.006653353295715964</v>
       </c>
-      <c r="W1">
+      <c r="Z1">
         <v>0.0001400348751304675</v>
       </c>
-      <c r="X1">
+      <c r="AA1">
         <v>0.006653353295715964</v>
-      </c>
-      <c r="Y1">
-        <v>0.01126709889836981</v>
-      </c>
-      <c r="Z1">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AA1">
-        <v>0.01126709889836981</v>
       </c>
       <c r="AB1">
         <v>0.01126709889836981</v>
@@ -447,13 +447,13 @@
         <v>0.01126709889836981</v>
       </c>
       <c r="AH1">
-        <v>0.0001648236055669436</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.0001648236055669436</v>
+        <v>0.01126709889836981</v>
       </c>
       <c r="AK1">
         <v>0.0001648236055669436</v>
@@ -465,22 +465,22 @@
         <v>0.0001648236055669436</v>
       </c>
       <c r="AN1">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="AO1">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AP1">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="AQ1">
         <v>0.001175430265398609</v>
       </c>
-      <c r="AO1">
+      <c r="AR1">
         <v>0.0001527405366339252</v>
       </c>
-      <c r="AP1">
+      <c r="AS1">
         <v>0.001175430265398609</v>
-      </c>
-      <c r="AQ1">
-        <v>0.003204207242957014</v>
-      </c>
-      <c r="AR1">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AS1">
-        <v>0.003204207242957014</v>
       </c>
       <c r="AT1">
         <v>0.003204207242957014</v>
@@ -492,13 +492,13 @@
         <v>0.003204207242957014</v>
       </c>
       <c r="AW1">
-        <v>0.0001648236055669436</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.0001648236055669436</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AZ1">
         <v>0.0001648236055669436</v>
@@ -509,8 +509,17 @@
       <c r="BB1">
         <v>0.0001648236055669436</v>
       </c>
+      <c r="BC1">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="BD1">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BE1">
+        <v>0.0001648236055669436</v>
+      </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:57">
       <c r="A2">
         <v>0.01331514114706135</v>
       </c>
@@ -575,22 +584,22 @@
         <v>0.02262491053503307</v>
       </c>
       <c r="V2">
+        <v>0.02262491053503307</v>
+      </c>
+      <c r="W2">
+        <v>0.1512910435046977</v>
+      </c>
+      <c r="X2">
+        <v>0.02262491053503307</v>
+      </c>
+      <c r="Y2">
         <v>0.01258396833395928</v>
       </c>
-      <c r="W2">
+      <c r="Z2">
         <v>0.1008989035205063</v>
       </c>
-      <c r="X2">
+      <c r="AA2">
         <v>0.01258396833395928</v>
-      </c>
-      <c r="Y2">
-        <v>0.01312583227429785</v>
-      </c>
-      <c r="Z2">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AA2">
-        <v>0.01312583227429785</v>
       </c>
       <c r="AB2">
         <v>0.01312583227429785</v>
@@ -611,13 +620,13 @@
         <v>0.01312583227429785</v>
       </c>
       <c r="AH2">
-        <v>0.006479769352745266</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.006479769352745266</v>
+        <v>0.01312583227429785</v>
       </c>
       <c r="AK2">
         <v>0.006479769352745266</v>
@@ -629,22 +638,22 @@
         <v>0.006479769352745266</v>
       </c>
       <c r="AN2">
+        <v>0.006479769352745266</v>
+      </c>
+      <c r="AO2">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AP2">
+        <v>0.006479769352745266</v>
+      </c>
+      <c r="AQ2">
         <v>0.02262491053503307</v>
       </c>
-      <c r="AO2">
+      <c r="AR2">
         <v>0.1512910435046977</v>
       </c>
-      <c r="AP2">
+      <c r="AS2">
         <v>0.02262491053503307</v>
-      </c>
-      <c r="AQ2">
-        <v>0.01306272931671001</v>
-      </c>
-      <c r="AR2">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AS2">
-        <v>0.01306272931671001</v>
       </c>
       <c r="AT2">
         <v>0.01306272931671001</v>
@@ -656,13 +665,13 @@
         <v>0.01306272931671001</v>
       </c>
       <c r="AW2">
-        <v>0.006479769352745266</v>
+        <v>0.01306272931671001</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.006479769352745266</v>
+        <v>0.01306272931671001</v>
       </c>
       <c r="AZ2">
         <v>0.006479769352745266</v>
@@ -673,8 +682,17 @@
       <c r="BB2">
         <v>0.006479769352745266</v>
       </c>
+      <c r="BC2">
+        <v>0.006479769352745266</v>
+      </c>
+      <c r="BD2">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BE2">
+        <v>0.006479769352745266</v>
+      </c>
     </row>
-    <row r="3" spans="1:54">
+    <row r="3" spans="1:57">
       <c r="A3">
         <v>0.01051194564093447</v>
       </c>
@@ -739,22 +757,22 @@
         <v>0.01374566675163806</v>
       </c>
       <c r="V3">
+        <v>0.01374566675163806</v>
+      </c>
+      <c r="W3">
+        <v>0.3311108033259505</v>
+      </c>
+      <c r="X3">
+        <v>0.01374566675163806</v>
+      </c>
+      <c r="Y3">
         <v>0.01272778309089564</v>
       </c>
-      <c r="W3">
+      <c r="Z3">
         <v>0.3238510920252826</v>
       </c>
-      <c r="X3">
+      <c r="AA3">
         <v>0.01272778309089564</v>
-      </c>
-      <c r="Y3">
-        <v>0.01381443835817066</v>
-      </c>
-      <c r="Z3">
-        <v>0.309331669423947</v>
-      </c>
-      <c r="AA3">
-        <v>0.01381443835817066</v>
       </c>
       <c r="AB3">
         <v>0.01381443835817066</v>
@@ -775,13 +793,13 @@
         <v>0.01381443835817066</v>
       </c>
       <c r="AH3">
-        <v>0.01004553072597439</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="AI3">
         <v>0.309331669423947</v>
       </c>
       <c r="AJ3">
-        <v>0.01004553072597439</v>
+        <v>0.01381443835817066</v>
       </c>
       <c r="AK3">
         <v>0.01004553072597439</v>
@@ -793,22 +811,22 @@
         <v>0.01004553072597439</v>
       </c>
       <c r="AN3">
+        <v>0.01004553072597439</v>
+      </c>
+      <c r="AO3">
+        <v>0.309331669423947</v>
+      </c>
+      <c r="AP3">
+        <v>0.01004553072597439</v>
+      </c>
+      <c r="AQ3">
         <v>0.01374566675163806</v>
       </c>
-      <c r="AO3">
+      <c r="AR3">
         <v>0.3311108033259505</v>
       </c>
-      <c r="AP3">
+      <c r="AS3">
         <v>0.01374566675163806</v>
-      </c>
-      <c r="AQ3">
-        <v>0.01491526926391605</v>
-      </c>
-      <c r="AR3">
-        <v>0.309331669423947</v>
-      </c>
-      <c r="AS3">
-        <v>0.01491526926391605</v>
       </c>
       <c r="AT3">
         <v>0.01491526926391605</v>
@@ -820,13 +838,13 @@
         <v>0.01491526926391605</v>
       </c>
       <c r="AW3">
-        <v>0.01004553072597439</v>
+        <v>0.01491526926391605</v>
       </c>
       <c r="AX3">
         <v>0.309331669423947</v>
       </c>
       <c r="AY3">
-        <v>0.01004553072597439</v>
+        <v>0.01491526926391605</v>
       </c>
       <c r="AZ3">
         <v>0.01004553072597439</v>
@@ -837,8 +855,17 @@
       <c r="BB3">
         <v>0.01004553072597439</v>
       </c>
+      <c r="BC3">
+        <v>0.01004553072597439</v>
+      </c>
+      <c r="BD3">
+        <v>0.309331669423947</v>
+      </c>
+      <c r="BE3">
+        <v>0.01004553072597439</v>
+      </c>
     </row>
-    <row r="4" spans="1:54">
+    <row r="4" spans="1:57">
       <c r="A4">
         <v>0.01218671493848782</v>
       </c>
@@ -903,22 +930,22 @@
         <v>0.008830914452507423</v>
       </c>
       <c r="V4">
+        <v>0.008830914452507423</v>
+      </c>
+      <c r="W4">
+        <v>0.1803031754725153</v>
+      </c>
+      <c r="X4">
+        <v>0.008830914452507423</v>
+      </c>
+      <c r="Y4">
         <v>0.009587958428762032</v>
       </c>
-      <c r="W4">
+      <c r="Z4">
         <v>0.2002385385131124</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>0.009587958428762032</v>
-      </c>
-      <c r="Y4">
-        <v>0.01056493977132024</v>
-      </c>
-      <c r="Z4">
-        <v>0.2401092645943063</v>
-      </c>
-      <c r="AA4">
-        <v>0.01056493977132024</v>
       </c>
       <c r="AB4">
         <v>0.01056493977132024</v>
@@ -939,13 +966,13 @@
         <v>0.01056493977132024</v>
       </c>
       <c r="AH4">
-        <v>0.008012517731772919</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="AI4">
         <v>0.2401092645943063</v>
       </c>
       <c r="AJ4">
-        <v>0.008012517731772919</v>
+        <v>0.01056493977132024</v>
       </c>
       <c r="AK4">
         <v>0.008012517731772919</v>
@@ -957,22 +984,22 @@
         <v>0.008012517731772919</v>
       </c>
       <c r="AN4">
+        <v>0.008012517731772919</v>
+      </c>
+      <c r="AO4">
+        <v>0.2401092645943063</v>
+      </c>
+      <c r="AP4">
+        <v>0.008012517731772919</v>
+      </c>
+      <c r="AQ4">
         <v>0.008830914452507423</v>
       </c>
-      <c r="AO4">
+      <c r="AR4">
         <v>0.1803031754725153</v>
       </c>
-      <c r="AP4">
+      <c r="AS4">
         <v>0.008830914452507423</v>
-      </c>
-      <c r="AQ4">
-        <v>0.01002434804893105</v>
-      </c>
-      <c r="AR4">
-        <v>0.2401092645943063</v>
-      </c>
-      <c r="AS4">
-        <v>0.01002434804893105</v>
       </c>
       <c r="AT4">
         <v>0.01002434804893105</v>
@@ -984,13 +1011,13 @@
         <v>0.01002434804893105</v>
       </c>
       <c r="AW4">
-        <v>0.008012517731772919</v>
+        <v>0.01002434804893105</v>
       </c>
       <c r="AX4">
         <v>0.2401092645943063</v>
       </c>
       <c r="AY4">
-        <v>0.008012517731772919</v>
+        <v>0.01002434804893105</v>
       </c>
       <c r="AZ4">
         <v>0.008012517731772919</v>
@@ -1001,8 +1028,17 @@
       <c r="BB4">
         <v>0.008012517731772919</v>
       </c>
+      <c r="BC4">
+        <v>0.008012517731772919</v>
+      </c>
+      <c r="BD4">
+        <v>0.2401092645943063</v>
+      </c>
+      <c r="BE4">
+        <v>0.008012517731772919</v>
+      </c>
     </row>
-    <row r="5" spans="1:54">
+    <row r="5" spans="1:57">
       <c r="A5">
         <v>0.009680657902577198</v>
       </c>
@@ -1067,22 +1103,22 @@
         <v>0.009385874096320437</v>
       </c>
       <c r="V5">
+        <v>0.009385874096320437</v>
+      </c>
+      <c r="W5">
+        <v>0.1279935295394772</v>
+      </c>
+      <c r="X5">
+        <v>0.009385874096320437</v>
+      </c>
+      <c r="Y5">
         <v>0.008955780224535791</v>
       </c>
-      <c r="W5">
+      <c r="Z5">
         <v>0.1369294622163093</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>0.008955780224535791</v>
-      </c>
-      <c r="Y5">
-        <v>0.01006922124099752</v>
-      </c>
-      <c r="Z5">
-        <v>0.1548013275699734</v>
-      </c>
-      <c r="AA5">
-        <v>0.01006922124099752</v>
       </c>
       <c r="AB5">
         <v>0.01006922124099752</v>
@@ -1103,13 +1139,13 @@
         <v>0.01006922124099752</v>
       </c>
       <c r="AH5">
-        <v>0.006513851255720016</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="AI5">
         <v>0.1548013275699734</v>
       </c>
       <c r="AJ5">
-        <v>0.006513851255720016</v>
+        <v>0.01006922124099752</v>
       </c>
       <c r="AK5">
         <v>0.006513851255720016</v>
@@ -1121,22 +1157,22 @@
         <v>0.006513851255720016</v>
       </c>
       <c r="AN5">
+        <v>0.006513851255720016</v>
+      </c>
+      <c r="AO5">
+        <v>0.1548013275699734</v>
+      </c>
+      <c r="AP5">
+        <v>0.006513851255720016</v>
+      </c>
+      <c r="AQ5">
         <v>0.009385874096320437</v>
       </c>
-      <c r="AO5">
+      <c r="AR5">
         <v>0.1279935295394772</v>
       </c>
-      <c r="AP5">
+      <c r="AS5">
         <v>0.009385874096320437</v>
-      </c>
-      <c r="AQ5">
-        <v>0.01019874235380429</v>
-      </c>
-      <c r="AR5">
-        <v>0.1548013275699734</v>
-      </c>
-      <c r="AS5">
-        <v>0.01019874235380429</v>
       </c>
       <c r="AT5">
         <v>0.01019874235380429</v>
@@ -1148,13 +1184,13 @@
         <v>0.01019874235380429</v>
       </c>
       <c r="AW5">
-        <v>0.006513851255720016</v>
+        <v>0.01019874235380429</v>
       </c>
       <c r="AX5">
         <v>0.1548013275699734</v>
       </c>
       <c r="AY5">
-        <v>0.006513851255720016</v>
+        <v>0.01019874235380429</v>
       </c>
       <c r="AZ5">
         <v>0.006513851255720016</v>
@@ -1165,8 +1201,17 @@
       <c r="BB5">
         <v>0.006513851255720016</v>
       </c>
+      <c r="BC5">
+        <v>0.006513851255720016</v>
+      </c>
+      <c r="BD5">
+        <v>0.1548013275699734</v>
+      </c>
+      <c r="BE5">
+        <v>0.006513851255720016</v>
+      </c>
     </row>
-    <row r="6" spans="1:54">
+    <row r="6" spans="1:57">
       <c r="A6">
         <v>0.007503798698266477</v>
       </c>
@@ -1231,22 +1276,22 @@
         <v>0.003394023396034468</v>
       </c>
       <c r="V6">
+        <v>0.003394023396034468</v>
+      </c>
+      <c r="W6">
+        <v>0.1494313824275443</v>
+      </c>
+      <c r="X6">
+        <v>0.003394023396034468</v>
+      </c>
+      <c r="Y6">
         <v>0.007022701431492167</v>
       </c>
-      <c r="W6">
+      <c r="Z6">
         <v>0.125006887507649</v>
       </c>
-      <c r="X6">
+      <c r="AA6">
         <v>0.007022701431492167</v>
-      </c>
-      <c r="Y6">
-        <v>0.008072229298499904</v>
-      </c>
-      <c r="Z6">
-        <v>0.07615789766785841</v>
-      </c>
-      <c r="AA6">
-        <v>0.008072229298499904</v>
       </c>
       <c r="AB6">
         <v>0.008072229298499904</v>
@@ -1267,13 +1312,13 @@
         <v>0.008072229298499904</v>
       </c>
       <c r="AH6">
-        <v>0.006737984715205545</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="AI6">
         <v>0.07615789766785841</v>
       </c>
       <c r="AJ6">
-        <v>0.006737984715205545</v>
+        <v>0.008072229298499904</v>
       </c>
       <c r="AK6">
         <v>0.006737984715205545</v>
@@ -1285,22 +1330,22 @@
         <v>0.006737984715205545</v>
       </c>
       <c r="AN6">
+        <v>0.006737984715205545</v>
+      </c>
+      <c r="AO6">
+        <v>0.07615789766785841</v>
+      </c>
+      <c r="AP6">
+        <v>0.006737984715205545</v>
+      </c>
+      <c r="AQ6">
         <v>0.003394023396034468</v>
       </c>
-      <c r="AO6">
+      <c r="AR6">
         <v>0.1494313824275443</v>
       </c>
-      <c r="AP6">
+      <c r="AS6">
         <v>0.003394023396034468</v>
-      </c>
-      <c r="AQ6">
-        <v>0.00826170616524438</v>
-      </c>
-      <c r="AR6">
-        <v>0.07615789766785841</v>
-      </c>
-      <c r="AS6">
-        <v>0.00826170616524438</v>
       </c>
       <c r="AT6">
         <v>0.00826170616524438</v>
@@ -1312,13 +1357,13 @@
         <v>0.00826170616524438</v>
       </c>
       <c r="AW6">
-        <v>0.006737984715205545</v>
+        <v>0.00826170616524438</v>
       </c>
       <c r="AX6">
         <v>0.07615789766785841</v>
       </c>
       <c r="AY6">
-        <v>0.006737984715205545</v>
+        <v>0.00826170616524438</v>
       </c>
       <c r="AZ6">
         <v>0.006737984715205545</v>
@@ -1329,8 +1374,17 @@
       <c r="BB6">
         <v>0.006737984715205545</v>
       </c>
+      <c r="BC6">
+        <v>0.006737984715205545</v>
+      </c>
+      <c r="BD6">
+        <v>0.07615789766785841</v>
+      </c>
+      <c r="BE6">
+        <v>0.006737984715205545</v>
+      </c>
     </row>
-    <row r="7" spans="1:54">
+    <row r="7" spans="1:57">
       <c r="A7">
         <v>0.004619230646090584</v>
       </c>
@@ -1395,22 +1449,22 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="V7">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="W7">
+        <v>0.03729258762855925</v>
+      </c>
+      <c r="X7">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="Y7">
         <v>0.003249069490238883</v>
       </c>
-      <c r="W7">
+      <c r="Z7">
         <v>0.02489993293641402</v>
       </c>
-      <c r="X7">
+      <c r="AA7">
         <v>0.003249069490238883</v>
-      </c>
-      <c r="Y7">
-        <v>0.004887828862775059</v>
-      </c>
-      <c r="Z7">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AA7">
-        <v>0.004887828862775059</v>
       </c>
       <c r="AB7">
         <v>0.004887828862775059</v>
@@ -1431,13 +1485,13 @@
         <v>0.004887828862775059</v>
       </c>
       <c r="AH7">
-        <v>0.001503619736861317</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.001503619736861317</v>
+        <v>0.004887828862775059</v>
       </c>
       <c r="AK7">
         <v>0.001503619736861317</v>
@@ -1449,22 +1503,22 @@
         <v>0.001503619736861317</v>
       </c>
       <c r="AN7">
-        <v>0.0001849315068493151</v>
+        <v>0.001503619736861317</v>
       </c>
       <c r="AO7">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AP7">
+        <v>0.001503619736861317</v>
+      </c>
+      <c r="AQ7">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="AR7">
         <v>0.03729258762855925</v>
       </c>
-      <c r="AP7">
-        <v>0.0001849315068493151</v>
-      </c>
-      <c r="AQ7">
-        <v>0.004977361601669884</v>
-      </c>
-      <c r="AR7">
-        <v>0.0001146235521235521</v>
-      </c>
       <c r="AS7">
-        <v>0.004977361601669884</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AT7">
         <v>0.004977361601669884</v>
@@ -1476,13 +1530,13 @@
         <v>0.004977361601669884</v>
       </c>
       <c r="AW7">
-        <v>0.001503619736861317</v>
+        <v>0.004977361601669884</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.001503619736861317</v>
+        <v>0.004977361601669884</v>
       </c>
       <c r="AZ7">
         <v>0.001503619736861317</v>
@@ -1493,8 +1547,17 @@
       <c r="BB7">
         <v>0.001503619736861317</v>
       </c>
+      <c r="BC7">
+        <v>0.001503619736861317</v>
+      </c>
+      <c r="BD7">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BE7">
+        <v>0.001503619736861317</v>
+      </c>
     </row>
-    <row r="8" spans="1:54">
+    <row r="8" spans="1:57">
       <c r="A8">
         <v>0.000235106866757617</v>
       </c>
@@ -1559,22 +1622,22 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="V8">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="W8">
+        <v>0.02211925649135387</v>
+      </c>
+      <c r="X8">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="Y8">
         <v>0.0003698114948764792</v>
       </c>
-      <c r="W8">
+      <c r="Z8">
         <v>0.01478437884494376</v>
       </c>
-      <c r="X8">
+      <c r="AA8">
         <v>0.0003698114948764792</v>
-      </c>
-      <c r="Y8">
-        <v>0.0005185254365380381</v>
-      </c>
-      <c r="Z8">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AA8">
-        <v>0.0005185254365380381</v>
       </c>
       <c r="AB8">
         <v>0.0005185254365380381</v>
@@ -1595,13 +1658,13 @@
         <v>0.0005185254365380381</v>
       </c>
       <c r="AH8">
-        <v>0.0001648236055669436</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.0001648236055669436</v>
+        <v>0.0005185254365380381</v>
       </c>
       <c r="AK8">
         <v>0.0001648236055669436</v>
@@ -1613,22 +1676,22 @@
         <v>0.0001648236055669436</v>
       </c>
       <c r="AN8">
-        <v>0.0001849315068493151</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AO8">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AP8">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="AQ8">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="AR8">
         <v>0.02211925649135387</v>
       </c>
-      <c r="AP8">
-        <v>0.0001849315068493151</v>
-      </c>
-      <c r="AQ8">
-        <v>0.0006129982931315117</v>
-      </c>
-      <c r="AR8">
-        <v>0.0001146235521235521</v>
-      </c>
       <c r="AS8">
-        <v>0.0006129982931315117</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AT8">
         <v>0.0006129982931315117</v>
@@ -1640,13 +1703,13 @@
         <v>0.0006129982931315117</v>
       </c>
       <c r="AW8">
-        <v>0.0001648236055669436</v>
+        <v>0.0006129982931315117</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.0001648236055669436</v>
+        <v>0.0006129982931315117</v>
       </c>
       <c r="AZ8">
         <v>0.0001648236055669436</v>
@@ -1657,8 +1720,17 @@
       <c r="BB8">
         <v>0.0001648236055669436</v>
       </c>
+      <c r="BC8">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="BD8">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BE8">
+        <v>0.0001648236055669436</v>
+      </c>
     </row>
-    <row r="9" spans="1:54">
+    <row r="9" spans="1:57">
       <c r="A9">
         <v>0.000235106866757617</v>
       </c>
@@ -1723,22 +1795,22 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="V9">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="W9">
+        <v>0.0001527405366339252</v>
+      </c>
+      <c r="X9">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="Y9">
         <v>0.0002136034642349976</v>
       </c>
-      <c r="W9">
+      <c r="Z9">
         <v>0.0001400348751304675</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>0.0002136034642349976</v>
-      </c>
-      <c r="Y9">
-        <v>0.0002451613829154453</v>
-      </c>
-      <c r="Z9">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AA9">
-        <v>0.0002451613829154453</v>
       </c>
       <c r="AB9">
         <v>0.0002451613829154453</v>
@@ -1759,13 +1831,13 @@
         <v>0.0002451613829154453</v>
       </c>
       <c r="AH9">
-        <v>0.0001648236055669436</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AI9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ9">
-        <v>0.0001648236055669436</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AK9">
         <v>0.0001648236055669436</v>
@@ -1777,22 +1849,22 @@
         <v>0.0001648236055669436</v>
       </c>
       <c r="AN9">
-        <v>0.0001849315068493151</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AO9">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AP9">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="AQ9">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="AR9">
         <v>0.0001527405366339252</v>
       </c>
-      <c r="AP9">
-        <v>0.0001849315068493151</v>
-      </c>
-      <c r="AQ9">
-        <v>0.000248512888301388</v>
-      </c>
-      <c r="AR9">
-        <v>0.0001146235521235521</v>
-      </c>
       <c r="AS9">
-        <v>0.000248512888301388</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AT9">
         <v>0.000248512888301388</v>
@@ -1804,13 +1876,13 @@
         <v>0.000248512888301388</v>
       </c>
       <c r="AW9">
-        <v>0.0001648236055669436</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AX9">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY9">
-        <v>0.0001648236055669436</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AZ9">
         <v>0.0001648236055669436</v>
@@ -1821,8 +1893,17 @@
       <c r="BB9">
         <v>0.0001648236055669436</v>
       </c>
+      <c r="BC9">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="BD9">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BE9">
+        <v>0.0001648236055669436</v>
+      </c>
     </row>
-    <row r="10" spans="1:54">
+    <row r="10" spans="1:57">
       <c r="A10">
         <v>0.000235106866757617</v>
       </c>
@@ -1887,22 +1968,22 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="V10">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="W10">
+        <v>0.0001527405366339252</v>
+      </c>
+      <c r="X10">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="Y10">
         <v>0.0002136034642349976</v>
       </c>
-      <c r="W10">
+      <c r="Z10">
         <v>0.0001400348751304675</v>
       </c>
-      <c r="X10">
+      <c r="AA10">
         <v>0.0002136034642349976</v>
-      </c>
-      <c r="Y10">
-        <v>0.0002451613829154453</v>
-      </c>
-      <c r="Z10">
-        <v>0.0001146235521235521</v>
-      </c>
-      <c r="AA10">
-        <v>0.0002451613829154453</v>
       </c>
       <c r="AB10">
         <v>0.0002451613829154453</v>
@@ -1923,13 +2004,13 @@
         <v>0.0002451613829154453</v>
       </c>
       <c r="AH10">
-        <v>0.0001648236055669436</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AI10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ10">
-        <v>0.0001648236055669436</v>
+        <v>0.0002451613829154453</v>
       </c>
       <c r="AK10">
         <v>0.0001648236055669436</v>
@@ -1941,22 +2022,22 @@
         <v>0.0001648236055669436</v>
       </c>
       <c r="AN10">
-        <v>0.0001849315068493151</v>
+        <v>0.0001648236055669436</v>
       </c>
       <c r="AO10">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="AP10">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="AQ10">
+        <v>0.0001849315068493151</v>
+      </c>
+      <c r="AR10">
         <v>0.0001527405366339252</v>
       </c>
-      <c r="AP10">
-        <v>0.0001849315068493151</v>
-      </c>
-      <c r="AQ10">
-        <v>0.000248512888301388</v>
-      </c>
-      <c r="AR10">
-        <v>0.0001146235521235521</v>
-      </c>
       <c r="AS10">
-        <v>0.000248512888301388</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AT10">
         <v>0.000248512888301388</v>
@@ -1968,13 +2049,13 @@
         <v>0.000248512888301388</v>
       </c>
       <c r="AW10">
-        <v>0.0001648236055669436</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AX10">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY10">
-        <v>0.0001648236055669436</v>
+        <v>0.000248512888301388</v>
       </c>
       <c r="AZ10">
         <v>0.0001648236055669436</v>
@@ -1983,6 +2064,15 @@
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB10">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="BC10">
+        <v>0.0001648236055669436</v>
+      </c>
+      <c r="BD10">
+        <v>0.0001146235521235521</v>
+      </c>
+      <c r="BE10">
         <v>0.0001648236055669436</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Get stubble sim working again and re-run using the most up-to-date sgen. Plus add p axis to sup.
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,112 +348,112 @@
   <sheetData>
     <row r="1" spans="1:57">
       <c r="A1">
-        <v>0.03545577386460821</v>
+        <v>0.03546614488291291</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.03545577386460821</v>
+        <v>0.03546614488291291</v>
       </c>
       <c r="D1">
-        <v>0.03545577386460821</v>
+        <v>0.03546614488291291</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.03545577386460821</v>
+        <v>0.03546614488291291</v>
       </c>
       <c r="G1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="H1">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="I1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="J1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="M1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="N1">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="O1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="P1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="Q1">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="R1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="S1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="T1">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="U1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="V1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="W1">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="X1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="Y1">
-        <v>0.006653353295715964</v>
+        <v>0.00853535631384668</v>
       </c>
       <c r="Z1">
-        <v>0.0001400348751304675</v>
+        <v>0.0001402202031142261</v>
       </c>
       <c r="AA1">
-        <v>0.006653353295715964</v>
+        <v>0.00853535631384668</v>
       </c>
       <c r="AB1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="AE1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="AH1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.01126709889836981</v>
+        <v>0.0121900220344118</v>
       </c>
       <c r="AK1">
         <v>0.0001648236055669436</v>
@@ -474,31 +474,31 @@
         <v>0.0001648236055669436</v>
       </c>
       <c r="AQ1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="AR1">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="AS1">
-        <v>0.001175430265398609</v>
+        <v>0.01065775884814567</v>
       </c>
       <c r="AT1">
-        <v>0.003204207242957014</v>
+        <v>0.004431314418244764</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.003204207242957014</v>
+        <v>0.004431314418244764</v>
       </c>
       <c r="AW1">
-        <v>0.003204207242957014</v>
+        <v>0.004431314418244764</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.003204207242957014</v>
+        <v>0.004431314418244764</v>
       </c>
       <c r="AZ1">
         <v>0.0001648236055669436</v>
@@ -521,911 +521,911 @@
     </row>
     <row r="2" spans="1:57">
       <c r="A2">
-        <v>0.01331514114706135</v>
+        <v>0.01332633397302849</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.01331514114706135</v>
+        <v>0.01332633397302849</v>
       </c>
       <c r="D2">
-        <v>0.01331514114706135</v>
+        <v>0.01332633397302849</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.01331514114706135</v>
+        <v>0.01332633397302849</v>
       </c>
       <c r="G2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="H2">
-        <v>0.1512910435046977</v>
+        <v>0.1469630793008418</v>
       </c>
       <c r="I2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="J2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="M2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="N2">
-        <v>0.1512910435046977</v>
+        <v>0.1469630793008418</v>
       </c>
       <c r="O2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="P2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="Q2">
-        <v>0.1512910435046977</v>
+        <v>0.1469630793008418</v>
       </c>
       <c r="R2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="S2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="T2">
-        <v>0.1512910435046977</v>
+        <v>0.1469630793008418</v>
       </c>
       <c r="U2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="V2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="W2">
-        <v>0.1512910435046977</v>
+        <v>0.1469630793008418</v>
       </c>
       <c r="X2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="Y2">
-        <v>0.01258396833395928</v>
+        <v>0.01374602572713187</v>
       </c>
       <c r="Z2">
-        <v>0.1008989035205063</v>
+        <v>0.09801359405126905</v>
       </c>
       <c r="AA2">
-        <v>0.01258396833395928</v>
+        <v>0.01374602572713187</v>
       </c>
       <c r="AB2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="AE2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="AH2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.01312583227429785</v>
+        <v>0.01291371067363524</v>
       </c>
       <c r="AK2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
       <c r="AL2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
       <c r="AN2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
       <c r="AO2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
       <c r="AQ2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="AR2">
-        <v>0.1512910435046977</v>
+        <v>0.1469630793008418</v>
       </c>
       <c r="AS2">
-        <v>0.02262491053503307</v>
+        <v>0.03080610777059984</v>
       </c>
       <c r="AT2">
-        <v>0.01306272931671001</v>
+        <v>0.01277616957383749</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.01306272931671001</v>
+        <v>0.01277616957383749</v>
       </c>
       <c r="AW2">
-        <v>0.01306272931671001</v>
+        <v>0.01277616957383749</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.01306272931671001</v>
+        <v>0.01277616957383749</v>
       </c>
       <c r="AZ2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
       <c r="BA2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
       <c r="BC2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
       <c r="BD2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BE2">
-        <v>0.006479769352745266</v>
+        <v>0.006880614812391151</v>
       </c>
     </row>
     <row r="3" spans="1:57">
       <c r="A3">
-        <v>0.01051194564093447</v>
+        <v>0.01052340617798367</v>
       </c>
       <c r="B3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="C3">
-        <v>0.01051194564093447</v>
+        <v>0.01052340617798367</v>
       </c>
       <c r="D3">
-        <v>0.01051194564093447</v>
+        <v>0.01052340617798367</v>
       </c>
       <c r="E3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="F3">
-        <v>0.01051194564093447</v>
+        <v>0.01052340617798367</v>
       </c>
       <c r="G3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="H3">
-        <v>0.3311108033259505</v>
+        <v>0.3317162293534002</v>
       </c>
       <c r="I3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="J3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="K3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="L3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="M3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="N3">
-        <v>0.3311108033259505</v>
+        <v>0.3317162293534002</v>
       </c>
       <c r="O3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="P3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="Q3">
-        <v>0.3311108033259505</v>
+        <v>0.3317162293534002</v>
       </c>
       <c r="R3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="S3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="T3">
-        <v>0.3311108033259505</v>
+        <v>0.3317162293534002</v>
       </c>
       <c r="U3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="V3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="W3">
-        <v>0.3311108033259505</v>
+        <v>0.3317162293534002</v>
       </c>
       <c r="X3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="Y3">
-        <v>0.01272778309089564</v>
+        <v>0.01298291562096301</v>
       </c>
       <c r="Z3">
-        <v>0.3238510920252826</v>
+        <v>0.3298467614002561</v>
       </c>
       <c r="AA3">
-        <v>0.01272778309089564</v>
+        <v>0.01298291562096301</v>
       </c>
       <c r="AB3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="AC3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="AD3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="AE3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="AF3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="AG3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="AH3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="AI3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="AJ3">
-        <v>0.01381443835817066</v>
+        <v>0.01363626179490493</v>
       </c>
       <c r="AK3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
       <c r="AL3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="AM3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
       <c r="AN3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
       <c r="AO3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="AP3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
       <c r="AQ3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="AR3">
-        <v>0.3311108033259505</v>
+        <v>0.3317162293534002</v>
       </c>
       <c r="AS3">
-        <v>0.01374566675163806</v>
+        <v>0.01623772226398872</v>
       </c>
       <c r="AT3">
-        <v>0.01491526926391605</v>
+        <v>0.01467388033387868</v>
       </c>
       <c r="AU3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="AV3">
-        <v>0.01491526926391605</v>
+        <v>0.01467388033387868</v>
       </c>
       <c r="AW3">
-        <v>0.01491526926391605</v>
+        <v>0.01467388033387868</v>
       </c>
       <c r="AX3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="AY3">
-        <v>0.01491526926391605</v>
+        <v>0.01467388033387868</v>
       </c>
       <c r="AZ3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
       <c r="BA3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="BB3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
       <c r="BC3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
       <c r="BD3">
-        <v>0.309331669423947</v>
+        <v>0.326107825493968</v>
       </c>
       <c r="BE3">
-        <v>0.01004553072597439</v>
+        <v>0.01004881995156634</v>
       </c>
     </row>
     <row r="4" spans="1:57">
       <c r="A4">
-        <v>0.01218671493848782</v>
+        <v>0.01220446518046994</v>
       </c>
       <c r="B4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="C4">
-        <v>0.01218671493848782</v>
+        <v>0.01220446518046994</v>
       </c>
       <c r="D4">
-        <v>0.01218671493848782</v>
+        <v>0.01220446518046994</v>
       </c>
       <c r="E4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="F4">
-        <v>0.01218671493848782</v>
+        <v>0.01220446518046994</v>
       </c>
       <c r="G4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="H4">
-        <v>0.1803031754725153</v>
+        <v>0.1769669385797322</v>
       </c>
       <c r="I4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="J4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="K4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="L4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="M4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="N4">
-        <v>0.1803031754725153</v>
+        <v>0.1769669385797322</v>
       </c>
       <c r="O4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="P4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="Q4">
-        <v>0.1803031754725153</v>
+        <v>0.1769669385797322</v>
       </c>
       <c r="R4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="S4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="T4">
-        <v>0.1803031754725153</v>
+        <v>0.1769669385797322</v>
       </c>
       <c r="U4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="V4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="W4">
-        <v>0.1803031754725153</v>
+        <v>0.1769669385797322</v>
       </c>
       <c r="X4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="Y4">
-        <v>0.009587958428762032</v>
+        <v>0.01071965335842769</v>
       </c>
       <c r="Z4">
-        <v>0.2002385385131124</v>
+        <v>0.1903754586637219</v>
       </c>
       <c r="AA4">
-        <v>0.009587958428762032</v>
+        <v>0.01071965335842769</v>
       </c>
       <c r="AB4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="AC4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="AD4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="AE4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="AF4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="AG4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="AH4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="AI4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="AJ4">
-        <v>0.01056493977132024</v>
+        <v>0.01073808468063451</v>
       </c>
       <c r="AK4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
       <c r="AL4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="AM4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
       <c r="AN4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
       <c r="AO4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="AP4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
       <c r="AQ4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="AR4">
-        <v>0.1803031754725153</v>
+        <v>0.1769669385797322</v>
       </c>
       <c r="AS4">
-        <v>0.008830914452507423</v>
+        <v>0.01671275040825515</v>
       </c>
       <c r="AT4">
-        <v>0.01002434804893105</v>
+        <v>0.01024929118068937</v>
       </c>
       <c r="AU4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="AV4">
-        <v>0.01002434804893105</v>
+        <v>0.01024929118068937</v>
       </c>
       <c r="AW4">
-        <v>0.01002434804893105</v>
+        <v>0.01024929118068937</v>
       </c>
       <c r="AX4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="AY4">
-        <v>0.01002434804893105</v>
+        <v>0.01024929118068937</v>
       </c>
       <c r="AZ4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
       <c r="BA4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="BB4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
       <c r="BC4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
       <c r="BD4">
-        <v>0.2401092645943063</v>
+        <v>0.2171924988317014</v>
       </c>
       <c r="BE4">
-        <v>0.008012517731772919</v>
+        <v>0.007686242189100319</v>
       </c>
     </row>
     <row r="5" spans="1:57">
       <c r="A5">
-        <v>0.009680657902577198</v>
+        <v>0.009698175402116061</v>
       </c>
       <c r="B5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="C5">
-        <v>0.009680657902577198</v>
+        <v>0.009698175402116061</v>
       </c>
       <c r="D5">
-        <v>0.009680657902577198</v>
+        <v>0.009698175402116061</v>
       </c>
       <c r="E5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="F5">
-        <v>0.009680657902577198</v>
+        <v>0.009698175402116061</v>
       </c>
       <c r="G5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H5">
-        <v>0.1279935295394772</v>
+        <v>0.1350304976632463</v>
       </c>
       <c r="I5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="K5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="L5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="M5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N5">
-        <v>0.1279935295394772</v>
+        <v>0.1350304976632463</v>
       </c>
       <c r="O5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q5">
-        <v>0.1279935295394772</v>
+        <v>0.1350304976632463</v>
       </c>
       <c r="R5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T5">
-        <v>0.1279935295394772</v>
+        <v>0.1350304976632463</v>
       </c>
       <c r="U5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="W5">
-        <v>0.1279935295394772</v>
+        <v>0.1350304976632463</v>
       </c>
       <c r="X5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Y5">
-        <v>0.008955780224535791</v>
+        <v>0.007556343267930988</v>
       </c>
       <c r="Z5">
-        <v>0.1369294622163093</v>
+        <v>0.1388962589468278</v>
       </c>
       <c r="AA5">
-        <v>0.008955780224535791</v>
+        <v>0.007556343267930988</v>
       </c>
       <c r="AB5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="AC5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="AD5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="AE5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="AF5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="AG5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="AH5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="AI5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="AJ5">
-        <v>0.01006922124099752</v>
+        <v>0.009772820099179347</v>
       </c>
       <c r="AK5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
       <c r="AL5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="AM5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
       <c r="AN5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
       <c r="AO5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="AP5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
       <c r="AQ5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AR5">
-        <v>0.1279935295394772</v>
+        <v>0.1350304976632463</v>
       </c>
       <c r="AS5">
-        <v>0.009385874096320437</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AT5">
-        <v>0.01019874235380429</v>
+        <v>0.00979770166486711</v>
       </c>
       <c r="AU5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="AV5">
-        <v>0.01019874235380429</v>
+        <v>0.00979770166486711</v>
       </c>
       <c r="AW5">
-        <v>0.01019874235380429</v>
+        <v>0.00979770166486711</v>
       </c>
       <c r="AX5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="AY5">
-        <v>0.01019874235380429</v>
+        <v>0.00979770166486711</v>
       </c>
       <c r="AZ5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
       <c r="BA5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="BB5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
       <c r="BC5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
       <c r="BD5">
-        <v>0.1548013275699734</v>
+        <v>0.1466277815139906</v>
       </c>
       <c r="BE5">
-        <v>0.006513851255720016</v>
+        <v>0.006809095485975105</v>
       </c>
     </row>
     <row r="6" spans="1:57">
       <c r="A6">
-        <v>0.007503798698266477</v>
+        <v>0.007518590801563001</v>
       </c>
       <c r="B6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="C6">
-        <v>0.007503798698266477</v>
+        <v>0.007518590801563001</v>
       </c>
       <c r="D6">
-        <v>0.007503798698266477</v>
+        <v>0.007518590801563001</v>
       </c>
       <c r="E6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="F6">
-        <v>0.007503798698266477</v>
+        <v>0.007518590801563001</v>
       </c>
       <c r="G6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="H6">
-        <v>0.1494313824275443</v>
+        <v>0.1469265467189451</v>
       </c>
       <c r="I6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="J6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="K6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="L6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="M6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="N6">
-        <v>0.1494313824275443</v>
+        <v>0.1469265467189451</v>
       </c>
       <c r="O6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="P6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Q6">
-        <v>0.1494313824275443</v>
+        <v>0.1469265467189451</v>
       </c>
       <c r="R6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="S6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="T6">
-        <v>0.1494313824275443</v>
+        <v>0.1469265467189451</v>
       </c>
       <c r="U6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="V6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="W6">
-        <v>0.1494313824275443</v>
+        <v>0.1469265467189451</v>
       </c>
       <c r="X6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="Y6">
-        <v>0.007022701431492167</v>
+        <v>0.006493611973198488</v>
       </c>
       <c r="Z6">
-        <v>0.125006887507649</v>
+        <v>0.1389076671321314</v>
       </c>
       <c r="AA6">
-        <v>0.007022701431492167</v>
+        <v>0.006493611973198488</v>
       </c>
       <c r="AB6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="AC6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="AD6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="AE6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="AF6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="AG6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="AH6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="AI6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="AJ6">
-        <v>0.008072229298499904</v>
+        <v>0.007948316857439757</v>
       </c>
       <c r="AK6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
       <c r="AL6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="AM6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
       <c r="AN6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
       <c r="AO6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="AP6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
       <c r="AQ6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AR6">
-        <v>0.1494313824275443</v>
+        <v>0.1469265467189451</v>
       </c>
       <c r="AS6">
-        <v>0.003394023396034468</v>
+        <v>0.0001849315068493151</v>
       </c>
       <c r="AT6">
-        <v>0.00826170616524438</v>
+        <v>0.00809155887606534</v>
       </c>
       <c r="AU6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="AV6">
-        <v>0.00826170616524438</v>
+        <v>0.00809155887606534</v>
       </c>
       <c r="AW6">
-        <v>0.00826170616524438</v>
+        <v>0.00809155887606534</v>
       </c>
       <c r="AX6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="AY6">
-        <v>0.00826170616524438</v>
+        <v>0.00809155887606534</v>
       </c>
       <c r="AZ6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
       <c r="BA6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="BB6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
       <c r="BC6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
       <c r="BD6">
-        <v>0.07615789766785841</v>
+        <v>0.1228699079585041</v>
       </c>
       <c r="BE6">
-        <v>0.006737984715205545</v>
+        <v>0.006738542437890538</v>
       </c>
     </row>
     <row r="7" spans="1:57">
       <c r="A7">
-        <v>0.004619230646090584</v>
+        <v>0.004628616415328602</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.004619230646090584</v>
+        <v>0.004628616415328602</v>
       </c>
       <c r="D7">
-        <v>0.004619230646090584</v>
+        <v>0.004628616415328602</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.004619230646090584</v>
+        <v>0.004628616415328602</v>
       </c>
       <c r="G7">
         <v>0.0001849315068493151</v>
       </c>
       <c r="H7">
-        <v>0.03729258762855925</v>
+        <v>0.03976329111914859</v>
       </c>
       <c r="I7">
         <v>0.0001849315068493151</v>
       </c>
       <c r="J7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="M7">
         <v>0.0001849315068493151</v>
       </c>
       <c r="N7">
-        <v>0.03729258762855925</v>
+        <v>0.03976329111914859</v>
       </c>
       <c r="O7">
         <v>0.0001849315068493151</v>
@@ -1434,7 +1434,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="Q7">
-        <v>0.03729258762855925</v>
+        <v>0.03976329111914859</v>
       </c>
       <c r="R7">
         <v>0.0001849315068493151</v>
@@ -1443,7 +1443,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="T7">
-        <v>0.03729258762855925</v>
+        <v>0.03976329111914859</v>
       </c>
       <c r="U7">
         <v>0.0001849315068493151</v>
@@ -1452,109 +1452,109 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="W7">
-        <v>0.03729258762855925</v>
+        <v>0.03976329111914859</v>
       </c>
       <c r="X7">
         <v>0.0001849315068493151</v>
       </c>
       <c r="Y7">
-        <v>0.003249069490238883</v>
+        <v>0.003220273384676921</v>
       </c>
       <c r="Z7">
-        <v>0.02489993293641402</v>
+        <v>0.02654706859680691</v>
       </c>
       <c r="AA7">
-        <v>0.003249069490238883</v>
+        <v>0.003220273384676921</v>
       </c>
       <c r="AB7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="AE7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="AH7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.004887828862775059</v>
+        <v>0.004890286753711106</v>
       </c>
       <c r="AK7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
       <c r="AL7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
       <c r="AN7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
       <c r="AO7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
       <c r="AQ7">
         <v>0.0001849315068493151</v>
       </c>
       <c r="AR7">
-        <v>0.03729258762855925</v>
+        <v>0.03976329111914859</v>
       </c>
       <c r="AS7">
         <v>0.0001849315068493151</v>
       </c>
       <c r="AT7">
-        <v>0.004977361601669884</v>
+        <v>0.004977510199838607</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.004977361601669884</v>
+        <v>0.004977510199838607</v>
       </c>
       <c r="AW7">
-        <v>0.004977361601669884</v>
+        <v>0.004977510199838607</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.004977361601669884</v>
+        <v>0.004977510199838607</v>
       </c>
       <c r="AZ7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
       <c r="BA7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
       <c r="BC7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
       <c r="BD7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BE7">
-        <v>0.001503619736861317</v>
+        <v>0.001397917585522355</v>
       </c>
     </row>
     <row r="8" spans="1:57">
@@ -1580,25 +1580,25 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="H8">
-        <v>0.02211925649135387</v>
+        <v>0.02217436167885712</v>
       </c>
       <c r="I8">
         <v>0.0001849315068493151</v>
       </c>
       <c r="J8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="M8">
         <v>0.0001849315068493151</v>
       </c>
       <c r="N8">
-        <v>0.02211925649135387</v>
+        <v>0.02217436167885712</v>
       </c>
       <c r="O8">
         <v>0.0001849315068493151</v>
@@ -1607,7 +1607,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="Q8">
-        <v>0.02211925649135387</v>
+        <v>0.02217436167885712</v>
       </c>
       <c r="R8">
         <v>0.0001849315068493151</v>
@@ -1616,7 +1616,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="T8">
-        <v>0.02211925649135387</v>
+        <v>0.02217436167885712</v>
       </c>
       <c r="U8">
         <v>0.0001849315068493151</v>
@@ -1625,46 +1625,46 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="W8">
-        <v>0.02211925649135387</v>
+        <v>0.02217436167885712</v>
       </c>
       <c r="X8">
         <v>0.0001849315068493151</v>
       </c>
       <c r="Y8">
-        <v>0.0003698114948764792</v>
+        <v>0.0003698042370484211</v>
       </c>
       <c r="Z8">
-        <v>0.01478437884494376</v>
+        <v>0.0148211156366126</v>
       </c>
       <c r="AA8">
-        <v>0.0003698114948764792</v>
+        <v>0.0003698042370484211</v>
       </c>
       <c r="AB8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="AE8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="AH8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.0005185254365380381</v>
+        <v>0.0005185127353389364</v>
       </c>
       <c r="AK8">
         <v>0.0001648236055669436</v>
@@ -1688,28 +1688,28 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="AR8">
-        <v>0.02211925649135387</v>
+        <v>0.02217436167885712</v>
       </c>
       <c r="AS8">
         <v>0.0001849315068493151</v>
       </c>
       <c r="AT8">
-        <v>0.0006129982931315117</v>
+        <v>0.0006129813581993762</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.0006129982931315117</v>
+        <v>0.0006129813581993762</v>
       </c>
       <c r="AW8">
-        <v>0.0006129982931315117</v>
+        <v>0.0006129813581993762</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.0006129982931315117</v>
+        <v>0.0006129813581993762</v>
       </c>
       <c r="AZ8">
         <v>0.0001648236055669436</v>
@@ -1753,7 +1753,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="H9">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="I9">
         <v>0.0001849315068493151</v>
@@ -1771,7 +1771,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="N9">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="O9">
         <v>0.0001849315068493151</v>
@@ -1780,7 +1780,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="Q9">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="R9">
         <v>0.0001849315068493151</v>
@@ -1789,7 +1789,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="T9">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="U9">
         <v>0.0001849315068493151</v>
@@ -1798,7 +1798,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="W9">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="X9">
         <v>0.0001849315068493151</v>
@@ -1807,7 +1807,7 @@
         <v>0.0002136034642349976</v>
       </c>
       <c r="Z9">
-        <v>0.0001400348751304675</v>
+        <v>0.0001402202031142261</v>
       </c>
       <c r="AA9">
         <v>0.0002136034642349976</v>
@@ -1861,7 +1861,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="AR9">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="AS9">
         <v>0.0001849315068493151</v>
@@ -1926,7 +1926,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="H10">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="I10">
         <v>0.0001849315068493151</v>
@@ -1944,7 +1944,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="N10">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="O10">
         <v>0.0001849315068493151</v>
@@ -1953,7 +1953,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="Q10">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="R10">
         <v>0.0001849315068493151</v>
@@ -1962,7 +1962,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="T10">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="U10">
         <v>0.0001849315068493151</v>
@@ -1971,7 +1971,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="W10">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="X10">
         <v>0.0001849315068493151</v>
@@ -1980,7 +1980,7 @@
         <v>0.0002136034642349976</v>
       </c>
       <c r="Z10">
-        <v>0.0001400348751304675</v>
+        <v>0.0001402202031142261</v>
       </c>
       <c r="AA10">
         <v>0.0002136034642349976</v>
@@ -2034,7 +2034,7 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="AR10">
-        <v>0.0001527405366339252</v>
+        <v>0.0001530185286095631</v>
       </c>
       <c r="AS10">
         <v>0.0001849315068493151</v>

</xml_diff>

<commit_message>
1. distribute rainfall when using stub sim (no profit impact). 2. increase FOO in stub sim inputs to 3000 (because stubble has RA=1 in cropresidue.py therefore we should simulate with high foo so it matches) - profit down ~4k.
</commit_message>
<xml_diff>
--- a/ExcelInputs/stubble sim.xlsx
+++ b/ExcelInputs/stubble sim.xlsx
@@ -348,112 +348,112 @@
   <sheetData>
     <row r="1" spans="1:57">
       <c r="A1">
-        <v>0.03546614488291291</v>
+        <v>0.0335925515058287</v>
       </c>
       <c r="B1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C1">
-        <v>0.03546614488291291</v>
+        <v>0.0335925515058287</v>
       </c>
       <c r="D1">
-        <v>0.03546614488291291</v>
+        <v>0.0335925515058287</v>
       </c>
       <c r="E1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F1">
-        <v>0.03546614488291291</v>
+        <v>0.0335925515058287</v>
       </c>
       <c r="G1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="H1">
         <v>0.0001530185286095631</v>
       </c>
       <c r="I1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="J1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="K1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="M1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="N1">
         <v>0.0001530185286095631</v>
       </c>
       <c r="O1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="P1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="Q1">
         <v>0.0001530185286095631</v>
       </c>
       <c r="R1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="S1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="T1">
         <v>0.0001530185286095631</v>
       </c>
       <c r="U1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="V1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="W1">
         <v>0.0001530185286095631</v>
       </c>
       <c r="X1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="Y1">
-        <v>0.00853535631384668</v>
+        <v>0.006812599091287491</v>
       </c>
       <c r="Z1">
         <v>0.0001402202031142261</v>
       </c>
       <c r="AA1">
-        <v>0.00853535631384668</v>
+        <v>0.006812599091287491</v>
       </c>
       <c r="AB1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="AC1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="AE1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="AF1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="AH1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="AI1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ1">
-        <v>0.0121900220344118</v>
+        <v>0.01080129330867494</v>
       </c>
       <c r="AK1">
         <v>0.0001648236055669436</v>
@@ -474,31 +474,31 @@
         <v>0.0001648236055669436</v>
       </c>
       <c r="AQ1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="AR1">
         <v>0.0001530185286095631</v>
       </c>
       <c r="AS1">
-        <v>0.01065775884814567</v>
+        <v>0.00415337319317881</v>
       </c>
       <c r="AT1">
-        <v>0.004431314418244764</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AU1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV1">
-        <v>0.004431314418244764</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AW1">
-        <v>0.004431314418244764</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AX1">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY1">
-        <v>0.004431314418244764</v>
+        <v>0.003204207242957014</v>
       </c>
       <c r="AZ1">
         <v>0.0001648236055669436</v>
@@ -521,714 +521,714 @@
     </row>
     <row r="2" spans="1:57">
       <c r="A2">
-        <v>0.01332633397302849</v>
+        <v>0.01329569268477082</v>
       </c>
       <c r="B2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C2">
-        <v>0.01332633397302849</v>
+        <v>0.01329569268477082</v>
       </c>
       <c r="D2">
-        <v>0.01332633397302849</v>
+        <v>0.01329569268477082</v>
       </c>
       <c r="E2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F2">
-        <v>0.01332633397302849</v>
+        <v>0.01329569268477082</v>
       </c>
       <c r="G2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="H2">
         <v>0.1469630793008418</v>
       </c>
       <c r="I2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="J2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="K2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="M2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="N2">
         <v>0.1469630793008418</v>
       </c>
       <c r="O2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="P2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="Q2">
         <v>0.1469630793008418</v>
       </c>
       <c r="R2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="S2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="T2">
         <v>0.1469630793008418</v>
       </c>
       <c r="U2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="V2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="W2">
         <v>0.1469630793008418</v>
       </c>
       <c r="X2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="Y2">
-        <v>0.01374602572713187</v>
+        <v>0.0139836561524329</v>
       </c>
       <c r="Z2">
         <v>0.09801359405126905</v>
       </c>
       <c r="AA2">
-        <v>0.01374602572713187</v>
+        <v>0.0139836561524329</v>
       </c>
       <c r="AB2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="AC2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="AE2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="AF2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="AH2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="AI2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ2">
-        <v>0.01291371067363524</v>
+        <v>0.01256237976152273</v>
       </c>
       <c r="AK2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
       <c r="AL2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
       <c r="AN2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
       <c r="AO2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
       <c r="AQ2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="AR2">
         <v>0.1469630793008418</v>
       </c>
       <c r="AS2">
-        <v>0.03080610777059984</v>
+        <v>0.03547460314413775</v>
       </c>
       <c r="AT2">
-        <v>0.01277616957383749</v>
+        <v>0.01231794212044003</v>
       </c>
       <c r="AU2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV2">
-        <v>0.01277616957383749</v>
+        <v>0.01231794212044003</v>
       </c>
       <c r="AW2">
-        <v>0.01277616957383749</v>
+        <v>0.01231794212044003</v>
       </c>
       <c r="AX2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY2">
-        <v>0.01277616957383749</v>
+        <v>0.01231794212044003</v>
       </c>
       <c r="AZ2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
       <c r="BA2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
       <c r="BC2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
       <c r="BD2">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BE2">
-        <v>0.006880614812391151</v>
+        <v>0.006080735438400828</v>
       </c>
     </row>
     <row r="3" spans="1:57">
       <c r="A3">
-        <v>0.01052340617798367</v>
+        <v>0.009016779748564735</v>
       </c>
       <c r="B3">
         <v>0.326107825493968</v>
       </c>
       <c r="C3">
-        <v>0.01052340617798367</v>
+        <v>0.009016779748564735</v>
       </c>
       <c r="D3">
-        <v>0.01052340617798367</v>
+        <v>0.009016779748564735</v>
       </c>
       <c r="E3">
         <v>0.326107825493968</v>
       </c>
       <c r="F3">
-        <v>0.01052340617798367</v>
+        <v>0.009016779748564735</v>
       </c>
       <c r="G3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="H3">
         <v>0.3317162293534002</v>
       </c>
       <c r="I3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="J3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="K3">
         <v>0.326107825493968</v>
       </c>
       <c r="L3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="M3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="N3">
         <v>0.3317162293534002</v>
       </c>
       <c r="O3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="P3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="Q3">
         <v>0.3317162293534002</v>
       </c>
       <c r="R3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="S3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="T3">
         <v>0.3317162293534002</v>
       </c>
       <c r="U3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="V3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="W3">
         <v>0.3317162293534002</v>
       </c>
       <c r="X3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="Y3">
-        <v>0.01298291562096301</v>
+        <v>0.01229076004851318</v>
       </c>
       <c r="Z3">
         <v>0.3298467614002561</v>
       </c>
       <c r="AA3">
-        <v>0.01298291562096301</v>
+        <v>0.01229076004851318</v>
       </c>
       <c r="AB3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="AC3">
         <v>0.326107825493968</v>
       </c>
       <c r="AD3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="AE3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="AF3">
         <v>0.326107825493968</v>
       </c>
       <c r="AG3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="AH3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="AI3">
         <v>0.326107825493968</v>
       </c>
       <c r="AJ3">
-        <v>0.01363626179490493</v>
+        <v>0.01306817444397589</v>
       </c>
       <c r="AK3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
       <c r="AL3">
         <v>0.326107825493968</v>
       </c>
       <c r="AM3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
       <c r="AN3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
       <c r="AO3">
         <v>0.326107825493968</v>
       </c>
       <c r="AP3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
       <c r="AQ3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="AR3">
         <v>0.3317162293534002</v>
       </c>
       <c r="AS3">
-        <v>0.01623772226398872</v>
+        <v>0.01506335219405633</v>
       </c>
       <c r="AT3">
-        <v>0.01467388033387868</v>
+        <v>0.01441863934244628</v>
       </c>
       <c r="AU3">
         <v>0.326107825493968</v>
       </c>
       <c r="AV3">
-        <v>0.01467388033387868</v>
+        <v>0.01441863934244628</v>
       </c>
       <c r="AW3">
-        <v>0.01467388033387868</v>
+        <v>0.01441863934244628</v>
       </c>
       <c r="AX3">
         <v>0.326107825493968</v>
       </c>
       <c r="AY3">
-        <v>0.01467388033387868</v>
+        <v>0.01441863934244628</v>
       </c>
       <c r="AZ3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
       <c r="BA3">
         <v>0.326107825493968</v>
       </c>
       <c r="BB3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
       <c r="BC3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
       <c r="BD3">
         <v>0.326107825493968</v>
       </c>
       <c r="BE3">
-        <v>0.01004881995156634</v>
+        <v>0.009349635184816175</v>
       </c>
     </row>
     <row r="4" spans="1:57">
       <c r="A4">
-        <v>0.01220446518046994</v>
+        <v>0.01080975467967811</v>
       </c>
       <c r="B4">
         <v>0.2171924988317014</v>
       </c>
       <c r="C4">
-        <v>0.01220446518046994</v>
+        <v>0.01080975467967811</v>
       </c>
       <c r="D4">
-        <v>0.01220446518046994</v>
+        <v>0.01080975467967811</v>
       </c>
       <c r="E4">
         <v>0.2171924988317014</v>
       </c>
       <c r="F4">
-        <v>0.01220446518046994</v>
+        <v>0.01080975467967811</v>
       </c>
       <c r="G4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="H4">
         <v>0.1769669385797322</v>
       </c>
       <c r="I4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="J4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="K4">
         <v>0.2171924988317014</v>
       </c>
       <c r="L4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="M4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="N4">
         <v>0.1769669385797322</v>
       </c>
       <c r="O4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="P4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="Q4">
         <v>0.1769669385797322</v>
       </c>
       <c r="R4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="S4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="T4">
         <v>0.1769669385797322</v>
       </c>
       <c r="U4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="V4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="W4">
         <v>0.1769669385797322</v>
       </c>
       <c r="X4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="Y4">
-        <v>0.01071965335842769</v>
+        <v>0.01031864210849662</v>
       </c>
       <c r="Z4">
         <v>0.1903754586637219</v>
       </c>
       <c r="AA4">
-        <v>0.01071965335842769</v>
+        <v>0.01031864210849662</v>
       </c>
       <c r="AB4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="AC4">
         <v>0.2171924988317014</v>
       </c>
       <c r="AD4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="AE4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="AF4">
         <v>0.2171924988317014</v>
       </c>
       <c r="AG4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="AH4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="AI4">
         <v>0.2171924988317014</v>
       </c>
       <c r="AJ4">
-        <v>0.01073808468063451</v>
+        <v>0.01003982395500032</v>
       </c>
       <c r="AK4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
       <c r="AL4">
         <v>0.2171924988317014</v>
       </c>
       <c r="AM4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
       <c r="AN4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
       <c r="AO4">
         <v>0.2171924988317014</v>
       </c>
       <c r="AP4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
       <c r="AQ4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="AR4">
         <v>0.1769669385797322</v>
       </c>
       <c r="AS4">
-        <v>0.01671275040825515</v>
+        <v>0.01669895148551608</v>
       </c>
       <c r="AT4">
-        <v>0.01024929118068937</v>
+        <v>0.009783180380107722</v>
       </c>
       <c r="AU4">
         <v>0.2171924988317014</v>
       </c>
       <c r="AV4">
-        <v>0.01024929118068937</v>
+        <v>0.009783180380107722</v>
       </c>
       <c r="AW4">
-        <v>0.01024929118068937</v>
+        <v>0.009783180380107722</v>
       </c>
       <c r="AX4">
         <v>0.2171924988317014</v>
       </c>
       <c r="AY4">
-        <v>0.01024929118068937</v>
+        <v>0.009783180380107722</v>
       </c>
       <c r="AZ4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
       <c r="BA4">
         <v>0.2171924988317014</v>
       </c>
       <c r="BB4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
       <c r="BC4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
       <c r="BD4">
         <v>0.2171924988317014</v>
       </c>
       <c r="BE4">
-        <v>0.007686242189100319</v>
+        <v>0.0076861237269795</v>
       </c>
     </row>
     <row r="5" spans="1:57">
       <c r="A5">
-        <v>0.009698175402116061</v>
+        <v>0.01089133042749333</v>
       </c>
       <c r="B5">
         <v>0.1466277815139906</v>
       </c>
       <c r="C5">
-        <v>0.009698175402116061</v>
+        <v>0.01089133042749333</v>
       </c>
       <c r="D5">
-        <v>0.009698175402116061</v>
+        <v>0.01089133042749333</v>
       </c>
       <c r="E5">
         <v>0.1466277815139906</v>
       </c>
       <c r="F5">
-        <v>0.009698175402116061</v>
+        <v>0.01089133042749333</v>
       </c>
       <c r="G5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="H5">
         <v>0.1350304976632463</v>
       </c>
       <c r="I5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="J5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="K5">
         <v>0.1466277815139906</v>
       </c>
       <c r="L5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="M5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="N5">
         <v>0.1350304976632463</v>
       </c>
       <c r="O5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="P5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="Q5">
         <v>0.1350304976632463</v>
       </c>
       <c r="R5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="S5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="T5">
         <v>0.1350304976632463</v>
       </c>
       <c r="U5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="V5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="W5">
         <v>0.1350304976632463</v>
       </c>
       <c r="X5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="Y5">
-        <v>0.007556343267930988</v>
+        <v>0.007562330893504463</v>
       </c>
       <c r="Z5">
         <v>0.1388962589468278</v>
       </c>
       <c r="AA5">
-        <v>0.007556343267930988</v>
+        <v>0.007562330893504463</v>
       </c>
       <c r="AB5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="AC5">
         <v>0.1466277815139906</v>
       </c>
       <c r="AD5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="AE5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="AF5">
         <v>0.1466277815139906</v>
       </c>
       <c r="AG5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="AH5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="AI5">
         <v>0.1466277815139906</v>
       </c>
       <c r="AJ5">
-        <v>0.009772820099179347</v>
+        <v>0.009512934771852246</v>
       </c>
       <c r="AK5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
       <c r="AL5">
         <v>0.1466277815139906</v>
       </c>
       <c r="AM5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
       <c r="AN5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
       <c r="AO5">
         <v>0.1466277815139906</v>
       </c>
       <c r="AP5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
       <c r="AQ5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="AR5">
         <v>0.1350304976632463</v>
       </c>
       <c r="AS5">
-        <v>0.0001849315068493151</v>
+        <v>0.001845113746186173</v>
       </c>
       <c r="AT5">
-        <v>0.00979770166486711</v>
+        <v>0.009053469553305216</v>
       </c>
       <c r="AU5">
         <v>0.1466277815139906</v>
       </c>
       <c r="AV5">
-        <v>0.00979770166486711</v>
+        <v>0.009053469553305216</v>
       </c>
       <c r="AW5">
-        <v>0.00979770166486711</v>
+        <v>0.009053469553305216</v>
       </c>
       <c r="AX5">
         <v>0.1466277815139906</v>
       </c>
       <c r="AY5">
-        <v>0.00979770166486711</v>
+        <v>0.009053469553305216</v>
       </c>
       <c r="AZ5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
       <c r="BA5">
         <v>0.1466277815139906</v>
       </c>
       <c r="BB5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
       <c r="BC5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
       <c r="BD5">
         <v>0.1466277815139906</v>
       </c>
       <c r="BE5">
-        <v>0.006809095485975105</v>
+        <v>0.006519731710468045</v>
       </c>
     </row>
     <row r="6" spans="1:57">
       <c r="A6">
-        <v>0.007518590801563001</v>
+        <v>0.007484115743621659</v>
       </c>
       <c r="B6">
         <v>0.1228699079585041</v>
       </c>
       <c r="C6">
-        <v>0.007518590801563001</v>
+        <v>0.007484115743621659</v>
       </c>
       <c r="D6">
-        <v>0.007518590801563001</v>
+        <v>0.007484115743621659</v>
       </c>
       <c r="E6">
         <v>0.1228699079585041</v>
       </c>
       <c r="F6">
-        <v>0.007518590801563001</v>
+        <v>0.007484115743621659</v>
       </c>
       <c r="G6">
         <v>0.0001849315068493151</v>
@@ -1240,13 +1240,13 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="J6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="K6">
         <v>0.1228699079585041</v>
       </c>
       <c r="L6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="M6">
         <v>0.0001849315068493151</v>
@@ -1285,58 +1285,58 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="Y6">
-        <v>0.006493611973198488</v>
+        <v>0.006571276703108419</v>
       </c>
       <c r="Z6">
         <v>0.1389076671321314</v>
       </c>
       <c r="AA6">
-        <v>0.006493611973198488</v>
+        <v>0.006571276703108419</v>
       </c>
       <c r="AB6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="AC6">
         <v>0.1228699079585041</v>
       </c>
       <c r="AD6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="AE6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="AF6">
         <v>0.1228699079585041</v>
       </c>
       <c r="AG6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="AH6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="AI6">
         <v>0.1228699079585041</v>
       </c>
       <c r="AJ6">
-        <v>0.007948316857439757</v>
+        <v>0.008351383692089775</v>
       </c>
       <c r="AK6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
       <c r="AL6">
         <v>0.1228699079585041</v>
       </c>
       <c r="AM6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
       <c r="AN6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
       <c r="AO6">
         <v>0.1228699079585041</v>
       </c>
       <c r="AP6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
       <c r="AQ6">
         <v>0.0001849315068493151</v>
@@ -1348,60 +1348,60 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="AT6">
-        <v>0.00809155887606534</v>
+        <v>0.008640473008245815</v>
       </c>
       <c r="AU6">
         <v>0.1228699079585041</v>
       </c>
       <c r="AV6">
-        <v>0.00809155887606534</v>
+        <v>0.008640473008245815</v>
       </c>
       <c r="AW6">
-        <v>0.00809155887606534</v>
+        <v>0.008640473008245815</v>
       </c>
       <c r="AX6">
         <v>0.1228699079585041</v>
       </c>
       <c r="AY6">
-        <v>0.00809155887606534</v>
+        <v>0.008640473008245815</v>
       </c>
       <c r="AZ6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
       <c r="BA6">
         <v>0.1228699079585041</v>
       </c>
       <c r="BB6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
       <c r="BC6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
       <c r="BD6">
         <v>0.1228699079585041</v>
       </c>
       <c r="BE6">
-        <v>0.006738542437890538</v>
+        <v>0.006204235323275257</v>
       </c>
     </row>
     <row r="7" spans="1:57">
       <c r="A7">
-        <v>0.004628616415328602</v>
+        <v>0.005554174131977045</v>
       </c>
       <c r="B7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C7">
-        <v>0.004628616415328602</v>
+        <v>0.005554174131977045</v>
       </c>
       <c r="D7">
-        <v>0.004628616415328602</v>
+        <v>0.005554174131977045</v>
       </c>
       <c r="E7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F7">
-        <v>0.004628616415328602</v>
+        <v>0.005554174131977045</v>
       </c>
       <c r="G7">
         <v>0.0001849315068493151</v>
@@ -1413,13 +1413,13 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="J7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="K7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="M7">
         <v>0.0001849315068493151</v>
@@ -1458,58 +1458,58 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="Y7">
-        <v>0.003220273384676921</v>
+        <v>0.003855230184347192</v>
       </c>
       <c r="Z7">
         <v>0.02654706859680691</v>
       </c>
       <c r="AA7">
-        <v>0.003220273384676921</v>
+        <v>0.003855230184347192</v>
       </c>
       <c r="AB7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="AC7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="AE7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="AF7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="AH7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="AI7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ7">
-        <v>0.004890286753711106</v>
+        <v>0.00531149095487475</v>
       </c>
       <c r="AK7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
       <c r="AL7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AM7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
       <c r="AN7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
       <c r="AO7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AP7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
       <c r="AQ7">
         <v>0.0001849315068493151</v>
@@ -1521,60 +1521,60 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="AT7">
-        <v>0.004977510199838607</v>
+        <v>0.005230596562507317</v>
       </c>
       <c r="AU7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV7">
-        <v>0.004977510199838607</v>
+        <v>0.005230596562507317</v>
       </c>
       <c r="AW7">
-        <v>0.004977510199838607</v>
+        <v>0.005230596562507317</v>
       </c>
       <c r="AX7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY7">
-        <v>0.004977510199838607</v>
+        <v>0.005230596562507317</v>
       </c>
       <c r="AZ7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
       <c r="BA7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BB7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
       <c r="BC7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
       <c r="BD7">
         <v>0.0001146235521235521</v>
       </c>
       <c r="BE7">
-        <v>0.001397917585522355</v>
+        <v>0.002777857982041016</v>
       </c>
     </row>
     <row r="8" spans="1:57">
       <c r="A8">
-        <v>0.000235106866757617</v>
+        <v>0.0007570548562017816</v>
       </c>
       <c r="B8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="C8">
-        <v>0.000235106866757617</v>
+        <v>0.0007570548562017816</v>
       </c>
       <c r="D8">
-        <v>0.000235106866757617</v>
+        <v>0.0007570548562017816</v>
       </c>
       <c r="E8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="F8">
-        <v>0.000235106866757617</v>
+        <v>0.0007570548562017816</v>
       </c>
       <c r="G8">
         <v>0.0001849315068493151</v>
@@ -1586,13 +1586,13 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="J8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="K8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="L8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="M8">
         <v>0.0001849315068493151</v>
@@ -1631,40 +1631,40 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="Y8">
-        <v>0.0003698042370484211</v>
+        <v>0.0007914360112777169</v>
       </c>
       <c r="Z8">
         <v>0.0148211156366126</v>
       </c>
       <c r="AA8">
-        <v>0.0003698042370484211</v>
+        <v>0.0007914360112777169</v>
       </c>
       <c r="AB8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="AC8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AD8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="AE8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="AF8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AG8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="AH8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="AI8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AJ8">
-        <v>0.0005185127353389364</v>
+        <v>0.001256368340240204</v>
       </c>
       <c r="AK8">
         <v>0.0001648236055669436</v>
@@ -1694,22 +1694,22 @@
         <v>0.0001849315068493151</v>
       </c>
       <c r="AT8">
-        <v>0.0006129813581993762</v>
+        <v>0.001422806168253012</v>
       </c>
       <c r="AU8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AV8">
-        <v>0.0006129813581993762</v>
+        <v>0.001422806168253012</v>
       </c>
       <c r="AW8">
-        <v>0.0006129813581993762</v>
+        <v>0.001422806168253012</v>
       </c>
       <c r="AX8">
         <v>0.0001146235521235521</v>
       </c>
       <c r="AY8">
-        <v>0.0006129813581993762</v>
+        <v>0.001422806168253012</v>
       </c>
       <c r="AZ8">
         <v>0.0001648236055669436</v>

</xml_diff>